<commit_message>
Turns every 'Group' into a 'BrokerageNote' when all 'Lines' in the 'Group' have the same 'TradingDate' and 'BrokerageNote'.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA9AC50-4F36-4043-8F7C-E6CA1CB1DF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D8F8F3-5FE9-4F5B-8EDC-C654FC2CD3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" activeTab="1" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
+    <sheet name="2" sheetId="7" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,9 +36,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+  <si>
+    <t>BBAS3</t>
+  </si>
+  <si>
+    <t>PETR4</t>
+  </si>
   <si>
     <t>GGBR4</t>
+  </si>
+  <si>
+    <t>ITSA4</t>
+  </si>
+  <si>
+    <t>VALE5</t>
   </si>
   <si>
     <t>Total</t>
@@ -448,7 +461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB4B250-0980-498E-BE81-900F19EFBBA1}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -490,40 +503,40 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="AC1" s="5"/>
     </row>
@@ -535,7 +548,7 @@
         <v>1662</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1">
         <v>100</v>
@@ -568,6 +581,645 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
+  <dimension ref="A1:AC14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="1"/>
+    <col min="18" max="18" width="10.28515625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="4"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="5"/>
+    </row>
+    <row r="2" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>100</v>
+      </c>
+      <c r="E2" s="2">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="2">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="2">
+        <f>0.74*(F2/SUM(F2:F4))</f>
+        <v>0.12177215189873417</v>
+      </c>
+      <c r="H2" s="2">
+        <f>2.51*(F2/SUM(F2:F4))</f>
+        <v>0.41303797468354425</v>
+      </c>
+      <c r="I2" s="2">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2">
+        <f>F2+G2+H2+I2</f>
+        <v>1550.5248101265822</v>
+      </c>
+      <c r="M2" s="4"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+    </row>
+    <row r="3" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>39757</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1662</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>200</v>
+      </c>
+      <c r="E3" s="2">
+        <v>25.19</v>
+      </c>
+      <c r="F3" s="2">
+        <f>D3*E3</f>
+        <v>5038</v>
+      </c>
+      <c r="G3" s="2">
+        <f>0.74*(F3/SUM(F2:F4))</f>
+        <v>0.39992705428019737</v>
+      </c>
+      <c r="H3" s="2">
+        <f>2.51*(F3/SUM(F2:F4))</f>
+        <v>1.3565093327612099</v>
+      </c>
+      <c r="I3" s="2">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2">
+        <f>F3+G3+H3+I3</f>
+        <v>5055.7464363870413</v>
+      </c>
+      <c r="M3" s="4"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+    </row>
+    <row r="4" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1662</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>100</v>
+      </c>
+      <c r="E4" s="2">
+        <v>27.5</v>
+      </c>
+      <c r="F4" s="2">
+        <f>D4*E4</f>
+        <v>2750</v>
+      </c>
+      <c r="G4" s="2">
+        <f>0.74*(F4/SUM(F2:F4))</f>
+        <v>0.21830079382106843</v>
+      </c>
+      <c r="H4" s="2">
+        <f>2.51*(F4/SUM(F2:F4))</f>
+        <v>0.74045269255524548</v>
+      </c>
+      <c r="I4" s="2">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2">
+        <f>F4+G4+H4+I4</f>
+        <v>2766.9487534863761</v>
+      </c>
+      <c r="M4" s="4"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+    </row>
+    <row r="5" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2">
+        <f>SUM(F2:F4)</f>
+        <v>9322</v>
+      </c>
+      <c r="G5" s="2">
+        <f>SUM(G2:G4)</f>
+        <v>0.74</v>
+      </c>
+      <c r="H5" s="2">
+        <f>SUM(H2:H4)</f>
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="I5" s="2">
+        <f>SUM(I2:I4)</f>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="2">
+        <f>SUM(J2:J4)</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2">
+        <f>SUM(L2:L4)</f>
+        <v>9373.2199999999993</v>
+      </c>
+      <c r="M5" s="4"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+    </row>
+    <row r="6" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="4"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+    </row>
+    <row r="7" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>39758</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1344</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>100</v>
+      </c>
+      <c r="E7" s="2">
+        <v>15.2</v>
+      </c>
+      <c r="F7" s="2">
+        <f>D7*E7</f>
+        <v>1520</v>
+      </c>
+      <c r="G7" s="2">
+        <f>0.2*(F7/SUM(F7:F8))</f>
+        <v>0.13280908693752733</v>
+      </c>
+      <c r="H7" s="2">
+        <f>0.69*(F7/SUM(F7:F8))</f>
+        <v>0.45819134993446919</v>
+      </c>
+      <c r="I7" s="2">
+        <v>15.99</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2">
+        <f>F7+G7+H7+I7</f>
+        <v>1536.5810004368718</v>
+      </c>
+      <c r="M7" s="4"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+    </row>
+    <row r="8" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>39758</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1344</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>100</v>
+      </c>
+      <c r="E8" s="2">
+        <v>7.69</v>
+      </c>
+      <c r="F8" s="2">
+        <f>D8*E8</f>
+        <v>769</v>
+      </c>
+      <c r="G8" s="2">
+        <f>0.2*(F8/SUM(F7:F8))</f>
+        <v>6.7190913062472699E-2</v>
+      </c>
+      <c r="H8" s="2">
+        <f>0.69*(F8/SUM(F7:F8))</f>
+        <v>0.23180865006553075</v>
+      </c>
+      <c r="I8" s="2">
+        <v>15.99</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2">
+        <f>F8+G8+H8+I8</f>
+        <v>785.28899956312807</v>
+      </c>
+      <c r="M8" s="4"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+    </row>
+    <row r="9" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2">
+        <f>SUM(F7:F8)</f>
+        <v>2289</v>
+      </c>
+      <c r="G9" s="2">
+        <f>SUM(G7:G8)</f>
+        <v>0.2</v>
+      </c>
+      <c r="H9" s="2">
+        <f>SUM(H7:H8)</f>
+        <v>0.69</v>
+      </c>
+      <c r="I9" s="2">
+        <f>SUM(I7:I8)</f>
+        <v>31.98</v>
+      </c>
+      <c r="J9" s="2">
+        <f>SUM(J7:J8)</f>
+        <v>1.6</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2">
+        <f>SUM(L7:L8)</f>
+        <v>2321.87</v>
+      </c>
+      <c r="M9" s="4"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+    </row>
+    <row r="10" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="4"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+    </row>
+    <row r="11" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>39849</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1319</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1">
+        <v>100</v>
+      </c>
+      <c r="E11" s="2">
+        <v>31.5</v>
+      </c>
+      <c r="F11" s="2">
+        <f>D11*E11</f>
+        <v>3150</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="I11" s="2">
+        <v>15.99</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <f>F11-G11-H11-I11-K11</f>
+        <v>3132.9100000000003</v>
+      </c>
+      <c r="M11" s="4"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+    </row>
+    <row r="12" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="4"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+    </row>
+    <row r="13" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>39853</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1362</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>100</v>
+      </c>
+      <c r="E13" s="2">
+        <v>17.7</v>
+      </c>
+      <c r="F13" s="2">
+        <f>D13*E13</f>
+        <v>1770</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="I13" s="2">
+        <v>15.99</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <f>F13-G13-H13-I13-K13</f>
+        <v>1753.3999999999999</v>
+      </c>
+      <c r="M13" s="4"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+    </row>
+    <row r="14" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="4"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Turns every 'SummaryLine' into a 'FinancialSummary'.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D8F8F3-5FE9-4F5B-8EDC-C654FC2CD3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90CF90B-D0F6-4572-91BA-B082269F366C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" activeTab="1" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" activeTab="2" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
     <sheet name="2" sheetId="7" r:id="rId2"/>
+    <sheet name="3" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="17">
   <si>
     <t>BBAS3</t>
   </si>
@@ -592,7 +593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
@@ -1225,4 +1226,351 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
+  <dimension ref="A1:AC11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="1"/>
+    <col min="18" max="18" width="10.28515625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC1" s="5"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>100</v>
+      </c>
+      <c r="E2" s="2">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="2">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="2">
+        <f>0.74*(F2/SUM(F2:F4))</f>
+        <v>0.12177215189873417</v>
+      </c>
+      <c r="H2" s="2">
+        <f>2.51*(F2/SUM(F2:F4))</f>
+        <v>0.41303797468354425</v>
+      </c>
+      <c r="I2" s="2">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L2" s="2">
+        <f>F2+G2+H2+I2</f>
+        <v>1550.5248101265822</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>39757</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1662</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>200</v>
+      </c>
+      <c r="E3" s="2">
+        <v>25.19</v>
+      </c>
+      <c r="F3" s="2">
+        <f>D3*E3</f>
+        <v>5038</v>
+      </c>
+      <c r="G3" s="2">
+        <f>0.74*(F3/SUM(F2:F4))</f>
+        <v>0.39992705428019737</v>
+      </c>
+      <c r="H3" s="2">
+        <f>2.51*(F3/SUM(F2:F4))</f>
+        <v>1.3565093327612099</v>
+      </c>
+      <c r="I3" s="2">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L3" s="2">
+        <f>F3+G3+H3+I3</f>
+        <v>5055.7464363870413</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1662</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>100</v>
+      </c>
+      <c r="E4" s="2">
+        <v>27.5</v>
+      </c>
+      <c r="F4" s="2">
+        <f>D4*E4</f>
+        <v>2750</v>
+      </c>
+      <c r="G4" s="2">
+        <f>0.74*(F4/SUM(F2:F4))</f>
+        <v>0.21830079382106843</v>
+      </c>
+      <c r="H4" s="2">
+        <f>2.51*(F4/SUM(F2:F4))</f>
+        <v>0.74045269255524548</v>
+      </c>
+      <c r="I4" s="2">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L4" s="2">
+        <f>F4+G4+H4+I4</f>
+        <v>2766.9487534863761</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="F5" s="2">
+        <f>SUM(F2:F4)</f>
+        <v>9322</v>
+      </c>
+      <c r="G5" s="2">
+        <f>SUM(G2:G4)</f>
+        <v>0.74</v>
+      </c>
+      <c r="H5" s="2">
+        <f>SUM(H2:H4)</f>
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="I5" s="2">
+        <f>SUM(I2:I4)</f>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="2">
+        <f>SUM(J2:J4)</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="L5" s="2">
+        <f>SUM(L2:L4)</f>
+        <v>9373.2199999999993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>39758</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1344</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>100</v>
+      </c>
+      <c r="E7" s="2">
+        <v>15.2</v>
+      </c>
+      <c r="F7" s="2">
+        <f>D7*E7</f>
+        <v>1520</v>
+      </c>
+      <c r="G7" s="2">
+        <f>0.2*(F7/SUM(F7:F8))</f>
+        <v>0.13280908693752733</v>
+      </c>
+      <c r="H7" s="2">
+        <f>0.69*(F7/SUM(F7:F8))</f>
+        <v>0.45819134993446919</v>
+      </c>
+      <c r="I7" s="2">
+        <v>15.99</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L7" s="2">
+        <f>F7+G7+H7+I7</f>
+        <v>1536.5810004368718</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>39758</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1344</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>100</v>
+      </c>
+      <c r="E8" s="2">
+        <v>7.69</v>
+      </c>
+      <c r="F8" s="2">
+        <f>D8*E8</f>
+        <v>769</v>
+      </c>
+      <c r="G8" s="2">
+        <f>0.2*(F8/SUM(F7:F8))</f>
+        <v>6.7190913062472699E-2</v>
+      </c>
+      <c r="H8" s="2">
+        <f>0.69*(F8/SUM(F7:F8))</f>
+        <v>0.23180865006553075</v>
+      </c>
+      <c r="I8" s="2">
+        <v>15.99</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L8" s="2">
+        <f>F8+G8+H8+I8</f>
+        <v>785.28899956312807</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="F9" s="2">
+        <f>SUM(F7:F8)</f>
+        <v>2289</v>
+      </c>
+      <c r="G9" s="2">
+        <f>SUM(G7:G8)</f>
+        <v>0.2</v>
+      </c>
+      <c r="H9" s="2">
+        <f>SUM(H7:H8)</f>
+        <v>0.69</v>
+      </c>
+      <c r="I9" s="2">
+        <f>SUM(I7:I8)</f>
+        <v>31.98</v>
+      </c>
+      <c r="J9" s="2">
+        <f>SUM(J7:J8)</f>
+        <v>1.6</v>
+      </c>
+      <c r="L9" s="2">
+        <f>SUM(L7:L8)</f>
+        <v>2321.87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Generates a 'FinancialSummary', for 'Groups' of one 'Line', whose fields would replicate the corresponding ones from the one 'Line' in the 'Group'.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B45AB79-8EF1-48BA-9FF1-C80757E993AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3080159E-835A-42BD-8773-15ECB064320F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" activeTab="3" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" activeTab="4" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
     <sheet name="2" sheetId="7" r:id="rId2"/>
     <sheet name="3" sheetId="8" r:id="rId3"/>
     <sheet name="4" sheetId="9" r:id="rId4"/>
+    <sheet name="5" sheetId="10" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,8 +38,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Avell</author>
+  </authors>
+  <commentList>
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{6F3110C4-1405-4638-8B6C-6C5B4E20B248}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Avell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Encontrado no extrato</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K4" authorId="0" shapeId="0" xr:uid="{1C2F5EF2-608C-48D4-BF2E-277E20FC5F8D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Avell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Encontrado no extrato</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="22">
   <si>
     <t>BBAS3</t>
   </si>
@@ -55,6 +114,9 @@
     <t>VALE5</t>
   </si>
   <si>
+    <t>KLBN4</t>
+  </si>
+  <si>
     <t>MMXM3</t>
   </si>
   <si>
@@ -62,6 +124,9 @@
   </si>
   <si>
     <t>ARCZ6</t>
+  </si>
+  <si>
+    <t>VCPA4</t>
   </si>
   <si>
     <t>Total</t>
@@ -108,7 +173,7 @@
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +217,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -179,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -194,6 +272,7 @@
     <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -533,7 +612,7 @@
     <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="16" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
     <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="9.140625" style="12"/>
@@ -556,45 +635,45 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="F1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC1" s="17"/>
+      <c r="AC1" s="18"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="15">
         <v>39757</v>
       </c>
       <c r="B2" s="12">
@@ -633,7 +712,7 @@
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+      <c r="A3" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -664,7 +743,7 @@
     <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="16" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
     <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="9.140625" style="12"/>
@@ -687,42 +766,42 @@
   <sheetData>
     <row r="1" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="F1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="16"/>
+      <c r="M1" s="17"/>
       <c r="R1" s="13"/>
       <c r="S1" s="13"/>
       <c r="T1" s="13"/>
@@ -734,10 +813,10 @@
       <c r="Z1" s="13"/>
       <c r="AA1" s="13"/>
       <c r="AB1" s="13"/>
-      <c r="AC1" s="17"/>
+      <c r="AC1" s="18"/>
     </row>
     <row r="2" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="15">
         <v>39757</v>
       </c>
       <c r="B2" s="12">
@@ -775,7 +854,7 @@
         <f>F2+G2+H2+I2</f>
         <v>1550.5248101265822</v>
       </c>
-      <c r="M2" s="16"/>
+      <c r="M2" s="17"/>
       <c r="R2" s="13"/>
       <c r="S2" s="13"/>
       <c r="T2" s="13"/>
@@ -789,7 +868,7 @@
       <c r="AB2" s="13"/>
     </row>
     <row r="3" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="A3" s="15">
         <v>39757</v>
       </c>
       <c r="B3" s="12">
@@ -827,7 +906,7 @@
         <f>F3+G3+H3+I3</f>
         <v>5055.7464363870413</v>
       </c>
-      <c r="M3" s="16"/>
+      <c r="M3" s="17"/>
       <c r="R3" s="13"/>
       <c r="S3" s="13"/>
       <c r="T3" s="13"/>
@@ -841,7 +920,7 @@
       <c r="AB3" s="13"/>
     </row>
     <row r="4" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
+      <c r="A4" s="15">
         <v>39757</v>
       </c>
       <c r="B4" s="12">
@@ -879,7 +958,7 @@
         <f>F4+G4+H4+I4</f>
         <v>2766.9487534863761</v>
       </c>
-      <c r="M4" s="16"/>
+      <c r="M4" s="17"/>
       <c r="R4" s="13"/>
       <c r="S4" s="13"/>
       <c r="T4" s="13"/>
@@ -893,7 +972,7 @@
       <c r="AB4" s="13"/>
     </row>
     <row r="5" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
+      <c r="A5" s="15"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13">
         <f>SUM(F2:F4)</f>
@@ -920,7 +999,7 @@
         <f>SUM(L2:L4)</f>
         <v>9373.2199999999993</v>
       </c>
-      <c r="M5" s="16"/>
+      <c r="M5" s="17"/>
       <c r="R5" s="13"/>
       <c r="S5" s="13"/>
       <c r="T5" s="13"/>
@@ -934,7 +1013,7 @@
       <c r="AB5" s="13"/>
     </row>
     <row r="6" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="15"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -943,7 +1022,7 @@
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
-      <c r="M6" s="16"/>
+      <c r="M6" s="17"/>
       <c r="R6" s="13"/>
       <c r="S6" s="13"/>
       <c r="T6" s="13"/>
@@ -957,7 +1036,7 @@
       <c r="AB6" s="13"/>
     </row>
     <row r="7" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
+      <c r="A7" s="15">
         <v>39758</v>
       </c>
       <c r="B7" s="12">
@@ -995,7 +1074,7 @@
         <f>F7+G7+H7+I7</f>
         <v>1536.5810004368718</v>
       </c>
-      <c r="M7" s="16"/>
+      <c r="M7" s="17"/>
       <c r="R7" s="13"/>
       <c r="S7" s="13"/>
       <c r="T7" s="13"/>
@@ -1009,7 +1088,7 @@
       <c r="AB7" s="13"/>
     </row>
     <row r="8" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
+      <c r="A8" s="15">
         <v>39758</v>
       </c>
       <c r="B8" s="12">
@@ -1047,7 +1126,7 @@
         <f>F8+G8+H8+I8</f>
         <v>785.28899956312807</v>
       </c>
-      <c r="M8" s="16"/>
+      <c r="M8" s="17"/>
       <c r="R8" s="13"/>
       <c r="S8" s="13"/>
       <c r="T8" s="13"/>
@@ -1061,7 +1140,7 @@
       <c r="AB8" s="13"/>
     </row>
     <row r="9" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="15"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13">
         <f>SUM(F7:F8)</f>
@@ -1088,7 +1167,7 @@
         <f>SUM(L7:L8)</f>
         <v>2321.87</v>
       </c>
-      <c r="M9" s="16"/>
+      <c r="M9" s="17"/>
       <c r="R9" s="13"/>
       <c r="S9" s="13"/>
       <c r="T9" s="13"/>
@@ -1102,7 +1181,7 @@
       <c r="AB9" s="13"/>
     </row>
     <row r="10" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+      <c r="A10" s="15"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
@@ -1111,7 +1190,7 @@
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
-      <c r="M10" s="16"/>
+      <c r="M10" s="17"/>
       <c r="R10" s="13"/>
       <c r="S10" s="13"/>
       <c r="T10" s="13"/>
@@ -1125,7 +1204,7 @@
       <c r="AB10" s="13"/>
     </row>
     <row r="11" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
+      <c r="A11" s="15">
         <v>39849</v>
       </c>
       <c r="B11" s="12">
@@ -1163,7 +1242,7 @@
         <f>F11-G11-H11-I11-K11</f>
         <v>3132.9100000000003</v>
       </c>
-      <c r="M11" s="16"/>
+      <c r="M11" s="17"/>
       <c r="R11" s="13"/>
       <c r="S11" s="13"/>
       <c r="T11" s="13"/>
@@ -1177,7 +1256,7 @@
       <c r="AB11" s="13"/>
     </row>
     <row r="12" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="15"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
@@ -1186,7 +1265,7 @@
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
-      <c r="M12" s="16"/>
+      <c r="M12" s="17"/>
       <c r="R12" s="13"/>
       <c r="S12" s="13"/>
       <c r="T12" s="13"/>
@@ -1200,7 +1279,7 @@
       <c r="AB12" s="13"/>
     </row>
     <row r="13" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
+      <c r="A13" s="15">
         <v>39853</v>
       </c>
       <c r="B13" s="12">
@@ -1238,7 +1317,7 @@
         <f>F13-G13-H13-I13-K13</f>
         <v>1753.3999999999999</v>
       </c>
-      <c r="M13" s="16"/>
+      <c r="M13" s="17"/>
       <c r="R13" s="13"/>
       <c r="S13" s="13"/>
       <c r="T13" s="13"/>
@@ -1252,7 +1331,7 @@
       <c r="AB13" s="13"/>
     </row>
     <row r="14" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="15"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
@@ -1261,7 +1340,7 @@
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
-      <c r="M14" s="16"/>
+      <c r="M14" s="17"/>
       <c r="R14" s="13"/>
       <c r="S14" s="13"/>
       <c r="T14" s="13"/>
@@ -1303,7 +1382,7 @@
     <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="16" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
     <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="9.140625" style="12"/>
@@ -1326,45 +1405,45 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="F1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC1" s="17"/>
+      <c r="AC1" s="18"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="15">
         <v>39757</v>
       </c>
       <c r="B2" s="12">
@@ -1403,7 +1482,7 @@
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="A3" s="15">
         <v>39757</v>
       </c>
       <c r="B3" s="12">
@@ -1442,7 +1521,7 @@
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
+      <c r="A4" s="15">
         <v>39757</v>
       </c>
       <c r="B4" s="12">
@@ -1481,7 +1560,7 @@
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
+      <c r="A5" s="15"/>
       <c r="F5" s="13">
         <f>SUM(F2:F4)</f>
         <v>9322</v>
@@ -1508,10 +1587,10 @@
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="15"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
+      <c r="A7" s="15">
         <v>39758</v>
       </c>
       <c r="B7" s="12">
@@ -1550,7 +1629,7 @@
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
+      <c r="A8" s="15">
         <v>39758</v>
       </c>
       <c r="B8" s="12">
@@ -1589,7 +1668,7 @@
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="15"/>
       <c r="F9" s="13">
         <f>SUM(F7:F8)</f>
         <v>2289</v>
@@ -1616,10 +1695,10 @@
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+      <c r="A10" s="15"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+      <c r="A11" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1630,6 +1709,890 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="3">
+        <f>0.74*(F2/SUM(F2:F4))</f>
+        <v>0.12177215189873417</v>
+      </c>
+      <c r="H2" s="3">
+        <f>2.51*(F2/SUM(F2:F4))</f>
+        <v>0.41303797468354425</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2</f>
+        <v>1550.5248101265822</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>200</v>
+      </c>
+      <c r="E3" s="3">
+        <v>25.19</v>
+      </c>
+      <c r="F3" s="3">
+        <f>D3*E3</f>
+        <v>5038</v>
+      </c>
+      <c r="G3" s="3">
+        <f>0.74*(F3/SUM(F2:F4))</f>
+        <v>0.39992705428019737</v>
+      </c>
+      <c r="H3" s="3">
+        <f>2.51*(F3/SUM(F2:F4))</f>
+        <v>1.3565093327612099</v>
+      </c>
+      <c r="I3" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3</f>
+        <v>5055.7464363870413</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4">
+        <v>100</v>
+      </c>
+      <c r="E4" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F4" s="3">
+        <f>D4*E4</f>
+        <v>2750</v>
+      </c>
+      <c r="G4" s="3">
+        <f>0.74*(F4/SUM(F2:F4))</f>
+        <v>0.21830079382106843</v>
+      </c>
+      <c r="H4" s="3">
+        <f>2.51*(F4/SUM(F2:F4))</f>
+        <v>0.74045269255524548</v>
+      </c>
+      <c r="I4" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3">
+        <f>F4+G4+H4+I4</f>
+        <v>2766.9487534863761</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="7">
+        <f>SUM(F2:F4)</f>
+        <v>9322</v>
+      </c>
+      <c r="G5" s="7">
+        <f>SUM(G2:G4)</f>
+        <v>0.74</v>
+      </c>
+      <c r="H5" s="7">
+        <f>SUM(H2:H4)</f>
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="I5" s="7">
+        <f>SUM(I2:I4)</f>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="7">
+        <f>SUM(J2:J4)</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7">
+        <f>SUM(L2:L4)</f>
+        <v>9373.2199999999993</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+    </row>
+    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="6"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+    </row>
+    <row r="7" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>39758</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1344</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4">
+        <v>100</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2.68</v>
+      </c>
+      <c r="F7" s="3">
+        <f>D7*E7</f>
+        <v>268</v>
+      </c>
+      <c r="G7" s="3">
+        <f>0.2*(F7/SUM(F7:F9))</f>
+        <v>2.0962064919827925E-2</v>
+      </c>
+      <c r="H7" s="3">
+        <f>0.69*(F7/SUM(F7:F9))</f>
+        <v>7.2319123973406341E-2</v>
+      </c>
+      <c r="I7" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3">
+        <f>F7+G7+H7+I7</f>
+        <v>284.08328118889324</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+    </row>
+    <row r="8" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>39758</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1344</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>100</v>
+      </c>
+      <c r="E8" s="3">
+        <v>15.2</v>
+      </c>
+      <c r="F8" s="3">
+        <f>D8*E8</f>
+        <v>1520</v>
+      </c>
+      <c r="G8" s="3">
+        <f>0.2*(F8/SUM(F7:F9))</f>
+        <v>0.11888932342588972</v>
+      </c>
+      <c r="H8" s="3">
+        <f>0.69*(F8/SUM(F7:F9))</f>
+        <v>0.41016816581931947</v>
+      </c>
+      <c r="I8" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3">
+        <f>F8+G8+H8+I8</f>
+        <v>1536.5190574892454</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+    </row>
+    <row r="9" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>39758</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1344</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4">
+        <v>100</v>
+      </c>
+      <c r="E9" s="3">
+        <v>7.69</v>
+      </c>
+      <c r="F9" s="3">
+        <f>D9*E9</f>
+        <v>769</v>
+      </c>
+      <c r="G9" s="3">
+        <f>0.2*(F9/SUM(F7:F9))</f>
+        <v>6.0148611654282362E-2</v>
+      </c>
+      <c r="H9" s="3">
+        <f>0.69*(F9/SUM(F7:F9))</f>
+        <v>0.20751271020727413</v>
+      </c>
+      <c r="I9" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3">
+        <f>F9+G9+H9+I9</f>
+        <v>785.25766132186163</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+    </row>
+    <row r="10" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="7">
+        <f>SUM(F7:F9)</f>
+        <v>2557</v>
+      </c>
+      <c r="G10" s="7">
+        <f>SUM(G7:G9)</f>
+        <v>0.2</v>
+      </c>
+      <c r="H10" s="7">
+        <f>SUM(H7:H9)</f>
+        <v>0.69</v>
+      </c>
+      <c r="I10" s="7">
+        <f>SUM(I7:I9)</f>
+        <v>47.97</v>
+      </c>
+      <c r="J10" s="7">
+        <f>SUM(J7:J9)</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7">
+        <f>SUM(L7:L9)</f>
+        <v>2605.86</v>
+      </c>
+      <c r="M10" s="6"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+    </row>
+    <row r="11" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="6"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+    </row>
+    <row r="12" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B12" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="9">
+        <v>200</v>
+      </c>
+      <c r="E12" s="8">
+        <v>35.15</v>
+      </c>
+      <c r="F12" s="8">
+        <f>D12*E12</f>
+        <v>7030</v>
+      </c>
+      <c r="G12" s="8">
+        <f>1.16*(F12/SUM(F12:F14))</f>
+        <v>0.42000412031314377</v>
+      </c>
+      <c r="H12" s="8">
+        <f>5.53*(F12/SUM(F12:F14))</f>
+        <v>2.0022610218376595</v>
+      </c>
+      <c r="I12" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K12" s="8">
+        <v>0</v>
+      </c>
+      <c r="L12" s="8">
+        <f>F12-G12-H12-I12-K12</f>
+        <v>7011.5877348578497</v>
+      </c>
+      <c r="M12" s="6"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="8"/>
+    </row>
+    <row r="13" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B13" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="9">
+        <v>200</v>
+      </c>
+      <c r="E13" s="8">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="F13" s="8">
+        <f>D13*E13</f>
+        <v>6895.9999999999991</v>
+      </c>
+      <c r="G13" s="8">
+        <f>1.16*(F13/SUM(F12:F14))</f>
+        <v>0.41199835187474243</v>
+      </c>
+      <c r="H13" s="8">
+        <f>5.53*(F13/SUM(F12:F14))</f>
+        <v>1.964095591264936</v>
+      </c>
+      <c r="I13" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K13" s="8">
+        <v>0</v>
+      </c>
+      <c r="L13" s="8">
+        <f>F13-G13-H13-I13-K13</f>
+        <v>6877.6339060568598</v>
+      </c>
+      <c r="M13" s="6"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
+    </row>
+    <row r="14" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="9">
+        <v>200</v>
+      </c>
+      <c r="E14" s="8">
+        <v>27.45</v>
+      </c>
+      <c r="F14" s="8">
+        <f>D14*E14</f>
+        <v>5490</v>
+      </c>
+      <c r="G14" s="8">
+        <f>1.16*(F14/SUM(F12:F14))</f>
+        <v>0.32799752781211372</v>
+      </c>
+      <c r="H14" s="8">
+        <f>5.53*(F14/SUM(F12:F14))</f>
+        <v>1.5636433868974042</v>
+      </c>
+      <c r="I14" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J14" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K14" s="8">
+        <v>0</v>
+      </c>
+      <c r="L14" s="8">
+        <f>F14-G14-H14-I14-K14</f>
+        <v>5472.1183590852906</v>
+      </c>
+      <c r="M14" s="6"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
+    </row>
+    <row r="15" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="11">
+        <f>SUM(F12:F14)</f>
+        <v>19416</v>
+      </c>
+      <c r="G15" s="11">
+        <f>SUM(G12:G14)</f>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="H15" s="11">
+        <f>SUM(H12:H14)</f>
+        <v>5.5299999999999994</v>
+      </c>
+      <c r="I15" s="11">
+        <f>SUM(I12:I14)</f>
+        <v>47.97</v>
+      </c>
+      <c r="J15" s="11">
+        <f>SUM(J12:J14)</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11">
+        <f>SUM(L12:L14)</f>
+        <v>19361.34</v>
+      </c>
+      <c r="M15" s="6"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="8"/>
+      <c r="AA15" s="8"/>
+      <c r="AB15" s="8"/>
+    </row>
+    <row r="17" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>40158</v>
+      </c>
+      <c r="B17" s="9">
+        <v>1171</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="9">
+        <v>500</v>
+      </c>
+      <c r="E17" s="8">
+        <v>26.1</v>
+      </c>
+      <c r="F17" s="8">
+        <f>D17*E17</f>
+        <v>13050</v>
+      </c>
+      <c r="G17" s="8">
+        <f>1.51*(F17/SUM(F17:F18))</f>
+        <v>0.78289630512514907</v>
+      </c>
+      <c r="H17" s="8">
+        <f>7.17*(F17/SUM(F17:F18))</f>
+        <v>3.7174612634088202</v>
+      </c>
+      <c r="I17" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K17" s="8">
+        <f>1.25*(F17/SUM(F17:F18))</f>
+        <v>0.64809296781883197</v>
+      </c>
+      <c r="L17" s="8">
+        <f>F17-G17-H17-I17-K17</f>
+        <v>13028.861549463649</v>
+      </c>
+      <c r="M17" s="6"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="8"/>
+      <c r="AA17" s="8"/>
+      <c r="AB17" s="8"/>
+    </row>
+    <row r="18" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>40158</v>
+      </c>
+      <c r="B18" s="9">
+        <v>1171</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="9">
+        <v>1000</v>
+      </c>
+      <c r="E18" s="8">
+        <v>12.12</v>
+      </c>
+      <c r="F18" s="8">
+        <f>D18*E18</f>
+        <v>12120</v>
+      </c>
+      <c r="G18" s="8">
+        <f>1.51*(F18/SUM(F17:F18))</f>
+        <v>0.72710369487485105</v>
+      </c>
+      <c r="H18" s="8">
+        <f>7.17*(F18/SUM(F17:F18))</f>
+        <v>3.4525387365911802</v>
+      </c>
+      <c r="I18" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J18" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K18" s="8">
+        <f>1.25*(F18/SUM(F17:F18))</f>
+        <v>0.60190703218116803</v>
+      </c>
+      <c r="L18" s="8">
+        <f>F18-G18-H18-I18-K18</f>
+        <v>12099.228450536351</v>
+      </c>
+      <c r="M18" s="6"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+      <c r="Y18" s="8"/>
+      <c r="Z18" s="8"/>
+      <c r="AA18" s="8"/>
+      <c r="AB18" s="8"/>
+    </row>
+    <row r="19" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="11">
+        <f>SUM(F17:F18)</f>
+        <v>25170</v>
+      </c>
+      <c r="G19" s="11">
+        <f>SUM(G17:G18)</f>
+        <v>1.5100000000000002</v>
+      </c>
+      <c r="H19" s="11">
+        <f>SUM(H17:H18)</f>
+        <v>7.17</v>
+      </c>
+      <c r="I19" s="11">
+        <f>SUM(I17:I18)</f>
+        <v>31.98</v>
+      </c>
+      <c r="J19" s="11">
+        <f>SUM(J17:J18)</f>
+        <v>1.6</v>
+      </c>
+      <c r="K19" s="11">
+        <f>SUM(K17:K18)</f>
+        <v>1.25</v>
+      </c>
+      <c r="L19" s="11">
+        <f>SUM(L17:L18)</f>
+        <v>25128.09</v>
+      </c>
+      <c r="M19" s="6"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+      <c r="Y19" s="8"/>
+      <c r="Z19" s="8"/>
+      <c r="AA19" s="8"/>
+      <c r="AB19" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
+  <dimension ref="A1:AC6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1671,250 +2634,192 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>39959</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1430</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC1" s="15"/>
-    </row>
-    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4">
-        <v>100</v>
-      </c>
-      <c r="E2" s="3">
-        <v>15.34</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="D2" s="9">
+        <v>200</v>
+      </c>
+      <c r="E2" s="8">
+        <v>23.4</v>
+      </c>
+      <c r="F2" s="8">
         <f>D2*E2</f>
-        <v>1534</v>
-      </c>
-      <c r="G2" s="3">
-        <f>0.74*(F2/SUM(F2:F4))</f>
-        <v>0.12177215189873417</v>
-      </c>
-      <c r="H2" s="3">
-        <f>2.51*(F2/SUM(F2:F4))</f>
-        <v>0.41303797468354425</v>
-      </c>
-      <c r="I2" s="3">
+        <v>4680</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1.33</v>
+      </c>
+      <c r="I2" s="8">
         <v>15.99</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="8">
         <v>0.8</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2</f>
-        <v>1550.5248101265822</v>
+      <c r="K2" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="L2" s="8">
+        <f>F2-G2-H2-I2</f>
+        <v>4662.4000000000005</v>
       </c>
       <c r="M2" s="6"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-    </row>
-    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>39960</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1681</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D4" s="9">
         <v>200</v>
       </c>
-      <c r="E3" s="3">
-        <v>25.19</v>
-      </c>
-      <c r="F3" s="3">
-        <f>D3*E3</f>
-        <v>5038</v>
-      </c>
-      <c r="G3" s="3">
-        <f>0.74*(F3/SUM(F2:F4))</f>
-        <v>0.39992705428019737</v>
-      </c>
-      <c r="H3" s="3">
-        <f>2.51*(F3/SUM(F2:F4))</f>
-        <v>1.3565093327612099</v>
-      </c>
-      <c r="I3" s="3">
+      <c r="E4" s="8">
+        <v>34.04</v>
+      </c>
+      <c r="F4" s="8">
+        <f>D4*E4</f>
+        <v>6808</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="H4" s="8">
+        <v>1.94</v>
+      </c>
+      <c r="I4" s="8">
         <v>15.99</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J4" s="8">
         <v>0.8</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3</f>
-        <v>5055.7464363870413</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4">
-        <v>100</v>
-      </c>
-      <c r="E4" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F4" s="3">
-        <f>D4*E4</f>
-        <v>2750</v>
-      </c>
-      <c r="G4" s="3">
-        <f>0.74*(F4/SUM(F2:F4))</f>
-        <v>0.21830079382106843</v>
-      </c>
-      <c r="H4" s="3">
-        <f>2.51*(F4/SUM(F2:F4))</f>
-        <v>0.74045269255524548</v>
-      </c>
-      <c r="I4" s="3">
+      <c r="K4" s="8">
+        <v>0.34</v>
+      </c>
+      <c r="L4" s="8">
+        <f>F4-G4-H4-I4</f>
+        <v>6789.670000000001</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>39961</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1246</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E6" s="3">
+        <v>3.31</v>
+      </c>
+      <c r="F6" s="3">
+        <f>D6*E6</f>
+        <v>3310</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="I6" s="3">
         <v>15.99</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J6" s="3">
         <v>0.8</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3">
-        <f>F4+G4+H4+I4</f>
-        <v>2766.9487534863761</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="7">
-        <f>SUM(F2:F4)</f>
-        <v>9322</v>
-      </c>
-      <c r="G5" s="7">
-        <f>SUM(G2:G4)</f>
-        <v>0.74</v>
-      </c>
-      <c r="H5" s="7">
-        <f>SUM(H2:H4)</f>
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="I5" s="7">
-        <f>SUM(I2:I4)</f>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="7">
-        <f>SUM(J2:J4)</f>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7">
-        <f>SUM(L2:L4)</f>
-        <v>9373.2199999999993</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-    </row>
-    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3">
+        <f>F6+G6+H6+I6</f>
+        <v>3327.12</v>
+      </c>
       <c r="M6" s="6"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
@@ -1928,585 +2833,9 @@
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
     </row>
-    <row r="7" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="4">
-        <v>100</v>
-      </c>
-      <c r="E7" s="3">
-        <v>2.68</v>
-      </c>
-      <c r="F7" s="3">
-        <f>D7*E7</f>
-        <v>268</v>
-      </c>
-      <c r="G7" s="3">
-        <f>0.2*(F7/SUM(F7:F9))</f>
-        <v>2.0962064919827925E-2</v>
-      </c>
-      <c r="H7" s="3">
-        <f>0.69*(F7/SUM(F7:F9))</f>
-        <v>7.2319123973406341E-2</v>
-      </c>
-      <c r="I7" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3">
-        <f>F7+G7+H7+I7</f>
-        <v>284.08328118889324</v>
-      </c>
-      <c r="M7" s="6"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-    </row>
-    <row r="8" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>100</v>
-      </c>
-      <c r="E8" s="3">
-        <v>15.2</v>
-      </c>
-      <c r="F8" s="3">
-        <f>D8*E8</f>
-        <v>1520</v>
-      </c>
-      <c r="G8" s="3">
-        <f>0.2*(F8/SUM(F7:F9))</f>
-        <v>0.11888932342588972</v>
-      </c>
-      <c r="H8" s="3">
-        <f>0.69*(F8/SUM(F7:F9))</f>
-        <v>0.41016816581931947</v>
-      </c>
-      <c r="I8" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3">
-        <f>F8+G8+H8+I8</f>
-        <v>1536.5190574892454</v>
-      </c>
-      <c r="M8" s="6"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-    </row>
-    <row r="9" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B9" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="4">
-        <v>100</v>
-      </c>
-      <c r="E9" s="3">
-        <v>7.69</v>
-      </c>
-      <c r="F9" s="3">
-        <f>D9*E9</f>
-        <v>769</v>
-      </c>
-      <c r="G9" s="3">
-        <f>0.2*(F9/SUM(F7:F9))</f>
-        <v>6.0148611654282362E-2</v>
-      </c>
-      <c r="H9" s="3">
-        <f>0.69*(F9/SUM(F7:F9))</f>
-        <v>0.20751271020727413</v>
-      </c>
-      <c r="I9" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3">
-        <f>F9+G9+H9+I9</f>
-        <v>785.25766132186163</v>
-      </c>
-      <c r="M9" s="6"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-    </row>
-    <row r="10" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="7">
-        <f>SUM(F7:F9)</f>
-        <v>2557</v>
-      </c>
-      <c r="G10" s="7">
-        <f>SUM(G7:G9)</f>
-        <v>0.2</v>
-      </c>
-      <c r="H10" s="7">
-        <f>SUM(H7:H9)</f>
-        <v>0.69</v>
-      </c>
-      <c r="I10" s="7">
-        <f>SUM(I7:I9)</f>
-        <v>47.97</v>
-      </c>
-      <c r="J10" s="7">
-        <f>SUM(J7:J9)</f>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7">
-        <f>SUM(L7:L9)</f>
-        <v>2605.86</v>
-      </c>
-      <c r="M10" s="6"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
-      <c r="AB10" s="3"/>
-    </row>
-    <row r="11" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="6"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="3"/>
-      <c r="AB11" s="3"/>
-    </row>
-    <row r="12" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B12" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="9">
-        <v>200</v>
-      </c>
-      <c r="E12" s="8">
-        <v>35.15</v>
-      </c>
-      <c r="F12" s="8">
-        <f>D12*E12</f>
-        <v>7030</v>
-      </c>
-      <c r="G12" s="8">
-        <f>1.16*(F12/SUM(F12:F14))</f>
-        <v>0.42000412031314377</v>
-      </c>
-      <c r="H12" s="8">
-        <f>5.53*(F12/SUM(F12:F14))</f>
-        <v>2.0022610218376595</v>
-      </c>
-      <c r="I12" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J12" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K12" s="8">
-        <v>0</v>
-      </c>
-      <c r="L12" s="8">
-        <f>F12-G12-H12-I12-K12</f>
-        <v>7011.5877348578497</v>
-      </c>
-      <c r="M12" s="6"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="8"/>
-      <c r="X12" s="8"/>
-      <c r="Y12" s="8"/>
-      <c r="Z12" s="8"/>
-      <c r="AA12" s="8"/>
-      <c r="AB12" s="8"/>
-    </row>
-    <row r="13" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B13" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="9">
-        <v>200</v>
-      </c>
-      <c r="E13" s="8">
-        <v>34.479999999999997</v>
-      </c>
-      <c r="F13" s="8">
-        <f>D13*E13</f>
-        <v>6895.9999999999991</v>
-      </c>
-      <c r="G13" s="8">
-        <f>1.16*(F13/SUM(F12:F14))</f>
-        <v>0.41199835187474243</v>
-      </c>
-      <c r="H13" s="8">
-        <f>5.53*(F13/SUM(F12:F14))</f>
-        <v>1.964095591264936</v>
-      </c>
-      <c r="I13" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J13" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K13" s="8">
-        <v>0</v>
-      </c>
-      <c r="L13" s="8">
-        <f>F13-G13-H13-I13-K13</f>
-        <v>6877.6339060568598</v>
-      </c>
-      <c r="M13" s="6"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="8"/>
-      <c r="AA13" s="8"/>
-      <c r="AB13" s="8"/>
-    </row>
-    <row r="14" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B14" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="9">
-        <v>200</v>
-      </c>
-      <c r="E14" s="8">
-        <v>27.45</v>
-      </c>
-      <c r="F14" s="8">
-        <f>D14*E14</f>
-        <v>5490</v>
-      </c>
-      <c r="G14" s="8">
-        <f>1.16*(F14/SUM(F12:F14))</f>
-        <v>0.32799752781211372</v>
-      </c>
-      <c r="H14" s="8">
-        <f>5.53*(F14/SUM(F12:F14))</f>
-        <v>1.5636433868974042</v>
-      </c>
-      <c r="I14" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J14" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K14" s="8">
-        <v>0</v>
-      </c>
-      <c r="L14" s="8">
-        <f>F14-G14-H14-I14-K14</f>
-        <v>5472.1183590852906</v>
-      </c>
-      <c r="M14" s="6"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="8"/>
-      <c r="AA14" s="8"/>
-      <c r="AB14" s="8"/>
-    </row>
-    <row r="15" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="11">
-        <f>SUM(F12:F14)</f>
-        <v>19416</v>
-      </c>
-      <c r="G15" s="11">
-        <f>SUM(G12:G14)</f>
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="H15" s="11">
-        <f>SUM(H12:H14)</f>
-        <v>5.5299999999999994</v>
-      </c>
-      <c r="I15" s="11">
-        <f>SUM(I12:I14)</f>
-        <v>47.97</v>
-      </c>
-      <c r="J15" s="11">
-        <f>SUM(J12:J14)</f>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11">
-        <f>SUM(L12:L14)</f>
-        <v>19361.34</v>
-      </c>
-      <c r="M15" s="6"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="8"/>
-      <c r="Z15" s="8"/>
-      <c r="AA15" s="8"/>
-      <c r="AB15" s="8"/>
-    </row>
-    <row r="17" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
-        <v>40158</v>
-      </c>
-      <c r="B17" s="9">
-        <v>1171</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="9">
-        <v>500</v>
-      </c>
-      <c r="E17" s="8">
-        <v>26.1</v>
-      </c>
-      <c r="F17" s="8">
-        <f>D17*E17</f>
-        <v>13050</v>
-      </c>
-      <c r="G17" s="8">
-        <f>1.51*(F17/SUM(F17:F18))</f>
-        <v>0.78289630512514907</v>
-      </c>
-      <c r="H17" s="8">
-        <f>7.17*(F17/SUM(F17:F18))</f>
-        <v>3.7174612634088202</v>
-      </c>
-      <c r="I17" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J17" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K17" s="8">
-        <f>1.25*(F17/SUM(F17:F18))</f>
-        <v>0.64809296781883197</v>
-      </c>
-      <c r="L17" s="8">
-        <f>F17-G17-H17-I17-K17</f>
-        <v>13028.861549463649</v>
-      </c>
-      <c r="M17" s="6"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="8"/>
-      <c r="Z17" s="8"/>
-      <c r="AA17" s="8"/>
-      <c r="AB17" s="8"/>
-    </row>
-    <row r="18" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>40158</v>
-      </c>
-      <c r="B18" s="9">
-        <v>1171</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="9">
-        <v>1000</v>
-      </c>
-      <c r="E18" s="8">
-        <v>12.12</v>
-      </c>
-      <c r="F18" s="8">
-        <f>D18*E18</f>
-        <v>12120</v>
-      </c>
-      <c r="G18" s="8">
-        <f>1.51*(F18/SUM(F17:F18))</f>
-        <v>0.72710369487485105</v>
-      </c>
-      <c r="H18" s="8">
-        <f>7.17*(F18/SUM(F17:F18))</f>
-        <v>3.4525387365911802</v>
-      </c>
-      <c r="I18" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J18" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K18" s="8">
-        <f>1.25*(F18/SUM(F17:F18))</f>
-        <v>0.60190703218116803</v>
-      </c>
-      <c r="L18" s="8">
-        <f>F18-G18-H18-I18-K18</f>
-        <v>12099.228450536351</v>
-      </c>
-      <c r="M18" s="6"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="8"/>
-      <c r="X18" s="8"/>
-      <c r="Y18" s="8"/>
-      <c r="Z18" s="8"/>
-      <c r="AA18" s="8"/>
-      <c r="AB18" s="8"/>
-    </row>
-    <row r="19" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="11">
-        <f>SUM(F17:F18)</f>
-        <v>25170</v>
-      </c>
-      <c r="G19" s="11">
-        <f>SUM(G17:G18)</f>
-        <v>1.5100000000000002</v>
-      </c>
-      <c r="H19" s="11">
-        <f>SUM(H17:H18)</f>
-        <v>7.17</v>
-      </c>
-      <c r="I19" s="11">
-        <f>SUM(I17:I18)</f>
-        <v>31.98</v>
-      </c>
-      <c r="J19" s="11">
-        <f>SUM(J17:J18)</f>
-        <v>1.6</v>
-      </c>
-      <c r="K19" s="11">
-        <f>SUM(K17:K18)</f>
-        <v>1.25</v>
-      </c>
-      <c r="L19" s="11">
-        <f>SUM(L17:L18)</f>
-        <v>25128.09</v>
-      </c>
-      <c r="M19" s="6"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="8"/>
-      <c r="V19" s="8"/>
-      <c r="W19" s="8"/>
-      <c r="X19" s="8"/>
-      <c r="Y19" s="8"/>
-      <c r="Z19" s="8"/>
-      <c r="AA19" s="8"/>
-      <c r="AB19" s="8"/>
-    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fails when trying to create a 'BrokerageNotesWorksheetReader' from a 'Worksheet' whose 'BrokerageNotes' have different 'TradingDate's.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3080159E-835A-42BD-8773-15ECB064320F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2D926E-DB38-4E07-AA1B-13FBDEE9C6F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" activeTab="4" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" activeTab="1" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
-    <sheet name="2" sheetId="7" r:id="rId2"/>
-    <sheet name="3" sheetId="8" r:id="rId3"/>
-    <sheet name="4" sheetId="9" r:id="rId4"/>
-    <sheet name="5" sheetId="10" r:id="rId5"/>
+    <sheet name="GroupWithDifferentTradingDates" sheetId="11" r:id="rId2"/>
+    <sheet name="2" sheetId="7" r:id="rId3"/>
+    <sheet name="3" sheetId="8" r:id="rId4"/>
+    <sheet name="4" sheetId="9" r:id="rId5"/>
+    <sheet name="5" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -97,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="22">
   <si>
     <t>BBAS3</t>
   </si>
@@ -596,7 +597,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,13 +722,443 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03306DC6-EFFD-4226-8075-7FFC9D0F7B34}">
+  <dimension ref="A1:AC14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="12"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC1" s="18"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="12">
+        <v>100</v>
+      </c>
+      <c r="E2" s="13">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="13">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="13">
+        <f>0.74*(F2/SUM(F2:F4))</f>
+        <v>0.12177215189873417</v>
+      </c>
+      <c r="H2" s="13">
+        <f>2.51*(F2/SUM(F2:F4))</f>
+        <v>0.41303797468354425</v>
+      </c>
+      <c r="I2" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="L2" s="13">
+        <f>F2+G2+H2+I2</f>
+        <v>1550.5248101265822</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>39758</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1662</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12">
+        <v>200</v>
+      </c>
+      <c r="E3" s="13">
+        <v>25.19</v>
+      </c>
+      <c r="F3" s="13">
+        <f>D3*E3</f>
+        <v>5038</v>
+      </c>
+      <c r="G3" s="13">
+        <f>0.74*(F3/SUM(F2:F4))</f>
+        <v>0.39992705428019737</v>
+      </c>
+      <c r="H3" s="13">
+        <f>2.51*(F3/SUM(F2:F4))</f>
+        <v>1.3565093327612099</v>
+      </c>
+      <c r="I3" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="L3" s="13">
+        <f>F3+G3+H3+I3</f>
+        <v>5055.7464363870413</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="12">
+        <v>1662</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="12">
+        <v>100</v>
+      </c>
+      <c r="E4" s="13">
+        <v>27.5</v>
+      </c>
+      <c r="F4" s="13">
+        <f>D4*E4</f>
+        <v>2750</v>
+      </c>
+      <c r="G4" s="13">
+        <f>0.74*(F4/SUM(F2:F4))</f>
+        <v>0.21830079382106843</v>
+      </c>
+      <c r="H4" s="13">
+        <f>2.51*(F4/SUM(F2:F4))</f>
+        <v>0.74045269255524548</v>
+      </c>
+      <c r="I4" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="L4" s="13">
+        <f>F4+G4+H4+I4</f>
+        <v>2766.9487534863761</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="F5" s="13">
+        <f>SUM(F2:F4)</f>
+        <v>9322</v>
+      </c>
+      <c r="G5" s="13">
+        <f>SUM(G2:G4)</f>
+        <v>0.74</v>
+      </c>
+      <c r="H5" s="13">
+        <f>SUM(H2:H4)</f>
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="I5" s="13">
+        <f>SUM(I2:I4)</f>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="13">
+        <f>SUM(J2:J4)</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="L5" s="13">
+        <f>SUM(L2:L4)</f>
+        <v>9373.2199999999993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>39758</v>
+      </c>
+      <c r="B7" s="12">
+        <v>1344</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12">
+        <v>100</v>
+      </c>
+      <c r="E7" s="13">
+        <v>15.2</v>
+      </c>
+      <c r="F7" s="13">
+        <f>D7*E7</f>
+        <v>1520</v>
+      </c>
+      <c r="G7" s="13">
+        <f>0.2*(F7/SUM(F7:F8))</f>
+        <v>0.13280908693752733</v>
+      </c>
+      <c r="H7" s="13">
+        <f>0.69*(F7/SUM(F7:F8))</f>
+        <v>0.45819134993446919</v>
+      </c>
+      <c r="I7" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J7" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="L7" s="13">
+        <f>F7+G7+H7+I7</f>
+        <v>1536.5810004368718</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>39758</v>
+      </c>
+      <c r="B8" s="12">
+        <v>1344</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="12">
+        <v>100</v>
+      </c>
+      <c r="E8" s="13">
+        <v>7.69</v>
+      </c>
+      <c r="F8" s="13">
+        <f>D8*E8</f>
+        <v>769</v>
+      </c>
+      <c r="G8" s="13">
+        <f>0.2*(F8/SUM(F7:F8))</f>
+        <v>6.7190913062472699E-2</v>
+      </c>
+      <c r="H8" s="13">
+        <f>0.69*(F8/SUM(F7:F8))</f>
+        <v>0.23180865006553075</v>
+      </c>
+      <c r="I8" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J8" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="L8" s="13">
+        <f>F8+G8+H8+I8</f>
+        <v>785.28899956312807</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="F9" s="13">
+        <f>SUM(F7:F8)</f>
+        <v>2289</v>
+      </c>
+      <c r="G9" s="13">
+        <f>SUM(G7:G8)</f>
+        <v>0.2</v>
+      </c>
+      <c r="H9" s="13">
+        <f>SUM(H7:H8)</f>
+        <v>0.69</v>
+      </c>
+      <c r="I9" s="13">
+        <f>SUM(I7:I8)</f>
+        <v>31.98</v>
+      </c>
+      <c r="J9" s="13">
+        <f>SUM(J7:J8)</f>
+        <v>1.6</v>
+      </c>
+      <c r="L9" s="13">
+        <f>SUM(L7:L8)</f>
+        <v>2321.87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>39849</v>
+      </c>
+      <c r="B11" s="12">
+        <v>1319</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="12">
+        <v>100</v>
+      </c>
+      <c r="E11" s="13">
+        <v>31.5</v>
+      </c>
+      <c r="F11" s="13">
+        <f>D11*E11</f>
+        <v>3150</v>
+      </c>
+      <c r="G11" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="H11" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="I11" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J11" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="K11" s="13">
+        <v>0</v>
+      </c>
+      <c r="L11" s="13">
+        <f>F11-G11-H11-I11-K11</f>
+        <v>3132.9100000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>39853</v>
+      </c>
+      <c r="B13" s="12">
+        <v>1362</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="12">
+        <v>100</v>
+      </c>
+      <c r="E13" s="13">
+        <v>17.7</v>
+      </c>
+      <c r="F13" s="13">
+        <f>D13*E13</f>
+        <v>1770</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H13" s="13">
+        <v>0.47</v>
+      </c>
+      <c r="I13" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J13" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="K13" s="13">
+        <v>0</v>
+      </c>
+      <c r="L13" s="13">
+        <f>F13-G13-H13-I13-K13</f>
+        <v>1753.3999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1359,7 +1790,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
@@ -1706,7 +2137,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
@@ -2590,11 +3021,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Fails when trying to create a 'BrokerageNotesWorksheetReader' from a 'Worksheet' whose 'BrokerageNotes' have different 'NoteNumber's.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2D926E-DB38-4E07-AA1B-13FBDEE9C6F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6181E28C-F4CE-46AF-B2B0-C0E179EF7AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" activeTab="1" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" firstSheet="2" activeTab="2" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
     <sheet name="GroupWithDifferentTradingDates" sheetId="11" r:id="rId2"/>
-    <sheet name="2" sheetId="7" r:id="rId3"/>
-    <sheet name="3" sheetId="8" r:id="rId4"/>
-    <sheet name="4" sheetId="9" r:id="rId5"/>
-    <sheet name="5" sheetId="10" r:id="rId6"/>
+    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId3"/>
+    <sheet name="2" sheetId="7" r:id="rId4"/>
+    <sheet name="3" sheetId="8" r:id="rId5"/>
+    <sheet name="4" sheetId="9" r:id="rId6"/>
+    <sheet name="5" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -98,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="22">
   <si>
     <t>BBAS3</t>
   </si>
@@ -172,7 +173,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -275,9 +276,9 @@
     <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,7 +726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03306DC6-EFFD-4226-8075-7FFC9D0F7B34}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1152,6 +1153,436 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
+  <dimension ref="A1:AC14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="12"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC1" s="18"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="12">
+        <v>100</v>
+      </c>
+      <c r="E2" s="13">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="13">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="13">
+        <f>0.74*(F2/SUM(F2:F4))</f>
+        <v>0.12177215189873417</v>
+      </c>
+      <c r="H2" s="13">
+        <f>2.51*(F2/SUM(F2:F4))</f>
+        <v>0.41303797468354425</v>
+      </c>
+      <c r="I2" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="L2" s="13">
+        <f>F2+G2+H2+I2</f>
+        <v>1550.5248101265822</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>39757</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1663</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12">
+        <v>200</v>
+      </c>
+      <c r="E3" s="13">
+        <v>25.19</v>
+      </c>
+      <c r="F3" s="13">
+        <f>D3*E3</f>
+        <v>5038</v>
+      </c>
+      <c r="G3" s="13">
+        <f>0.74*(F3/SUM(F2:F4))</f>
+        <v>0.39992705428019737</v>
+      </c>
+      <c r="H3" s="13">
+        <f>2.51*(F3/SUM(F2:F4))</f>
+        <v>1.3565093327612099</v>
+      </c>
+      <c r="I3" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="L3" s="13">
+        <f>F3+G3+H3+I3</f>
+        <v>5055.7464363870413</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="12">
+        <v>1662</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="12">
+        <v>100</v>
+      </c>
+      <c r="E4" s="13">
+        <v>27.5</v>
+      </c>
+      <c r="F4" s="13">
+        <f>D4*E4</f>
+        <v>2750</v>
+      </c>
+      <c r="G4" s="13">
+        <f>0.74*(F4/SUM(F2:F4))</f>
+        <v>0.21830079382106843</v>
+      </c>
+      <c r="H4" s="13">
+        <f>2.51*(F4/SUM(F2:F4))</f>
+        <v>0.74045269255524548</v>
+      </c>
+      <c r="I4" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="L4" s="13">
+        <f>F4+G4+H4+I4</f>
+        <v>2766.9487534863761</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="F5" s="13">
+        <f>SUM(F2:F4)</f>
+        <v>9322</v>
+      </c>
+      <c r="G5" s="13">
+        <f>SUM(G2:G4)</f>
+        <v>0.74</v>
+      </c>
+      <c r="H5" s="13">
+        <f>SUM(H2:H4)</f>
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="I5" s="13">
+        <f>SUM(I2:I4)</f>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="13">
+        <f>SUM(J2:J4)</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="L5" s="13">
+        <f>SUM(L2:L4)</f>
+        <v>9373.2199999999993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>39758</v>
+      </c>
+      <c r="B7" s="12">
+        <v>1344</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12">
+        <v>100</v>
+      </c>
+      <c r="E7" s="13">
+        <v>15.2</v>
+      </c>
+      <c r="F7" s="13">
+        <f>D7*E7</f>
+        <v>1520</v>
+      </c>
+      <c r="G7" s="13">
+        <f>0.2*(F7/SUM(F7:F8))</f>
+        <v>0.13280908693752733</v>
+      </c>
+      <c r="H7" s="13">
+        <f>0.69*(F7/SUM(F7:F8))</f>
+        <v>0.45819134993446919</v>
+      </c>
+      <c r="I7" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J7" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="L7" s="13">
+        <f>F7+G7+H7+I7</f>
+        <v>1536.5810004368718</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>39758</v>
+      </c>
+      <c r="B8" s="12">
+        <v>1344</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="12">
+        <v>100</v>
+      </c>
+      <c r="E8" s="13">
+        <v>7.69</v>
+      </c>
+      <c r="F8" s="13">
+        <f>D8*E8</f>
+        <v>769</v>
+      </c>
+      <c r="G8" s="13">
+        <f>0.2*(F8/SUM(F7:F8))</f>
+        <v>6.7190913062472699E-2</v>
+      </c>
+      <c r="H8" s="13">
+        <f>0.69*(F8/SUM(F7:F8))</f>
+        <v>0.23180865006553075</v>
+      </c>
+      <c r="I8" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J8" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="L8" s="13">
+        <f>F8+G8+H8+I8</f>
+        <v>785.28899956312807</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="F9" s="13">
+        <f>SUM(F7:F8)</f>
+        <v>2289</v>
+      </c>
+      <c r="G9" s="13">
+        <f>SUM(G7:G8)</f>
+        <v>0.2</v>
+      </c>
+      <c r="H9" s="13">
+        <f>SUM(H7:H8)</f>
+        <v>0.69</v>
+      </c>
+      <c r="I9" s="13">
+        <f>SUM(I7:I8)</f>
+        <v>31.98</v>
+      </c>
+      <c r="J9" s="13">
+        <f>SUM(J7:J8)</f>
+        <v>1.6</v>
+      </c>
+      <c r="L9" s="13">
+        <f>SUM(L7:L8)</f>
+        <v>2321.87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>39849</v>
+      </c>
+      <c r="B11" s="12">
+        <v>1319</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="12">
+        <v>100</v>
+      </c>
+      <c r="E11" s="13">
+        <v>31.5</v>
+      </c>
+      <c r="F11" s="13">
+        <f>D11*E11</f>
+        <v>3150</v>
+      </c>
+      <c r="G11" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="H11" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="I11" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J11" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="K11" s="13">
+        <v>0</v>
+      </c>
+      <c r="L11" s="13">
+        <f>F11-G11-H11-I11-K11</f>
+        <v>3132.9100000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>39853</v>
+      </c>
+      <c r="B13" s="12">
+        <v>1362</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="12">
+        <v>100</v>
+      </c>
+      <c r="E13" s="13">
+        <v>17.7</v>
+      </c>
+      <c r="F13" s="13">
+        <f>D13*E13</f>
+        <v>1770</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H13" s="13">
+        <v>0.47</v>
+      </c>
+      <c r="I13" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J13" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="K13" s="13">
+        <v>0</v>
+      </c>
+      <c r="L13" s="13">
+        <f>F13-G13-H13-I13-K13</f>
+        <v>1753.3999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -1195,7 +1626,7 @@
     <col min="32" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>21</v>
       </c>
@@ -1232,21 +1663,9 @@
       <c r="L1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="17"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
       <c r="AC1" s="18"/>
     </row>
-    <row r="2" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>39757</v>
       </c>
@@ -1280,25 +1699,12 @@
       <c r="J2" s="13">
         <v>0.8</v>
       </c>
-      <c r="K2" s="13"/>
       <c r="L2" s="13">
         <f>F2+G2+H2+I2</f>
         <v>1550.5248101265822</v>
       </c>
-      <c r="M2" s="17"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="13"/>
-    </row>
-    <row r="3" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>39757</v>
       </c>
@@ -1332,25 +1738,12 @@
       <c r="J3" s="13">
         <v>0.8</v>
       </c>
-      <c r="K3" s="13"/>
       <c r="L3" s="13">
         <f>F3+G3+H3+I3</f>
         <v>5055.7464363870413</v>
       </c>
-      <c r="M3" s="17"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="13"/>
-      <c r="Z3" s="13"/>
-      <c r="AA3" s="13"/>
-      <c r="AB3" s="13"/>
-    </row>
-    <row r="4" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>39757</v>
       </c>
@@ -1384,27 +1777,13 @@
       <c r="J4" s="13">
         <v>0.8</v>
       </c>
-      <c r="K4" s="13"/>
       <c r="L4" s="13">
         <f>F4+G4+H4+I4</f>
         <v>2766.9487534863761</v>
       </c>
-      <c r="M4" s="17"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="13"/>
-      <c r="AB4" s="13"/>
-    </row>
-    <row r="5" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
-      <c r="E5" s="13"/>
       <c r="F5" s="13">
         <f>SUM(F2:F4)</f>
         <v>9322</v>
@@ -1425,48 +1804,15 @@
         <f>SUM(J2:J4)</f>
         <v>2.4000000000000004</v>
       </c>
-      <c r="K5" s="13"/>
       <c r="L5" s="13">
         <f>SUM(L2:L4)</f>
         <v>9373.2199999999993</v>
       </c>
-      <c r="M5" s="17"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="13"/>
-      <c r="AB5" s="13"/>
-    </row>
-    <row r="6" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="17"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="13"/>
-      <c r="AB6" s="13"/>
-    </row>
-    <row r="7" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>39758</v>
       </c>
@@ -1500,25 +1846,12 @@
       <c r="J7" s="13">
         <v>0.8</v>
       </c>
-      <c r="K7" s="13"/>
       <c r="L7" s="13">
         <f>F7+G7+H7+I7</f>
         <v>1536.5810004368718</v>
       </c>
-      <c r="M7" s="17"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
-      <c r="Z7" s="13"/>
-      <c r="AA7" s="13"/>
-      <c r="AB7" s="13"/>
-    </row>
-    <row r="8" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>39758</v>
       </c>
@@ -1552,27 +1885,13 @@
       <c r="J8" s="13">
         <v>0.8</v>
       </c>
-      <c r="K8" s="13"/>
       <c r="L8" s="13">
         <f>F8+G8+H8+I8</f>
         <v>785.28899956312807</v>
       </c>
-      <c r="M8" s="17"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="13"/>
-      <c r="Y8" s="13"/>
-      <c r="Z8" s="13"/>
-      <c r="AA8" s="13"/>
-      <c r="AB8" s="13"/>
-    </row>
-    <row r="9" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
-      <c r="E9" s="13"/>
       <c r="F9" s="13">
         <f>SUM(F7:F8)</f>
         <v>2289</v>
@@ -1593,48 +1912,15 @@
         <f>SUM(J7:J8)</f>
         <v>1.6</v>
       </c>
-      <c r="K9" s="13"/>
       <c r="L9" s="13">
         <f>SUM(L7:L8)</f>
         <v>2321.87</v>
       </c>
-      <c r="M9" s="17"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="13"/>
-      <c r="Y9" s="13"/>
-      <c r="Z9" s="13"/>
-      <c r="AA9" s="13"/>
-      <c r="AB9" s="13"/>
-    </row>
-    <row r="10" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="17"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
-      <c r="W10" s="13"/>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="13"/>
-      <c r="Z10" s="13"/>
-      <c r="AA10" s="13"/>
-      <c r="AB10" s="13"/>
-    </row>
-    <row r="11" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>39849</v>
       </c>
@@ -1673,43 +1959,11 @@
         <f>F11-G11-H11-I11-K11</f>
         <v>3132.9100000000003</v>
       </c>
-      <c r="M11" s="17"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="13"/>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="13"/>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="13"/>
-      <c r="AB11" s="13"/>
-    </row>
-    <row r="12" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="17"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13"/>
-      <c r="U12" s="13"/>
-      <c r="V12" s="13"/>
-      <c r="W12" s="13"/>
-      <c r="X12" s="13"/>
-      <c r="Y12" s="13"/>
-      <c r="Z12" s="13"/>
-      <c r="AA12" s="13"/>
-      <c r="AB12" s="13"/>
-    </row>
-    <row r="13" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>39853</v>
       </c>
@@ -1748,41 +2002,9 @@
         <f>F13-G13-H13-I13-K13</f>
         <v>1753.3999999999999</v>
       </c>
-      <c r="M13" s="17"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
-      <c r="U13" s="13"/>
-      <c r="V13" s="13"/>
-      <c r="W13" s="13"/>
-      <c r="X13" s="13"/>
-      <c r="Y13" s="13"/>
-      <c r="Z13" s="13"/>
-      <c r="AA13" s="13"/>
-      <c r="AB13" s="13"/>
-    </row>
-    <row r="14" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="17"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="13"/>
-      <c r="V14" s="13"/>
-      <c r="W14" s="13"/>
-      <c r="X14" s="13"/>
-      <c r="Y14" s="13"/>
-      <c r="Z14" s="13"/>
-      <c r="AA14" s="13"/>
-      <c r="AB14" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1790,7 +2012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
@@ -2137,7 +2359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
@@ -2975,31 +3197,31 @@
       <c r="A19" s="10"/>
       <c r="E19" s="8"/>
       <c r="F19" s="11">
-        <f>SUM(F17:F18)</f>
+        <f t="shared" ref="F19:L19" si="0">SUM(F17:F18)</f>
         <v>25170</v>
       </c>
       <c r="G19" s="11">
-        <f>SUM(G17:G18)</f>
+        <f t="shared" si="0"/>
         <v>1.5100000000000002</v>
       </c>
       <c r="H19" s="11">
-        <f>SUM(H17:H18)</f>
+        <f t="shared" si="0"/>
         <v>7.17</v>
       </c>
       <c r="I19" s="11">
-        <f>SUM(I17:I18)</f>
+        <f t="shared" si="0"/>
         <v>31.98</v>
       </c>
       <c r="J19" s="11">
-        <f>SUM(J17:J18)</f>
+        <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
       <c r="K19" s="11">
-        <f>SUM(K17:K18)</f>
+        <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
       <c r="L19" s="11">
-        <f>SUM(L17:L18)</f>
+        <f t="shared" si="0"/>
         <v>25128.09</v>
       </c>
       <c r="M19" s="6"/>
@@ -3021,7 +3243,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
   <dimension ref="A1:AC6"/>
   <sheetViews>

</xml_diff>

<commit_message>
Fails when trying to create a 'BrokerageNotesWorksheetReader' from a 'Worksheet' whose 'Line's have 'Cell's with different 'FontColor's.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6181E28C-F4CE-46AF-B2B0-C0E179EF7AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D67CDB-5210-403C-9A17-DA046CA2D077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" firstSheet="2" activeTab="2" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" firstSheet="3" activeTab="3" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
     <sheet name="GroupWithDifferentTradingDates" sheetId="11" r:id="rId2"/>
     <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId3"/>
-    <sheet name="2" sheetId="7" r:id="rId4"/>
-    <sheet name="3" sheetId="8" r:id="rId5"/>
-    <sheet name="4" sheetId="9" r:id="rId6"/>
-    <sheet name="5" sheetId="10" r:id="rId7"/>
+    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId4"/>
+    <sheet name="2" sheetId="7" r:id="rId5"/>
+    <sheet name="3" sheetId="8" r:id="rId6"/>
+    <sheet name="4" sheetId="9" r:id="rId7"/>
+    <sheet name="5" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -99,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="22">
   <si>
     <t>BBAS3</t>
   </si>
@@ -175,7 +176,7 @@
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,6 +233,13 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -259,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -279,6 +287,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1156,6 +1165,436 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="12"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC1" s="18"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="12">
+        <v>100</v>
+      </c>
+      <c r="E2" s="13">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="13">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="13">
+        <f>0.74*(F2/SUM(F2:F4))</f>
+        <v>0.12177215189873417</v>
+      </c>
+      <c r="H2" s="13">
+        <f>2.51*(F2/SUM(F2:F4))</f>
+        <v>0.41303797468354425</v>
+      </c>
+      <c r="I2" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="L2" s="13">
+        <f>F2+G2+H2+I2</f>
+        <v>1550.5248101265822</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>39757</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1663</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12">
+        <v>200</v>
+      </c>
+      <c r="E3" s="13">
+        <v>25.19</v>
+      </c>
+      <c r="F3" s="13">
+        <f>D3*E3</f>
+        <v>5038</v>
+      </c>
+      <c r="G3" s="13">
+        <f>0.74*(F3/SUM(F2:F4))</f>
+        <v>0.39992705428019737</v>
+      </c>
+      <c r="H3" s="13">
+        <f>2.51*(F3/SUM(F2:F4))</f>
+        <v>1.3565093327612099</v>
+      </c>
+      <c r="I3" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="L3" s="13">
+        <f>F3+G3+H3+I3</f>
+        <v>5055.7464363870413</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="12">
+        <v>1662</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="12">
+        <v>100</v>
+      </c>
+      <c r="E4" s="13">
+        <v>27.5</v>
+      </c>
+      <c r="F4" s="13">
+        <f>D4*E4</f>
+        <v>2750</v>
+      </c>
+      <c r="G4" s="13">
+        <f>0.74*(F4/SUM(F2:F4))</f>
+        <v>0.21830079382106843</v>
+      </c>
+      <c r="H4" s="13">
+        <f>2.51*(F4/SUM(F2:F4))</f>
+        <v>0.74045269255524548</v>
+      </c>
+      <c r="I4" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="L4" s="13">
+        <f>F4+G4+H4+I4</f>
+        <v>2766.9487534863761</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="F5" s="13">
+        <f>SUM(F2:F4)</f>
+        <v>9322</v>
+      </c>
+      <c r="G5" s="13">
+        <f>SUM(G2:G4)</f>
+        <v>0.74</v>
+      </c>
+      <c r="H5" s="13">
+        <f>SUM(H2:H4)</f>
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="I5" s="13">
+        <f>SUM(I2:I4)</f>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="13">
+        <f>SUM(J2:J4)</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="L5" s="13">
+        <f>SUM(L2:L4)</f>
+        <v>9373.2199999999993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>39758</v>
+      </c>
+      <c r="B7" s="12">
+        <v>1344</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12">
+        <v>100</v>
+      </c>
+      <c r="E7" s="13">
+        <v>15.2</v>
+      </c>
+      <c r="F7" s="13">
+        <f>D7*E7</f>
+        <v>1520</v>
+      </c>
+      <c r="G7" s="13">
+        <f>0.2*(F7/SUM(F7:F8))</f>
+        <v>0.13280908693752733</v>
+      </c>
+      <c r="H7" s="13">
+        <f>0.69*(F7/SUM(F7:F8))</f>
+        <v>0.45819134993446919</v>
+      </c>
+      <c r="I7" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J7" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="L7" s="13">
+        <f>F7+G7+H7+I7</f>
+        <v>1536.5810004368718</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>39758</v>
+      </c>
+      <c r="B8" s="12">
+        <v>1344</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="12">
+        <v>100</v>
+      </c>
+      <c r="E8" s="13">
+        <v>7.69</v>
+      </c>
+      <c r="F8" s="13">
+        <f>D8*E8</f>
+        <v>769</v>
+      </c>
+      <c r="G8" s="13">
+        <f>0.2*(F8/SUM(F7:F8))</f>
+        <v>6.7190913062472699E-2</v>
+      </c>
+      <c r="H8" s="13">
+        <f>0.69*(F8/SUM(F7:F8))</f>
+        <v>0.23180865006553075</v>
+      </c>
+      <c r="I8" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J8" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="L8" s="13">
+        <f>F8+G8+H8+I8</f>
+        <v>785.28899956312807</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="F9" s="13">
+        <f>SUM(F7:F8)</f>
+        <v>2289</v>
+      </c>
+      <c r="G9" s="13">
+        <f>SUM(G7:G8)</f>
+        <v>0.2</v>
+      </c>
+      <c r="H9" s="13">
+        <f>SUM(H7:H8)</f>
+        <v>0.69</v>
+      </c>
+      <c r="I9" s="13">
+        <f>SUM(I7:I8)</f>
+        <v>31.98</v>
+      </c>
+      <c r="J9" s="13">
+        <f>SUM(J7:J8)</f>
+        <v>1.6</v>
+      </c>
+      <c r="L9" s="13">
+        <f>SUM(L7:L8)</f>
+        <v>2321.87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>39849</v>
+      </c>
+      <c r="B11" s="12">
+        <v>1319</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="12">
+        <v>100</v>
+      </c>
+      <c r="E11" s="13">
+        <v>31.5</v>
+      </c>
+      <c r="F11" s="13">
+        <f>D11*E11</f>
+        <v>3150</v>
+      </c>
+      <c r="G11" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="H11" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="I11" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J11" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="K11" s="13">
+        <v>0</v>
+      </c>
+      <c r="L11" s="13">
+        <f>F11-G11-H11-I11-K11</f>
+        <v>3132.9100000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>39853</v>
+      </c>
+      <c r="B13" s="12">
+        <v>1362</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="12">
+        <v>100</v>
+      </c>
+      <c r="E13" s="13">
+        <v>17.7</v>
+      </c>
+      <c r="F13" s="13">
+        <f>D13*E13</f>
+        <v>1770</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H13" s="13">
+        <v>0.47</v>
+      </c>
+      <c r="I13" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J13" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="K13" s="13">
+        <v>0</v>
+      </c>
+      <c r="L13" s="13">
+        <f>F13-G13-H13-I13-K13</f>
+        <v>1753.3999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384BB7C-DF07-4187-ADF0-23E50C2BA287}">
+  <dimension ref="A1:AC7"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
@@ -1235,346 +1674,208 @@
       </c>
       <c r="AC1" s="18"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>39757</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="4">
         <v>1662</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="4">
         <v>100</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="3">
         <v>15.34</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="3">
         <f>D2*E2</f>
         <v>1534</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="3">
         <f>0.74*(F2/SUM(F2:F4))</f>
         <v>0.12177215189873417</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="3">
         <f>2.51*(F2/SUM(F2:F4))</f>
         <v>0.41303797468354425</v>
       </c>
-      <c r="I2" s="13">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="13">
-        <v>0.8</v>
-      </c>
-      <c r="L2" s="13">
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3">
         <f>F2+G2+H2+I2</f>
         <v>1550.5248101265822</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>39757</v>
       </c>
-      <c r="B3" s="12">
-        <v>1663</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="19">
+        <v>1662</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="4">
         <v>200</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="3">
         <v>25.19</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="3">
         <f>D3*E3</f>
         <v>5038</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="3">
         <f>0.74*(F3/SUM(F2:F4))</f>
         <v>0.39992705428019737</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="3">
         <f>2.51*(F3/SUM(F2:F4))</f>
         <v>1.3565093327612099</v>
       </c>
-      <c r="I3" s="13">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="13">
-        <v>0.8</v>
-      </c>
-      <c r="L3" s="13">
+      <c r="I3" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
         <f>F3+G3+H3+I3</f>
         <v>5055.7464363870413</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+      <c r="M3" s="6"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>39757</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="4">
         <v>1662</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="4">
         <v>100</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="3">
         <v>27.5</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="3">
         <f>D4*E4</f>
         <v>2750</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="3">
         <f>0.74*(F4/SUM(F2:F4))</f>
         <v>0.21830079382106843</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="3">
         <f>2.51*(F4/SUM(F2:F4))</f>
         <v>0.74045269255524548</v>
       </c>
-      <c r="I4" s="13">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="13">
-        <v>0.8</v>
-      </c>
-      <c r="L4" s="13">
+      <c r="I4" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3">
         <f>F4+G4+H4+I4</f>
         <v>2766.9487534863761</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="F5" s="13">
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="7">
         <f>SUM(F2:F4)</f>
         <v>9322</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="7">
         <f>SUM(G2:G4)</f>
         <v>0.74</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="7">
         <f>SUM(H2:H4)</f>
         <v>2.5099999999999998</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="7">
         <f>SUM(I2:I4)</f>
         <v>47.97</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="7">
         <f>SUM(J2:J4)</f>
         <v>2.4000000000000004</v>
       </c>
-      <c r="L5" s="13">
+      <c r="K5" s="7"/>
+      <c r="L5" s="7">
         <f>SUM(L2:L4)</f>
         <v>9373.2199999999993</v>
       </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
-        <v>39758</v>
-      </c>
-      <c r="B7" s="12">
-        <v>1344</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="12">
-        <v>100</v>
-      </c>
-      <c r="E7" s="13">
-        <v>15.2</v>
-      </c>
-      <c r="F7" s="13">
-        <f>D7*E7</f>
-        <v>1520</v>
-      </c>
-      <c r="G7" s="13">
-        <f>0.2*(F7/SUM(F7:F8))</f>
-        <v>0.13280908693752733</v>
-      </c>
-      <c r="H7" s="13">
-        <f>0.69*(F7/SUM(F7:F8))</f>
-        <v>0.45819134993446919</v>
-      </c>
-      <c r="I7" s="13">
-        <v>15.99</v>
-      </c>
-      <c r="J7" s="13">
-        <v>0.8</v>
-      </c>
-      <c r="L7" s="13">
-        <f>F7+G7+H7+I7</f>
-        <v>1536.5810004368718</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
-        <v>39758</v>
-      </c>
-      <c r="B8" s="12">
-        <v>1344</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="12">
-        <v>100</v>
-      </c>
-      <c r="E8" s="13">
-        <v>7.69</v>
-      </c>
-      <c r="F8" s="13">
-        <f>D8*E8</f>
-        <v>769</v>
-      </c>
-      <c r="G8" s="13">
-        <f>0.2*(F8/SUM(F7:F8))</f>
-        <v>6.7190913062472699E-2</v>
-      </c>
-      <c r="H8" s="13">
-        <f>0.69*(F8/SUM(F7:F8))</f>
-        <v>0.23180865006553075</v>
-      </c>
-      <c r="I8" s="13">
-        <v>15.99</v>
-      </c>
-      <c r="J8" s="13">
-        <v>0.8</v>
-      </c>
-      <c r="L8" s="13">
-        <f>F8+G8+H8+I8</f>
-        <v>785.28899956312807</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="F9" s="13">
-        <f>SUM(F7:F8)</f>
-        <v>2289</v>
-      </c>
-      <c r="G9" s="13">
-        <f>SUM(G7:G8)</f>
-        <v>0.2</v>
-      </c>
-      <c r="H9" s="13">
-        <f>SUM(H7:H8)</f>
-        <v>0.69</v>
-      </c>
-      <c r="I9" s="13">
-        <f>SUM(I7:I8)</f>
-        <v>31.98</v>
-      </c>
-      <c r="J9" s="13">
-        <f>SUM(J7:J8)</f>
-        <v>1.6</v>
-      </c>
-      <c r="L9" s="13">
-        <f>SUM(L7:L8)</f>
-        <v>2321.87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
-        <v>39849</v>
-      </c>
-      <c r="B11" s="12">
-        <v>1319</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="12">
-        <v>100</v>
-      </c>
-      <c r="E11" s="13">
-        <v>31.5</v>
-      </c>
-      <c r="F11" s="13">
-        <f>D11*E11</f>
-        <v>3150</v>
-      </c>
-      <c r="G11" s="13">
-        <v>0.25</v>
-      </c>
-      <c r="H11" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="I11" s="13">
-        <v>15.99</v>
-      </c>
-      <c r="J11" s="13">
-        <v>0.8</v>
-      </c>
-      <c r="K11" s="13">
-        <v>0</v>
-      </c>
-      <c r="L11" s="13">
-        <f>F11-G11-H11-I11-K11</f>
-        <v>3132.9100000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
-        <v>39853</v>
-      </c>
-      <c r="B13" s="12">
-        <v>1362</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="12">
-        <v>100</v>
-      </c>
-      <c r="E13" s="13">
-        <v>17.7</v>
-      </c>
-      <c r="F13" s="13">
-        <f>D13*E13</f>
-        <v>1770</v>
-      </c>
-      <c r="G13" s="13">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="H13" s="13">
-        <v>0.47</v>
-      </c>
-      <c r="I13" s="13">
-        <v>15.99</v>
-      </c>
-      <c r="J13" s="13">
-        <v>0.8</v>
-      </c>
-      <c r="K13" s="13">
-        <v>0</v>
-      </c>
-      <c r="L13" s="13">
-        <f>F13-G13-H13-I13-K13</f>
-        <v>1753.3999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
+      <c r="A7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1582,7 +1883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -2012,7 +2313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
@@ -2359,7 +2660,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
@@ -3243,7 +3544,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
   <dimension ref="A1:AC6"/>
   <sheetViews>

</xml_diff>

<commit_message>
Fails when trying to create a 'BrokerageNotesWorksheetReader' from a 'Worksheet' whose 'Line's have 'Cell's whose values are supposed to have been calculated from other 'Cell's but, do not pass the recalculation test. Here, specifically, the 'Volume' from an 'Operation'.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD854A71-EEE7-487A-888C-CE0EF1A6B272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86CC5A7-B24E-490E-96AB-339F6A631E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" firstSheet="7" activeTab="8" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" firstSheet="8" activeTab="9" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="GroupsWithSummary" sheetId="8" r:id="rId7"/>
     <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId8"/>
     <sheet name="SingleLineGroups" sheetId="10" r:id="rId9"/>
+    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -101,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="22">
   <si>
     <t>BBAS3</t>
   </si>
@@ -732,6 +733,295 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7618D34E-0B33-4181-8E63-6765777C5B7E}">
+  <dimension ref="A1:AC5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9">
+        <v>200</v>
+      </c>
+      <c r="E2" s="8">
+        <v>35.15</v>
+      </c>
+      <c r="F2" s="8">
+        <v>7030.01</v>
+      </c>
+      <c r="G2" s="8">
+        <f>1.16*(F2/SUM(F2:F4))</f>
+        <v>0.42000450143979118</v>
+      </c>
+      <c r="H2" s="8">
+        <f>5.53*(F2/SUM(F2:F4))</f>
+        <v>2.0022628387603842</v>
+      </c>
+      <c r="I2" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0</v>
+      </c>
+      <c r="L2" s="8">
+        <f>F2-G2-H2-I2-K2</f>
+        <v>7011.5977326598004</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9">
+        <v>200</v>
+      </c>
+      <c r="E3" s="8">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3*E3</f>
+        <v>6895.9999999999991</v>
+      </c>
+      <c r="G3" s="8">
+        <f>1.16*(F3/SUM(F2:F4))</f>
+        <v>0.41199813967957366</v>
+      </c>
+      <c r="H3" s="8">
+        <f>5.53*(F3/SUM(F2:F4))</f>
+        <v>1.9640945796793472</v>
+      </c>
+      <c r="I3" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="8">
+        <v>0</v>
+      </c>
+      <c r="L3" s="8">
+        <f>F3-G3-H3-I3-K3</f>
+        <v>6877.6339072806404</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="9">
+        <v>200</v>
+      </c>
+      <c r="E4" s="8">
+        <v>27.45</v>
+      </c>
+      <c r="F4" s="8">
+        <f>D4*E4</f>
+        <v>5490</v>
+      </c>
+      <c r="G4" s="8">
+        <f>1.16*(F4/SUM(F2:F4))</f>
+        <v>0.32799735888063514</v>
+      </c>
+      <c r="H4" s="8">
+        <f>5.53*(F4/SUM(F2:F4))</f>
+        <v>1.5636425815602693</v>
+      </c>
+      <c r="I4" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="8">
+        <v>0</v>
+      </c>
+      <c r="L4" s="8">
+        <f>F4-G4-H4-I4-K4</f>
+        <v>5472.1183600595596</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="11">
+        <f>SUM(F2:F4)</f>
+        <v>19416.009999999998</v>
+      </c>
+      <c r="G5" s="11">
+        <f>SUM(G2:G4)</f>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="H5" s="11">
+        <f>SUM(H2:H4)</f>
+        <v>5.53</v>
+      </c>
+      <c r="I5" s="11">
+        <f>SUM(I2:I4)</f>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="11">
+        <f>SUM(J2:J4)</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11">
+        <f>SUM(L2:L4)</f>
+        <v>19361.349999999999</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03306DC6-EFFD-4226-8075-7FFC9D0F7B34}">
   <dimension ref="A1:AC14"/>
@@ -3206,7 +3496,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="1" sqref="A7:XFD7 A12:XFD12"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="1" sqref="A2:XFD2 A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4087,7 +4377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="A6" activeCellId="2" sqref="A2:XFD2 A4:XFD4 A6:XFD6"/>

</xml_diff>

<commit_message>
Fails when trying to create a 'BrokerageNotesWorksheetReader' from a 'Worksheet' whose 'Line's have 'Cell's whose values are supposed to have been calculated from other 'Cell's but, do not pass the recalculation test. Here, specifically, the 'SettlementFee', which should equal the 'Volume' * 'SettlementFee' for the 'OperationalMode' when the 'OperationalMode' is 'Normal'.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86CC5A7-B24E-490E-96AB-339F6A631E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F568317-70D1-4BF8-AAE7-C6388D85769A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" firstSheet="8" activeTab="9" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" firstSheet="6" activeTab="6" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId8"/>
     <sheet name="SingleLineGroups" sheetId="10" r:id="rId9"/>
     <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId10"/>
+    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -102,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="24">
   <si>
     <t>BBAS3</t>
   </si>
@@ -168,6 +169,12 @@
   </si>
   <si>
     <t>Data Pregão</t>
+  </si>
+  <si>
+    <t>AZUL4</t>
+  </si>
+  <si>
+    <t>EMBR3</t>
   </si>
 </sst>
 </file>
@@ -737,7 +744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7618D34E-0B33-4181-8E63-6765777C5B7E}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
@@ -1015,6 +1022,218 @@
       <c r="Z5" s="8"/>
       <c r="AA5" s="8"/>
       <c r="AB5" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19EF43A-AB48-4760-8CB3-D62FBA7ABFD8}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <v>2.76</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.429349999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>SUM(F2:F3)</f>
+        <v>22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
+        <v>5.66</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="2"/>
+        <v>22611.028699999995</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1986,8 +2205,8 @@
         <v>1534</v>
       </c>
       <c r="G2" s="3">
-        <f>0.74*(F2/SUM(F2:F4))</f>
-        <v>0.12177215189873417</v>
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
       </c>
       <c r="H2" s="3">
         <f>2.51*(F2/SUM(F2:F4))</f>
@@ -2002,7 +2221,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2</f>
-        <v>1550.5248101265822</v>
+        <v>1550.8248879746834</v>
       </c>
       <c r="M2" s="6"/>
       <c r="R2" s="3"/>
@@ -2038,8 +2257,8 @@
         <v>5038</v>
       </c>
       <c r="G3" s="3">
-        <f>0.74*(F3/SUM(F2:F4))</f>
-        <v>0.39992705428019737</v>
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.3854500000000001</v>
       </c>
       <c r="H3" s="3">
         <f>2.51*(F3/SUM(F2:F4))</f>
@@ -2054,7 +2273,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3</f>
-        <v>5055.7464363870413</v>
+        <v>5056.7319593327611</v>
       </c>
       <c r="M3" s="6"/>
       <c r="R3" s="3"/>
@@ -2090,8 +2309,8 @@
         <v>2750</v>
       </c>
       <c r="G4" s="3">
-        <f>0.74*(F4/SUM(F2:F4))</f>
-        <v>0.21830079382106843</v>
+        <f t="shared" si="0"/>
+        <v>0.75625000000000009</v>
       </c>
       <c r="H4" s="3">
         <f>2.51*(F4/SUM(F2:F4))</f>
@@ -2106,7 +2325,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3">
         <f>F4+G4+H4+I4</f>
-        <v>2766.9487534863761</v>
+        <v>2767.4867026925549</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -2130,7 +2349,7 @@
       </c>
       <c r="G5" s="7">
         <f>SUM(G2:G4)</f>
-        <v>0.74</v>
+        <v>2.5635500000000002</v>
       </c>
       <c r="H5" s="7">
         <f>SUM(H2:H4)</f>
@@ -2147,7 +2366,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7">
         <f>SUM(L2:L4)</f>
-        <v>9373.2199999999993</v>
+        <v>9375.0435499999985</v>
       </c>
       <c r="M5" s="6"/>
       <c r="R5" s="3"/>
@@ -2517,8 +2736,8 @@
         <v>1534</v>
       </c>
       <c r="G2" s="3">
-        <f>0.74*(F2/SUM(F2:F4))</f>
-        <v>0.12177215189873417</v>
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
       </c>
       <c r="H2" s="3">
         <f>2.51*(F2/SUM(F2:F4))</f>
@@ -2533,7 +2752,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2</f>
-        <v>1550.5248101265822</v>
+        <v>1550.8248879746834</v>
       </c>
       <c r="M2" s="6"/>
       <c r="R2" s="3"/>
@@ -2569,8 +2788,8 @@
         <v>5038</v>
       </c>
       <c r="G3" s="3">
-        <f>0.74*(F3/SUM(F2:F4))</f>
-        <v>0.39992705428019737</v>
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.3854500000000001</v>
       </c>
       <c r="H3" s="3">
         <f>2.51*(F3/SUM(F2:F4))</f>
@@ -2585,7 +2804,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3</f>
-        <v>5055.7464363870413</v>
+        <v>5056.7319593327611</v>
       </c>
       <c r="M3" s="6"/>
       <c r="R3" s="3"/>
@@ -2621,8 +2840,8 @@
         <v>2750</v>
       </c>
       <c r="G4" s="3">
-        <f>0.74*(F4/SUM(F2:F4))</f>
-        <v>0.21830079382106843</v>
+        <f t="shared" si="0"/>
+        <v>0.75625000000000009</v>
       </c>
       <c r="H4" s="3">
         <f>2.51*(F4/SUM(F2:F4))</f>
@@ -2637,7 +2856,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3">
         <f>F4+G4+H4+I4</f>
-        <v>2766.9487534863761</v>
+        <v>2767.4867026925549</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -2661,7 +2880,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM(G2:G4)</f>
-        <v>0.74</v>
+        <v>2.5635500000000002</v>
       </c>
       <c r="H5" s="3">
         <f>SUM(H2:H4)</f>
@@ -2678,7 +2897,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3">
         <f>SUM(L2:L4)</f>
-        <v>9373.2199999999993</v>
+        <v>9375.0435499999985</v>
       </c>
       <c r="M5" s="6"/>
       <c r="R5" s="3"/>
@@ -2737,8 +2956,8 @@
         <v>1520</v>
       </c>
       <c r="G7" s="3">
-        <f>0.2*(F7/SUM(F7:F8))</f>
-        <v>0.13280908693752733</v>
+        <f>F7*0.0275%</f>
+        <v>0.41800000000000004</v>
       </c>
       <c r="H7" s="3">
         <f>0.69*(F7/SUM(F7:F8))</f>
@@ -2753,7 +2972,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3">
         <f>F7+G7+H7+I7</f>
-        <v>1536.5810004368718</v>
+        <v>1536.8661913499343</v>
       </c>
       <c r="M7" s="6"/>
       <c r="R7" s="3"/>
@@ -2789,8 +3008,8 @@
         <v>769</v>
       </c>
       <c r="G8" s="3">
-        <f>0.2*(F8/SUM(F7:F8))</f>
-        <v>6.7190913062472699E-2</v>
+        <f>F8*0.0275%</f>
+        <v>0.21147500000000002</v>
       </c>
       <c r="H8" s="3">
         <f>0.69*(F8/SUM(F7:F8))</f>
@@ -2805,7 +3024,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3">
         <f>F8+G8+H8+I8</f>
-        <v>785.28899956312807</v>
+        <v>785.4332836500655</v>
       </c>
       <c r="M8" s="6"/>
       <c r="R8" s="3"/>
@@ -2829,7 +3048,7 @@
       </c>
       <c r="G9" s="3">
         <f>SUM(G7:G8)</f>
-        <v>0.2</v>
+        <v>0.62947500000000001</v>
       </c>
       <c r="H9" s="3">
         <f>SUM(H7:H8)</f>
@@ -2846,7 +3065,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3">
         <f>SUM(L7:L8)</f>
-        <v>2321.87</v>
+        <v>2322.2994749999998</v>
       </c>
       <c r="M9" s="6"/>
       <c r="R9" s="3"/>
@@ -2885,7 +3104,8 @@
         <v>3150</v>
       </c>
       <c r="G11" s="8">
-        <v>0.25</v>
+        <f>F11*0.0275%</f>
+        <v>0.86625000000000008</v>
       </c>
       <c r="H11" s="8">
         <v>0.85</v>
@@ -2901,7 +3121,7 @@
       </c>
       <c r="L11" s="8">
         <f>F11-G11-H11-I11-K11</f>
-        <v>3132.9100000000003</v>
+        <v>3132.2937500000003</v>
       </c>
       <c r="M11" s="6"/>
       <c r="R11" s="8"/>
@@ -2940,7 +3160,8 @@
         <v>1770</v>
       </c>
       <c r="G13" s="8">
-        <v>0.14000000000000001</v>
+        <f>F13*0.0275%</f>
+        <v>0.48675000000000002</v>
       </c>
       <c r="H13" s="8">
         <v>0.47</v>
@@ -2956,7 +3177,7 @@
       </c>
       <c r="L13" s="8">
         <f>F13-G13-H13-I13-K13</f>
-        <v>1753.3999999999999</v>
+        <v>1753.0532499999999</v>
       </c>
       <c r="M13" s="6"/>
       <c r="R13" s="8"/>
@@ -2984,7 +3205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="A10" activeCellId="1" sqref="A5:XFD5 A10:XFD10"/>
@@ -3084,8 +3305,8 @@
         <v>1534</v>
       </c>
       <c r="G2" s="3">
-        <f>0.74*(F2/SUM(F2:F4))</f>
-        <v>0.12177215189873417</v>
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
       </c>
       <c r="H2" s="3">
         <f>2.51*(F2/SUM(F2:F4))</f>
@@ -3100,7 +3321,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2</f>
-        <v>1550.5248101265822</v>
+        <v>1550.8248879746834</v>
       </c>
       <c r="M2" s="6"/>
       <c r="R2" s="3"/>
@@ -3136,8 +3357,8 @@
         <v>5038</v>
       </c>
       <c r="G3" s="3">
-        <f>0.74*(F3/SUM(F2:F4))</f>
-        <v>0.39992705428019737</v>
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.3854500000000001</v>
       </c>
       <c r="H3" s="3">
         <f>2.51*(F3/SUM(F2:F4))</f>
@@ -3152,7 +3373,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3</f>
-        <v>5055.7464363870413</v>
+        <v>5056.7319593327611</v>
       </c>
       <c r="M3" s="6"/>
       <c r="R3" s="3"/>
@@ -3188,8 +3409,8 @@
         <v>2750</v>
       </c>
       <c r="G4" s="3">
-        <f>0.74*(F4/SUM(F2:F4))</f>
-        <v>0.21830079382106843</v>
+        <f t="shared" si="0"/>
+        <v>0.75625000000000009</v>
       </c>
       <c r="H4" s="3">
         <f>2.51*(F4/SUM(F2:F4))</f>
@@ -3204,7 +3425,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3">
         <f>F4+G4+H4+I4</f>
-        <v>2766.9487534863761</v>
+        <v>2767.4867026925549</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -3228,7 +3449,7 @@
       </c>
       <c r="G5" s="7">
         <f>SUM(G2:G4)</f>
-        <v>0.74</v>
+        <v>2.5635500000000002</v>
       </c>
       <c r="H5" s="7">
         <f>SUM(H2:H4)</f>
@@ -3245,7 +3466,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7">
         <f>SUM(L2:L4)</f>
-        <v>9373.2199999999993</v>
+        <v>9375.0435499999985</v>
       </c>
       <c r="M5" s="6"/>
       <c r="R5" s="3"/>
@@ -3304,8 +3525,8 @@
         <v>268</v>
       </c>
       <c r="G7" s="3">
-        <f>0.2*(F7/SUM(F7:F9))</f>
-        <v>2.0962064919827925E-2</v>
+        <f>F7*0.0275%</f>
+        <v>7.3700000000000002E-2</v>
       </c>
       <c r="H7" s="3">
         <f>0.69*(F7/SUM(F7:F9))</f>
@@ -3320,7 +3541,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3">
         <f>F7+G7+H7+I7</f>
-        <v>284.08328118889324</v>
+        <v>284.13601912397337</v>
       </c>
       <c r="M7" s="6"/>
       <c r="R7" s="3"/>
@@ -3356,8 +3577,8 @@
         <v>1520</v>
       </c>
       <c r="G8" s="3">
-        <f>0.2*(F8/SUM(F7:F9))</f>
-        <v>0.11888932342588972</v>
+        <f t="shared" ref="G8:G9" si="1">F8*0.0275%</f>
+        <v>0.41800000000000004</v>
       </c>
       <c r="H8" s="3">
         <f>0.69*(F8/SUM(F7:F9))</f>
@@ -3372,7 +3593,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3">
         <f>F8+G8+H8+I8</f>
-        <v>1536.5190574892454</v>
+        <v>1536.8181681658193</v>
       </c>
       <c r="M8" s="6"/>
       <c r="R8" s="3"/>
@@ -3408,8 +3629,8 @@
         <v>769</v>
       </c>
       <c r="G9" s="3">
-        <f>0.2*(F9/SUM(F7:F9))</f>
-        <v>6.0148611654282362E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.21147500000000002</v>
       </c>
       <c r="H9" s="3">
         <f>0.69*(F9/SUM(F7:F9))</f>
@@ -3424,7 +3645,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3">
         <f>F9+G9+H9+I9</f>
-        <v>785.25766132186163</v>
+        <v>785.40898771020727</v>
       </c>
       <c r="M9" s="6"/>
       <c r="R9" s="3"/>
@@ -3448,7 +3669,7 @@
       </c>
       <c r="G10" s="7">
         <f>SUM(G7:G9)</f>
-        <v>0.2</v>
+        <v>0.70317500000000011</v>
       </c>
       <c r="H10" s="7">
         <f>SUM(H7:H9)</f>
@@ -3465,7 +3686,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7">
         <f>SUM(L7:L9)</f>
-        <v>2605.86</v>
+        <v>2606.363175</v>
       </c>
       <c r="M10" s="6"/>
       <c r="R10" s="3"/>
@@ -3496,7 +3717,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="1" sqref="A2:XFD2 A12:XFD12"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="1" sqref="A12:XFD12 A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3591,8 +3812,8 @@
         <v>1534</v>
       </c>
       <c r="G2" s="3">
-        <f>0.74*(F2/SUM(F2:F4))</f>
-        <v>0.12177215189873417</v>
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
       </c>
       <c r="H2" s="3">
         <f>2.51*(F2/SUM(F2:F4))</f>
@@ -3607,7 +3828,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2</f>
-        <v>1550.5248101265822</v>
+        <v>1550.8248879746834</v>
       </c>
       <c r="M2" s="6"/>
       <c r="R2" s="3"/>
@@ -3643,8 +3864,8 @@
         <v>5038</v>
       </c>
       <c r="G3" s="3">
-        <f>0.74*(F3/SUM(F2:F4))</f>
-        <v>0.39992705428019737</v>
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.3854500000000001</v>
       </c>
       <c r="H3" s="3">
         <f>2.51*(F3/SUM(F2:F4))</f>
@@ -3659,7 +3880,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3</f>
-        <v>5055.7464363870413</v>
+        <v>5056.7319593327611</v>
       </c>
       <c r="M3" s="6"/>
       <c r="R3" s="3"/>
@@ -3695,8 +3916,8 @@
         <v>2750</v>
       </c>
       <c r="G4" s="3">
-        <f>0.74*(F4/SUM(F2:F4))</f>
-        <v>0.21830079382106843</v>
+        <f t="shared" si="0"/>
+        <v>0.75625000000000009</v>
       </c>
       <c r="H4" s="3">
         <f>2.51*(F4/SUM(F2:F4))</f>
@@ -3711,7 +3932,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3">
         <f>F4+G4+H4+I4</f>
-        <v>2766.9487534863761</v>
+        <v>2767.4867026925549</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -3735,7 +3956,7 @@
       </c>
       <c r="G5" s="7">
         <f>SUM(G2:G4)</f>
-        <v>0.74</v>
+        <v>2.5635500000000002</v>
       </c>
       <c r="H5" s="7">
         <f>SUM(H2:H4)</f>
@@ -3752,7 +3973,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7">
         <f>SUM(L2:L4)</f>
-        <v>9373.2199999999993</v>
+        <v>9375.0435499999985</v>
       </c>
       <c r="M5" s="6"/>
       <c r="R5" s="3"/>
@@ -3811,8 +4032,8 @@
         <v>268</v>
       </c>
       <c r="G7" s="3">
-        <f>0.2*(F7/SUM(F7:F9))</f>
-        <v>2.0962064919827925E-2</v>
+        <f>F7*0.0275%</f>
+        <v>7.3700000000000002E-2</v>
       </c>
       <c r="H7" s="3">
         <f>0.69*(F7/SUM(F7:F9))</f>
@@ -3827,7 +4048,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3">
         <f>F7+G7+H7+I7</f>
-        <v>284.08328118889324</v>
+        <v>284.13601912397337</v>
       </c>
       <c r="M7" s="6"/>
       <c r="R7" s="3"/>
@@ -3863,8 +4084,8 @@
         <v>1520</v>
       </c>
       <c r="G8" s="3">
-        <f>0.2*(F8/SUM(F7:F9))</f>
-        <v>0.11888932342588972</v>
+        <f t="shared" ref="G8:G9" si="1">F8*0.0275%</f>
+        <v>0.41800000000000004</v>
       </c>
       <c r="H8" s="3">
         <f>0.69*(F8/SUM(F7:F9))</f>
@@ -3879,7 +4100,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3">
         <f>F8+G8+H8+I8</f>
-        <v>1536.5190574892454</v>
+        <v>1536.8181681658193</v>
       </c>
       <c r="M8" s="6"/>
       <c r="R8" s="3"/>
@@ -3915,8 +4136,8 @@
         <v>769</v>
       </c>
       <c r="G9" s="3">
-        <f>0.2*(F9/SUM(F7:F9))</f>
-        <v>6.0148611654282362E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.21147500000000002</v>
       </c>
       <c r="H9" s="3">
         <f>0.69*(F9/SUM(F7:F9))</f>
@@ -3931,7 +4152,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3">
         <f>F9+G9+H9+I9</f>
-        <v>785.25766132186163</v>
+        <v>785.40898771020727</v>
       </c>
       <c r="M9" s="6"/>
       <c r="R9" s="3"/>
@@ -3955,7 +4176,7 @@
       </c>
       <c r="G10" s="7">
         <f>SUM(G7:G9)</f>
-        <v>0.2</v>
+        <v>0.70317500000000011</v>
       </c>
       <c r="H10" s="7">
         <f>SUM(H7:H9)</f>
@@ -3972,7 +4193,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7">
         <f>SUM(L7:L9)</f>
-        <v>2605.86</v>
+        <v>2606.363175</v>
       </c>
       <c r="M10" s="6"/>
       <c r="R10" s="3"/>
@@ -4031,8 +4252,8 @@
         <v>7030</v>
       </c>
       <c r="G12" s="8">
-        <f>1.16*(F12/SUM(F12:F14))</f>
-        <v>0.42000412031314377</v>
+        <f>F12*0.0275%</f>
+        <v>1.9332500000000001</v>
       </c>
       <c r="H12" s="8">
         <f>5.53*(F12/SUM(F12:F14))</f>
@@ -4049,7 +4270,7 @@
       </c>
       <c r="L12" s="8">
         <f>F12-G12-H12-I12-K12</f>
-        <v>7011.5877348578497</v>
+        <v>7010.0744889781627</v>
       </c>
       <c r="M12" s="6"/>
       <c r="R12" s="8"/>
@@ -4085,8 +4306,8 @@
         <v>6895.9999999999991</v>
       </c>
       <c r="G13" s="8">
-        <f>1.16*(F13/SUM(F12:F14))</f>
-        <v>0.41199835187474243</v>
+        <f t="shared" ref="G13:G14" si="2">F13*0.0275%</f>
+        <v>1.8963999999999999</v>
       </c>
       <c r="H13" s="8">
         <f>5.53*(F13/SUM(F12:F14))</f>
@@ -4103,7 +4324,7 @@
       </c>
       <c r="L13" s="8">
         <f>F13-G13-H13-I13-K13</f>
-        <v>6877.6339060568598</v>
+        <v>6876.1495044087351</v>
       </c>
       <c r="M13" s="6"/>
       <c r="R13" s="8"/>
@@ -4139,8 +4360,8 @@
         <v>5490</v>
       </c>
       <c r="G14" s="8">
-        <f>1.16*(F14/SUM(F12:F14))</f>
-        <v>0.32799752781211372</v>
+        <f t="shared" si="2"/>
+        <v>1.5097500000000001</v>
       </c>
       <c r="H14" s="8">
         <f>5.53*(F14/SUM(F12:F14))</f>
@@ -4157,7 +4378,7 @@
       </c>
       <c r="L14" s="8">
         <f>F14-G14-H14-I14-K14</f>
-        <v>5472.1183590852906</v>
+        <v>5470.9366066131024</v>
       </c>
       <c r="M14" s="6"/>
       <c r="R14" s="8"/>
@@ -4181,7 +4402,7 @@
       </c>
       <c r="G15" s="11">
         <f>SUM(G12:G14)</f>
-        <v>1.1599999999999999</v>
+        <v>5.3394000000000004</v>
       </c>
       <c r="H15" s="11">
         <f>SUM(H12:H14)</f>
@@ -4198,7 +4419,7 @@
       <c r="K15" s="11"/>
       <c r="L15" s="11">
         <f>SUM(L12:L14)</f>
-        <v>19361.34</v>
+        <v>19357.160600000003</v>
       </c>
       <c r="M15" s="6"/>
       <c r="R15" s="8"/>
@@ -4234,8 +4455,8 @@
         <v>13050</v>
       </c>
       <c r="G17" s="8">
-        <f>1.51*(F17/SUM(F17:F18))</f>
-        <v>0.78289630512514907</v>
+        <f>F17*0.0275%</f>
+        <v>3.5887500000000001</v>
       </c>
       <c r="H17" s="8">
         <f>7.17*(F17/SUM(F17:F18))</f>
@@ -4253,7 +4474,7 @@
       </c>
       <c r="L17" s="8">
         <f>F17-G17-H17-I17-K17</f>
-        <v>13028.861549463649</v>
+        <v>13026.055695768773</v>
       </c>
       <c r="M17" s="6"/>
       <c r="R17" s="8"/>
@@ -4289,8 +4510,8 @@
         <v>12120</v>
       </c>
       <c r="G18" s="8">
-        <f>1.51*(F18/SUM(F17:F18))</f>
-        <v>0.72710369487485105</v>
+        <f>F18*0.0275%</f>
+        <v>3.3330000000000002</v>
       </c>
       <c r="H18" s="8">
         <f>7.17*(F18/SUM(F17:F18))</f>
@@ -4308,7 +4529,7 @@
       </c>
       <c r="L18" s="8">
         <f>F18-G18-H18-I18-K18</f>
-        <v>12099.228450536351</v>
+        <v>12096.622554231226</v>
       </c>
       <c r="M18" s="6"/>
       <c r="R18" s="8"/>
@@ -4327,32 +4548,32 @@
       <c r="A19" s="10"/>
       <c r="E19" s="8"/>
       <c r="F19" s="11">
-        <f t="shared" ref="F19:L19" si="0">SUM(F17:F18)</f>
+        <f t="shared" ref="F19:L19" si="3">SUM(F17:F18)</f>
         <v>25170</v>
       </c>
       <c r="G19" s="11">
-        <f t="shared" si="0"/>
-        <v>1.5100000000000002</v>
+        <f t="shared" si="3"/>
+        <v>6.9217500000000003</v>
       </c>
       <c r="H19" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7.17</v>
       </c>
       <c r="I19" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>31.98</v>
       </c>
       <c r="J19" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.6</v>
       </c>
       <c r="K19" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.25</v>
       </c>
       <c r="L19" s="11">
-        <f t="shared" si="0"/>
-        <v>25128.09</v>
+        <f t="shared" si="3"/>
+        <v>25122.678249999997</v>
       </c>
       <c r="M19" s="6"/>
       <c r="R19" s="8"/>

</xml_diff>

<commit_message>
Fails when trying to create a 'BrokerageNotesWorksheetReader' from a 'Worksheet' whose 'Line's have 'Cell's whose values are supposed to have been calculated from other 'Cell's but, do not pass the recalculation test. Here, specifically, the 'NegotiationFees', which should equal 'Volume' * 'NegotiationFeesRate' at 'TradingTime'.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F568317-70D1-4BF8-AAE7-C6388D85769A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12906ED-76D2-447D-82AC-69D08F46AD13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" firstSheet="6" activeTab="6" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" firstSheet="10" activeTab="11" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="SingleLineGroups" sheetId="10" r:id="rId9"/>
     <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId10"/>
     <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId11"/>
+    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -103,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="24">
   <si>
     <t>BBAS3</t>
   </si>
@@ -1036,7 +1037,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,6 +1206,218 @@
       <c r="H4" s="7">
         <f t="shared" si="2"/>
         <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="2"/>
+        <v>22611.028699999995</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.429349999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>SUM(F2:F3)</f>
+        <v>22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1400000000000001</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" si="2"/>
@@ -2108,7 +2321,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="A3:B3"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2209,8 +2422,8 @@
         <v>0.42185</v>
       </c>
       <c r="H2" s="3">
-        <f>2.51*(F2/SUM(F2:F4))</f>
-        <v>0.41303797468354425</v>
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
       </c>
       <c r="I2" s="3">
         <v>15.99</v>
@@ -2221,7 +2434,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2</f>
-        <v>1550.8248879746834</v>
+        <v>1550.5192299999999</v>
       </c>
       <c r="M2" s="6"/>
       <c r="R2" s="3"/>
@@ -2261,8 +2474,8 @@
         <v>1.3854500000000001</v>
       </c>
       <c r="H3" s="3">
-        <f>2.51*(F3/SUM(F2:F4))</f>
-        <v>1.3565093327612099</v>
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.35266000000000003</v>
       </c>
       <c r="I3" s="3">
         <v>15.99</v>
@@ -2273,7 +2486,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3</f>
-        <v>5056.7319593327611</v>
+        <v>5055.7281099999991</v>
       </c>
       <c r="M3" s="6"/>
       <c r="R3" s="3"/>
@@ -2313,8 +2526,8 @@
         <v>0.75625000000000009</v>
       </c>
       <c r="H4" s="3">
-        <f>2.51*(F4/SUM(F2:F4))</f>
-        <v>0.74045269255524548</v>
+        <f t="shared" si="1"/>
+        <v>0.19250000000000003</v>
       </c>
       <c r="I4" s="3">
         <v>15.99</v>
@@ -2325,7 +2538,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3">
         <f>F4+G4+H4+I4</f>
-        <v>2767.4867026925549</v>
+        <v>2766.9387499999998</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -2353,7 +2566,7 @@
       </c>
       <c r="H5" s="7">
         <f>SUM(H2:H4)</f>
-        <v>2.5099999999999998</v>
+        <v>0.65254000000000012</v>
       </c>
       <c r="I5" s="7">
         <f>SUM(I2:I4)</f>
@@ -2366,7 +2579,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7">
         <f>SUM(L2:L4)</f>
-        <v>9375.0435499999985</v>
+        <v>9373.1860899999992</v>
       </c>
       <c r="M5" s="6"/>
       <c r="R5" s="3"/>
@@ -2740,8 +2953,8 @@
         <v>0.42185</v>
       </c>
       <c r="H2" s="3">
-        <f>2.51*(F2/SUM(F2:F4))</f>
-        <v>0.41303797468354425</v>
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
       </c>
       <c r="I2" s="3">
         <v>15.99</v>
@@ -2752,7 +2965,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2</f>
-        <v>1550.8248879746834</v>
+        <v>1550.5192299999999</v>
       </c>
       <c r="M2" s="6"/>
       <c r="R2" s="3"/>
@@ -2792,8 +3005,8 @@
         <v>1.3854500000000001</v>
       </c>
       <c r="H3" s="3">
-        <f>2.51*(F3/SUM(F2:F4))</f>
-        <v>1.3565093327612099</v>
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.35266000000000003</v>
       </c>
       <c r="I3" s="3">
         <v>15.99</v>
@@ -2804,7 +3017,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3</f>
-        <v>5056.7319593327611</v>
+        <v>5055.7281099999991</v>
       </c>
       <c r="M3" s="6"/>
       <c r="R3" s="3"/>
@@ -2844,8 +3057,8 @@
         <v>0.75625000000000009</v>
       </c>
       <c r="H4" s="3">
-        <f>2.51*(F4/SUM(F2:F4))</f>
-        <v>0.74045269255524548</v>
+        <f t="shared" si="1"/>
+        <v>0.19250000000000003</v>
       </c>
       <c r="I4" s="3">
         <v>15.99</v>
@@ -2856,7 +3069,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3">
         <f>F4+G4+H4+I4</f>
-        <v>2767.4867026925549</v>
+        <v>2766.9387499999998</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -2884,7 +3097,7 @@
       </c>
       <c r="H5" s="3">
         <f>SUM(H2:H4)</f>
-        <v>2.5099999999999998</v>
+        <v>0.65254000000000012</v>
       </c>
       <c r="I5" s="3">
         <f>SUM(I2:I4)</f>
@@ -2897,7 +3110,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3">
         <f>SUM(L2:L4)</f>
-        <v>9375.0435499999985</v>
+        <v>9373.1860899999992</v>
       </c>
       <c r="M5" s="6"/>
       <c r="R5" s="3"/>
@@ -2960,8 +3173,8 @@
         <v>0.41800000000000004</v>
       </c>
       <c r="H7" s="3">
-        <f>0.69*(F7/SUM(F7:F8))</f>
-        <v>0.45819134993446919</v>
+        <f>F7*0.007%</f>
+        <v>0.10640000000000001</v>
       </c>
       <c r="I7" s="3">
         <v>15.99</v>
@@ -2972,7 +3185,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3">
         <f>F7+G7+H7+I7</f>
-        <v>1536.8661913499343</v>
+        <v>1536.5143999999998</v>
       </c>
       <c r="M7" s="6"/>
       <c r="R7" s="3"/>
@@ -3012,8 +3225,8 @@
         <v>0.21147500000000002</v>
       </c>
       <c r="H8" s="3">
-        <f>0.69*(F8/SUM(F7:F8))</f>
-        <v>0.23180865006553075</v>
+        <f>F8*0.007%</f>
+        <v>5.3830000000000003E-2</v>
       </c>
       <c r="I8" s="3">
         <v>15.99</v>
@@ -3024,7 +3237,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3">
         <f>F8+G8+H8+I8</f>
-        <v>785.4332836500655</v>
+        <v>785.25530499999991</v>
       </c>
       <c r="M8" s="6"/>
       <c r="R8" s="3"/>
@@ -3052,7 +3265,7 @@
       </c>
       <c r="H9" s="3">
         <f>SUM(H7:H8)</f>
-        <v>0.69</v>
+        <v>0.16023000000000001</v>
       </c>
       <c r="I9" s="3">
         <f>SUM(I7:I8)</f>
@@ -3065,7 +3278,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3">
         <f>SUM(L7:L8)</f>
-        <v>2322.2994749999998</v>
+        <v>2321.7697049999997</v>
       </c>
       <c r="M9" s="6"/>
       <c r="R9" s="3"/>
@@ -3108,7 +3321,8 @@
         <v>0.86625000000000008</v>
       </c>
       <c r="H11" s="8">
-        <v>0.85</v>
+        <f>F11*0.007%</f>
+        <v>0.22050000000000003</v>
       </c>
       <c r="I11" s="8">
         <v>15.99</v>
@@ -3121,7 +3335,7 @@
       </c>
       <c r="L11" s="8">
         <f>F11-G11-H11-I11-K11</f>
-        <v>3132.2937500000003</v>
+        <v>3132.9232500000003</v>
       </c>
       <c r="M11" s="6"/>
       <c r="R11" s="8"/>
@@ -3164,7 +3378,8 @@
         <v>0.48675000000000002</v>
       </c>
       <c r="H13" s="8">
-        <v>0.47</v>
+        <f>F13*0.007%</f>
+        <v>0.12390000000000001</v>
       </c>
       <c r="I13" s="8">
         <v>15.99</v>
@@ -3177,7 +3392,7 @@
       </c>
       <c r="L13" s="8">
         <f>F13-G13-H13-I13-K13</f>
-        <v>1753.0532499999999</v>
+        <v>1753.3993499999999</v>
       </c>
       <c r="M13" s="6"/>
       <c r="R13" s="8"/>
@@ -3205,7 +3420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="A10" activeCellId="1" sqref="A5:XFD5 A10:XFD10"/>
@@ -3309,8 +3524,8 @@
         <v>0.42185</v>
       </c>
       <c r="H2" s="3">
-        <f>2.51*(F2/SUM(F2:F4))</f>
-        <v>0.41303797468354425</v>
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
       </c>
       <c r="I2" s="3">
         <v>15.99</v>
@@ -3321,7 +3536,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2</f>
-        <v>1550.8248879746834</v>
+        <v>1550.5192299999999</v>
       </c>
       <c r="M2" s="6"/>
       <c r="R2" s="3"/>
@@ -3361,8 +3576,8 @@
         <v>1.3854500000000001</v>
       </c>
       <c r="H3" s="3">
-        <f>2.51*(F3/SUM(F2:F4))</f>
-        <v>1.3565093327612099</v>
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.35266000000000003</v>
       </c>
       <c r="I3" s="3">
         <v>15.99</v>
@@ -3373,7 +3588,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3</f>
-        <v>5056.7319593327611</v>
+        <v>5055.7281099999991</v>
       </c>
       <c r="M3" s="6"/>
       <c r="R3" s="3"/>
@@ -3413,8 +3628,8 @@
         <v>0.75625000000000009</v>
       </c>
       <c r="H4" s="3">
-        <f>2.51*(F4/SUM(F2:F4))</f>
-        <v>0.74045269255524548</v>
+        <f t="shared" si="1"/>
+        <v>0.19250000000000003</v>
       </c>
       <c r="I4" s="3">
         <v>15.99</v>
@@ -3425,7 +3640,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3">
         <f>F4+G4+H4+I4</f>
-        <v>2767.4867026925549</v>
+        <v>2766.9387499999998</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -3453,7 +3668,7 @@
       </c>
       <c r="H5" s="7">
         <f>SUM(H2:H4)</f>
-        <v>2.5099999999999998</v>
+        <v>0.65254000000000012</v>
       </c>
       <c r="I5" s="7">
         <f>SUM(I2:I4)</f>
@@ -3466,7 +3681,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7">
         <f>SUM(L2:L4)</f>
-        <v>9375.0435499999985</v>
+        <v>9373.1860899999992</v>
       </c>
       <c r="M5" s="6"/>
       <c r="R5" s="3"/>
@@ -3529,8 +3744,8 @@
         <v>7.3700000000000002E-2</v>
       </c>
       <c r="H7" s="3">
-        <f>0.69*(F7/SUM(F7:F9))</f>
-        <v>7.2319123973406341E-2</v>
+        <f>F7*0.007%</f>
+        <v>1.8760000000000002E-2</v>
       </c>
       <c r="I7" s="3">
         <v>15.99</v>
@@ -3541,7 +3756,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3">
         <f>F7+G7+H7+I7</f>
-        <v>284.13601912397337</v>
+        <v>284.08245999999997</v>
       </c>
       <c r="M7" s="6"/>
       <c r="R7" s="3"/>
@@ -3577,12 +3792,12 @@
         <v>1520</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" ref="G8:G9" si="1">F8*0.0275%</f>
+        <f t="shared" ref="G8:G9" si="2">F8*0.0275%</f>
         <v>0.41800000000000004</v>
       </c>
       <c r="H8" s="3">
-        <f>0.69*(F8/SUM(F7:F9))</f>
-        <v>0.41016816581931947</v>
+        <f t="shared" ref="H8:H9" si="3">F8*0.007%</f>
+        <v>0.10640000000000001</v>
       </c>
       <c r="I8" s="3">
         <v>15.99</v>
@@ -3593,7 +3808,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3">
         <f>F8+G8+H8+I8</f>
-        <v>1536.8181681658193</v>
+        <v>1536.5143999999998</v>
       </c>
       <c r="M8" s="6"/>
       <c r="R8" s="3"/>
@@ -3629,12 +3844,12 @@
         <v>769</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.21147500000000002</v>
       </c>
       <c r="H9" s="3">
-        <f>0.69*(F9/SUM(F7:F9))</f>
-        <v>0.20751271020727413</v>
+        <f t="shared" si="3"/>
+        <v>5.3830000000000003E-2</v>
       </c>
       <c r="I9" s="3">
         <v>15.99</v>
@@ -3645,7 +3860,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3">
         <f>F9+G9+H9+I9</f>
-        <v>785.40898771020727</v>
+        <v>785.25530499999991</v>
       </c>
       <c r="M9" s="6"/>
       <c r="R9" s="3"/>
@@ -3673,7 +3888,7 @@
       </c>
       <c r="H10" s="7">
         <f>SUM(H7:H9)</f>
-        <v>0.69</v>
+        <v>0.17899000000000004</v>
       </c>
       <c r="I10" s="7">
         <f>SUM(I7:I9)</f>
@@ -3686,7 +3901,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7">
         <f>SUM(L7:L9)</f>
-        <v>2606.363175</v>
+        <v>2605.8521649999993</v>
       </c>
       <c r="M10" s="6"/>
       <c r="R10" s="3"/>
@@ -3717,7 +3932,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="1" sqref="A12:XFD12 A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="1" sqref="A2:XFD2 A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3816,8 +4031,8 @@
         <v>0.42185</v>
       </c>
       <c r="H2" s="3">
-        <f>2.51*(F2/SUM(F2:F4))</f>
-        <v>0.41303797468354425</v>
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
       </c>
       <c r="I2" s="3">
         <v>15.99</v>
@@ -3828,7 +4043,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2</f>
-        <v>1550.8248879746834</v>
+        <v>1550.5192299999999</v>
       </c>
       <c r="M2" s="6"/>
       <c r="R2" s="3"/>
@@ -3868,8 +4083,8 @@
         <v>1.3854500000000001</v>
       </c>
       <c r="H3" s="3">
-        <f>2.51*(F3/SUM(F2:F4))</f>
-        <v>1.3565093327612099</v>
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.35266000000000003</v>
       </c>
       <c r="I3" s="3">
         <v>15.99</v>
@@ -3880,7 +4095,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3</f>
-        <v>5056.7319593327611</v>
+        <v>5055.7281099999991</v>
       </c>
       <c r="M3" s="6"/>
       <c r="R3" s="3"/>
@@ -3920,8 +4135,8 @@
         <v>0.75625000000000009</v>
       </c>
       <c r="H4" s="3">
-        <f>2.51*(F4/SUM(F2:F4))</f>
-        <v>0.74045269255524548</v>
+        <f t="shared" si="1"/>
+        <v>0.19250000000000003</v>
       </c>
       <c r="I4" s="3">
         <v>15.99</v>
@@ -3932,7 +4147,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3">
         <f>F4+G4+H4+I4</f>
-        <v>2767.4867026925549</v>
+        <v>2766.9387499999998</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -3960,7 +4175,7 @@
       </c>
       <c r="H5" s="7">
         <f>SUM(H2:H4)</f>
-        <v>2.5099999999999998</v>
+        <v>0.65254000000000012</v>
       </c>
       <c r="I5" s="7">
         <f>SUM(I2:I4)</f>
@@ -3973,7 +4188,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7">
         <f>SUM(L2:L4)</f>
-        <v>9375.0435499999985</v>
+        <v>9373.1860899999992</v>
       </c>
       <c r="M5" s="6"/>
       <c r="R5" s="3"/>
@@ -4036,8 +4251,8 @@
         <v>7.3700000000000002E-2</v>
       </c>
       <c r="H7" s="3">
-        <f>0.69*(F7/SUM(F7:F9))</f>
-        <v>7.2319123973406341E-2</v>
+        <f>F7*0.007%</f>
+        <v>1.8760000000000002E-2</v>
       </c>
       <c r="I7" s="3">
         <v>15.99</v>
@@ -4048,7 +4263,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3">
         <f>F7+G7+H7+I7</f>
-        <v>284.13601912397337</v>
+        <v>284.08245999999997</v>
       </c>
       <c r="M7" s="6"/>
       <c r="R7" s="3"/>
@@ -4084,12 +4299,12 @@
         <v>1520</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" ref="G8:G9" si="1">F8*0.0275%</f>
+        <f t="shared" ref="G8:G9" si="2">F8*0.0275%</f>
         <v>0.41800000000000004</v>
       </c>
       <c r="H8" s="3">
-        <f>0.69*(F8/SUM(F7:F9))</f>
-        <v>0.41016816581931947</v>
+        <f t="shared" ref="H8:H9" si="3">F8*0.007%</f>
+        <v>0.10640000000000001</v>
       </c>
       <c r="I8" s="3">
         <v>15.99</v>
@@ -4100,7 +4315,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3">
         <f>F8+G8+H8+I8</f>
-        <v>1536.8181681658193</v>
+        <v>1536.5143999999998</v>
       </c>
       <c r="M8" s="6"/>
       <c r="R8" s="3"/>
@@ -4136,12 +4351,12 @@
         <v>769</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.21147500000000002</v>
       </c>
       <c r="H9" s="3">
-        <f>0.69*(F9/SUM(F7:F9))</f>
-        <v>0.20751271020727413</v>
+        <f t="shared" si="3"/>
+        <v>5.3830000000000003E-2</v>
       </c>
       <c r="I9" s="3">
         <v>15.99</v>
@@ -4152,7 +4367,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3">
         <f>F9+G9+H9+I9</f>
-        <v>785.40898771020727</v>
+        <v>785.25530499999991</v>
       </c>
       <c r="M9" s="6"/>
       <c r="R9" s="3"/>
@@ -4180,7 +4395,7 @@
       </c>
       <c r="H10" s="7">
         <f>SUM(H7:H9)</f>
-        <v>0.69</v>
+        <v>0.17899000000000004</v>
       </c>
       <c r="I10" s="7">
         <f>SUM(I7:I9)</f>
@@ -4193,7 +4408,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7">
         <f>SUM(L7:L9)</f>
-        <v>2606.363175</v>
+        <v>2605.8521649999993</v>
       </c>
       <c r="M10" s="6"/>
       <c r="R10" s="3"/>
@@ -4256,8 +4471,8 @@
         <v>1.9332500000000001</v>
       </c>
       <c r="H12" s="8">
-        <f>5.53*(F12/SUM(F12:F14))</f>
-        <v>2.0022610218376595</v>
+        <f>F12*0.007%</f>
+        <v>0.49210000000000004</v>
       </c>
       <c r="I12" s="8">
         <v>15.99</v>
@@ -4270,7 +4485,7 @@
       </c>
       <c r="L12" s="8">
         <f>F12-G12-H12-I12-K12</f>
-        <v>7010.0744889781627</v>
+        <v>7011.5846499999998</v>
       </c>
       <c r="M12" s="6"/>
       <c r="R12" s="8"/>
@@ -4306,12 +4521,12 @@
         <v>6895.9999999999991</v>
       </c>
       <c r="G13" s="8">
-        <f t="shared" ref="G13:G14" si="2">F13*0.0275%</f>
+        <f t="shared" ref="G13:G14" si="4">F13*0.0275%</f>
         <v>1.8963999999999999</v>
       </c>
       <c r="H13" s="8">
-        <f>5.53*(F13/SUM(F12:F14))</f>
-        <v>1.964095591264936</v>
+        <f t="shared" ref="H13:H14" si="5">F13*0.007%</f>
+        <v>0.48271999999999998</v>
       </c>
       <c r="I13" s="8">
         <v>15.99</v>
@@ -4324,7 +4539,7 @@
       </c>
       <c r="L13" s="8">
         <f>F13-G13-H13-I13-K13</f>
-        <v>6876.1495044087351</v>
+        <v>6877.6308799999997</v>
       </c>
       <c r="M13" s="6"/>
       <c r="R13" s="8"/>
@@ -4360,12 +4575,12 @@
         <v>5490</v>
       </c>
       <c r="G14" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5097500000000001</v>
       </c>
       <c r="H14" s="8">
-        <f>5.53*(F14/SUM(F12:F14))</f>
-        <v>1.5636433868974042</v>
+        <f t="shared" si="5"/>
+        <v>0.38430000000000003</v>
       </c>
       <c r="I14" s="8">
         <v>15.99</v>
@@ -4378,7 +4593,7 @@
       </c>
       <c r="L14" s="8">
         <f>F14-G14-H14-I14-K14</f>
-        <v>5470.9366066131024</v>
+        <v>5472.1159500000003</v>
       </c>
       <c r="M14" s="6"/>
       <c r="R14" s="8"/>
@@ -4406,7 +4621,7 @@
       </c>
       <c r="H15" s="11">
         <f>SUM(H12:H14)</f>
-        <v>5.5299999999999994</v>
+        <v>1.3591200000000001</v>
       </c>
       <c r="I15" s="11">
         <f>SUM(I12:I14)</f>
@@ -4419,7 +4634,7 @@
       <c r="K15" s="11"/>
       <c r="L15" s="11">
         <f>SUM(L12:L14)</f>
-        <v>19357.160600000003</v>
+        <v>19361.331480000001</v>
       </c>
       <c r="M15" s="6"/>
       <c r="R15" s="8"/>
@@ -4459,8 +4674,8 @@
         <v>3.5887500000000001</v>
       </c>
       <c r="H17" s="8">
-        <f>7.17*(F17/SUM(F17:F18))</f>
-        <v>3.7174612634088202</v>
+        <f>F17*0.007%</f>
+        <v>0.91350000000000009</v>
       </c>
       <c r="I17" s="8">
         <v>15.99</v>
@@ -4474,7 +4689,7 @@
       </c>
       <c r="L17" s="8">
         <f>F17-G17-H17-I17-K17</f>
-        <v>13026.055695768773</v>
+        <v>13028.859657032181</v>
       </c>
       <c r="M17" s="6"/>
       <c r="R17" s="8"/>
@@ -4514,8 +4729,8 @@
         <v>3.3330000000000002</v>
       </c>
       <c r="H18" s="8">
-        <f>7.17*(F18/SUM(F17:F18))</f>
-        <v>3.4525387365911802</v>
+        <f>F18*0.007%</f>
+        <v>0.84840000000000004</v>
       </c>
       <c r="I18" s="8">
         <v>15.99</v>
@@ -4529,7 +4744,7 @@
       </c>
       <c r="L18" s="8">
         <f>F18-G18-H18-I18-K18</f>
-        <v>12096.622554231226</v>
+        <v>12099.226692967817</v>
       </c>
       <c r="M18" s="6"/>
       <c r="R18" s="8"/>
@@ -4548,32 +4763,32 @@
       <c r="A19" s="10"/>
       <c r="E19" s="8"/>
       <c r="F19" s="11">
-        <f t="shared" ref="F19:L19" si="3">SUM(F17:F18)</f>
+        <f t="shared" ref="F19:L19" si="6">SUM(F17:F18)</f>
         <v>25170</v>
       </c>
       <c r="G19" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.9217500000000003</v>
       </c>
       <c r="H19" s="11">
-        <f t="shared" si="3"/>
-        <v>7.17</v>
+        <f t="shared" si="6"/>
+        <v>1.7619000000000002</v>
       </c>
       <c r="I19" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>31.98</v>
       </c>
       <c r="J19" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.6</v>
       </c>
       <c r="K19" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.25</v>
       </c>
       <c r="L19" s="11">
-        <f t="shared" si="3"/>
-        <v>25122.678249999997</v>
+        <f t="shared" si="6"/>
+        <v>25128.086349999998</v>
       </c>
       <c r="M19" s="6"/>
       <c r="R19" s="8"/>

</xml_diff>

<commit_message>
Fails when trying to create a 'BrokerageNotesWorksheetReader' from a 'Worksheet' whose 'Line's have 'Cell's whose values are supposed to have been calculated from other 'Cell's but, do not pass the recalculation test. Here, specifically, the 'ServiceTax', which should equal the 'Brokerage' * 'ServiceTaxRate' at 'TradingDate' in 'BrokerCity'.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12906ED-76D2-447D-82AC-69D08F46AD13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B219AEF-9C10-47D4-9551-998A40515F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" firstSheet="10" activeTab="11" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="11" activeTab="12" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId10"/>
     <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId11"/>
     <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId12"/>
+    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -104,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="24">
   <si>
     <t>BBAS3</t>
   </si>
@@ -1246,7 +1247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
@@ -1434,6 +1435,218 @@
       <c r="L4" s="7">
         <f t="shared" si="2"/>
         <v>22611.028699999995</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1583F5-F968-4E69-BCCF-4B8530FA0CCB}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" ref="J2:J3" si="1">I3*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>SUM(F2:F3)</f>
+        <v>22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.24934999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="2"/>
+        <v>22611.00935</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>

</xml_diff>

<commit_message>
Fails when trying to create a 'BrokerageNotesWorksheetReader' from a 'Worksheet' whose 'Line's have 'Cell's whose values are supposed to have been calculated from other 'Cell's but, do not pass the recalculation test. Here, specifically, the 'IncomeTaxAtSource', which, for 'SellingOperations', should equal (('Volume' - 'SettlementFee' - 'NegotiationFees' - 'Brokerage' - 'ServiceTax') - ('AverageStockPrice' for the 'Ticker' * 'Qty')) * 'IncomeTaxAtSourceRate' for the 'OperationalMode' when 'OperationalMode' is 'Normal'.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B219AEF-9C10-47D4-9551-998A40515F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65D73CB-2958-4AD5-AFD4-9F81091AD4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="11" activeTab="12" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="7" activeTab="7" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId11"/>
     <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId12"/>
     <sheet name="InvalidServiceTax" sheetId="18" r:id="rId13"/>
+    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -104,8 +105,31 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Andrei Diego Cardoso</author>
+  </authors>
+  <commentList>
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{D2A4F95B-CDBE-432B-B036-B0291D562E73}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>=((F2 - G2 - H2 - I2 - J2) - (O12 * D2)) * 0,005%</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="23">
   <si>
     <t>BBAS3</t>
   </si>
@@ -123,9 +147,6 @@
   </si>
   <si>
     <t>KLBN4</t>
-  </si>
-  <si>
-    <t>MMXM3</t>
   </si>
   <si>
     <t>RDCD3</t>
@@ -183,11 +204,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +273,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -278,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -299,6 +341,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,40 +702,40 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC1" s="18"/>
     </row>
@@ -786,40 +831,40 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC1" s="16"/>
     </row>
@@ -938,7 +983,7 @@
         <v>1462</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="9">
         <v>200</v>
@@ -1075,40 +1120,40 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC1" s="16"/>
     </row>
@@ -1120,7 +1165,7 @@
         <v>85060</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="4">
         <v>400</v>
@@ -1160,7 +1205,7 @@
         <v>85060</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="4">
         <v>500</v>
@@ -1287,40 +1332,40 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC1" s="16"/>
     </row>
@@ -1332,7 +1377,7 @@
         <v>85060</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="4">
         <v>400</v>
@@ -1372,7 +1417,7 @@
         <v>85060</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="4">
         <v>500</v>
@@ -1459,7 +1504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1583F5-F968-4E69-BCCF-4B8530FA0CCB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
@@ -1499,40 +1544,40 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC1" s="16"/>
     </row>
@@ -1544,7 +1589,7 @@
         <v>85060</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="4">
         <v>400</v>
@@ -1584,7 +1629,7 @@
         <v>85060</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="4">
         <v>500</v>
@@ -1608,7 +1653,7 @@
         <v>1.99</v>
       </c>
       <c r="J3" s="3">
-        <f t="shared" ref="J2:J3" si="1">I3*6.5%</f>
+        <f t="shared" ref="J3" si="1">I3*6.5%</f>
         <v>0.12934999999999999</v>
       </c>
       <c r="K3" s="3"/>
@@ -1664,6 +1709,445 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
+  <dimension ref="A1:AC13"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9">
+        <v>200</v>
+      </c>
+      <c r="E2" s="8">
+        <v>40</v>
+      </c>
+      <c r="F2" s="8">
+        <f>D2*E2</f>
+        <v>8000</v>
+      </c>
+      <c r="G2" s="8">
+        <f>F2*0.0275%</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H2" s="8">
+        <f>F2*0.007%</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I2" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="L2" s="8">
+        <f>F2-G2-H2-I2-K2</f>
+        <v>7981.06</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9">
+        <v>200</v>
+      </c>
+      <c r="E3" s="8">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3*E3</f>
+        <v>6895.9999999999991</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.8963999999999999</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.48271999999999998</v>
+      </c>
+      <c r="I3" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="8">
+        <f>((F3 - G3 - H3 - I3 - J3) - (18.5 * D3)) * 0.005%</f>
+        <v>0.15884154399999997</v>
+      </c>
+      <c r="L3" s="8">
+        <f>F3-G3-H3-I3-K3</f>
+        <v>6877.4720384559996</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="9">
+        <v>200</v>
+      </c>
+      <c r="E4" s="8">
+        <v>27.45</v>
+      </c>
+      <c r="F4" s="8">
+        <f>D4*E4</f>
+        <v>5490</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5097500000000001</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" si="1"/>
+        <v>0.38430000000000003</v>
+      </c>
+      <c r="I4" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="8">
+        <f>((F4 - G4 - H4 - I4 - J4) - (22.3 * D4)) * 0.005%</f>
+        <v>5.0565797500000009E-2</v>
+      </c>
+      <c r="L4" s="8">
+        <f>F4-G4-H4-I4-K4</f>
+        <v>5472.0653842025004</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="11">
+        <f t="shared" ref="F5:L5" si="2">SUM(F2:F4)</f>
+        <v>20386</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="2"/>
+        <v>5.6061500000000004</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="2"/>
+        <v>1.4270200000000002</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="2"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="2"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="2"/>
+        <v>0.39940734150000001</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="2"/>
+        <v>20330.597422658502</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E9" s="20">
+        <v>100</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2750</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="I9" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K9" s="1">
+        <f>F9-G9-H9-I9-J9</f>
+        <v>2732.2500000000005</v>
+      </c>
+      <c r="L9" s="1">
+        <f>L8+K9</f>
+        <v>2732.2500000000005</v>
+      </c>
+      <c r="N9" s="20">
+        <f>N8+E9</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E10" s="20">
+        <v>200</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5940</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.47</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I10" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" ref="K10:K12" si="3">F10-G10-H10-I10-J10</f>
+        <v>5921.1399999999994</v>
+      </c>
+      <c r="L10" s="1">
+        <f>L9+K10</f>
+        <v>8653.39</v>
+      </c>
+      <c r="N10" s="20">
+        <f>N9+E10</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E11" s="20">
+        <v>-200</v>
+      </c>
+      <c r="F11" s="1">
+        <v>6630</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1.89</v>
+      </c>
+      <c r="I11" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="3"/>
+        <v>6610.9299999999994</v>
+      </c>
+      <c r="L11" s="1">
+        <f>L10+((L10/N10)*E11)</f>
+        <v>2884.4633333333331</v>
+      </c>
+      <c r="N11" s="20">
+        <f>N10+E11</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E12" s="20">
+        <v>200</v>
+      </c>
+      <c r="F12" s="1">
+        <v>6400</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1.82</v>
+      </c>
+      <c r="I12" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="3"/>
+        <v>6381.01</v>
+      </c>
+      <c r="L12" s="21">
+        <f>L11+K12</f>
+        <v>9265.4733333333334</v>
+      </c>
+      <c r="N12" s="22">
+        <f>N11+E12</f>
+        <v>300</v>
+      </c>
+      <c r="O12" s="1">
+        <f>L12/N12</f>
+        <v>30.884911111111112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E13" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1713,40 +2197,40 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC1" s="18"/>
     </row>
@@ -2143,40 +2627,40 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC1" s="18"/>
     </row>
@@ -2573,40 +3057,40 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC1" s="18"/>
     </row>
@@ -2865,40 +3349,40 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC1" s="18"/>
     </row>
@@ -3104,40 +3588,40 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC1" s="18"/>
     </row>
@@ -3675,40 +4159,40 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC1" s="18"/>
     </row>
@@ -3940,7 +4424,7 @@
         <v>1344</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="4">
         <v>100</v>
@@ -4142,10 +4626,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="1" sqref="A2:XFD2 A12:XFD12"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4159,11 +4643,11 @@
     <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
     <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
@@ -4182,40 +4666,40 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC1" s="16"/>
     </row>
@@ -4447,7 +4931,7 @@
         <v>1344</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="4">
         <v>100</v>
@@ -4694,11 +5178,12 @@
         <v>0.8</v>
       </c>
       <c r="K12" s="8">
-        <v>0</v>
+        <f>((F12 - G12 - H12 - I12 - J12) - (30.88 * D12)) * 0.005%</f>
+        <v>4.173923249999998E-2</v>
       </c>
       <c r="L12" s="8">
         <f>F12-G12-H12-I12-K12</f>
-        <v>7011.5846499999998</v>
+        <v>7011.5429107675</v>
       </c>
       <c r="M12" s="6"/>
       <c r="R12" s="8"/>
@@ -4721,7 +5206,7 @@
         <v>1462</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D13" s="9">
         <v>200</v>
@@ -4748,11 +5233,12 @@
         <v>0.8</v>
       </c>
       <c r="K13" s="8">
-        <v>0</v>
+        <f>((F13 - G13 - H13 - I13 - J13) - (30.88 * D13)) * 0.005%</f>
+        <v>3.504154399999998E-2</v>
       </c>
       <c r="L13" s="8">
         <f>F13-G13-H13-I13-K13</f>
-        <v>6877.6308799999997</v>
+        <v>6877.5958384559999</v>
       </c>
       <c r="M13" s="6"/>
       <c r="R13" s="8"/>
@@ -4775,25 +5261,25 @@
         <v>1462</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D14" s="9">
         <v>200</v>
       </c>
       <c r="E14" s="8">
-        <v>27.45</v>
+        <v>31</v>
       </c>
       <c r="F14" s="8">
         <f>D14*E14</f>
-        <v>5490</v>
+        <v>6200</v>
       </c>
       <c r="G14" s="8">
         <f t="shared" si="4"/>
-        <v>1.5097500000000001</v>
+        <v>1.7050000000000001</v>
       </c>
       <c r="H14" s="8">
         <f t="shared" si="5"/>
-        <v>0.38430000000000003</v>
+        <v>0.43400000000000005</v>
       </c>
       <c r="I14" s="8">
         <v>15.99</v>
@@ -4802,11 +5288,12 @@
         <v>0.8</v>
       </c>
       <c r="K14" s="8">
-        <v>0</v>
+        <f>((F14 - G14 - H14 - I14 - J14) - (30.88 * D14)) * 0.005%</f>
+        <v>2.5354999999999567E-4</v>
       </c>
       <c r="L14" s="8">
         <f>F14-G14-H14-I14-K14</f>
-        <v>5472.1159500000003</v>
+        <v>6181.8707464500003</v>
       </c>
       <c r="M14" s="6"/>
       <c r="R14" s="8"/>
@@ -4826,15 +5313,15 @@
       <c r="E15" s="8"/>
       <c r="F15" s="11">
         <f>SUM(F12:F14)</f>
-        <v>19416</v>
+        <v>20126</v>
       </c>
       <c r="G15" s="11">
         <f>SUM(G12:G14)</f>
-        <v>5.3394000000000004</v>
+        <v>5.5346500000000001</v>
       </c>
       <c r="H15" s="11">
         <f>SUM(H12:H14)</f>
-        <v>1.3591200000000001</v>
+        <v>1.40882</v>
       </c>
       <c r="I15" s="11">
         <f>SUM(I12:I14)</f>
@@ -4844,10 +5331,13 @@
         <f>SUM(J12:J14)</f>
         <v>2.4000000000000004</v>
       </c>
-      <c r="K15" s="11"/>
+      <c r="K15" s="11">
+        <f>SUM(K12:K14)</f>
+        <v>7.7034326499999944E-2</v>
+      </c>
       <c r="L15" s="11">
         <f>SUM(L12:L14)</f>
-        <v>19361.331480000001</v>
+        <v>20071.009495673501</v>
       </c>
       <c r="M15" s="6"/>
       <c r="R15" s="8"/>
@@ -4870,25 +5360,25 @@
         <v>1171</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D17" s="9">
         <v>500</v>
       </c>
       <c r="E17" s="8">
-        <v>26.1</v>
+        <v>31</v>
       </c>
       <c r="F17" s="8">
         <f>D17*E17</f>
-        <v>13050</v>
+        <v>15500</v>
       </c>
       <c r="G17" s="8">
         <f>F17*0.0275%</f>
-        <v>3.5887500000000001</v>
+        <v>4.2625000000000002</v>
       </c>
       <c r="H17" s="8">
         <f>F17*0.007%</f>
-        <v>0.91350000000000009</v>
+        <v>1.0850000000000002</v>
       </c>
       <c r="I17" s="8">
         <v>15.99</v>
@@ -4897,12 +5387,12 @@
         <v>0.8</v>
       </c>
       <c r="K17" s="8">
-        <f>1.25*(F17/SUM(F17:F18))</f>
-        <v>0.64809296781883197</v>
+        <f>((F17 - G17 - H17 - I17 - J17) - (30.88 * D17)) * 0.005%</f>
+        <v>1.8931250000000547E-3</v>
       </c>
       <c r="L17" s="8">
         <f>F17-G17-H17-I17-K17</f>
-        <v>13028.859657032181</v>
+        <v>15478.660606875001</v>
       </c>
       <c r="M17" s="6"/>
       <c r="R17" s="8"/>
@@ -4925,25 +5415,25 @@
         <v>1171</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D18" s="9">
         <v>1000</v>
       </c>
       <c r="E18" s="8">
-        <v>12.12</v>
+        <v>31</v>
       </c>
       <c r="F18" s="8">
         <f>D18*E18</f>
-        <v>12120</v>
+        <v>31000</v>
       </c>
       <c r="G18" s="8">
         <f>F18*0.0275%</f>
-        <v>3.3330000000000002</v>
+        <v>8.5250000000000004</v>
       </c>
       <c r="H18" s="8">
         <f>F18*0.007%</f>
-        <v>0.84840000000000004</v>
+        <v>2.1700000000000004</v>
       </c>
       <c r="I18" s="8">
         <v>15.99</v>
@@ -4952,12 +5442,12 @@
         <v>0.8</v>
       </c>
       <c r="K18" s="8">
-        <f>1.25*(F18/SUM(F17:F18))</f>
-        <v>0.60190703218116803</v>
+        <f>((F18 - G18 - H18 - I18 - J18) - (30.88 * D18)) * 0.005%</f>
+        <v>4.625749999999971E-3</v>
       </c>
       <c r="L18" s="8">
         <f>F18-G18-H18-I18-K18</f>
-        <v>12099.226692967817</v>
+        <v>30973.310374249999</v>
       </c>
       <c r="M18" s="6"/>
       <c r="R18" s="8"/>
@@ -4977,15 +5467,15 @@
       <c r="E19" s="8"/>
       <c r="F19" s="11">
         <f t="shared" ref="F19:L19" si="6">SUM(F17:F18)</f>
-        <v>25170</v>
+        <v>46500</v>
       </c>
       <c r="G19" s="11">
         <f t="shared" si="6"/>
-        <v>6.9217500000000003</v>
+        <v>12.787500000000001</v>
       </c>
       <c r="H19" s="11">
         <f t="shared" si="6"/>
-        <v>1.7619000000000002</v>
+        <v>3.2550000000000008</v>
       </c>
       <c r="I19" s="11">
         <f t="shared" si="6"/>
@@ -4997,11 +5487,11 @@
       </c>
       <c r="K19" s="11">
         <f t="shared" si="6"/>
-        <v>1.25</v>
+        <v>6.5188750000000255E-3</v>
       </c>
       <c r="L19" s="11">
         <f t="shared" si="6"/>
-        <v>25128.086349999998</v>
+        <v>46451.970981125</v>
       </c>
       <c r="M19" s="6"/>
       <c r="R19" s="8"/>
@@ -5017,6 +5507,7 @@
       <c r="AB19" s="8"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5066,40 +5557,40 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC1" s="16"/>
     </row>
@@ -5111,7 +5602,7 @@
         <v>1430</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="9">
         <v>200</v>

</xml_diff>

<commit_message>
Fails when trying to create a 'BrokerageNotesWorksheetReader' from a 'Worksheet' whose 'Line's have 'Cell's whose values are supposed to have been calculated from other 'Cell's but, do not pass the recalculation test. Here, specifically, the 'IncomeTaxAtSource', which, for 'BuyiungOperations', should not be calculated and, therefore, should not contain values that are either non-currencies or non-zero.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65D73CB-2958-4AD5-AFD4-9F81091AD4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48641BFE-D91F-438B-9FBD-CFD6BED09FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="7" activeTab="7" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="15" activeTab="15" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -27,6 +27,8 @@
     <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId12"/>
     <sheet name="InvalidServiceTax" sheetId="18" r:id="rId13"/>
     <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId14"/>
+    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId15"/>
+    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -129,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="23">
   <si>
     <t>BBAS3</t>
   </si>
@@ -204,10 +206,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="166" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -320,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -344,6 +347,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2151,6 +2155,436 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F402F95-319A-4797-B7E1-F3EB07A82FDD}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="23">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>SUM(F2:F3)</f>
+        <v>22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="2"/>
+        <v>22611.018699999997</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A590E594-CB91-4439-95F2-7F159495761F}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>SUM(F2:F3)</f>
+        <v>22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="2"/>
+        <v>22611.018699999997</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03306DC6-EFFD-4226-8075-7FFC9D0F7B34}">
   <dimension ref="A1:AC14"/>
@@ -4626,10 +5060,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="1" sqref="A2:XFD2 A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5312,31 +5746,31 @@
       <c r="A15" s="10"/>
       <c r="E15" s="8"/>
       <c r="F15" s="11">
-        <f>SUM(F12:F14)</f>
+        <f t="shared" ref="F15:L15" si="6">SUM(F12:F14)</f>
         <v>20126</v>
       </c>
       <c r="G15" s="11">
-        <f>SUM(G12:G14)</f>
+        <f t="shared" si="6"/>
         <v>5.5346500000000001</v>
       </c>
       <c r="H15" s="11">
-        <f>SUM(H12:H14)</f>
+        <f t="shared" si="6"/>
         <v>1.40882</v>
       </c>
       <c r="I15" s="11">
-        <f>SUM(I12:I14)</f>
+        <f t="shared" si="6"/>
         <v>47.97</v>
       </c>
       <c r="J15" s="11">
-        <f>SUM(J12:J14)</f>
+        <f t="shared" si="6"/>
         <v>2.4000000000000004</v>
       </c>
       <c r="K15" s="11">
-        <f>SUM(K12:K14)</f>
+        <f t="shared" si="6"/>
         <v>7.7034326499999944E-2</v>
       </c>
       <c r="L15" s="11">
-        <f>SUM(L12:L14)</f>
+        <f t="shared" si="6"/>
         <v>20071.009495673501</v>
       </c>
       <c r="M15" s="6"/>
@@ -5466,31 +5900,31 @@
       <c r="A19" s="10"/>
       <c r="E19" s="8"/>
       <c r="F19" s="11">
-        <f t="shared" ref="F19:L19" si="6">SUM(F17:F18)</f>
+        <f t="shared" ref="F19:L19" si="7">SUM(F17:F18)</f>
         <v>46500</v>
       </c>
       <c r="G19" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12.787500000000001</v>
       </c>
       <c r="H19" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.2550000000000008</v>
       </c>
       <c r="I19" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>31.98</v>
       </c>
       <c r="J19" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6</v>
       </c>
       <c r="K19" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.5188750000000255E-3</v>
       </c>
       <c r="L19" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>46451.970981125</v>
       </c>
       <c r="M19" s="6"/>

</xml_diff>

<commit_message>
Fails when trying to create a 'BrokerageNotesWorksheetReader' from a 'Worksheet' whose 'Line's have 'Cell's whose values are supposed to have been calculated from other 'Cell's but, do not pass the recalculation test. Here, specifically, the 'Total', which, for 'SellingOperations', should equal the 'Volume' - 'SettlementFee' - 'NegotiationFees' - 'Brokerage' - 'ServiceTax'.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48641BFE-D91F-438B-9FBD-CFD6BED09FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD82A30-DC00-4BF8-A4F0-EC8ACE883D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="15" activeTab="15" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="7" activeTab="7" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId14"/>
     <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId15"/>
     <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId16"/>
+    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -131,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="23">
   <si>
     <t>BBAS3</t>
   </si>
@@ -1720,7 +1721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
   <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
@@ -2374,7 +2375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A590E594-CB91-4439-95F2-7F159495761F}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
@@ -2578,6 +2579,304 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34F43A8-C89C-44C0-BF29-1F8134A0151F}">
+  <dimension ref="A1:AC8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9">
+        <v>200</v>
+      </c>
+      <c r="E2" s="8">
+        <v>35.15</v>
+      </c>
+      <c r="F2" s="8">
+        <f>D2*E2</f>
+        <v>7030</v>
+      </c>
+      <c r="G2" s="8">
+        <f>F2*0.0275%</f>
+        <v>1.9332500000000001</v>
+      </c>
+      <c r="H2" s="8">
+        <f>F2*0.007%</f>
+        <v>0.49210000000000004</v>
+      </c>
+      <c r="I2" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="8">
+        <f>((F2 - G2 - H2 - I2 - J2) - (30.88 * D2)) * 0.005%</f>
+        <v>4.173923249999998E-2</v>
+      </c>
+      <c r="L2" s="8">
+        <v>7010.81</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9">
+        <v>200</v>
+      </c>
+      <c r="E3" s="8">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3*E3</f>
+        <v>6895.9999999999991</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.8963999999999999</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.48271999999999998</v>
+      </c>
+      <c r="I3" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="8">
+        <f>((F3 - G3 - H3 - I3 - J3) - (30.88 * D3)) * 0.005%</f>
+        <v>3.504154399999998E-2</v>
+      </c>
+      <c r="L3" s="8">
+        <f t="shared" ref="L3:L4" si="2">F3-G3-H3-I3-J3</f>
+        <v>6876.8308799999995</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9">
+        <v>200</v>
+      </c>
+      <c r="E4" s="8">
+        <v>31</v>
+      </c>
+      <c r="F4" s="8">
+        <f>D4*E4</f>
+        <v>6200</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" si="0"/>
+        <v>1.7050000000000001</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" si="1"/>
+        <v>0.43400000000000005</v>
+      </c>
+      <c r="I4" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="8">
+        <f>((F4 - G4 - H4 - I4 - J4) - (30.88 * D4)) * 0.005%</f>
+        <v>2.5354999999999567E-4</v>
+      </c>
+      <c r="L4" s="8">
+        <f t="shared" si="2"/>
+        <v>6181.0709999999999</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="11">
+        <f t="shared" ref="F5:L5" si="3">SUM(F2:F4)</f>
+        <v>20126</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="3"/>
+        <v>5.5346500000000001</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="3"/>
+        <v>1.40882</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="3"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="3"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="3"/>
+        <v>7.7034326499999944E-2</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="3"/>
+        <v>20068.711879999999</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E8" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -5060,10 +5359,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="1" sqref="A2:XFD2 A12:XFD12"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="1" sqref="A12:XFD12 A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5616,8 +5915,8 @@
         <v>4.173923249999998E-2</v>
       </c>
       <c r="L12" s="8">
-        <f>F12-G12-H12-I12-K12</f>
-        <v>7011.5429107675</v>
+        <f>F12-G12-H12-I12-J12</f>
+        <v>7010.7846499999996</v>
       </c>
       <c r="M12" s="6"/>
       <c r="R12" s="8"/>
@@ -5671,8 +5970,8 @@
         <v>3.504154399999998E-2</v>
       </c>
       <c r="L13" s="8">
-        <f>F13-G13-H13-I13-K13</f>
-        <v>6877.5958384559999</v>
+        <f t="shared" ref="L13:L14" si="6">F13-G13-H13-I13-J13</f>
+        <v>6876.8308799999995</v>
       </c>
       <c r="M13" s="6"/>
       <c r="R13" s="8"/>
@@ -5726,8 +6025,8 @@
         <v>2.5354999999999567E-4</v>
       </c>
       <c r="L14" s="8">
-        <f>F14-G14-H14-I14-K14</f>
-        <v>6181.8707464500003</v>
+        <f t="shared" si="6"/>
+        <v>6181.0709999999999</v>
       </c>
       <c r="M14" s="6"/>
       <c r="R14" s="8"/>
@@ -5746,32 +6045,32 @@
       <c r="A15" s="10"/>
       <c r="E15" s="8"/>
       <c r="F15" s="11">
-        <f t="shared" ref="F15:L15" si="6">SUM(F12:F14)</f>
+        <f t="shared" ref="F15:L15" si="7">SUM(F12:F14)</f>
         <v>20126</v>
       </c>
       <c r="G15" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.5346500000000001</v>
       </c>
       <c r="H15" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.40882</v>
       </c>
       <c r="I15" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>47.97</v>
       </c>
       <c r="J15" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4000000000000004</v>
       </c>
       <c r="K15" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.7034326499999944E-2</v>
       </c>
       <c r="L15" s="11">
-        <f t="shared" si="6"/>
-        <v>20071.009495673501</v>
+        <f t="shared" si="7"/>
+        <v>20068.686529999999</v>
       </c>
       <c r="M15" s="6"/>
       <c r="R15" s="8"/>
@@ -5825,8 +6124,8 @@
         <v>1.8931250000000547E-3</v>
       </c>
       <c r="L17" s="8">
-        <f>F17-G17-H17-I17-K17</f>
-        <v>15478.660606875001</v>
+        <f>F17-G17-H17-I17-J17</f>
+        <v>15477.862500000001</v>
       </c>
       <c r="M17" s="6"/>
       <c r="R17" s="8"/>
@@ -5880,8 +6179,8 @@
         <v>4.625749999999971E-3</v>
       </c>
       <c r="L18" s="8">
-        <f>F18-G18-H18-I18-K18</f>
-        <v>30973.310374249999</v>
+        <f>F18-G18-H18-I18-J18</f>
+        <v>30972.514999999999</v>
       </c>
       <c r="M18" s="6"/>
       <c r="R18" s="8"/>
@@ -5900,32 +6199,32 @@
       <c r="A19" s="10"/>
       <c r="E19" s="8"/>
       <c r="F19" s="11">
-        <f t="shared" ref="F19:L19" si="7">SUM(F17:F18)</f>
+        <f t="shared" ref="F19:L19" si="8">SUM(F17:F18)</f>
         <v>46500</v>
       </c>
       <c r="G19" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>12.787500000000001</v>
       </c>
       <c r="H19" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.2550000000000008</v>
       </c>
       <c r="I19" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>31.98</v>
       </c>
       <c r="J19" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.6</v>
       </c>
       <c r="K19" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6.5188750000000255E-3</v>
       </c>
       <c r="L19" s="11">
-        <f t="shared" si="7"/>
-        <v>46451.970981125</v>
+        <f t="shared" si="8"/>
+        <v>46450.377500000002</v>
       </c>
       <c r="M19" s="6"/>
       <c r="R19" s="8"/>

</xml_diff>

<commit_message>
Fails when trying to create a 'BrokerageNotesWorksheetReader' from a 'Worksheet' whose 'Line's have 'Cell's whose values are supposed to have been calculated from other 'Cell's but, do not pass the recalculation test. Here, specifically, the 'Total', which, for 'BuyingOperations', should equal 'Volume' + 'SettlementFee' + 'NegotiationFees' + 'Brokerage' + 'ServiceTax'.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD82A30-DC00-4BF8-A4F0-EC8ACE883D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B85EF3-62DD-43E6-AA77-8AF2F5F94807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="7" activeTab="7" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="6" activeTab="7" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId15"/>
     <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId16"/>
     <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId17"/>
+    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -132,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="23">
   <si>
     <t>BBAS3</t>
   </si>
@@ -2884,6 +2885,218 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5AE87-00E8-4CF9-A517-EB6C0CA40610}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3">
+        <v>11005.45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>SUM(F2:F3)</f>
+        <v>22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="2"/>
+        <v>22611.049350000001</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03306DC6-EFFD-4226-8075-7FFC9D0F7B34}">
   <dimension ref="A1:AC14"/>
@@ -3751,7 +3964,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:B3"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="1" sqref="A3 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3863,8 +4076,8 @@
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3">
-        <f>F2+G2+H2+I2</f>
-        <v>1550.5192299999999</v>
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
       </c>
       <c r="M2" s="6"/>
       <c r="R2" s="3"/>
@@ -3915,8 +4128,8 @@
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3">
-        <f>F3+G3+H3+I3</f>
-        <v>5055.7281099999991</v>
+        <f>F3+G3+H3+I3+J3</f>
+        <v>5056.5281099999993</v>
       </c>
       <c r="M3" s="6"/>
       <c r="R3" s="3"/>
@@ -3967,8 +4180,8 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3">
-        <f>F4+G4+H4+I4</f>
-        <v>2766.9387499999998</v>
+        <f>F4+G4+H4+I4+J4</f>
+        <v>2767.73875</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -4009,7 +4222,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7">
         <f>SUM(L2:L4)</f>
-        <v>9373.1860899999992</v>
+        <v>9375.5860899999989</v>
       </c>
       <c r="M5" s="6"/>
       <c r="R5" s="3"/>
@@ -4394,8 +4607,8 @@
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3">
-        <f>F2+G2+H2+I2</f>
-        <v>1550.5192299999999</v>
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
       </c>
       <c r="M2" s="6"/>
       <c r="R2" s="3"/>
@@ -4446,8 +4659,8 @@
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3">
-        <f>F3+G3+H3+I3</f>
-        <v>5055.7281099999991</v>
+        <f t="shared" ref="L3:L4" si="2">F3+G3+H3+I3+J3</f>
+        <v>5056.5281099999993</v>
       </c>
       <c r="M3" s="6"/>
       <c r="R3" s="3"/>
@@ -4498,8 +4711,8 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3">
-        <f>F4+G4+H4+I4</f>
-        <v>2766.9387499999998</v>
+        <f t="shared" si="2"/>
+        <v>2767.73875</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -4540,7 +4753,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3">
         <f>SUM(L2:L4)</f>
-        <v>9373.1860899999992</v>
+        <v>9375.5860899999989</v>
       </c>
       <c r="M5" s="6"/>
       <c r="R5" s="3"/>
@@ -4614,8 +4827,8 @@
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3">
-        <f>F7+G7+H7+I7</f>
-        <v>1536.5143999999998</v>
+        <f>F7+G7+H7+I7+J7</f>
+        <v>1537.3143999999998</v>
       </c>
       <c r="M7" s="6"/>
       <c r="R7" s="3"/>
@@ -4666,8 +4879,8 @@
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3">
-        <f>F8+G8+H8+I8</f>
-        <v>785.25530499999991</v>
+        <f>F8+G8+H8+I8+J8</f>
+        <v>786.05530499999986</v>
       </c>
       <c r="M8" s="6"/>
       <c r="R8" s="3"/>
@@ -4708,7 +4921,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3">
         <f>SUM(L7:L8)</f>
-        <v>2321.7697049999997</v>
+        <v>2323.3697049999996</v>
       </c>
       <c r="M9" s="6"/>
       <c r="R9" s="3"/>
@@ -4965,8 +5178,8 @@
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3">
-        <f>F2+G2+H2+I2</f>
-        <v>1550.5192299999999</v>
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
       </c>
       <c r="M2" s="6"/>
       <c r="R2" s="3"/>
@@ -5017,8 +5230,8 @@
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3">
-        <f>F3+G3+H3+I3</f>
-        <v>5055.7281099999991</v>
+        <f>F3+G3+H3+I3+J3</f>
+        <v>5056.5281099999993</v>
       </c>
       <c r="M3" s="6"/>
       <c r="R3" s="3"/>
@@ -5069,8 +5282,8 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3">
-        <f>F4+G4+H4+I4</f>
-        <v>2766.9387499999998</v>
+        <f>F4+G4+H4+I4+J4</f>
+        <v>2767.73875</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -5111,7 +5324,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7">
         <f>SUM(L2:L4)</f>
-        <v>9373.1860899999992</v>
+        <v>9375.5860899999989</v>
       </c>
       <c r="M5" s="6"/>
       <c r="R5" s="3"/>
@@ -5185,8 +5398,8 @@
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3">
-        <f>F7+G7+H7+I7</f>
-        <v>284.08245999999997</v>
+        <f>F7+G7+H7+I7+J7</f>
+        <v>284.88245999999998</v>
       </c>
       <c r="M7" s="6"/>
       <c r="R7" s="3"/>
@@ -5237,8 +5450,8 @@
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3">
-        <f>F8+G8+H8+I8</f>
-        <v>1536.5143999999998</v>
+        <f>F8+G8+H8+I8+J8</f>
+        <v>1537.3143999999998</v>
       </c>
       <c r="M8" s="6"/>
       <c r="R8" s="3"/>
@@ -5289,8 +5502,8 @@
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3">
-        <f>F9+G9+H9+I9</f>
-        <v>785.25530499999991</v>
+        <f>F9+G9+H9+I9+J9</f>
+        <v>786.05530499999986</v>
       </c>
       <c r="M9" s="6"/>
       <c r="R9" s="3"/>
@@ -5331,7 +5544,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7">
         <f>SUM(L7:L9)</f>
-        <v>2605.8521649999993</v>
+        <v>2608.2521649999999</v>
       </c>
       <c r="M10" s="6"/>
       <c r="R10" s="3"/>
@@ -5362,7 +5575,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="1" sqref="A12:XFD12 A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="1" sqref="A2:XFD2 A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5472,8 +5685,8 @@
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3">
-        <f>F2+G2+H2+I2</f>
-        <v>1550.5192299999999</v>
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
       </c>
       <c r="M2" s="6"/>
       <c r="R2" s="3"/>
@@ -5524,8 +5737,8 @@
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3">
-        <f>F3+G3+H3+I3</f>
-        <v>5055.7281099999991</v>
+        <f>F3+G3+H3+I3+J3</f>
+        <v>5056.5281099999993</v>
       </c>
       <c r="M3" s="6"/>
       <c r="R3" s="3"/>
@@ -5576,8 +5789,8 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3">
-        <f>F4+G4+H4+I4</f>
-        <v>2766.9387499999998</v>
+        <f>F4+G4+H4+I4+J4</f>
+        <v>2767.73875</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -5618,7 +5831,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7">
         <f>SUM(L2:L4)</f>
-        <v>9373.1860899999992</v>
+        <v>9375.5860899999989</v>
       </c>
       <c r="M5" s="6"/>
       <c r="R5" s="3"/>
@@ -5692,8 +5905,8 @@
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3">
-        <f>F7+G7+H7+I7</f>
-        <v>284.08245999999997</v>
+        <f>F7+G7+H7+I7+J7</f>
+        <v>284.88245999999998</v>
       </c>
       <c r="M7" s="6"/>
       <c r="R7" s="3"/>
@@ -5744,8 +5957,8 @@
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3">
-        <f>F8+G8+H8+I8</f>
-        <v>1536.5143999999998</v>
+        <f>F8+G8+H8+I8+J8</f>
+        <v>1537.3143999999998</v>
       </c>
       <c r="M8" s="6"/>
       <c r="R8" s="3"/>
@@ -5796,8 +6009,8 @@
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3">
-        <f>F9+G9+H9+I9</f>
-        <v>785.25530499999991</v>
+        <f>F9+G9+H9+I9+J9</f>
+        <v>786.05530499999986</v>
       </c>
       <c r="M9" s="6"/>
       <c r="R9" s="3"/>
@@ -5838,7 +6051,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7">
         <f>SUM(L7:L9)</f>
-        <v>2605.8521649999993</v>
+        <v>2608.2521649999999</v>
       </c>
       <c r="M10" s="6"/>
       <c r="R10" s="3"/>

</xml_diff>

<commit_message>
Fails when trying to create a 'BrokerageNotesWorksheetReader' from a 'Worksheet' whose 'Groups' that contain more than one 'Operation' don't have a 'Summary'.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,29 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B85EF3-62DD-43E6-AA77-8AF2F5F94807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDF73BD-7883-494C-A9A6-27CD521804DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="6" activeTab="7" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="4" activeTab="4" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
     <sheet name="GroupWithDifferentTradingDates" sheetId="11" r:id="rId2"/>
     <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId3"/>
-    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId4"/>
-    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId5"/>
-    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId6"/>
-    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId7"/>
-    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId8"/>
-    <sheet name="SingleLineGroups" sheetId="10" r:id="rId9"/>
-    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId10"/>
-    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId11"/>
-    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId12"/>
-    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId13"/>
-    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId14"/>
-    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId15"/>
-    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId16"/>
-    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId17"/>
-    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId18"/>
+    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId4"/>
+    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId5"/>
+    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId6"/>
+    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId7"/>
+    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId8"/>
+    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId9"/>
+    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId10"/>
+    <sheet name="SingleLineGroups" sheetId="10" r:id="rId11"/>
+    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId12"/>
+    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId13"/>
+    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId14"/>
+    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId15"/>
+    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId16"/>
+    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId17"/>
+    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId18"/>
+    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId19"/>
+    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId20"/>
+    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -133,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="23">
   <si>
     <t>BBAS3</t>
   </si>
@@ -794,6 +797,1147 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
+  <dimension ref="A1:AC19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="1" sqref="A2:XFD2 A12:XFD12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>200</v>
+      </c>
+      <c r="E3" s="3">
+        <v>25.19</v>
+      </c>
+      <c r="F3" s="3">
+        <f>D3*E3</f>
+        <v>5038</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.3854500000000001</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.35266000000000003</v>
+      </c>
+      <c r="I3" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>5056.5281099999993</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4">
+        <v>100</v>
+      </c>
+      <c r="E4" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F4" s="3">
+        <f>D4*E4</f>
+        <v>2750</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.75625000000000009</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.19250000000000003</v>
+      </c>
+      <c r="I4" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3">
+        <f>F4+G4+H4+I4+J4</f>
+        <v>2767.73875</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="7">
+        <f>SUM(F2:F4)</f>
+        <v>9322</v>
+      </c>
+      <c r="G5" s="7">
+        <f>SUM(G2:G4)</f>
+        <v>2.5635500000000002</v>
+      </c>
+      <c r="H5" s="7">
+        <f>SUM(H2:H4)</f>
+        <v>0.65254000000000012</v>
+      </c>
+      <c r="I5" s="7">
+        <f>SUM(I2:I4)</f>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="7">
+        <f>SUM(J2:J4)</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7">
+        <f>SUM(L2:L4)</f>
+        <v>9375.5860899999989</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+    </row>
+    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="6"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+    </row>
+    <row r="7" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>39758</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1344</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4">
+        <v>100</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2.68</v>
+      </c>
+      <c r="F7" s="3">
+        <f>D7*E7</f>
+        <v>268</v>
+      </c>
+      <c r="G7" s="3">
+        <f>F7*0.0275%</f>
+        <v>7.3700000000000002E-2</v>
+      </c>
+      <c r="H7" s="3">
+        <f>F7*0.007%</f>
+        <v>1.8760000000000002E-2</v>
+      </c>
+      <c r="I7" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3">
+        <f>F7+G7+H7+I7+J7</f>
+        <v>284.88245999999998</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+    </row>
+    <row r="8" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>39758</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1344</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>100</v>
+      </c>
+      <c r="E8" s="3">
+        <v>15.2</v>
+      </c>
+      <c r="F8" s="3">
+        <f>D8*E8</f>
+        <v>1520</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" ref="G8:G9" si="2">F8*0.0275%</f>
+        <v>0.41800000000000004</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" ref="H8:H9" si="3">F8*0.007%</f>
+        <v>0.10640000000000001</v>
+      </c>
+      <c r="I8" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3">
+        <f>F8+G8+H8+I8+J8</f>
+        <v>1537.3143999999998</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+    </row>
+    <row r="9" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>39758</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1344</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4">
+        <v>100</v>
+      </c>
+      <c r="E9" s="3">
+        <v>7.69</v>
+      </c>
+      <c r="F9" s="3">
+        <f>D9*E9</f>
+        <v>769</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="2"/>
+        <v>0.21147500000000002</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="3"/>
+        <v>5.3830000000000003E-2</v>
+      </c>
+      <c r="I9" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3">
+        <f>F9+G9+H9+I9+J9</f>
+        <v>786.05530499999986</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+    </row>
+    <row r="10" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="7">
+        <f>SUM(F7:F9)</f>
+        <v>2557</v>
+      </c>
+      <c r="G10" s="7">
+        <f>SUM(G7:G9)</f>
+        <v>0.70317500000000011</v>
+      </c>
+      <c r="H10" s="7">
+        <f>SUM(H7:H9)</f>
+        <v>0.17899000000000004</v>
+      </c>
+      <c r="I10" s="7">
+        <f>SUM(I7:I9)</f>
+        <v>47.97</v>
+      </c>
+      <c r="J10" s="7">
+        <f>SUM(J7:J9)</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7">
+        <f>SUM(L7:L9)</f>
+        <v>2608.2521649999999</v>
+      </c>
+      <c r="M10" s="6"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+    </row>
+    <row r="11" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="6"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+    </row>
+    <row r="12" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B12" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="9">
+        <v>200</v>
+      </c>
+      <c r="E12" s="8">
+        <v>35.15</v>
+      </c>
+      <c r="F12" s="8">
+        <f>D12*E12</f>
+        <v>7030</v>
+      </c>
+      <c r="G12" s="8">
+        <f>F12*0.0275%</f>
+        <v>1.9332500000000001</v>
+      </c>
+      <c r="H12" s="8">
+        <f>F12*0.007%</f>
+        <v>0.49210000000000004</v>
+      </c>
+      <c r="I12" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K12" s="8">
+        <f>((F12 - G12 - H12 - I12 - J12) - (30.88 * D12)) * 0.005%</f>
+        <v>4.173923249999998E-2</v>
+      </c>
+      <c r="L12" s="8">
+        <f>F12-G12-H12-I12-J12</f>
+        <v>7010.7846499999996</v>
+      </c>
+      <c r="M12" s="6"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="8"/>
+    </row>
+    <row r="13" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B13" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="9">
+        <v>200</v>
+      </c>
+      <c r="E13" s="8">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="F13" s="8">
+        <f>D13*E13</f>
+        <v>6895.9999999999991</v>
+      </c>
+      <c r="G13" s="8">
+        <f t="shared" ref="G13:G14" si="4">F13*0.0275%</f>
+        <v>1.8963999999999999</v>
+      </c>
+      <c r="H13" s="8">
+        <f t="shared" ref="H13:H14" si="5">F13*0.007%</f>
+        <v>0.48271999999999998</v>
+      </c>
+      <c r="I13" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K13" s="8">
+        <f>((F13 - G13 - H13 - I13 - J13) - (30.88 * D13)) * 0.005%</f>
+        <v>3.504154399999998E-2</v>
+      </c>
+      <c r="L13" s="8">
+        <f t="shared" ref="L13:L14" si="6">F13-G13-H13-I13-J13</f>
+        <v>6876.8308799999995</v>
+      </c>
+      <c r="M13" s="6"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
+    </row>
+    <row r="14" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="9">
+        <v>200</v>
+      </c>
+      <c r="E14" s="8">
+        <v>31</v>
+      </c>
+      <c r="F14" s="8">
+        <f>D14*E14</f>
+        <v>6200</v>
+      </c>
+      <c r="G14" s="8">
+        <f t="shared" si="4"/>
+        <v>1.7050000000000001</v>
+      </c>
+      <c r="H14" s="8">
+        <f t="shared" si="5"/>
+        <v>0.43400000000000005</v>
+      </c>
+      <c r="I14" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J14" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K14" s="8">
+        <f>((F14 - G14 - H14 - I14 - J14) - (30.88 * D14)) * 0.005%</f>
+        <v>2.5354999999999567E-4</v>
+      </c>
+      <c r="L14" s="8">
+        <f t="shared" si="6"/>
+        <v>6181.0709999999999</v>
+      </c>
+      <c r="M14" s="6"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
+    </row>
+    <row r="15" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="11">
+        <f t="shared" ref="F15:L15" si="7">SUM(F12:F14)</f>
+        <v>20126</v>
+      </c>
+      <c r="G15" s="11">
+        <f t="shared" si="7"/>
+        <v>5.5346500000000001</v>
+      </c>
+      <c r="H15" s="11">
+        <f t="shared" si="7"/>
+        <v>1.40882</v>
+      </c>
+      <c r="I15" s="11">
+        <f t="shared" si="7"/>
+        <v>47.97</v>
+      </c>
+      <c r="J15" s="11">
+        <f t="shared" si="7"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K15" s="11">
+        <f t="shared" si="7"/>
+        <v>7.7034326499999944E-2</v>
+      </c>
+      <c r="L15" s="11">
+        <f t="shared" si="7"/>
+        <v>20068.686529999999</v>
+      </c>
+      <c r="M15" s="6"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="8"/>
+      <c r="AA15" s="8"/>
+      <c r="AB15" s="8"/>
+    </row>
+    <row r="17" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>40158</v>
+      </c>
+      <c r="B17" s="9">
+        <v>1171</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="9">
+        <v>500</v>
+      </c>
+      <c r="E17" s="8">
+        <v>31</v>
+      </c>
+      <c r="F17" s="8">
+        <f>D17*E17</f>
+        <v>15500</v>
+      </c>
+      <c r="G17" s="8">
+        <f>F17*0.0275%</f>
+        <v>4.2625000000000002</v>
+      </c>
+      <c r="H17" s="8">
+        <f>F17*0.007%</f>
+        <v>1.0850000000000002</v>
+      </c>
+      <c r="I17" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K17" s="8">
+        <f>((F17 - G17 - H17 - I17 - J17) - (30.88 * D17)) * 0.005%</f>
+        <v>1.8931250000000547E-3</v>
+      </c>
+      <c r="L17" s="8">
+        <f>F17-G17-H17-I17-J17</f>
+        <v>15477.862500000001</v>
+      </c>
+      <c r="M17" s="6"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="8"/>
+      <c r="AA17" s="8"/>
+      <c r="AB17" s="8"/>
+    </row>
+    <row r="18" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>40158</v>
+      </c>
+      <c r="B18" s="9">
+        <v>1171</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="9">
+        <v>1000</v>
+      </c>
+      <c r="E18" s="8">
+        <v>31</v>
+      </c>
+      <c r="F18" s="8">
+        <f>D18*E18</f>
+        <v>31000</v>
+      </c>
+      <c r="G18" s="8">
+        <f>F18*0.0275%</f>
+        <v>8.5250000000000004</v>
+      </c>
+      <c r="H18" s="8">
+        <f>F18*0.007%</f>
+        <v>2.1700000000000004</v>
+      </c>
+      <c r="I18" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J18" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K18" s="8">
+        <f>((F18 - G18 - H18 - I18 - J18) - (30.88 * D18)) * 0.005%</f>
+        <v>4.625749999999971E-3</v>
+      </c>
+      <c r="L18" s="8">
+        <f>F18-G18-H18-I18-J18</f>
+        <v>30972.514999999999</v>
+      </c>
+      <c r="M18" s="6"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+      <c r="Y18" s="8"/>
+      <c r="Z18" s="8"/>
+      <c r="AA18" s="8"/>
+      <c r="AB18" s="8"/>
+    </row>
+    <row r="19" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="11">
+        <f t="shared" ref="F19:L19" si="8">SUM(F17:F18)</f>
+        <v>46500</v>
+      </c>
+      <c r="G19" s="11">
+        <f t="shared" si="8"/>
+        <v>12.787500000000001</v>
+      </c>
+      <c r="H19" s="11">
+        <f t="shared" si="8"/>
+        <v>3.2550000000000008</v>
+      </c>
+      <c r="I19" s="11">
+        <f t="shared" si="8"/>
+        <v>31.98</v>
+      </c>
+      <c r="J19" s="11">
+        <f t="shared" si="8"/>
+        <v>1.6</v>
+      </c>
+      <c r="K19" s="11">
+        <f t="shared" si="8"/>
+        <v>6.5188750000000255E-3</v>
+      </c>
+      <c r="L19" s="11">
+        <f t="shared" si="8"/>
+        <v>46450.377500000002</v>
+      </c>
+      <c r="M19" s="6"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+      <c r="Y19" s="8"/>
+      <c r="Z19" s="8"/>
+      <c r="AA19" s="8"/>
+      <c r="AB19" s="8"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
+  <dimension ref="A1:AC6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="A6" activeCellId="2" sqref="A2:XFD2 A4:XFD4 A6:XFD6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>39959</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1430</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="9">
+        <v>200</v>
+      </c>
+      <c r="E2" s="8">
+        <v>23.4</v>
+      </c>
+      <c r="F2" s="8">
+        <f>D2*E2</f>
+        <v>4680</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1.33</v>
+      </c>
+      <c r="I2" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="L2" s="8">
+        <f>F2-G2-H2-I2</f>
+        <v>4662.4000000000005</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>39960</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1681</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9">
+        <v>200</v>
+      </c>
+      <c r="E4" s="8">
+        <v>34.04</v>
+      </c>
+      <c r="F4" s="8">
+        <f>D4*E4</f>
+        <v>6808</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="H4" s="8">
+        <v>1.94</v>
+      </c>
+      <c r="I4" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="8">
+        <v>0.34</v>
+      </c>
+      <c r="L4" s="8">
+        <f>F4-G4-H4-I4</f>
+        <v>6789.670000000001</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>39961</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1246</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E6" s="3">
+        <v>3.31</v>
+      </c>
+      <c r="F6" s="3">
+        <f>D6*E6</f>
+        <v>3310</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="I6" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3">
+        <f>F6+G6+H6+I6</f>
+        <v>3327.12</v>
+      </c>
+      <c r="M6" s="6"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7618D34E-0B33-4181-8E63-6765777C5B7E}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
@@ -1082,7 +2226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19EF43A-AB48-4760-8CB3-D62FBA7ABFD8}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -1294,7 +2438,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -1506,7 +2650,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1583F5-F968-4E69-BCCF-4B8530FA0CCB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -1718,7 +2862,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
   <dimension ref="A1:AC13"/>
   <sheetViews>
@@ -2157,7 +3301,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F402F95-319A-4797-B7E1-F3EB07A82FDD}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -2372,7 +3516,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A590E594-CB91-4439-95F2-7F159495761F}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -2587,7 +3731,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34F43A8-C89C-44C0-BF29-1F8134A0151F}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -2878,218 +4022,6 @@
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E8" s="22"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5AE87-00E8-4CF9-A517-EB6C0CA40610}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B2" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
-        <v>11000</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.025%</f>
-        <v>2.75</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3">
-        <v>11005.45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B3" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500</v>
-      </c>
-      <c r="E3" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" si="0"/>
-        <v>11600</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*0.025%</f>
-        <v>2.9</v>
-      </c>
-      <c r="H3" s="3">
-        <f>F3*0.005%</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>11605.599349999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7">
-        <f>SUM(F2:F3)</f>
-        <v>22600</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
-        <v>5.65</v>
-      </c>
-      <c r="H4" s="7">
-        <f t="shared" si="2"/>
-        <v>1.1300000000000001</v>
-      </c>
-      <c r="I4" s="7">
-        <f t="shared" si="2"/>
-        <v>3.98</v>
-      </c>
-      <c r="J4" s="7">
-        <f t="shared" si="2"/>
-        <v>0.25869999999999999</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="7">
-        <f t="shared" si="2"/>
-        <v>22611.049350000001</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3527,6 +4459,431 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5AE87-00E8-4CF9-A517-EB6C0CA40610}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3">
+        <v>11005.45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>SUM(F2:F3)</f>
+        <v>22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="2"/>
+        <v>22611.049350000001</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B51BEB4-905E-4036-959A-F9A0226AF070}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>SUM(F2:F3)</f>
+        <v>22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f>SUM(G2:G3) + 0.03</f>
+        <v>5.6800000000000006</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" ref="G4:L4" si="2">SUM(H2:H3)</f>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="2"/>
+        <v>22611.018699999997</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
   <dimension ref="A1:AC14"/>
@@ -3958,6 +5315,370 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F27D22B-36B9-402D-A19C-031FF2332945}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7579CBF-C87A-40BF-91B5-CE83CDC20ECE}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="F4" s="7">
+        <f>SUM(F1:F3)</f>
+        <v>22600</v>
+      </c>
+      <c r="G4" s="7">
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f>SUM(H1:H3)</f>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f>SUM(I1:I3)</f>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f>SUM(J1:J3)</f>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7">
+        <f>SUM(L1:L3)</f>
+        <v>22611.018699999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384BB7C-DF07-4187-ADF0-23E50C2BA287}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -4249,7 +5970,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EC0A3F-FFB0-437C-B726-EA72E0B69675}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -4488,7 +6209,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -5059,7 +6780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
@@ -5566,1145 +7287,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
-  <dimension ref="A1:AC19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="1" sqref="A2:XFD2 A12:XFD12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4">
-        <v>100</v>
-      </c>
-      <c r="E2" s="3">
-        <v>15.34</v>
-      </c>
-      <c r="F2" s="3">
-        <f>D2*E2</f>
-        <v>1534</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.0275%</f>
-        <v>0.42185</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.007%</f>
-        <v>0.10738000000000002</v>
-      </c>
-      <c r="I2" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>1551.3192299999998</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-    </row>
-    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" s="3">
-        <v>25.19</v>
-      </c>
-      <c r="F3" s="3">
-        <f>D3*E3</f>
-        <v>5038</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
-        <v>1.3854500000000001</v>
-      </c>
-      <c r="H3" s="3">
-        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
-        <v>0.35266000000000003</v>
-      </c>
-      <c r="I3" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>5056.5281099999993</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4">
-        <v>100</v>
-      </c>
-      <c r="E4" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F4" s="3">
-        <f>D4*E4</f>
-        <v>2750</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" si="0"/>
-        <v>0.75625000000000009</v>
-      </c>
-      <c r="H4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.19250000000000003</v>
-      </c>
-      <c r="I4" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3">
-        <f>F4+G4+H4+I4+J4</f>
-        <v>2767.73875</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="7">
-        <f>SUM(F2:F4)</f>
-        <v>9322</v>
-      </c>
-      <c r="G5" s="7">
-        <f>SUM(G2:G4)</f>
-        <v>2.5635500000000002</v>
-      </c>
-      <c r="H5" s="7">
-        <f>SUM(H2:H4)</f>
-        <v>0.65254000000000012</v>
-      </c>
-      <c r="I5" s="7">
-        <f>SUM(I2:I4)</f>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="7">
-        <f>SUM(J2:J4)</f>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7">
-        <f>SUM(L2:L4)</f>
-        <v>9375.5860899999989</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-    </row>
-    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="6"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-    </row>
-    <row r="7" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="4">
-        <v>100</v>
-      </c>
-      <c r="E7" s="3">
-        <v>2.68</v>
-      </c>
-      <c r="F7" s="3">
-        <f>D7*E7</f>
-        <v>268</v>
-      </c>
-      <c r="G7" s="3">
-        <f>F7*0.0275%</f>
-        <v>7.3700000000000002E-2</v>
-      </c>
-      <c r="H7" s="3">
-        <f>F7*0.007%</f>
-        <v>1.8760000000000002E-2</v>
-      </c>
-      <c r="I7" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3">
-        <f>F7+G7+H7+I7+J7</f>
-        <v>284.88245999999998</v>
-      </c>
-      <c r="M7" s="6"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-    </row>
-    <row r="8" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>100</v>
-      </c>
-      <c r="E8" s="3">
-        <v>15.2</v>
-      </c>
-      <c r="F8" s="3">
-        <f>D8*E8</f>
-        <v>1520</v>
-      </c>
-      <c r="G8" s="3">
-        <f t="shared" ref="G8:G9" si="2">F8*0.0275%</f>
-        <v>0.41800000000000004</v>
-      </c>
-      <c r="H8" s="3">
-        <f t="shared" ref="H8:H9" si="3">F8*0.007%</f>
-        <v>0.10640000000000001</v>
-      </c>
-      <c r="I8" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3">
-        <f>F8+G8+H8+I8+J8</f>
-        <v>1537.3143999999998</v>
-      </c>
-      <c r="M8" s="6"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-    </row>
-    <row r="9" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B9" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="4">
-        <v>100</v>
-      </c>
-      <c r="E9" s="3">
-        <v>7.69</v>
-      </c>
-      <c r="F9" s="3">
-        <f>D9*E9</f>
-        <v>769</v>
-      </c>
-      <c r="G9" s="3">
-        <f t="shared" si="2"/>
-        <v>0.21147500000000002</v>
-      </c>
-      <c r="H9" s="3">
-        <f t="shared" si="3"/>
-        <v>5.3830000000000003E-2</v>
-      </c>
-      <c r="I9" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3">
-        <f>F9+G9+H9+I9+J9</f>
-        <v>786.05530499999986</v>
-      </c>
-      <c r="M9" s="6"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-    </row>
-    <row r="10" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="7">
-        <f>SUM(F7:F9)</f>
-        <v>2557</v>
-      </c>
-      <c r="G10" s="7">
-        <f>SUM(G7:G9)</f>
-        <v>0.70317500000000011</v>
-      </c>
-      <c r="H10" s="7">
-        <f>SUM(H7:H9)</f>
-        <v>0.17899000000000004</v>
-      </c>
-      <c r="I10" s="7">
-        <f>SUM(I7:I9)</f>
-        <v>47.97</v>
-      </c>
-      <c r="J10" s="7">
-        <f>SUM(J7:J9)</f>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7">
-        <f>SUM(L7:L9)</f>
-        <v>2608.2521649999999</v>
-      </c>
-      <c r="M10" s="6"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
-      <c r="AB10" s="3"/>
-    </row>
-    <row r="11" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="6"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="3"/>
-      <c r="AB11" s="3"/>
-    </row>
-    <row r="12" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B12" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="9">
-        <v>200</v>
-      </c>
-      <c r="E12" s="8">
-        <v>35.15</v>
-      </c>
-      <c r="F12" s="8">
-        <f>D12*E12</f>
-        <v>7030</v>
-      </c>
-      <c r="G12" s="8">
-        <f>F12*0.0275%</f>
-        <v>1.9332500000000001</v>
-      </c>
-      <c r="H12" s="8">
-        <f>F12*0.007%</f>
-        <v>0.49210000000000004</v>
-      </c>
-      <c r="I12" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J12" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K12" s="8">
-        <f>((F12 - G12 - H12 - I12 - J12) - (30.88 * D12)) * 0.005%</f>
-        <v>4.173923249999998E-2</v>
-      </c>
-      <c r="L12" s="8">
-        <f>F12-G12-H12-I12-J12</f>
-        <v>7010.7846499999996</v>
-      </c>
-      <c r="M12" s="6"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="8"/>
-      <c r="X12" s="8"/>
-      <c r="Y12" s="8"/>
-      <c r="Z12" s="8"/>
-      <c r="AA12" s="8"/>
-      <c r="AB12" s="8"/>
-    </row>
-    <row r="13" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B13" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="9">
-        <v>200</v>
-      </c>
-      <c r="E13" s="8">
-        <v>34.479999999999997</v>
-      </c>
-      <c r="F13" s="8">
-        <f>D13*E13</f>
-        <v>6895.9999999999991</v>
-      </c>
-      <c r="G13" s="8">
-        <f t="shared" ref="G13:G14" si="4">F13*0.0275%</f>
-        <v>1.8963999999999999</v>
-      </c>
-      <c r="H13" s="8">
-        <f t="shared" ref="H13:H14" si="5">F13*0.007%</f>
-        <v>0.48271999999999998</v>
-      </c>
-      <c r="I13" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J13" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K13" s="8">
-        <f>((F13 - G13 - H13 - I13 - J13) - (30.88 * D13)) * 0.005%</f>
-        <v>3.504154399999998E-2</v>
-      </c>
-      <c r="L13" s="8">
-        <f t="shared" ref="L13:L14" si="6">F13-G13-H13-I13-J13</f>
-        <v>6876.8308799999995</v>
-      </c>
-      <c r="M13" s="6"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="8"/>
-      <c r="AA13" s="8"/>
-      <c r="AB13" s="8"/>
-    </row>
-    <row r="14" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B14" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="9">
-        <v>200</v>
-      </c>
-      <c r="E14" s="8">
-        <v>31</v>
-      </c>
-      <c r="F14" s="8">
-        <f>D14*E14</f>
-        <v>6200</v>
-      </c>
-      <c r="G14" s="8">
-        <f t="shared" si="4"/>
-        <v>1.7050000000000001</v>
-      </c>
-      <c r="H14" s="8">
-        <f t="shared" si="5"/>
-        <v>0.43400000000000005</v>
-      </c>
-      <c r="I14" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J14" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K14" s="8">
-        <f>((F14 - G14 - H14 - I14 - J14) - (30.88 * D14)) * 0.005%</f>
-        <v>2.5354999999999567E-4</v>
-      </c>
-      <c r="L14" s="8">
-        <f t="shared" si="6"/>
-        <v>6181.0709999999999</v>
-      </c>
-      <c r="M14" s="6"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="8"/>
-      <c r="AA14" s="8"/>
-      <c r="AB14" s="8"/>
-    </row>
-    <row r="15" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="11">
-        <f t="shared" ref="F15:L15" si="7">SUM(F12:F14)</f>
-        <v>20126</v>
-      </c>
-      <c r="G15" s="11">
-        <f t="shared" si="7"/>
-        <v>5.5346500000000001</v>
-      </c>
-      <c r="H15" s="11">
-        <f t="shared" si="7"/>
-        <v>1.40882</v>
-      </c>
-      <c r="I15" s="11">
-        <f t="shared" si="7"/>
-        <v>47.97</v>
-      </c>
-      <c r="J15" s="11">
-        <f t="shared" si="7"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K15" s="11">
-        <f t="shared" si="7"/>
-        <v>7.7034326499999944E-2</v>
-      </c>
-      <c r="L15" s="11">
-        <f t="shared" si="7"/>
-        <v>20068.686529999999</v>
-      </c>
-      <c r="M15" s="6"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="8"/>
-      <c r="Z15" s="8"/>
-      <c r="AA15" s="8"/>
-      <c r="AB15" s="8"/>
-    </row>
-    <row r="17" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
-        <v>40158</v>
-      </c>
-      <c r="B17" s="9">
-        <v>1171</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="9">
-        <v>500</v>
-      </c>
-      <c r="E17" s="8">
-        <v>31</v>
-      </c>
-      <c r="F17" s="8">
-        <f>D17*E17</f>
-        <v>15500</v>
-      </c>
-      <c r="G17" s="8">
-        <f>F17*0.0275%</f>
-        <v>4.2625000000000002</v>
-      </c>
-      <c r="H17" s="8">
-        <f>F17*0.007%</f>
-        <v>1.0850000000000002</v>
-      </c>
-      <c r="I17" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J17" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K17" s="8">
-        <f>((F17 - G17 - H17 - I17 - J17) - (30.88 * D17)) * 0.005%</f>
-        <v>1.8931250000000547E-3</v>
-      </c>
-      <c r="L17" s="8">
-        <f>F17-G17-H17-I17-J17</f>
-        <v>15477.862500000001</v>
-      </c>
-      <c r="M17" s="6"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="8"/>
-      <c r="Z17" s="8"/>
-      <c r="AA17" s="8"/>
-      <c r="AB17" s="8"/>
-    </row>
-    <row r="18" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>40158</v>
-      </c>
-      <c r="B18" s="9">
-        <v>1171</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="9">
-        <v>1000</v>
-      </c>
-      <c r="E18" s="8">
-        <v>31</v>
-      </c>
-      <c r="F18" s="8">
-        <f>D18*E18</f>
-        <v>31000</v>
-      </c>
-      <c r="G18" s="8">
-        <f>F18*0.0275%</f>
-        <v>8.5250000000000004</v>
-      </c>
-      <c r="H18" s="8">
-        <f>F18*0.007%</f>
-        <v>2.1700000000000004</v>
-      </c>
-      <c r="I18" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J18" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K18" s="8">
-        <f>((F18 - G18 - H18 - I18 - J18) - (30.88 * D18)) * 0.005%</f>
-        <v>4.625749999999971E-3</v>
-      </c>
-      <c r="L18" s="8">
-        <f>F18-G18-H18-I18-J18</f>
-        <v>30972.514999999999</v>
-      </c>
-      <c r="M18" s="6"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="8"/>
-      <c r="X18" s="8"/>
-      <c r="Y18" s="8"/>
-      <c r="Z18" s="8"/>
-      <c r="AA18" s="8"/>
-      <c r="AB18" s="8"/>
-    </row>
-    <row r="19" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="11">
-        <f t="shared" ref="F19:L19" si="8">SUM(F17:F18)</f>
-        <v>46500</v>
-      </c>
-      <c r="G19" s="11">
-        <f t="shared" si="8"/>
-        <v>12.787500000000001</v>
-      </c>
-      <c r="H19" s="11">
-        <f t="shared" si="8"/>
-        <v>3.2550000000000008</v>
-      </c>
-      <c r="I19" s="11">
-        <f t="shared" si="8"/>
-        <v>31.98</v>
-      </c>
-      <c r="J19" s="11">
-        <f t="shared" si="8"/>
-        <v>1.6</v>
-      </c>
-      <c r="K19" s="11">
-        <f t="shared" si="8"/>
-        <v>6.5188750000000255E-3</v>
-      </c>
-      <c r="L19" s="11">
-        <f t="shared" si="8"/>
-        <v>46450.377500000002</v>
-      </c>
-      <c r="M19" s="6"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="8"/>
-      <c r="V19" s="8"/>
-      <c r="W19" s="8"/>
-      <c r="X19" s="8"/>
-      <c r="Y19" s="8"/>
-      <c r="Z19" s="8"/>
-      <c r="AA19" s="8"/>
-      <c r="AB19" s="8"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
-  <dimension ref="A1:AC6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A6" activeCellId="2" sqref="A2:XFD2 A4:XFD4 A6:XFD6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>39959</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1430</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="9">
-        <v>200</v>
-      </c>
-      <c r="E2" s="8">
-        <v>23.4</v>
-      </c>
-      <c r="F2" s="8">
-        <f>D2*E2</f>
-        <v>4680</v>
-      </c>
-      <c r="G2" s="8">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="H2" s="8">
-        <v>1.33</v>
-      </c>
-      <c r="I2" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="8">
-        <v>0.23</v>
-      </c>
-      <c r="L2" s="8">
-        <f>F2-G2-H2-I2</f>
-        <v>4662.4000000000005</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>39960</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1681</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="9">
-        <v>200</v>
-      </c>
-      <c r="E4" s="8">
-        <v>34.04</v>
-      </c>
-      <c r="F4" s="8">
-        <f>D4*E4</f>
-        <v>6808</v>
-      </c>
-      <c r="G4" s="8">
-        <v>0.4</v>
-      </c>
-      <c r="H4" s="8">
-        <v>1.94</v>
-      </c>
-      <c r="I4" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="8">
-        <v>0.34</v>
-      </c>
-      <c r="L4" s="8">
-        <f>F4-G4-H4-I4</f>
-        <v>6789.670000000001</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>39961</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1246</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1000</v>
-      </c>
-      <c r="E6" s="3">
-        <v>3.31</v>
-      </c>
-      <c r="F6" s="3">
-        <f>D6*E6</f>
-        <v>3310</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.19</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.94</v>
-      </c>
-      <c r="I6" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3">
-        <f>F6+G6+H6+I6</f>
-        <v>3327.12</v>
-      </c>
-      <c r="M6" s="6"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fails when trying to create a 'BrokerageNotesWorksheetReader' from a 'Worksheet' whose 'Line's have 'Cell's whose values are supposed to have been calculated from other 'Cell's but, do not pass the recalculation test. Here, specifically, the 'NegotiationFees', which, for 'FinancialSummary's, should equal the sum of all 'Operation's 'NegotiationFees' in the 'BrokerageNote'.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDF73BD-7883-494C-A9A6-27CD521804DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67ACFB32-CFFC-45B1-A9C2-DC199AEB0737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="4" activeTab="4" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="20" activeTab="21" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -34,6 +34,7 @@
     <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId19"/>
     <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId20"/>
     <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId21"/>
+    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -136,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="23">
   <si>
     <t>BBAS3</t>
   </si>
@@ -4846,8 +4847,221 @@
         <v>5.6800000000000006</v>
       </c>
       <c r="H4" s="7">
-        <f t="shared" ref="G4:L4" si="2">SUM(H2:H3)</f>
+        <f t="shared" ref="H4:L4" si="2">SUM(H2:H3)</f>
         <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="2"/>
+        <v>22611.018699999997</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B7349E-D984-4817-800E-2EB4836D5B5D}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>SUM(F2:F3)</f>
+        <v>22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f>SUM(H2:H3) - 0.03</f>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" si="2"/>
@@ -5487,7 +5701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7579CBF-C87A-40BF-91B5-CE83CDC20ECE}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>

</xml_diff>

<commit_message>
Fails when trying to create a 'BrokerageNotesWorksheetReader' from a 'Worksheet' whose 'Line's have 'Cell's whose values are supposed to have been calculated from other 'Cell's but, do not pass the recalculation test. Here, specifically, the 'Brokerage', which, for 'FinancialSummary's, should equal the sum of all 'Operation's 'Brokerage' in the 'BrokerageNote'.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67ACFB32-CFFC-45B1-A9C2-DC199AEB0737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451F9DE6-583F-4556-8E4D-F20D2F26F335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="20" activeTab="21" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="21" activeTab="22" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId20"/>
     <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId21"/>
     <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId22"/>
+    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -137,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="23">
   <si>
     <t>BBAS3</t>
   </si>
@@ -4889,7 +4890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B7349E-D984-4817-800E-2EB4836D5B5D}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
@@ -5066,6 +5067,219 @@
       <c r="I4" s="7">
         <f t="shared" si="2"/>
         <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="2"/>
+        <v>22611.018699999997</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA65F892-A6B4-4288-ADB5-125D04E295EB}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>SUM(F2:F3)</f>
+        <v>22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f>SUM(H2:H3)</f>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f>SUM(I2:I3) - 0.03</f>
+        <v>3.95</v>
       </c>
       <c r="J4" s="7">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Fails when trying to create a 'BrokerageNotesWorksheetReader' from a 'Worksheet' whose 'Line's have 'Cell's whose values are supposed to have been calculated from other 'Cell's but, do not pass the recalculation test. Here, specifically, the 'ServiceTaxSummary', which, for 'FinancialSummary's, should equal the sum of all 'Operation's 'ServiceTax' in the 'BrokerageNote'.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451F9DE6-583F-4556-8E4D-F20D2F26F335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F35B850-4A60-4118-B377-7A10DD4CE07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="21" activeTab="22" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="22" activeTab="23" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId21"/>
     <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId22"/>
     <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId23"/>
+    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -138,7 +139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="23">
   <si>
     <t>BBAS3</t>
   </si>
@@ -5103,7 +5104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA65F892-A6B4-4288-ADB5-125D04E295EB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
@@ -5284,6 +5285,219 @@
       <c r="J4" s="7">
         <f t="shared" si="2"/>
         <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="2"/>
+        <v>22611.018699999997</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421F9D80-1D28-4F3C-95F7-8DE9883A26F0}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>SUM(F2:F3)</f>
+        <v>22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f>SUM(H2:H3)</f>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f>SUM(I2:I3)</f>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f>SUM(J2:J3) + 0.03</f>
+        <v>0.28869999999999996</v>
       </c>
       <c r="K4" s="7">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Fails when trying to create a 'BrokerageNotesWorksheetReader' from a 'Worksheet' whose 'Line's have 'Cell's whose values are supposed to have been calculated from other 'Cell's but, do not pass the recalculation test. Here, specifically, the 'IncomeTaxAtSource', which, for 'FinancialSummary's, should equal the sum of all 'Operation's 'IncomeTaxAtSource' in the 'BrokerageNote'.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F35B850-4A60-4118-B377-7A10DD4CE07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F834A58-39F1-41C7-A6F7-9558C21308AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="22" activeTab="23" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="8" activeTab="9" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -37,6 +37,7 @@
     <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId22"/>
     <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId23"/>
     <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId24"/>
+    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -139,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="23">
   <si>
     <t>BBAS3</t>
   </si>
@@ -803,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="A12" activeCellId="1" sqref="A2:XFD2 A12:XFD12"/>
@@ -914,7 +915,9 @@
       <c r="J2" s="3">
         <v>0.8</v>
       </c>
-      <c r="K2" s="3"/>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2+J2</f>
         <v>1551.3192299999998</v>
@@ -966,7 +969,9 @@
       <c r="J3" s="3">
         <v>0.8</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3+J3</f>
         <v>5056.5281099999993</v>
@@ -1018,7 +1023,9 @@
       <c r="J4" s="3">
         <v>0.8</v>
       </c>
-      <c r="K4" s="3"/>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
       <c r="L4" s="3">
         <f>F4+G4+H4+I4+J4</f>
         <v>2767.73875</v>
@@ -1059,7 +1066,10 @@
         <f>SUM(J2:J4)</f>
         <v>2.4000000000000004</v>
       </c>
-      <c r="K5" s="7"/>
+      <c r="K5" s="7">
+        <f>SUM(K2:K4)</f>
+        <v>0</v>
+      </c>
       <c r="L5" s="7">
         <f>SUM(L2:L4)</f>
         <v>9375.5860899999989</v>
@@ -1134,7 +1144,9 @@
       <c r="J7" s="3">
         <v>0.8</v>
       </c>
-      <c r="K7" s="3"/>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
       <c r="L7" s="3">
         <f>F7+G7+H7+I7+J7</f>
         <v>284.88245999999998</v>
@@ -1186,7 +1198,9 @@
       <c r="J8" s="3">
         <v>0.8</v>
       </c>
-      <c r="K8" s="3"/>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
       <c r="L8" s="3">
         <f>F8+G8+H8+I8+J8</f>
         <v>1537.3143999999998</v>
@@ -1238,7 +1252,9 @@
       <c r="J9" s="3">
         <v>0.8</v>
       </c>
-      <c r="K9" s="3"/>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
       <c r="L9" s="3">
         <f>F9+G9+H9+I9+J9</f>
         <v>786.05530499999986</v>
@@ -1279,7 +1295,10 @@
         <f>SUM(J7:J9)</f>
         <v>2.4000000000000004</v>
       </c>
-      <c r="K10" s="7"/>
+      <c r="K10" s="7">
+        <f>SUM(K7:K9)</f>
+        <v>0</v>
+      </c>
       <c r="L10" s="7">
         <f>SUM(L7:L9)</f>
         <v>2608.2521649999999</v>
@@ -2205,7 +2224,10 @@
         <f>SUM(J2:J4)</f>
         <v>2.4000000000000004</v>
       </c>
-      <c r="K5" s="11"/>
+      <c r="K5" s="11">
+        <f>SUM(K2:K4)</f>
+        <v>0</v>
+      </c>
       <c r="L5" s="11">
         <f>SUM(L2:L4)</f>
         <v>19361.349999999999</v>
@@ -2344,7 +2366,9 @@
         <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
         <v>0.12934999999999999</v>
       </c>
-      <c r="K2" s="3"/>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2+J2</f>
         <v>11005.429349999999</v>
@@ -2385,7 +2409,9 @@
         <f t="shared" si="1"/>
         <v>0.12934999999999999</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3+J3</f>
         <v>11605.599349999999</v>
@@ -2556,7 +2582,9 @@
         <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
         <v>0.12934999999999999</v>
       </c>
-      <c r="K2" s="3"/>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2+J2</f>
         <v>11005.429349999999</v>
@@ -2597,7 +2625,9 @@
         <f t="shared" si="1"/>
         <v>0.12934999999999999</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3+J3</f>
         <v>11605.599349999999</v>
@@ -2768,7 +2798,9 @@
       <c r="J2" s="3">
         <v>0.12</v>
       </c>
-      <c r="K2" s="3"/>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2+J2</f>
         <v>11005.41</v>
@@ -2809,7 +2841,9 @@
         <f t="shared" ref="J3" si="1">I3*6.5%</f>
         <v>0.12934999999999999</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3+J3</f>
         <v>11605.599349999999</v>
@@ -3463,7 +3497,9 @@
         <f t="shared" si="1"/>
         <v>0.12934999999999999</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3+J3</f>
         <v>11605.599349999999</v>
@@ -3678,7 +3714,9 @@
         <f t="shared" si="1"/>
         <v>0.12934999999999999</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3+J3</f>
         <v>11605.599349999999</v>
@@ -3741,7 +3779,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4149,6 +4187,9 @@
       <c r="J2" s="13">
         <v>0.8</v>
       </c>
+      <c r="K2" s="13">
+        <v>0</v>
+      </c>
       <c r="L2" s="13">
         <f>F2+G2+H2+I2</f>
         <v>1550.5248101265822</v>
@@ -4188,6 +4229,9 @@
       <c r="J3" s="13">
         <v>0.8</v>
       </c>
+      <c r="K3" s="13">
+        <v>0</v>
+      </c>
       <c r="L3" s="13">
         <f>F3+G3+H3+I3</f>
         <v>5055.7464363870413</v>
@@ -4226,6 +4270,9 @@
       </c>
       <c r="J4" s="13">
         <v>0.8</v>
+      </c>
+      <c r="K4" s="13">
+        <v>0</v>
       </c>
       <c r="L4" s="13">
         <f>F4+G4+H4+I4</f>
@@ -4254,6 +4301,10 @@
         <f>SUM(J2:J4)</f>
         <v>2.4000000000000004</v>
       </c>
+      <c r="K5" s="13">
+        <f>SUM(K2:K4)</f>
+        <v>0</v>
+      </c>
       <c r="L5" s="13">
         <f>SUM(L2:L4)</f>
         <v>9373.2199999999993</v>
@@ -4296,6 +4347,9 @@
       <c r="J7" s="13">
         <v>0.8</v>
       </c>
+      <c r="K7" s="13">
+        <v>0</v>
+      </c>
       <c r="L7" s="13">
         <f>F7+G7+H7+I7</f>
         <v>1536.5810004368718</v>
@@ -4334,6 +4388,9 @@
       </c>
       <c r="J8" s="13">
         <v>0.8</v>
+      </c>
+      <c r="K8" s="13">
+        <v>0</v>
       </c>
       <c r="L8" s="13">
         <f>F8+G8+H8+I8</f>
@@ -4361,6 +4418,10 @@
       <c r="J9" s="13">
         <f>SUM(J7:J8)</f>
         <v>1.6</v>
+      </c>
+      <c r="K9" s="13">
+        <f>SUM(K7:K8)</f>
+        <v>0</v>
       </c>
       <c r="L9" s="13">
         <f>SUM(L7:L8)</f>
@@ -4578,7 +4639,9 @@
         <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
         <v>0.12934999999999999</v>
       </c>
-      <c r="K2" s="3"/>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
       <c r="L2" s="3">
         <v>11005.45</v>
       </c>
@@ -4618,7 +4681,9 @@
         <f t="shared" si="1"/>
         <v>0.12934999999999999</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3+J3</f>
         <v>11605.599349999999</v>
@@ -5317,7 +5382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421F9D80-1D28-4F3C-95F7-8DE9883A26F0}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
@@ -5519,6 +5584,305 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D25BF0F-8645-49A4-A6C8-BE755BFA7BE7}">
+  <dimension ref="A1:AC8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9">
+        <v>200</v>
+      </c>
+      <c r="E2" s="8">
+        <v>35.15</v>
+      </c>
+      <c r="F2" s="8">
+        <f>D2*E2</f>
+        <v>7030</v>
+      </c>
+      <c r="G2" s="8">
+        <f>F2*0.0275%</f>
+        <v>1.9332500000000001</v>
+      </c>
+      <c r="H2" s="8">
+        <f>F2*0.007%</f>
+        <v>0.49210000000000004</v>
+      </c>
+      <c r="I2" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="8">
+        <f>((F2 - G2 - H2 - I2 - J2) - (30.88 * D2)) * 0.005%</f>
+        <v>4.173923249999998E-2</v>
+      </c>
+      <c r="L2" s="8">
+        <f t="shared" ref="L2:L4" si="0">F2-G2-H2-I2-J2</f>
+        <v>7010.7846499999996</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9">
+        <v>200</v>
+      </c>
+      <c r="E3" s="8">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3*E3</f>
+        <v>6895.9999999999991</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" ref="G3:G4" si="1">F3*0.0275%</f>
+        <v>1.8963999999999999</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" ref="H3:H4" si="2">F3*0.007%</f>
+        <v>0.48271999999999998</v>
+      </c>
+      <c r="I3" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="8">
+        <f>((F3 - G3 - H3 - I3 - J3) - (30.88 * D3)) * 0.005%</f>
+        <v>3.504154399999998E-2</v>
+      </c>
+      <c r="L3" s="8">
+        <f t="shared" si="0"/>
+        <v>6876.8308799999995</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9">
+        <v>200</v>
+      </c>
+      <c r="E4" s="8">
+        <v>31</v>
+      </c>
+      <c r="F4" s="8">
+        <f>D4*E4</f>
+        <v>6200</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" si="1"/>
+        <v>1.7050000000000001</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" si="2"/>
+        <v>0.43400000000000005</v>
+      </c>
+      <c r="I4" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="8">
+        <f>((F4 - G4 - H4 - I4 - J4) - (30.88 * D4)) * 0.005%</f>
+        <v>2.5354999999999567E-4</v>
+      </c>
+      <c r="L4" s="8">
+        <f t="shared" si="0"/>
+        <v>6181.0709999999999</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="11">
+        <f t="shared" ref="F5:L5" si="3">SUM(F2:F4)</f>
+        <v>20126</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="3"/>
+        <v>5.5346500000000001</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="3"/>
+        <v>1.40882</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="3"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="3"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="11">
+        <f>SUM(K2:K4) - 0.03</f>
+        <v>4.7034326499999946E-2</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="3"/>
+        <v>20068.686529999999</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E8" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -5643,6 +6007,9 @@
       <c r="J2" s="13">
         <v>0.8</v>
       </c>
+      <c r="K2" s="13">
+        <v>0</v>
+      </c>
       <c r="L2" s="13">
         <f>F2+G2+H2+I2</f>
         <v>1550.5248101265822</v>
@@ -5682,6 +6049,9 @@
       <c r="J3" s="13">
         <v>0.8</v>
       </c>
+      <c r="K3" s="13">
+        <v>0</v>
+      </c>
       <c r="L3" s="13">
         <f>F3+G3+H3+I3</f>
         <v>5055.7464363870413</v>
@@ -5720,6 +6090,9 @@
       </c>
       <c r="J4" s="13">
         <v>0.8</v>
+      </c>
+      <c r="K4" s="13">
+        <v>0</v>
       </c>
       <c r="L4" s="13">
         <f>F4+G4+H4+I4</f>
@@ -5748,6 +6121,10 @@
         <f>SUM(J2:J4)</f>
         <v>2.4000000000000004</v>
       </c>
+      <c r="K5" s="13">
+        <f>SUM(K2:K4)</f>
+        <v>0</v>
+      </c>
       <c r="L5" s="13">
         <f>SUM(L2:L4)</f>
         <v>9373.2199999999993</v>
@@ -5790,6 +6167,9 @@
       <c r="J7" s="13">
         <v>0.8</v>
       </c>
+      <c r="K7" s="13">
+        <v>0</v>
+      </c>
       <c r="L7" s="13">
         <f>F7+G7+H7+I7</f>
         <v>1536.5810004368718</v>
@@ -5828,6 +6208,9 @@
       </c>
       <c r="J8" s="13">
         <v>0.8</v>
+      </c>
+      <c r="K8" s="13">
+        <v>0</v>
       </c>
       <c r="L8" s="13">
         <f>F8+G8+H8+I8</f>
@@ -5855,6 +6238,10 @@
       <c r="J9" s="13">
         <f>SUM(J7:J8)</f>
         <v>1.6</v>
+      </c>
+      <c r="K9" s="13">
+        <f>SUM(K7:K8)</f>
+        <v>0</v>
       </c>
       <c r="L9" s="13">
         <f>SUM(L7:L8)</f>
@@ -6327,7 +6714,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="1" sqref="A3 B3"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6437,7 +6824,9 @@
       <c r="J2" s="3">
         <v>0.8</v>
       </c>
-      <c r="K2" s="3"/>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2+J2</f>
         <v>1551.3192299999998</v>
@@ -6489,7 +6878,9 @@
       <c r="J3" s="3">
         <v>0.8</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3+J3</f>
         <v>5056.5281099999993</v>
@@ -6541,7 +6932,9 @@
       <c r="J4" s="3">
         <v>0.8</v>
       </c>
-      <c r="K4" s="3"/>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
       <c r="L4" s="3">
         <f>F4+G4+H4+I4+J4</f>
         <v>2767.73875</v>
@@ -6582,7 +6975,10 @@
         <f>SUM(J2:J4)</f>
         <v>2.4000000000000004</v>
       </c>
-      <c r="K5" s="7"/>
+      <c r="K5" s="7">
+        <f>SUM(K2:K4)</f>
+        <v>0</v>
+      </c>
       <c r="L5" s="7">
         <f>SUM(L2:L4)</f>
         <v>9375.5860899999989</v>
@@ -6729,6 +7125,9 @@
       <c r="J2" s="13">
         <v>0.8</v>
       </c>
+      <c r="K2" s="13">
+        <v>0</v>
+      </c>
       <c r="L2" s="13">
         <f>F2+G2+H2+I2</f>
         <v>1550.5248101265822</v>
@@ -6768,6 +7167,9 @@
       <c r="J3" s="13">
         <v>0.8</v>
       </c>
+      <c r="K3" s="13">
+        <v>0</v>
+      </c>
       <c r="L3" s="13">
         <f>F3+G3+H3+I3</f>
         <v>5055.7464363870413</v>
@@ -6806,6 +7208,9 @@
       </c>
       <c r="J4" s="13">
         <v>0.8</v>
+      </c>
+      <c r="K4" s="13">
+        <v>0</v>
       </c>
       <c r="L4" s="13">
         <f>F4+G4+H4+I4</f>
@@ -6833,6 +7238,10 @@
       <c r="J5" s="13">
         <f>SUM(J2:J4)</f>
         <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="13">
+        <f>SUM(K2:K4)</f>
+        <v>0</v>
       </c>
       <c r="L5" s="13">
         <f>SUM(L2:L4)</f>
@@ -6968,7 +7377,9 @@
       <c r="J2" s="3">
         <v>0.8</v>
       </c>
-      <c r="K2" s="3"/>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2+J2</f>
         <v>1551.3192299999998</v>
@@ -7020,7 +7431,9 @@
       <c r="J3" s="3">
         <v>0.8</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
       <c r="L3" s="3">
         <f t="shared" ref="L3:L4" si="2">F3+G3+H3+I3+J3</f>
         <v>5056.5281099999993</v>
@@ -7072,7 +7485,9 @@
       <c r="J4" s="3">
         <v>0.8</v>
       </c>
-      <c r="K4" s="3"/>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
       <c r="L4" s="3">
         <f t="shared" si="2"/>
         <v>2767.73875</v>
@@ -7113,7 +7528,10 @@
         <f>SUM(J2:J4)</f>
         <v>2.4000000000000004</v>
       </c>
-      <c r="K5" s="3"/>
+      <c r="K5" s="3">
+        <f>SUM(K2:K4)</f>
+        <v>0</v>
+      </c>
       <c r="L5" s="3">
         <f>SUM(L2:L4)</f>
         <v>9375.5860899999989</v>
@@ -7188,7 +7606,9 @@
       <c r="J7" s="3">
         <v>0.8</v>
       </c>
-      <c r="K7" s="3"/>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
       <c r="L7" s="3">
         <f>F7+G7+H7+I7+J7</f>
         <v>1537.3143999999998</v>
@@ -7240,7 +7660,9 @@
       <c r="J8" s="3">
         <v>0.8</v>
       </c>
-      <c r="K8" s="3"/>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
       <c r="L8" s="3">
         <f>F8+G8+H8+I8+J8</f>
         <v>786.05530499999986</v>
@@ -7281,7 +7703,10 @@
         <f>SUM(J7:J8)</f>
         <v>1.6</v>
       </c>
-      <c r="K9" s="3"/>
+      <c r="K9" s="3">
+        <f>SUM(K7:K8)</f>
+        <v>0</v>
+      </c>
       <c r="L9" s="3">
         <f>SUM(L7:L8)</f>
         <v>2323.3697049999996</v>
@@ -7539,7 +7964,9 @@
       <c r="J2" s="3">
         <v>0.8</v>
       </c>
-      <c r="K2" s="3"/>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2+J2</f>
         <v>1551.3192299999998</v>
@@ -7591,7 +8018,9 @@
       <c r="J3" s="3">
         <v>0.8</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3+J3</f>
         <v>5056.5281099999993</v>
@@ -7643,7 +8072,9 @@
       <c r="J4" s="3">
         <v>0.8</v>
       </c>
-      <c r="K4" s="3"/>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
       <c r="L4" s="3">
         <f>F4+G4+H4+I4+J4</f>
         <v>2767.73875</v>
@@ -7684,7 +8115,10 @@
         <f>SUM(J2:J4)</f>
         <v>2.4000000000000004</v>
       </c>
-      <c r="K5" s="7"/>
+      <c r="K5" s="7">
+        <f>SUM(K2:K4)</f>
+        <v>0</v>
+      </c>
       <c r="L5" s="7">
         <f>SUM(L2:L4)</f>
         <v>9375.5860899999989</v>
@@ -7759,7 +8193,9 @@
       <c r="J7" s="3">
         <v>0.8</v>
       </c>
-      <c r="K7" s="3"/>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
       <c r="L7" s="3">
         <f>F7+G7+H7+I7+J7</f>
         <v>284.88245999999998</v>
@@ -7811,7 +8247,9 @@
       <c r="J8" s="3">
         <v>0.8</v>
       </c>
-      <c r="K8" s="3"/>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
       <c r="L8" s="3">
         <f>F8+G8+H8+I8+J8</f>
         <v>1537.3143999999998</v>
@@ -7863,7 +8301,9 @@
       <c r="J9" s="3">
         <v>0.8</v>
       </c>
-      <c r="K9" s="3"/>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
       <c r="L9" s="3">
         <f>F9+G9+H9+I9+J9</f>
         <v>786.05530499999986</v>
@@ -7904,7 +8344,10 @@
         <f>SUM(J7:J9)</f>
         <v>2.4000000000000004</v>
       </c>
-      <c r="K10" s="7"/>
+      <c r="K10" s="7">
+        <f>SUM(K7:K9)</f>
+        <v>0</v>
+      </c>
       <c r="L10" s="7">
         <f>SUM(L7:L9)</f>
         <v>2608.2521649999999</v>

</xml_diff>

<commit_message>
Fails when trying to create a 'BrokerageNotesWorksheetReader' from a 'Worksheet' whose 'Line's have 'Cell's whose values are supposed to have been calculated from other 'Cell's but, do not pass the recalculation test. Here, specifically, the 'Volume', which, for 'FinancialSummary's, should consider 'SellingOperations' as increasing and 'BuyingOperations' as decreasing the result.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F834A58-39F1-41C7-A6F7-9558C21308AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B10C4FD-8BEB-4F62-BB3A-9A27F0191C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="8" activeTab="9" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
@@ -38,6 +38,7 @@
     <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId23"/>
     <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId24"/>
     <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId25"/>
+    <sheet name="InvalidMixedBrokerageNote" sheetId="31" r:id="rId26"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -140,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="25">
   <si>
     <t>BBAS3</t>
   </si>
@@ -209,6 +210,12 @@
   </si>
   <si>
     <t>EMBR3</t>
+  </si>
+  <si>
+    <t>SLCE3</t>
+  </si>
+  <si>
+    <t>RAIL3</t>
   </si>
 </sst>
 </file>
@@ -1047,32 +1054,32 @@
       <c r="A5" s="5"/>
       <c r="E5" s="3"/>
       <c r="F5" s="7">
-        <f>SUM(F2:F4)</f>
-        <v>9322</v>
+        <f>-SUM(F2:F4)</f>
+        <v>-9322</v>
       </c>
       <c r="G5" s="7">
-        <f>SUM(G2:G4)</f>
+        <f t="shared" ref="F5:L5" si="2">SUM(G2:G4)</f>
         <v>2.5635500000000002</v>
       </c>
       <c r="H5" s="7">
-        <f>SUM(H2:H4)</f>
+        <f t="shared" si="2"/>
         <v>0.65254000000000012</v>
       </c>
       <c r="I5" s="7">
-        <f>SUM(I2:I4)</f>
+        <f t="shared" si="2"/>
         <v>47.97</v>
       </c>
       <c r="J5" s="7">
-        <f>SUM(J2:J4)</f>
+        <f t="shared" si="2"/>
         <v>2.4000000000000004</v>
       </c>
       <c r="K5" s="7">
-        <f>SUM(K2:K4)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L5" s="7">
-        <f>SUM(L2:L4)</f>
-        <v>9375.5860899999989</v>
+        <f>-SUM(L2:L4)</f>
+        <v>-9375.5860899999989</v>
       </c>
       <c r="M5" s="6"/>
       <c r="R5" s="3"/>
@@ -1185,11 +1192,11 @@
         <v>1520</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" ref="G8:G9" si="2">F8*0.0275%</f>
+        <f t="shared" ref="G8:G9" si="3">F8*0.0275%</f>
         <v>0.41800000000000004</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" ref="H8:H9" si="3">F8*0.007%</f>
+        <f t="shared" ref="H8:H9" si="4">F8*0.007%</f>
         <v>0.10640000000000001</v>
       </c>
       <c r="I8" s="3">
@@ -1239,11 +1246,11 @@
         <v>769</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.21147500000000002</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.3830000000000003E-2</v>
       </c>
       <c r="I9" s="3">
@@ -1276,32 +1283,32 @@
       <c r="A10" s="5"/>
       <c r="E10" s="3"/>
       <c r="F10" s="7">
-        <f>SUM(F7:F9)</f>
-        <v>2557</v>
+        <f>-SUM(F7:F9)</f>
+        <v>-2557</v>
       </c>
       <c r="G10" s="7">
-        <f>SUM(G7:G9)</f>
+        <f t="shared" ref="F10:L10" si="5">SUM(G7:G9)</f>
         <v>0.70317500000000011</v>
       </c>
       <c r="H10" s="7">
-        <f>SUM(H7:H9)</f>
+        <f t="shared" si="5"/>
         <v>0.17899000000000004</v>
       </c>
       <c r="I10" s="7">
-        <f>SUM(I7:I9)</f>
+        <f t="shared" si="5"/>
         <v>47.97</v>
       </c>
       <c r="J10" s="7">
-        <f>SUM(J7:J9)</f>
+        <f t="shared" si="5"/>
         <v>2.4000000000000004</v>
       </c>
       <c r="K10" s="7">
-        <f>SUM(K7:K9)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L10" s="7">
-        <f>SUM(L7:L9)</f>
-        <v>2608.2521649999999</v>
+        <f>-SUM(L7:L9)</f>
+        <v>-2608.2521649999999</v>
       </c>
       <c r="M10" s="6"/>
       <c r="R10" s="3"/>
@@ -1415,11 +1422,11 @@
         <v>6895.9999999999991</v>
       </c>
       <c r="G13" s="8">
-        <f t="shared" ref="G13:G14" si="4">F13*0.0275%</f>
+        <f t="shared" ref="G13:G14" si="6">F13*0.0275%</f>
         <v>1.8963999999999999</v>
       </c>
       <c r="H13" s="8">
-        <f t="shared" ref="H13:H14" si="5">F13*0.007%</f>
+        <f t="shared" ref="H13:H14" si="7">F13*0.007%</f>
         <v>0.48271999999999998</v>
       </c>
       <c r="I13" s="8">
@@ -1433,7 +1440,7 @@
         <v>3.504154399999998E-2</v>
       </c>
       <c r="L13" s="8">
-        <f t="shared" ref="L13:L14" si="6">F13-G13-H13-I13-J13</f>
+        <f t="shared" ref="L13:L14" si="8">F13-G13-H13-I13-J13</f>
         <v>6876.8308799999995</v>
       </c>
       <c r="M13" s="6"/>
@@ -1470,11 +1477,11 @@
         <v>6200</v>
       </c>
       <c r="G14" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.7050000000000001</v>
       </c>
       <c r="H14" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.43400000000000005</v>
       </c>
       <c r="I14" s="8">
@@ -1488,7 +1495,7 @@
         <v>2.5354999999999567E-4</v>
       </c>
       <c r="L14" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>6181.0709999999999</v>
       </c>
       <c r="M14" s="6"/>
@@ -1508,31 +1515,31 @@
       <c r="A15" s="10"/>
       <c r="E15" s="8"/>
       <c r="F15" s="11">
-        <f t="shared" ref="F15:L15" si="7">SUM(F12:F14)</f>
+        <f t="shared" ref="F15:L15" si="9">SUM(F12:F14)</f>
         <v>20126</v>
       </c>
       <c r="G15" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5.5346500000000001</v>
       </c>
       <c r="H15" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.40882</v>
       </c>
       <c r="I15" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>47.97</v>
       </c>
       <c r="J15" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.4000000000000004</v>
       </c>
       <c r="K15" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7.7034326499999944E-2</v>
       </c>
       <c r="L15" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>20068.686529999999</v>
       </c>
       <c r="M15" s="6"/>
@@ -1662,31 +1669,31 @@
       <c r="A19" s="10"/>
       <c r="E19" s="8"/>
       <c r="F19" s="11">
-        <f t="shared" ref="F19:L19" si="8">SUM(F17:F18)</f>
+        <f t="shared" ref="F19:L19" si="10">SUM(F17:F18)</f>
         <v>46500</v>
       </c>
       <c r="G19" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12.787500000000001</v>
       </c>
       <c r="H19" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.2550000000000008</v>
       </c>
       <c r="I19" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>31.98</v>
       </c>
       <c r="J19" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.6</v>
       </c>
       <c r="K19" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6.5188750000000255E-3</v>
       </c>
       <c r="L19" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>46450.377500000002</v>
       </c>
       <c r="M19" s="6"/>
@@ -2205,31 +2212,31 @@
       <c r="A5" s="10"/>
       <c r="E5" s="8"/>
       <c r="F5" s="11">
-        <f>SUM(F2:F4)</f>
+        <f t="shared" ref="F5:L5" si="0">SUM(F2:F4)</f>
         <v>19416.009999999998</v>
       </c>
       <c r="G5" s="11">
-        <f>SUM(G2:G4)</f>
+        <f t="shared" si="0"/>
         <v>1.1599999999999999</v>
       </c>
       <c r="H5" s="11">
-        <f>SUM(H2:H4)</f>
+        <f t="shared" si="0"/>
         <v>5.53</v>
       </c>
       <c r="I5" s="11">
-        <f>SUM(I2:I4)</f>
+        <f t="shared" si="0"/>
         <v>47.97</v>
       </c>
       <c r="J5" s="11">
-        <f>SUM(J2:J4)</f>
+        <f t="shared" si="0"/>
         <v>2.4000000000000004</v>
       </c>
       <c r="K5" s="11">
-        <f>SUM(K2:K4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L5" s="11">
-        <f>SUM(L2:L4)</f>
+        <f t="shared" si="0"/>
         <v>19361.349999999999</v>
       </c>
       <c r="M5" s="6"/>
@@ -2267,13 +2274,13 @@
     <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -2421,8 +2428,8 @@
       <c r="A4" s="5"/>
       <c r="E4" s="3"/>
       <c r="F4" s="7">
-        <f>SUM(F2:F3)</f>
-        <v>22600</v>
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
       </c>
       <c r="G4" s="7">
         <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
@@ -2445,8 +2452,8 @@
         <v>0</v>
       </c>
       <c r="L4" s="7">
-        <f t="shared" si="2"/>
-        <v>22611.028699999995</v>
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.028699999995</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -2483,13 +2490,13 @@
     <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -2637,8 +2644,8 @@
       <c r="A4" s="5"/>
       <c r="E4" s="3"/>
       <c r="F4" s="7">
-        <f>SUM(F2:F3)</f>
-        <v>22600</v>
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
       </c>
       <c r="G4" s="7">
         <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
@@ -2661,8 +2668,8 @@
         <v>0</v>
       </c>
       <c r="L4" s="7">
-        <f t="shared" si="2"/>
-        <v>22611.028699999995</v>
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.028699999995</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -2699,13 +2706,13 @@
     <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -2853,8 +2860,8 @@
       <c r="A4" s="5"/>
       <c r="E4" s="3"/>
       <c r="F4" s="7">
-        <f>SUM(F2:F3)</f>
-        <v>22600</v>
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
       </c>
       <c r="G4" s="7">
         <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
@@ -2877,8 +2884,8 @@
         <v>0</v>
       </c>
       <c r="L4" s="7">
-        <f t="shared" si="2"/>
-        <v>22611.00935</v>
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.00935</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -3354,13 +3361,13 @@
     <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -3509,8 +3516,8 @@
       <c r="A4" s="5"/>
       <c r="E4" s="3"/>
       <c r="F4" s="7">
-        <f>SUM(F2:F3)</f>
-        <v>22600</v>
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
       </c>
       <c r="G4" s="7">
         <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
@@ -3533,8 +3540,8 @@
         <v>1</v>
       </c>
       <c r="L4" s="7">
-        <f t="shared" si="2"/>
-        <v>22611.018699999997</v>
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.018699999997</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -3571,13 +3578,13 @@
     <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -3726,8 +3733,8 @@
       <c r="A4" s="5"/>
       <c r="E4" s="3"/>
       <c r="F4" s="7">
-        <f>SUM(F2:F3)</f>
-        <v>22600</v>
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
       </c>
       <c r="G4" s="7">
         <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
@@ -3750,8 +3757,8 @@
         <v>0.01</v>
       </c>
       <c r="L4" s="7">
-        <f t="shared" si="2"/>
-        <v>22611.018699999997</v>
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.018699999997</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -4282,31 +4289,31 @@
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="F5" s="13">
-        <f>SUM(F2:F4)</f>
+        <f t="shared" ref="F5:L5" si="0">SUM(F2:F4)</f>
         <v>9322</v>
       </c>
       <c r="G5" s="13">
-        <f>SUM(G2:G4)</f>
+        <f t="shared" si="0"/>
         <v>0.74</v>
       </c>
       <c r="H5" s="13">
-        <f>SUM(H2:H4)</f>
+        <f t="shared" si="0"/>
         <v>2.5099999999999998</v>
       </c>
       <c r="I5" s="13">
-        <f>SUM(I2:I4)</f>
+        <f t="shared" si="0"/>
         <v>47.97</v>
       </c>
       <c r="J5" s="13">
-        <f>SUM(J2:J4)</f>
+        <f t="shared" si="0"/>
         <v>2.4000000000000004</v>
       </c>
       <c r="K5" s="13">
-        <f>SUM(K2:K4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L5" s="13">
-        <f>SUM(L2:L4)</f>
+        <f t="shared" si="0"/>
         <v>9373.2199999999993</v>
       </c>
     </row>
@@ -4400,31 +4407,31 @@
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
       <c r="F9" s="13">
-        <f>SUM(F7:F8)</f>
+        <f t="shared" ref="F9:L9" si="1">SUM(F7:F8)</f>
         <v>2289</v>
       </c>
       <c r="G9" s="13">
-        <f>SUM(G7:G8)</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="H9" s="13">
-        <f>SUM(H7:H8)</f>
+        <f t="shared" si="1"/>
         <v>0.69</v>
       </c>
       <c r="I9" s="13">
-        <f>SUM(I7:I8)</f>
+        <f t="shared" si="1"/>
         <v>31.98</v>
       </c>
       <c r="J9" s="13">
-        <f>SUM(J7:J8)</f>
+        <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
       <c r="K9" s="13">
-        <f>SUM(K7:K8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L9" s="13">
-        <f>SUM(L7:L8)</f>
+        <f t="shared" si="1"/>
         <v>2321.87</v>
       </c>
     </row>
@@ -4539,13 +4546,13 @@
     <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -4693,8 +4700,8 @@
       <c r="A4" s="5"/>
       <c r="E4" s="3"/>
       <c r="F4" s="7">
-        <f>SUM(F2:F3)</f>
-        <v>22600</v>
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
       </c>
       <c r="G4" s="7">
         <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
@@ -4717,8 +4724,8 @@
         <v>0</v>
       </c>
       <c r="L4" s="7">
-        <f t="shared" si="2"/>
-        <v>22611.049350000001</v>
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.049350000001</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -4755,13 +4762,13 @@
     <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -4906,8 +4913,8 @@
       <c r="A4" s="5"/>
       <c r="E4" s="3"/>
       <c r="F4" s="7">
-        <f>SUM(F2:F3)</f>
-        <v>22600</v>
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
       </c>
       <c r="G4" s="7">
         <f>SUM(G2:G3) + 0.03</f>
@@ -4930,8 +4937,8 @@
         <v>0</v>
       </c>
       <c r="L4" s="7">
-        <f t="shared" si="2"/>
-        <v>22611.018699999997</v>
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.018699999997</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -4968,13 +4975,13 @@
     <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -5119,8 +5126,8 @@
       <c r="A4" s="5"/>
       <c r="E4" s="3"/>
       <c r="F4" s="7">
-        <f>SUM(F2:F3)</f>
-        <v>22600</v>
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
       </c>
       <c r="G4" s="7">
         <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
@@ -5143,8 +5150,8 @@
         <v>0</v>
       </c>
       <c r="L4" s="7">
-        <f t="shared" si="2"/>
-        <v>22611.018699999997</v>
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.018699999997</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -5181,13 +5188,13 @@
     <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -5332,8 +5339,8 @@
       <c r="A4" s="5"/>
       <c r="E4" s="3"/>
       <c r="F4" s="7">
-        <f>SUM(F2:F3)</f>
-        <v>22600</v>
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
       </c>
       <c r="G4" s="7">
         <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
@@ -5356,8 +5363,8 @@
         <v>0</v>
       </c>
       <c r="L4" s="7">
-        <f t="shared" si="2"/>
-        <v>22611.018699999997</v>
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.018699999997</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -5394,13 +5401,13 @@
     <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -5545,8 +5552,8 @@
       <c r="A4" s="5"/>
       <c r="E4" s="3"/>
       <c r="F4" s="7">
-        <f>SUM(F2:F3)</f>
-        <v>22600</v>
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
       </c>
       <c r="G4" s="7">
         <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
@@ -5569,8 +5576,8 @@
         <v>0</v>
       </c>
       <c r="L4" s="7">
-        <f t="shared" si="2"/>
-        <v>22611.018699999997</v>
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.018699999997</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -5598,7 +5605,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5887,6 +5894,241 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4721B46-AB87-4CAA-ABF7-E48CFDA36C4A}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>42996</v>
+      </c>
+      <c r="B2" s="4">
+        <v>168102</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>23.65</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>9460</v>
+      </c>
+      <c r="G2" s="3">
+        <f t="shared" ref="G2:G3" si="0">F2*0.0275%</f>
+        <v>2.6015000000000001</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.47300000000000003</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="J2" s="3">
+        <f>I2*5%</f>
+        <v>0.12450000000000001</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>9465.6890000000003</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>42996</v>
+      </c>
+      <c r="B3" s="9">
+        <v>168102</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="9">
+        <v>700</v>
+      </c>
+      <c r="E3" s="8">
+        <v>10.5</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3*E3</f>
+        <v>7350</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" si="0"/>
+        <v>2.0212500000000002</v>
+      </c>
+      <c r="H3" s="8">
+        <f>F3*0.005%</f>
+        <v>0.36749999999999999</v>
+      </c>
+      <c r="I3" s="8">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="J3" s="8">
+        <f>I3*5%</f>
+        <v>0.12450000000000001</v>
+      </c>
+      <c r="K3" s="8">
+        <v>0</v>
+      </c>
+      <c r="L3" s="8">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>7355.0032499999998</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>SUM(F2:F3)</f>
+        <v>16810</v>
+      </c>
+      <c r="G4" s="7">
+        <f>SUM(G2:G3)</f>
+        <v>4.6227499999999999</v>
+      </c>
+      <c r="H4" s="7">
+        <f>SUM(H2:H3)</f>
+        <v>0.84050000000000002</v>
+      </c>
+      <c r="I4" s="7">
+        <f>SUM(I2:I3)</f>
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="J4" s="7">
+        <f>SUM(J2:J3)</f>
+        <v>0.24900000000000003</v>
+      </c>
+      <c r="K4" s="7">
+        <f>SUM(K2:K3)</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f>SUM(L2:L3)</f>
+        <v>16820.69225</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -6102,31 +6344,31 @@
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="F5" s="13">
-        <f>SUM(F2:F4)</f>
+        <f t="shared" ref="F5:L5" si="0">SUM(F2:F4)</f>
         <v>9322</v>
       </c>
       <c r="G5" s="13">
-        <f>SUM(G2:G4)</f>
+        <f t="shared" si="0"/>
         <v>0.74</v>
       </c>
       <c r="H5" s="13">
-        <f>SUM(H2:H4)</f>
+        <f t="shared" si="0"/>
         <v>2.5099999999999998</v>
       </c>
       <c r="I5" s="13">
-        <f>SUM(I2:I4)</f>
+        <f t="shared" si="0"/>
         <v>47.97</v>
       </c>
       <c r="J5" s="13">
-        <f>SUM(J2:J4)</f>
+        <f t="shared" si="0"/>
         <v>2.4000000000000004</v>
       </c>
       <c r="K5" s="13">
-        <f>SUM(K2:K4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L5" s="13">
-        <f>SUM(L2:L4)</f>
+        <f t="shared" si="0"/>
         <v>9373.2199999999993</v>
       </c>
     </row>
@@ -6220,31 +6462,31 @@
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
       <c r="F9" s="13">
-        <f>SUM(F7:F8)</f>
+        <f t="shared" ref="F9:L9" si="1">SUM(F7:F8)</f>
         <v>2289</v>
       </c>
       <c r="G9" s="13">
-        <f>SUM(G7:G8)</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="H9" s="13">
-        <f>SUM(H7:H8)</f>
+        <f t="shared" si="1"/>
         <v>0.69</v>
       </c>
       <c r="I9" s="13">
-        <f>SUM(I7:I8)</f>
+        <f t="shared" si="1"/>
         <v>31.98</v>
       </c>
       <c r="J9" s="13">
-        <f>SUM(J7:J8)</f>
+        <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
       <c r="K9" s="13">
-        <f>SUM(K7:K8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L9" s="13">
-        <f>SUM(L7:L8)</f>
+        <f t="shared" si="1"/>
         <v>2321.87</v>
       </c>
     </row>
@@ -6956,32 +7198,32 @@
       <c r="A5" s="5"/>
       <c r="E5" s="3"/>
       <c r="F5" s="7">
-        <f>SUM(F2:F4)</f>
-        <v>9322</v>
+        <f>-SUM(F2:F4)</f>
+        <v>-9322</v>
       </c>
       <c r="G5" s="7">
-        <f>SUM(G2:G4)</f>
+        <f t="shared" ref="F5:L5" si="2">SUM(G2:G4)</f>
         <v>2.5635500000000002</v>
       </c>
       <c r="H5" s="7">
-        <f>SUM(H2:H4)</f>
+        <f t="shared" si="2"/>
         <v>0.65254000000000012</v>
       </c>
       <c r="I5" s="7">
-        <f>SUM(I2:I4)</f>
+        <f t="shared" si="2"/>
         <v>47.97</v>
       </c>
       <c r="J5" s="7">
-        <f>SUM(J2:J4)</f>
+        <f t="shared" si="2"/>
         <v>2.4000000000000004</v>
       </c>
       <c r="K5" s="7">
-        <f>SUM(K2:K4)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L5" s="7">
-        <f>SUM(L2:L4)</f>
-        <v>9375.5860899999989</v>
+        <f>-SUM(L2:L4)</f>
+        <v>-9375.5860899999989</v>
       </c>
       <c r="M5" s="6"/>
       <c r="R5" s="3"/>
@@ -7220,31 +7462,31 @@
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="F5" s="13">
-        <f>SUM(F2:F4)</f>
+        <f t="shared" ref="F5:L5" si="0">SUM(F2:F4)</f>
         <v>9322</v>
       </c>
       <c r="G5" s="13">
-        <f>SUM(G2:G4)</f>
+        <f t="shared" si="0"/>
         <v>0.74</v>
       </c>
       <c r="H5" s="13">
-        <f>SUM(H2:H4)</f>
+        <f t="shared" si="0"/>
         <v>2.5099999999999998</v>
       </c>
       <c r="I5" s="13">
-        <f>SUM(I2:I4)</f>
+        <f t="shared" si="0"/>
         <v>47.97</v>
       </c>
       <c r="J5" s="13">
-        <f>SUM(J2:J4)</f>
+        <f t="shared" si="0"/>
         <v>2.4000000000000004</v>
       </c>
       <c r="K5" s="13">
-        <f>SUM(K2:K4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L5" s="13">
-        <f>SUM(L2:L4)</f>
+        <f t="shared" si="0"/>
         <v>9373.2199999999993</v>
       </c>
     </row>
@@ -7509,32 +7751,32 @@
       <c r="A5" s="5"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3">
-        <f>SUM(F2:F4)</f>
-        <v>9322</v>
+        <f>-SUM(F2:F4)</f>
+        <v>-9322</v>
       </c>
       <c r="G5" s="3">
-        <f>SUM(G2:G4)</f>
+        <f t="shared" ref="F5:L5" si="3">SUM(G2:G4)</f>
         <v>2.5635500000000002</v>
       </c>
       <c r="H5" s="3">
-        <f>SUM(H2:H4)</f>
+        <f t="shared" si="3"/>
         <v>0.65254000000000012</v>
       </c>
       <c r="I5" s="3">
-        <f>SUM(I2:I4)</f>
+        <f t="shared" si="3"/>
         <v>47.97</v>
       </c>
       <c r="J5" s="3">
-        <f>SUM(J2:J4)</f>
+        <f t="shared" si="3"/>
         <v>2.4000000000000004</v>
       </c>
       <c r="K5" s="3">
-        <f>SUM(K2:K4)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L5" s="3">
-        <f>SUM(L2:L4)</f>
-        <v>9375.5860899999989</v>
+        <f>-SUM(L2:L4)</f>
+        <v>-9375.5860899999989</v>
       </c>
       <c r="M5" s="6"/>
       <c r="R5" s="3"/>
@@ -7684,32 +7926,32 @@
       <c r="A9" s="5"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3">
-        <f>SUM(F7:F8)</f>
-        <v>2289</v>
+        <f>-SUM(F7:F8)</f>
+        <v>-2289</v>
       </c>
       <c r="G9" s="3">
-        <f>SUM(G7:G8)</f>
+        <f t="shared" ref="F9:L9" si="4">SUM(G7:G8)</f>
         <v>0.62947500000000001</v>
       </c>
       <c r="H9" s="3">
-        <f>SUM(H7:H8)</f>
+        <f t="shared" si="4"/>
         <v>0.16023000000000001</v>
       </c>
       <c r="I9" s="3">
-        <f>SUM(I7:I8)</f>
+        <f t="shared" si="4"/>
         <v>31.98</v>
       </c>
       <c r="J9" s="3">
-        <f>SUM(J7:J8)</f>
+        <f t="shared" si="4"/>
         <v>1.6</v>
       </c>
       <c r="K9" s="3">
-        <f>SUM(K7:K8)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L9" s="3">
-        <f>SUM(L7:L8)</f>
-        <v>2323.3697049999996</v>
+        <f>-SUM(L7:L8)</f>
+        <v>-2323.3697049999996</v>
       </c>
       <c r="M9" s="6"/>
       <c r="R9" s="3"/>
@@ -8096,32 +8338,32 @@
       <c r="A5" s="5"/>
       <c r="E5" s="3"/>
       <c r="F5" s="7">
-        <f>SUM(F2:F4)</f>
-        <v>9322</v>
+        <f>-SUM(F2:F4)</f>
+        <v>-9322</v>
       </c>
       <c r="G5" s="7">
-        <f>SUM(G2:G4)</f>
+        <f t="shared" ref="F5:L5" si="2">SUM(G2:G4)</f>
         <v>2.5635500000000002</v>
       </c>
       <c r="H5" s="7">
-        <f>SUM(H2:H4)</f>
+        <f t="shared" si="2"/>
         <v>0.65254000000000012</v>
       </c>
       <c r="I5" s="7">
-        <f>SUM(I2:I4)</f>
+        <f t="shared" si="2"/>
         <v>47.97</v>
       </c>
       <c r="J5" s="7">
-        <f>SUM(J2:J4)</f>
+        <f t="shared" si="2"/>
         <v>2.4000000000000004</v>
       </c>
       <c r="K5" s="7">
-        <f>SUM(K2:K4)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L5" s="7">
-        <f>SUM(L2:L4)</f>
-        <v>9375.5860899999989</v>
+        <f>-SUM(L2:L4)</f>
+        <v>-9375.5860899999989</v>
       </c>
       <c r="M5" s="6"/>
       <c r="R5" s="3"/>
@@ -8234,11 +8476,11 @@
         <v>1520</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" ref="G8:G9" si="2">F8*0.0275%</f>
+        <f t="shared" ref="G8:G9" si="3">F8*0.0275%</f>
         <v>0.41800000000000004</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" ref="H8:H9" si="3">F8*0.007%</f>
+        <f t="shared" ref="H8:H9" si="4">F8*0.007%</f>
         <v>0.10640000000000001</v>
       </c>
       <c r="I8" s="3">
@@ -8288,11 +8530,11 @@
         <v>769</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.21147500000000002</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.3830000000000003E-2</v>
       </c>
       <c r="I9" s="3">
@@ -8325,32 +8567,32 @@
       <c r="A10" s="5"/>
       <c r="E10" s="3"/>
       <c r="F10" s="7">
-        <f>SUM(F7:F9)</f>
-        <v>2557</v>
+        <f>-SUM(F7:F9)</f>
+        <v>-2557</v>
       </c>
       <c r="G10" s="7">
-        <f>SUM(G7:G9)</f>
+        <f t="shared" ref="F10:L10" si="5">SUM(G7:G9)</f>
         <v>0.70317500000000011</v>
       </c>
       <c r="H10" s="7">
-        <f>SUM(H7:H9)</f>
+        <f t="shared" si="5"/>
         <v>0.17899000000000004</v>
       </c>
       <c r="I10" s="7">
-        <f>SUM(I7:I9)</f>
+        <f t="shared" si="5"/>
         <v>47.97</v>
       </c>
       <c r="J10" s="7">
-        <f>SUM(J7:J9)</f>
+        <f t="shared" si="5"/>
         <v>2.4000000000000004</v>
       </c>
       <c r="K10" s="7">
-        <f>SUM(K7:K9)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L10" s="7">
-        <f>SUM(L7:L9)</f>
-        <v>2608.2521649999999</v>
+        <f>-SUM(L7:L9)</f>
+        <v>-2608.2521649999999</v>
       </c>
       <c r="M10" s="6"/>
       <c r="R10" s="3"/>

</xml_diff>

<commit_message>
Fails when trying to create a 'BrokerageNotesWorksheetReader' from a 'Worksheet' whose 'Line's have 'Cell's whose values are supposed to have been calculated from other 'Cell's but, do not pass the recalculation test. Here, specifically, the 'Total', which, for 'FinancialSummary's, should consider 'SellingOperations' as increasing and 'BuyingOperations' as decreasing the result.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B10C4FD-8BEB-4F62-BB3A-9A27F0191C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E439C9CB-5AF0-4DBB-8AB4-18D509DB2CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="8" activeTab="9" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="25" activeTab="26" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,8 @@
     <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId23"/>
     <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId24"/>
     <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId25"/>
-    <sheet name="InvalidMixedBrokerageNote" sheetId="31" r:id="rId26"/>
+    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId26"/>
+    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId27"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -141,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="25">
   <si>
     <t>BBAS3</t>
   </si>
@@ -811,7 +812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="A12" activeCellId="1" sqref="A2:XFD2 A12:XFD12"/>
@@ -6111,6 +6112,241 @@
         <v>0</v>
       </c>
       <c r="L4" s="7">
+        <f>L3-L2</f>
+        <v>-2110.6857500000006</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF39107-DEBE-454A-A911-9FAC6360BB3B}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>42996</v>
+      </c>
+      <c r="B2" s="4">
+        <v>168102</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>23.65</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>9460</v>
+      </c>
+      <c r="G2" s="3">
+        <f t="shared" ref="G2:G3" si="0">F2*0.0275%</f>
+        <v>2.6015000000000001</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.47300000000000003</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="J2" s="3">
+        <f>I2*5%</f>
+        <v>0.12450000000000001</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>9465.6890000000003</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>42996</v>
+      </c>
+      <c r="B3" s="9">
+        <v>168102</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="9">
+        <v>700</v>
+      </c>
+      <c r="E3" s="8">
+        <v>10.5</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3*E3</f>
+        <v>7350</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" si="0"/>
+        <v>2.0212500000000002</v>
+      </c>
+      <c r="H3" s="8">
+        <f>F3*0.005%</f>
+        <v>0.36749999999999999</v>
+      </c>
+      <c r="I3" s="8">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="J3" s="8">
+        <f>I3*5%</f>
+        <v>0.12450000000000001</v>
+      </c>
+      <c r="K3" s="8">
+        <v>0</v>
+      </c>
+      <c r="L3" s="8">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>7355.0032499999998</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>F3-F2</f>
+        <v>-2110</v>
+      </c>
+      <c r="G4" s="7">
+        <f>SUM(G2:G3)</f>
+        <v>4.6227499999999999</v>
+      </c>
+      <c r="H4" s="7">
+        <f>SUM(H2:H3)</f>
+        <v>0.84050000000000002</v>
+      </c>
+      <c r="I4" s="7">
+        <f>SUM(I2:I3)</f>
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="J4" s="7">
+        <f>SUM(J2:J3)</f>
+        <v>0.24900000000000003</v>
+      </c>
+      <c r="K4" s="7">
+        <f>SUM(K2:K3)</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
         <f>SUM(L2:L3)</f>
         <v>16820.69225</v>
       </c>

</xml_diff>

<commit_message>
Exposes a bug in group formation to be addressed later on.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E439C9CB-5AF0-4DBB-8AB4-18D509DB2CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A27B25-0F52-4A0A-A304-FA8CA9C270B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="25" activeTab="26" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" firstSheet="2" activeTab="2" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
-    <sheet name="GroupWithDifferentTradingDates" sheetId="11" r:id="rId2"/>
+    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId2"/>
     <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId3"/>
     <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId4"/>
     <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId5"/>
@@ -29,17 +29,18 @@
     <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId14"/>
     <sheet name="InvalidServiceTax" sheetId="18" r:id="rId15"/>
     <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId16"/>
-    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId17"/>
-    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId18"/>
-    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId19"/>
-    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId20"/>
-    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId21"/>
-    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId22"/>
-    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId23"/>
-    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId24"/>
-    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId25"/>
-    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId26"/>
-    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId27"/>
+    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId17"/>
+    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId18"/>
+    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId19"/>
+    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId20"/>
+    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId21"/>
+    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId22"/>
+    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId23"/>
+    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId24"/>
+    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId25"/>
+    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId26"/>
+    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId27"/>
+    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId28"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -141,8 +142,31 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Andrei Diego Cardoso</author>
+  </authors>
+  <commentList>
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{A816318B-6C6C-417A-82FC-56C33FF54C9F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>=((F2 - G2 - H2 - I2 - J2) - (O12 * D2)) * 0,005%</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="25">
   <si>
     <t>BBAS3</t>
   </si>
@@ -229,7 +253,7 @@
     <numFmt numFmtId="165" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     <numFmt numFmtId="166" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,13 +309,6 @@
       <color indexed="81"/>
       <name val="Segoe UI"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -360,11 +377,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1059,7 +1076,7 @@
         <v>-9322</v>
       </c>
       <c r="G5" s="7">
-        <f t="shared" ref="F5:L5" si="2">SUM(G2:G4)</f>
+        <f t="shared" ref="G5:K5" si="2">SUM(G2:G4)</f>
         <v>2.5635500000000002</v>
       </c>
       <c r="H5" s="7">
@@ -1288,7 +1305,7 @@
         <v>-2557</v>
       </c>
       <c r="G10" s="7">
-        <f t="shared" ref="F10:L10" si="5">SUM(G7:G9)</f>
+        <f t="shared" ref="G10:K10" si="5">SUM(G7:G9)</f>
         <v>0.70317500000000011</v>
       </c>
       <c r="H10" s="7">
@@ -1711,7 +1728,7 @@
       <c r="AB19" s="8"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1819,10 +1836,12 @@
         <v>4680</v>
       </c>
       <c r="G2" s="8">
-        <v>0.28000000000000003</v>
+        <f>F2*0.0275%</f>
+        <v>1.2870000000000001</v>
       </c>
       <c r="H2" s="8">
-        <v>1.33</v>
+        <f>F2*0.007%</f>
+        <v>0.32760000000000006</v>
       </c>
       <c r="I2" s="8">
         <v>15.99</v>
@@ -1834,8 +1853,8 @@
         <v>0.23</v>
       </c>
       <c r="L2" s="8">
-        <f>F2-G2-H2-I2</f>
-        <v>4662.4000000000005</v>
+        <f>F2-G2-H2-I2-J2</f>
+        <v>4661.5954000000002</v>
       </c>
       <c r="M2" s="6"/>
       <c r="R2" s="8"/>
@@ -1875,10 +1894,12 @@
         <v>6808</v>
       </c>
       <c r="G4" s="8">
-        <v>0.4</v>
+        <f>F4*0.0275%</f>
+        <v>1.8722000000000001</v>
       </c>
       <c r="H4" s="8">
-        <v>1.94</v>
+        <f>F4*0.007%</f>
+        <v>0.47656000000000004</v>
       </c>
       <c r="I4" s="8">
         <v>15.99</v>
@@ -1890,8 +1911,8 @@
         <v>0.34</v>
       </c>
       <c r="L4" s="8">
-        <f>F4-G4-H4-I4</f>
-        <v>6789.670000000001</v>
+        <f>F4-G4-H4-I4-J4</f>
+        <v>6788.8612400000002</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="8"/>
@@ -1931,10 +1952,12 @@
         <v>3310</v>
       </c>
       <c r="G6" s="3">
-        <v>0.19</v>
+        <f>F6*0.0275%</f>
+        <v>0.91025</v>
       </c>
       <c r="H6" s="3">
-        <v>0.94</v>
+        <f>F6*0.007%</f>
+        <v>0.23170000000000002</v>
       </c>
       <c r="I6" s="3">
         <v>15.99</v>
@@ -1944,8 +1967,8 @@
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3">
-        <f>F6+G6+H6+I6</f>
-        <v>3327.12</v>
+        <f>F6+G6+H6+I6+J6</f>
+        <v>3327.9319499999997</v>
       </c>
       <c r="M6" s="6"/>
       <c r="R6" s="3"/>
@@ -2433,7 +2456,7 @@
         <v>-22600</v>
       </c>
       <c r="G4" s="7">
-        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
         <v>5.66</v>
       </c>
       <c r="H4" s="7">
@@ -2649,7 +2672,7 @@
         <v>-22600</v>
       </c>
       <c r="G4" s="7">
-        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
         <v>5.65</v>
       </c>
       <c r="H4" s="7">
@@ -2865,7 +2888,7 @@
         <v>-22600</v>
       </c>
       <c r="G4" s="7">
-        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
         <v>5.65</v>
       </c>
       <c r="H4" s="7">
@@ -2909,6 +2932,305 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
+  <dimension ref="A1:AC6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9">
+        <v>200</v>
+      </c>
+      <c r="E2" s="8">
+        <v>40</v>
+      </c>
+      <c r="F2" s="8">
+        <f>D2*E2</f>
+        <v>8000</v>
+      </c>
+      <c r="G2" s="8">
+        <f>F2*0.0275%</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H2" s="8">
+        <f>F2*0.007%</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I2" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="L2" s="8">
+        <f>F2-G2-H2-I2-K2</f>
+        <v>7981.06</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9">
+        <v>200</v>
+      </c>
+      <c r="E3" s="8">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3*E3</f>
+        <v>6895.9999999999991</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.8963999999999999</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.48271999999999998</v>
+      </c>
+      <c r="I3" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="8">
+        <f>((F3 - G3 - H3 - I3 - J3) - (18.5 * D3)) * 0.005%</f>
+        <v>0.15884154399999997</v>
+      </c>
+      <c r="L3" s="8">
+        <f>F3-G3-H3-I3-K3</f>
+        <v>6877.4720384559996</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="9">
+        <v>200</v>
+      </c>
+      <c r="E4" s="8">
+        <v>27.45</v>
+      </c>
+      <c r="F4" s="8">
+        <f>D4*E4</f>
+        <v>5490</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5097500000000001</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" si="1"/>
+        <v>0.38430000000000003</v>
+      </c>
+      <c r="I4" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="8">
+        <f>((F4 - G4 - H4 - I4 - J4) - (22.3 * D4)) * 0.005%</f>
+        <v>5.0565797500000009E-2</v>
+      </c>
+      <c r="L4" s="8">
+        <f>F4-G4-H4-I4-K4</f>
+        <v>5472.0653842025004</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="11">
+        <f t="shared" ref="F5:L5" si="2">SUM(F2:F4)</f>
+        <v>20386</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="2"/>
+        <v>5.6061500000000004</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="2"/>
+        <v>1.4270200000000002</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="2"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="2"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="2"/>
+        <v>0.39940734150000001</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="2"/>
+        <v>20330.597422658502</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E6" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E3E40E-BCAE-41DB-80FC-C74D9CCDCD28}">
   <dimension ref="A1:AC13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3205,7 +3527,7 @@
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E9" s="20">
+      <c r="E9" s="19">
         <v>100</v>
       </c>
       <c r="F9" s="1">
@@ -3231,13 +3553,13 @@
         <f>L8+K9</f>
         <v>2732.2500000000005</v>
       </c>
-      <c r="N9" s="20">
+      <c r="N9" s="19">
         <f>N8+E9</f>
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E10" s="20">
+      <c r="E10" s="19">
         <v>200</v>
       </c>
       <c r="F10" s="1">
@@ -3263,13 +3585,13 @@
         <f>L9+K10</f>
         <v>8653.39</v>
       </c>
-      <c r="N10" s="20">
+      <c r="N10" s="19">
         <f>N9+E10</f>
         <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E11" s="20">
+      <c r="E11" s="19">
         <v>-200</v>
       </c>
       <c r="F11" s="1">
@@ -3295,13 +3617,13 @@
         <f>L10+((L10/N10)*E11)</f>
         <v>2884.4633333333331</v>
       </c>
-      <c r="N11" s="20">
+      <c r="N11" s="19">
         <f>N10+E11</f>
         <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E12" s="20">
+      <c r="E12" s="19">
         <v>200</v>
       </c>
       <c r="F12" s="1">
@@ -3323,11 +3645,11 @@
         <f t="shared" si="3"/>
         <v>6381.01</v>
       </c>
-      <c r="L12" s="21">
+      <c r="L12" s="20">
         <f>L11+K12</f>
         <v>9265.4733333333334</v>
       </c>
-      <c r="N12" s="22">
+      <c r="N12" s="21">
         <f>N11+E12</f>
         <v>300</v>
       </c>
@@ -3337,7 +3659,7 @@
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E13" s="22"/>
+      <c r="E13" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3346,7 +3668,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F402F95-319A-4797-B7E1-F3EB07A82FDD}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -3462,7 +3784,7 @@
         <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
         <v>0.12934999999999999</v>
       </c>
-      <c r="K2" s="23">
+      <c r="K2" s="22">
         <v>1</v>
       </c>
       <c r="L2" s="3">
@@ -3521,7 +3843,7 @@
         <v>-22600</v>
       </c>
       <c r="G4" s="7">
-        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
         <v>5.65</v>
       </c>
       <c r="H4" s="7">
@@ -3563,7 +3885,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A590E594-CB91-4439-95F2-7F159495761F}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -3738,7 +4060,7 @@
         <v>-22600</v>
       </c>
       <c r="G4" s="7">
-        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
         <v>5.65</v>
       </c>
       <c r="H4" s="7">
@@ -3780,306 +4102,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34F43A8-C89C-44C0-BF29-1F8134A0151F}">
-  <dimension ref="A1:AC8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="9">
-        <v>200</v>
-      </c>
-      <c r="E2" s="8">
-        <v>35.15</v>
-      </c>
-      <c r="F2" s="8">
-        <f>D2*E2</f>
-        <v>7030</v>
-      </c>
-      <c r="G2" s="8">
-        <f>F2*0.0275%</f>
-        <v>1.9332500000000001</v>
-      </c>
-      <c r="H2" s="8">
-        <f>F2*0.007%</f>
-        <v>0.49210000000000004</v>
-      </c>
-      <c r="I2" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="8">
-        <f>((F2 - G2 - H2 - I2 - J2) - (30.88 * D2)) * 0.005%</f>
-        <v>4.173923249999998E-2</v>
-      </c>
-      <c r="L2" s="8">
-        <v>7010.81</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-    </row>
-    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B3" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="9">
-        <v>200</v>
-      </c>
-      <c r="E3" s="8">
-        <v>34.479999999999997</v>
-      </c>
-      <c r="F3" s="8">
-        <f>D3*E3</f>
-        <v>6895.9999999999991</v>
-      </c>
-      <c r="G3" s="8">
-        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
-        <v>1.8963999999999999</v>
-      </c>
-      <c r="H3" s="8">
-        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
-        <v>0.48271999999999998</v>
-      </c>
-      <c r="I3" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="8">
-        <f>((F3 - G3 - H3 - I3 - J3) - (30.88 * D3)) * 0.005%</f>
-        <v>3.504154399999998E-2</v>
-      </c>
-      <c r="L3" s="8">
-        <f t="shared" ref="L3:L4" si="2">F3-G3-H3-I3-J3</f>
-        <v>6876.8308799999995</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-    </row>
-    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="9">
-        <v>200</v>
-      </c>
-      <c r="E4" s="8">
-        <v>31</v>
-      </c>
-      <c r="F4" s="8">
-        <f>D4*E4</f>
-        <v>6200</v>
-      </c>
-      <c r="G4" s="8">
-        <f t="shared" si="0"/>
-        <v>1.7050000000000001</v>
-      </c>
-      <c r="H4" s="8">
-        <f t="shared" si="1"/>
-        <v>0.43400000000000005</v>
-      </c>
-      <c r="I4" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="8">
-        <f>((F4 - G4 - H4 - I4 - J4) - (30.88 * D4)) * 0.005%</f>
-        <v>2.5354999999999567E-4</v>
-      </c>
-      <c r="L4" s="8">
-        <f t="shared" si="2"/>
-        <v>6181.0709999999999</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-    </row>
-    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="11">
-        <f t="shared" ref="F5:L5" si="3">SUM(F2:F4)</f>
-        <v>20126</v>
-      </c>
-      <c r="G5" s="11">
-        <f t="shared" si="3"/>
-        <v>5.5346500000000001</v>
-      </c>
-      <c r="H5" s="11">
-        <f t="shared" si="3"/>
-        <v>1.40882</v>
-      </c>
-      <c r="I5" s="11">
-        <f t="shared" si="3"/>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="11">
-        <f t="shared" si="3"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="11">
-        <f t="shared" si="3"/>
-        <v>7.7034326499999944E-2</v>
-      </c>
-      <c r="L5" s="11">
-        <f t="shared" si="3"/>
-        <v>20068.711879999999</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="8"/>
-      <c r="AB5" s="8"/>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E8" s="22"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03306DC6-EFFD-4226-8075-7FFC9D0F7B34}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF98C6E-C61C-4098-8811-20C737B2746F}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4161,366 +4185,500 @@
       </c>
       <c r="AC1" s="18"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>39757</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="4">
         <v>1662</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="4">
         <v>100</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="3">
         <v>15.34</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="3">
         <f>D2*E2</f>
         <v>1534</v>
       </c>
-      <c r="G2" s="13">
-        <f>0.74*(F2/SUM(F2:F4))</f>
-        <v>0.12177215189873417</v>
-      </c>
-      <c r="H2" s="13">
-        <f>2.51*(F2/SUM(F2:F4))</f>
-        <v>0.41303797468354425</v>
-      </c>
-      <c r="I2" s="13">
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
+      </c>
+      <c r="I2" s="3">
         <v>15.99</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="3">
         <v>0.8</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="3">
         <v>0</v>
       </c>
-      <c r="L2" s="13">
-        <f>F2+G2+H2+I2</f>
-        <v>1550.5248101265822</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>39758</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="4">
         <v>1662</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="4">
         <v>200</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="3">
         <v>25.19</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="3">
         <f>D3*E3</f>
         <v>5038</v>
       </c>
-      <c r="G3" s="13">
-        <f>0.74*(F3/SUM(F2:F4))</f>
-        <v>0.39992705428019737</v>
-      </c>
-      <c r="H3" s="13">
-        <f>2.51*(F3/SUM(F2:F4))</f>
-        <v>1.3565093327612099</v>
-      </c>
-      <c r="I3" s="13">
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.3854500000000001</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.35266000000000003</v>
+      </c>
+      <c r="I3" s="3">
         <v>15.99</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="3">
         <v>0.8</v>
       </c>
-      <c r="K3" s="13">
+      <c r="K3" s="3">
         <v>0</v>
       </c>
-      <c r="L3" s="13">
-        <f>F3+G3+H3+I3</f>
-        <v>5055.7464363870413</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+      <c r="L3" s="3">
+        <f t="shared" ref="L3:L4" si="2">F3+G3+H3+I3+J3</f>
+        <v>5056.5281099999993</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>39757</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="4">
         <v>1662</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="4">
         <v>100</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="3">
         <v>27.5</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="3">
         <f>D4*E4</f>
         <v>2750</v>
       </c>
-      <c r="G4" s="13">
-        <f>0.74*(F4/SUM(F2:F4))</f>
-        <v>0.21830079382106843</v>
-      </c>
-      <c r="H4" s="13">
-        <f>2.51*(F4/SUM(F2:F4))</f>
-        <v>0.74045269255524548</v>
-      </c>
-      <c r="I4" s="13">
+      <c r="G4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.75625000000000009</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.19250000000000003</v>
+      </c>
+      <c r="I4" s="3">
         <v>15.99</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="3">
         <v>0.8</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="3">
         <v>0</v>
       </c>
-      <c r="L4" s="13">
-        <f>F4+G4+H4+I4</f>
-        <v>2766.9487534863761</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="F5" s="13">
-        <f t="shared" ref="F5:L5" si="0">SUM(F2:F4)</f>
-        <v>9322</v>
-      </c>
-      <c r="G5" s="13">
-        <f t="shared" si="0"/>
-        <v>0.74</v>
-      </c>
-      <c r="H5" s="13">
-        <f t="shared" si="0"/>
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="I5" s="13">
-        <f t="shared" si="0"/>
+      <c r="L4" s="3">
+        <f t="shared" si="2"/>
+        <v>2767.73875</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3">
+        <f>-SUM(F2:F4)</f>
+        <v>-9322</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" ref="G5:K5" si="3">SUM(G2:G4)</f>
+        <v>2.5635500000000002</v>
+      </c>
+      <c r="H5" s="3">
+        <f t="shared" si="3"/>
+        <v>0.65254000000000012</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="3"/>
         <v>47.97</v>
       </c>
-      <c r="J5" s="13">
-        <f t="shared" si="0"/>
+      <c r="J5" s="3">
+        <f t="shared" si="3"/>
         <v>2.4000000000000004</v>
       </c>
-      <c r="K5" s="13">
-        <f t="shared" si="0"/>
+      <c r="K5" s="3">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L5" s="13">
-        <f t="shared" si="0"/>
-        <v>9373.2199999999993</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="L5" s="3">
+        <f>-SUM(L2:L4)</f>
+        <v>-9375.5860899999989</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+    </row>
+    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="6"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+    </row>
+    <row r="7" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>39758</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="4">
         <v>1344</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="4">
         <v>100</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="3">
         <v>15.2</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="3">
         <f>D7*E7</f>
         <v>1520</v>
       </c>
-      <c r="G7" s="13">
-        <f>0.2*(F7/SUM(F7:F8))</f>
-        <v>0.13280908693752733</v>
-      </c>
-      <c r="H7" s="13">
-        <f>0.69*(F7/SUM(F7:F8))</f>
-        <v>0.45819134993446919</v>
-      </c>
-      <c r="I7" s="13">
+      <c r="G7" s="3">
+        <f>F7*0.0275%</f>
+        <v>0.41800000000000004</v>
+      </c>
+      <c r="H7" s="3">
+        <f>F7*0.007%</f>
+        <v>0.10640000000000001</v>
+      </c>
+      <c r="I7" s="3">
         <v>15.99</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="3">
         <v>0.8</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="3">
         <v>0</v>
       </c>
-      <c r="L7" s="13">
-        <f>F7+G7+H7+I7</f>
-        <v>1536.5810004368718</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="L7" s="3">
+        <f>F7+G7+H7+I7+J7</f>
+        <v>1537.3143999999998</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+    </row>
+    <row r="8" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>39758</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="4">
         <v>1344</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="4">
         <v>100</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="3">
         <v>7.69</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="3">
         <f>D8*E8</f>
         <v>769</v>
       </c>
-      <c r="G8" s="13">
-        <f>0.2*(F8/SUM(F7:F8))</f>
-        <v>6.7190913062472699E-2</v>
-      </c>
-      <c r="H8" s="13">
-        <f>0.69*(F8/SUM(F7:F8))</f>
-        <v>0.23180865006553075</v>
-      </c>
-      <c r="I8" s="13">
+      <c r="G8" s="3">
+        <f>F8*0.0275%</f>
+        <v>0.21147500000000002</v>
+      </c>
+      <c r="H8" s="3">
+        <f>F8*0.007%</f>
+        <v>5.3830000000000003E-2</v>
+      </c>
+      <c r="I8" s="3">
         <v>15.99</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="3">
         <v>0.8</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="3">
         <v>0</v>
       </c>
-      <c r="L8" s="13">
-        <f>F8+G8+H8+I8</f>
-        <v>785.28899956312807</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="F9" s="13">
-        <f t="shared" ref="F9:L9" si="1">SUM(F7:F8)</f>
-        <v>2289</v>
-      </c>
-      <c r="G9" s="13">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="H9" s="13">
-        <f t="shared" si="1"/>
-        <v>0.69</v>
-      </c>
-      <c r="I9" s="13">
-        <f t="shared" si="1"/>
+      <c r="L8" s="3">
+        <f>F8+G8+H8+I8+J8</f>
+        <v>786.05530499999986</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+    </row>
+    <row r="9" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <f>-SUM(F7:F8)</f>
+        <v>-2289</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" ref="G9:K9" si="4">SUM(G7:G8)</f>
+        <v>0.62947500000000001</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="4"/>
+        <v>0.16023000000000001</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="4"/>
         <v>31.98</v>
       </c>
-      <c r="J9" s="13">
-        <f t="shared" si="1"/>
+      <c r="J9" s="3">
+        <f t="shared" si="4"/>
         <v>1.6</v>
       </c>
-      <c r="K9" s="13">
-        <f t="shared" si="1"/>
+      <c r="K9" s="3">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L9" s="13">
-        <f t="shared" si="1"/>
-        <v>2321.87</v>
-      </c>
+      <c r="L9" s="3">
+        <f>-SUM(L7:L8)</f>
+        <v>-2323.3697049999996</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+    <row r="11" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
         <v>39849</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="9">
         <v>1319</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="9">
         <v>100</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="8">
         <v>31.5</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="8">
         <f>D11*E11</f>
         <v>3150</v>
       </c>
-      <c r="G11" s="13">
-        <v>0.25</v>
-      </c>
-      <c r="H11" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="I11" s="13">
+      <c r="G11" s="8">
+        <f>F11*0.0275%</f>
+        <v>0.86625000000000008</v>
+      </c>
+      <c r="H11" s="8">
+        <f>F11*0.007%</f>
+        <v>0.22050000000000003</v>
+      </c>
+      <c r="I11" s="8">
         <v>15.99</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="8">
         <v>0.8</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K11" s="8">
         <v>0</v>
       </c>
-      <c r="L11" s="13">
-        <f>F11-G11-H11-I11-K11</f>
-        <v>3132.9100000000003</v>
-      </c>
+      <c r="L11" s="8">
+        <f>F11-G11-H11-I11-J11</f>
+        <v>3132.1232500000001</v>
+      </c>
+      <c r="M11" s="6"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
+    <row r="13" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
         <v>39853</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="9">
         <v>1362</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="12">
+      <c r="C13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="9">
         <v>100</v>
       </c>
-      <c r="E13" s="13">
-        <v>17.7</v>
-      </c>
-      <c r="F13" s="13">
+      <c r="E13" s="8">
+        <v>31.5</v>
+      </c>
+      <c r="F13" s="8">
         <f>D13*E13</f>
-        <v>1770</v>
-      </c>
-      <c r="G13" s="13">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="H13" s="13">
-        <v>0.47</v>
-      </c>
-      <c r="I13" s="13">
+        <v>3150</v>
+      </c>
+      <c r="G13" s="8">
+        <f>F13*0.0275%</f>
+        <v>0.86625000000000008</v>
+      </c>
+      <c r="H13" s="8">
+        <f>F13*0.007%</f>
+        <v>0.22050000000000003</v>
+      </c>
+      <c r="I13" s="8">
         <v>15.99</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="8">
         <v>0.8</v>
       </c>
-      <c r="K13" s="13">
+      <c r="K13" s="8">
         <v>0</v>
       </c>
-      <c r="L13" s="13">
-        <f>F13-G13-H13-I13-K13</f>
-        <v>1753.3999999999999</v>
-      </c>
+      <c r="L13" s="8">
+        <f>F13-G13-H13-I13-J13</f>
+        <v>3132.1232500000001</v>
+      </c>
+      <c r="M13" s="6"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
@@ -4532,6 +4690,304 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34F43A8-C89C-44C0-BF29-1F8134A0151F}">
+  <dimension ref="A1:AC8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9">
+        <v>200</v>
+      </c>
+      <c r="E2" s="8">
+        <v>35.15</v>
+      </c>
+      <c r="F2" s="8">
+        <f>D2*E2</f>
+        <v>7030</v>
+      </c>
+      <c r="G2" s="8">
+        <f>F2*0.0275%</f>
+        <v>1.9332500000000001</v>
+      </c>
+      <c r="H2" s="8">
+        <f>F2*0.007%</f>
+        <v>0.49210000000000004</v>
+      </c>
+      <c r="I2" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="8">
+        <f>((F2 - G2 - H2 - I2 - J2) - (30.88 * D2)) * 0.005%</f>
+        <v>4.173923249999998E-2</v>
+      </c>
+      <c r="L2" s="8">
+        <v>7010.81</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9">
+        <v>200</v>
+      </c>
+      <c r="E3" s="8">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3*E3</f>
+        <v>6895.9999999999991</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.8963999999999999</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.48271999999999998</v>
+      </c>
+      <c r="I3" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="8">
+        <f>((F3 - G3 - H3 - I3 - J3) - (30.88 * D3)) * 0.005%</f>
+        <v>3.504154399999998E-2</v>
+      </c>
+      <c r="L3" s="8">
+        <f t="shared" ref="L3:L4" si="2">F3-G3-H3-I3-J3</f>
+        <v>6876.8308799999995</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9">
+        <v>200</v>
+      </c>
+      <c r="E4" s="8">
+        <v>31</v>
+      </c>
+      <c r="F4" s="8">
+        <f>D4*E4</f>
+        <v>6200</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" si="0"/>
+        <v>1.7050000000000001</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" si="1"/>
+        <v>0.43400000000000005</v>
+      </c>
+      <c r="I4" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="8">
+        <f>((F4 - G4 - H4 - I4 - J4) - (30.88 * D4)) * 0.005%</f>
+        <v>2.5354999999999567E-4</v>
+      </c>
+      <c r="L4" s="8">
+        <f t="shared" si="2"/>
+        <v>6181.0709999999999</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="11">
+        <f t="shared" ref="F5:L5" si="3">SUM(F2:F4)</f>
+        <v>20126</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="3"/>
+        <v>5.5346500000000001</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="3"/>
+        <v>1.40882</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="3"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="3"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="3"/>
+        <v>7.7034326499999944E-2</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="3"/>
+        <v>20068.711879999999</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E8" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5AE87-00E8-4CF9-A517-EB6C0CA40610}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -4705,7 +5161,7 @@
         <v>-22600</v>
       </c>
       <c r="G4" s="7">
-        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
         <v>5.65</v>
       </c>
       <c r="H4" s="7">
@@ -4747,7 +5203,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B51BEB4-905E-4036-959A-F9A0226AF070}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -4863,7 +5319,9 @@
         <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
         <v>0.12934999999999999</v>
       </c>
-      <c r="K2" s="3"/>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2+J2</f>
         <v>11005.419349999998</v>
@@ -4904,7 +5362,9 @@
         <f t="shared" si="1"/>
         <v>0.12934999999999999</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3+J3</f>
         <v>11605.599349999999</v>
@@ -4922,7 +5382,7 @@
         <v>5.6800000000000006</v>
       </c>
       <c r="H4" s="7">
-        <f t="shared" ref="H4:L4" si="2">SUM(H2:H3)</f>
+        <f t="shared" ref="H4:K4" si="2">SUM(H2:H3)</f>
         <v>1.1300000000000001</v>
       </c>
       <c r="I4" s="7">
@@ -4960,7 +5420,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B7349E-D984-4817-800E-2EB4836D5B5D}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -5076,7 +5536,9 @@
         <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
         <v>0.12934999999999999</v>
       </c>
-      <c r="K2" s="3"/>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2+J2</f>
         <v>11005.419349999998</v>
@@ -5117,7 +5579,9 @@
         <f t="shared" si="1"/>
         <v>0.12934999999999999</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3+J3</f>
         <v>11605.599349999999</v>
@@ -5131,7 +5595,7 @@
         <v>-22600</v>
       </c>
       <c r="G4" s="7">
-        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
         <v>5.65</v>
       </c>
       <c r="H4" s="7">
@@ -5173,7 +5637,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA65F892-A6B4-4288-ADB5-125D04E295EB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -5289,7 +5753,9 @@
         <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
         <v>0.12934999999999999</v>
       </c>
-      <c r="K2" s="3"/>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2+J2</f>
         <v>11005.419349999998</v>
@@ -5330,7 +5796,9 @@
         <f t="shared" si="1"/>
         <v>0.12934999999999999</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3+J3</f>
         <v>11605.599349999999</v>
@@ -5344,7 +5812,7 @@
         <v>-22600</v>
       </c>
       <c r="G4" s="7">
-        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
         <v>5.65</v>
       </c>
       <c r="H4" s="7">
@@ -5386,7 +5854,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421F9D80-1D28-4F3C-95F7-8DE9883A26F0}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -5502,7 +5970,9 @@
         <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
         <v>0.12934999999999999</v>
       </c>
-      <c r="K2" s="3"/>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2+J2</f>
         <v>11005.419349999998</v>
@@ -5543,7 +6013,9 @@
         <f t="shared" si="1"/>
         <v>0.12934999999999999</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
       <c r="L3" s="3">
         <f>F3+G3+H3+I3+J3</f>
         <v>11605.599349999999</v>
@@ -5557,7 +6029,7 @@
         <v>-22600</v>
       </c>
       <c r="G4" s="7">
-        <f t="shared" ref="G4:L4" si="2">SUM(G2:G3)</f>
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
         <v>5.65</v>
       </c>
       <c r="H4" s="7">
@@ -5599,7 +6071,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D25BF0F-8645-49A4-A6C8-BE755BFA7BE7}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -5890,7 +6362,7 @@
       <c r="AB5" s="8"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E8" s="22"/>
+      <c r="E8" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -5898,7 +6370,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4721B46-AB87-4CAA-ABF7-E48CFDA36C4A}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6088,27 +6560,27 @@
       <c r="A4" s="5"/>
       <c r="E4" s="3"/>
       <c r="F4" s="7">
-        <f>SUM(F2:F3)</f>
+        <f t="shared" ref="F4:K4" si="1">SUM(F2:F3)</f>
         <v>16810</v>
       </c>
       <c r="G4" s="7">
-        <f>SUM(G2:G3)</f>
+        <f t="shared" si="1"/>
         <v>4.6227499999999999</v>
       </c>
       <c r="H4" s="7">
-        <f>SUM(H2:H3)</f>
+        <f t="shared" si="1"/>
         <v>0.84050000000000002</v>
       </c>
       <c r="I4" s="7">
-        <f>SUM(I2:I3)</f>
+        <f t="shared" si="1"/>
         <v>4.9800000000000004</v>
       </c>
       <c r="J4" s="7">
-        <f>SUM(J2:J3)</f>
+        <f t="shared" si="1"/>
         <v>0.24900000000000003</v>
       </c>
       <c r="K4" s="7">
-        <f>SUM(K2:K3)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L4" s="7">
@@ -6133,11 +6605,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF39107-DEBE-454A-A911-9FAC6360BB3B}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
     </sheetView>
@@ -6327,27 +6799,27 @@
         <v>-2110</v>
       </c>
       <c r="G4" s="7">
-        <f>SUM(G2:G3)</f>
+        <f t="shared" ref="G4:L4" si="1">SUM(G2:G3)</f>
         <v>4.6227499999999999</v>
       </c>
       <c r="H4" s="7">
-        <f>SUM(H2:H3)</f>
+        <f t="shared" si="1"/>
         <v>0.84050000000000002</v>
       </c>
       <c r="I4" s="7">
-        <f>SUM(I2:I3)</f>
+        <f t="shared" si="1"/>
         <v>4.9800000000000004</v>
       </c>
       <c r="J4" s="7">
-        <f>SUM(J2:J3)</f>
+        <f t="shared" si="1"/>
         <v>0.24900000000000003</v>
       </c>
       <c r="K4" s="7">
-        <f>SUM(K2:K3)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L4" s="7">
-        <f>SUM(L2:L3)</f>
+        <f t="shared" si="1"/>
         <v>16820.69225</v>
       </c>
       <c r="M4" s="6"/>
@@ -6372,7 +6844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2:B3"/>
@@ -6451,366 +6923,500 @@
       </c>
       <c r="AC1" s="18"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>39757</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="4">
         <v>1662</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="4">
         <v>100</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="3">
         <v>15.34</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="3">
         <f>D2*E2</f>
         <v>1534</v>
       </c>
-      <c r="G2" s="13">
-        <f>0.74*(F2/SUM(F2:F4))</f>
-        <v>0.12177215189873417</v>
-      </c>
-      <c r="H2" s="13">
-        <f>2.51*(F2/SUM(F2:F4))</f>
-        <v>0.41303797468354425</v>
-      </c>
-      <c r="I2" s="13">
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
+      </c>
+      <c r="I2" s="3">
         <v>15.99</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="3">
         <v>0.8</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="3">
         <v>0</v>
       </c>
-      <c r="L2" s="13">
-        <f>F2+G2+H2+I2</f>
-        <v>1550.5248101265822</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>39757</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="4">
         <v>1663</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="4">
         <v>200</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="3">
         <v>25.19</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="3">
         <f>D3*E3</f>
         <v>5038</v>
       </c>
-      <c r="G3" s="13">
-        <f>0.74*(F3/SUM(F2:F4))</f>
-        <v>0.39992705428019737</v>
-      </c>
-      <c r="H3" s="13">
-        <f>2.51*(F3/SUM(F2:F4))</f>
-        <v>1.3565093327612099</v>
-      </c>
-      <c r="I3" s="13">
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.3854500000000001</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.35266000000000003</v>
+      </c>
+      <c r="I3" s="3">
         <v>15.99</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="3">
         <v>0.8</v>
       </c>
-      <c r="K3" s="13">
+      <c r="K3" s="3">
         <v>0</v>
       </c>
-      <c r="L3" s="13">
-        <f>F3+G3+H3+I3</f>
-        <v>5055.7464363870413</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+      <c r="L3" s="3">
+        <f t="shared" ref="L3:L4" si="2">F3+G3+H3+I3+J3</f>
+        <v>5056.5281099999993</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>39757</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="4">
         <v>1662</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="4">
         <v>100</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="3">
         <v>27.5</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="3">
         <f>D4*E4</f>
         <v>2750</v>
       </c>
-      <c r="G4" s="13">
-        <f>0.74*(F4/SUM(F2:F4))</f>
-        <v>0.21830079382106843</v>
-      </c>
-      <c r="H4" s="13">
-        <f>2.51*(F4/SUM(F2:F4))</f>
-        <v>0.74045269255524548</v>
-      </c>
-      <c r="I4" s="13">
+      <c r="G4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.75625000000000009</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.19250000000000003</v>
+      </c>
+      <c r="I4" s="3">
         <v>15.99</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="3">
         <v>0.8</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="3">
         <v>0</v>
       </c>
-      <c r="L4" s="13">
-        <f>F4+G4+H4+I4</f>
-        <v>2766.9487534863761</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="F5" s="13">
-        <f t="shared" ref="F5:L5" si="0">SUM(F2:F4)</f>
-        <v>9322</v>
-      </c>
-      <c r="G5" s="13">
-        <f t="shared" si="0"/>
-        <v>0.74</v>
-      </c>
-      <c r="H5" s="13">
-        <f t="shared" si="0"/>
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="I5" s="13">
-        <f t="shared" si="0"/>
+      <c r="L4" s="3">
+        <f t="shared" si="2"/>
+        <v>2767.73875</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3">
+        <f>-SUM(F2:F4)</f>
+        <v>-9322</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" ref="G5:K5" si="3">SUM(G2:G4)</f>
+        <v>2.5635500000000002</v>
+      </c>
+      <c r="H5" s="3">
+        <f t="shared" si="3"/>
+        <v>0.65254000000000012</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="3"/>
         <v>47.97</v>
       </c>
-      <c r="J5" s="13">
-        <f t="shared" si="0"/>
+      <c r="J5" s="3">
+        <f t="shared" si="3"/>
         <v>2.4000000000000004</v>
       </c>
-      <c r="K5" s="13">
-        <f t="shared" si="0"/>
+      <c r="K5" s="3">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L5" s="13">
-        <f t="shared" si="0"/>
-        <v>9373.2199999999993</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="L5" s="3">
+        <f>-SUM(L2:L4)</f>
+        <v>-9375.5860899999989</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+    </row>
+    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="6"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+    </row>
+    <row r="7" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>39758</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="4">
         <v>1344</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="4">
         <v>100</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="3">
         <v>15.2</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="3">
         <f>D7*E7</f>
         <v>1520</v>
       </c>
-      <c r="G7" s="13">
-        <f>0.2*(F7/SUM(F7:F8))</f>
-        <v>0.13280908693752733</v>
-      </c>
-      <c r="H7" s="13">
-        <f>0.69*(F7/SUM(F7:F8))</f>
-        <v>0.45819134993446919</v>
-      </c>
-      <c r="I7" s="13">
+      <c r="G7" s="3">
+        <f>F7*0.0275%</f>
+        <v>0.41800000000000004</v>
+      </c>
+      <c r="H7" s="3">
+        <f>F7*0.007%</f>
+        <v>0.10640000000000001</v>
+      </c>
+      <c r="I7" s="3">
         <v>15.99</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="3">
         <v>0.8</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="3">
         <v>0</v>
       </c>
-      <c r="L7" s="13">
-        <f>F7+G7+H7+I7</f>
-        <v>1536.5810004368718</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="L7" s="3">
+        <f>F7+G7+H7+I7+J7</f>
+        <v>1537.3143999999998</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+    </row>
+    <row r="8" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>39758</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="4">
         <v>1344</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="4">
         <v>100</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="3">
         <v>7.69</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="3">
         <f>D8*E8</f>
         <v>769</v>
       </c>
-      <c r="G8" s="13">
-        <f>0.2*(F8/SUM(F7:F8))</f>
-        <v>6.7190913062472699E-2</v>
-      </c>
-      <c r="H8" s="13">
-        <f>0.69*(F8/SUM(F7:F8))</f>
-        <v>0.23180865006553075</v>
-      </c>
-      <c r="I8" s="13">
+      <c r="G8" s="3">
+        <f>F8*0.0275%</f>
+        <v>0.21147500000000002</v>
+      </c>
+      <c r="H8" s="3">
+        <f>F8*0.007%</f>
+        <v>5.3830000000000003E-2</v>
+      </c>
+      <c r="I8" s="3">
         <v>15.99</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="3">
         <v>0.8</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="3">
         <v>0</v>
       </c>
-      <c r="L8" s="13">
-        <f>F8+G8+H8+I8</f>
-        <v>785.28899956312807</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="F9" s="13">
-        <f t="shared" ref="F9:L9" si="1">SUM(F7:F8)</f>
-        <v>2289</v>
-      </c>
-      <c r="G9" s="13">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="H9" s="13">
-        <f t="shared" si="1"/>
-        <v>0.69</v>
-      </c>
-      <c r="I9" s="13">
-        <f t="shared" si="1"/>
+      <c r="L8" s="3">
+        <f>F8+G8+H8+I8+J8</f>
+        <v>786.05530499999986</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+    </row>
+    <row r="9" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <f>-SUM(F7:F8)</f>
+        <v>-2289</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" ref="G9:K9" si="4">SUM(G7:G8)</f>
+        <v>0.62947500000000001</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="4"/>
+        <v>0.16023000000000001</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="4"/>
         <v>31.98</v>
       </c>
-      <c r="J9" s="13">
-        <f t="shared" si="1"/>
+      <c r="J9" s="3">
+        <f t="shared" si="4"/>
         <v>1.6</v>
       </c>
-      <c r="K9" s="13">
-        <f t="shared" si="1"/>
+      <c r="K9" s="3">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L9" s="13">
-        <f t="shared" si="1"/>
-        <v>2321.87</v>
-      </c>
+      <c r="L9" s="3">
+        <f>-SUM(L7:L8)</f>
+        <v>-2323.3697049999996</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+    <row r="11" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
         <v>39849</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="9">
         <v>1319</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="9">
         <v>100</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="8">
         <v>31.5</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="8">
         <f>D11*E11</f>
         <v>3150</v>
       </c>
-      <c r="G11" s="13">
-        <v>0.25</v>
-      </c>
-      <c r="H11" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="I11" s="13">
+      <c r="G11" s="8">
+        <f>F11*0.0275%</f>
+        <v>0.86625000000000008</v>
+      </c>
+      <c r="H11" s="8">
+        <f>F11*0.007%</f>
+        <v>0.22050000000000003</v>
+      </c>
+      <c r="I11" s="8">
         <v>15.99</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="8">
         <v>0.8</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K11" s="8">
         <v>0</v>
       </c>
-      <c r="L11" s="13">
-        <f>F11-G11-H11-I11-K11</f>
-        <v>3132.9100000000003</v>
-      </c>
+      <c r="L11" s="8">
+        <f>F11-G11-H11-I11-J11</f>
+        <v>3132.1232500000001</v>
+      </c>
+      <c r="M11" s="6"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
+    <row r="13" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
         <v>39853</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="9">
         <v>1362</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="12">
+      <c r="C13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="9">
         <v>100</v>
       </c>
-      <c r="E13" s="13">
-        <v>17.7</v>
-      </c>
-      <c r="F13" s="13">
+      <c r="E13" s="8">
+        <v>31.5</v>
+      </c>
+      <c r="F13" s="8">
         <f>D13*E13</f>
-        <v>1770</v>
-      </c>
-      <c r="G13" s="13">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="H13" s="13">
-        <v>0.47</v>
-      </c>
-      <c r="I13" s="13">
+        <v>3150</v>
+      </c>
+      <c r="G13" s="8">
+        <f>F13*0.0275%</f>
+        <v>0.86625000000000008</v>
+      </c>
+      <c r="H13" s="8">
+        <f>F13*0.007%</f>
+        <v>0.22050000000000003</v>
+      </c>
+      <c r="I13" s="8">
         <v>15.99</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="8">
         <v>0.8</v>
       </c>
-      <c r="K13" s="13">
+      <c r="K13" s="8">
         <v>0</v>
       </c>
-      <c r="L13" s="13">
-        <f>F13-G13-H13-I13-K13</f>
-        <v>1753.3999999999999</v>
-      </c>
+      <c r="L13" s="8">
+        <f>F13-G13-H13-I13-J13</f>
+        <v>3132.1232500000001</v>
+      </c>
+      <c r="M13" s="6"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
@@ -7192,13 +7798,14 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:B3"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="1" sqref="B3 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
@@ -7326,7 +7933,7 @@
       <c r="A3" s="5">
         <v>39757</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="23">
         <v>1662</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -7438,7 +8045,7 @@
         <v>-9322</v>
       </c>
       <c r="G5" s="7">
-        <f t="shared" ref="F5:L5" si="2">SUM(G2:G4)</f>
+        <f t="shared" ref="G5:K5" si="2">SUM(G2:G4)</f>
         <v>2.5635500000000002</v>
       </c>
       <c r="H5" s="7">
@@ -7590,12 +8197,12 @@
         <v>1534</v>
       </c>
       <c r="G2" s="13">
-        <f>0.74*(F2/SUM(F2:F4))</f>
-        <v>0.12177215189873417</v>
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
       </c>
       <c r="H2" s="13">
-        <f>2.51*(F2/SUM(F2:F4))</f>
-        <v>0.41303797468354425</v>
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
       </c>
       <c r="I2" s="13">
         <v>15.99</v>
@@ -7607,8 +8214,8 @@
         <v>0</v>
       </c>
       <c r="L2" s="13">
-        <f>F2+G2+H2+I2</f>
-        <v>1550.5248101265822</v>
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
@@ -7632,12 +8239,12 @@
         <v>5038</v>
       </c>
       <c r="G3" s="13">
-        <f>0.74*(F3/SUM(F2:F4))</f>
-        <v>0.39992705428019737</v>
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.3854500000000001</v>
       </c>
       <c r="H3" s="13">
-        <f>2.51*(F3/SUM(F2:F4))</f>
-        <v>1.3565093327612099</v>
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.35266000000000003</v>
       </c>
       <c r="I3" s="13">
         <v>15.99</v>
@@ -7649,8 +8256,8 @@
         <v>0</v>
       </c>
       <c r="L3" s="13">
-        <f>F3+G3+H3+I3</f>
-        <v>5055.7464363870413</v>
+        <f t="shared" ref="L3:L4" si="2">F3+G3+H3+I3+J3</f>
+        <v>5056.5281099999993</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
@@ -7674,12 +8281,12 @@
         <v>2750</v>
       </c>
       <c r="G4" s="13">
-        <f>0.74*(F4/SUM(F2:F4))</f>
-        <v>0.21830079382106843</v>
+        <f t="shared" si="0"/>
+        <v>0.75625000000000009</v>
       </c>
       <c r="H4" s="13">
-        <f>2.51*(F4/SUM(F2:F4))</f>
-        <v>0.74045269255524548</v>
+        <f t="shared" si="1"/>
+        <v>0.19250000000000003</v>
       </c>
       <c r="I4" s="13">
         <v>15.99</v>
@@ -7691,39 +8298,39 @@
         <v>0</v>
       </c>
       <c r="L4" s="13">
-        <f>F4+G4+H4+I4</f>
-        <v>2766.9487534863761</v>
+        <f t="shared" si="2"/>
+        <v>2767.73875</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="F5" s="13">
-        <f t="shared" ref="F5:L5" si="0">SUM(F2:F4)</f>
+        <f t="shared" ref="F5:L5" si="3">SUM(F2:F4)</f>
         <v>9322</v>
       </c>
       <c r="G5" s="13">
-        <f t="shared" si="0"/>
-        <v>0.74</v>
+        <f t="shared" si="3"/>
+        <v>2.5635500000000002</v>
       </c>
       <c r="H5" s="13">
-        <f t="shared" si="0"/>
-        <v>2.5099999999999998</v>
+        <f t="shared" si="3"/>
+        <v>0.65254000000000012</v>
       </c>
       <c r="I5" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>47.97</v>
       </c>
       <c r="J5" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.4000000000000004</v>
       </c>
       <c r="K5" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L5" s="13">
-        <f t="shared" si="0"/>
-        <v>9373.2199999999993</v>
+        <f t="shared" si="3"/>
+        <v>9375.5860899999989</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -7991,7 +8598,7 @@
         <v>-9322</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" ref="F5:L5" si="3">SUM(G2:G4)</f>
+        <f t="shared" ref="G5:K5" si="3">SUM(G2:G4)</f>
         <v>2.5635500000000002</v>
       </c>
       <c r="H5" s="3">
@@ -8166,7 +8773,7 @@
         <v>-2289</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" ref="F9:L9" si="4">SUM(G7:G8)</f>
+        <f t="shared" ref="G9:K9" si="4">SUM(G7:G8)</f>
         <v>0.62947500000000001</v>
       </c>
       <c r="H9" s="3">
@@ -8243,8 +8850,8 @@
         <v>0</v>
       </c>
       <c r="L11" s="8">
-        <f>F11-G11-H11-I11-K11</f>
-        <v>3132.9232500000003</v>
+        <f>F11-G11-H11-I11-J11</f>
+        <v>3132.1232500000001</v>
       </c>
       <c r="M11" s="6"/>
       <c r="R11" s="8"/>
@@ -8270,25 +8877,25 @@
         <v>1362</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D13" s="9">
         <v>100</v>
       </c>
       <c r="E13" s="8">
-        <v>17.7</v>
+        <v>31.5</v>
       </c>
       <c r="F13" s="8">
         <f>D13*E13</f>
-        <v>1770</v>
+        <v>3150</v>
       </c>
       <c r="G13" s="8">
         <f>F13*0.0275%</f>
-        <v>0.48675000000000002</v>
+        <v>0.86625000000000008</v>
       </c>
       <c r="H13" s="8">
         <f>F13*0.007%</f>
-        <v>0.12390000000000001</v>
+        <v>0.22050000000000003</v>
       </c>
       <c r="I13" s="8">
         <v>15.99</v>
@@ -8300,8 +8907,8 @@
         <v>0</v>
       </c>
       <c r="L13" s="8">
-        <f>F13-G13-H13-I13-K13</f>
-        <v>1753.3993499999999</v>
+        <f>F13-G13-H13-I13-J13</f>
+        <v>3132.1232500000001</v>
       </c>
       <c r="M13" s="6"/>
       <c r="R13" s="8"/>
@@ -8578,7 +9185,7 @@
         <v>-9322</v>
       </c>
       <c r="G5" s="7">
-        <f t="shared" ref="F5:L5" si="2">SUM(G2:G4)</f>
+        <f t="shared" ref="G5:K5" si="2">SUM(G2:G4)</f>
         <v>2.5635500000000002</v>
       </c>
       <c r="H5" s="7">
@@ -8807,7 +9414,7 @@
         <v>-2557</v>
       </c>
       <c r="G10" s="7">
-        <f t="shared" ref="F10:L10" si="5">SUM(G7:G9)</f>
+        <f t="shared" ref="G10:K10" si="5">SUM(G7:G9)</f>
         <v>0.70317500000000011</v>
       </c>
       <c r="H10" s="7">

</xml_diff>

<commit_message>
Introduces the 'CURRENCY' 'Cell' type.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A27B25-0F52-4A0A-A304-FA8CA9C270B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0CD489-3851-4800-AD0A-EFA7F47330F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" firstSheet="2" activeTab="2" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="15750" windowHeight="12600" firstSheet="17" activeTab="17" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -247,11 +247,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="165" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    <numFmt numFmtId="166" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+    <numFmt numFmtId="164" formatCode="0.00_ ;[Red]\-0.00\ "/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -374,14 +372,14 @@
     <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3672,7 +3670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F402F95-319A-4797-B7E1-F3EB07A82FDD}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
@@ -3784,8 +3782,8 @@
         <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
         <v>0.12934999999999999</v>
       </c>
-      <c r="K2" s="22">
-        <v>1</v>
+      <c r="K2" s="23">
+        <v>0</v>
       </c>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2+J2</f>
@@ -3860,7 +3858,7 @@
       </c>
       <c r="K4" s="7">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="7">
         <f>-SUM(L2:L3)</f>
@@ -6844,7 +6842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2:B3"/>
@@ -7933,7 +7931,7 @@
       <c r="A3" s="5">
         <v>39757</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="22">
         <v>1662</v>
       </c>
       <c r="C3" s="4" t="s">

</xml_diff>

<commit_message>
Introduces validation for missing 'NoteNumber'.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,41 +8,42 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D7F3E5-C6A6-47E4-9B72-2D709D89638C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68CA0F0-AEDE-4109-8296-0F7DD7562FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15285" activeTab="2" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="2" activeTab="3" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="NotUsed" sheetId="2" r:id="rId1"/>
     <sheet name="TradingDateMissing" sheetId="35" r:id="rId2"/>
     <sheet name="TradingDateBlack" sheetId="36" r:id="rId3"/>
-    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId4"/>
-    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId5"/>
-    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId6"/>
-    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId7"/>
-    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId8"/>
-    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId9"/>
-    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId10"/>
-    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId11"/>
-    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId12"/>
-    <sheet name="SingleLineGroups" sheetId="10" r:id="rId13"/>
-    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId14"/>
-    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId15"/>
-    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId16"/>
-    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId17"/>
-    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId18"/>
-    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId19"/>
-    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId20"/>
-    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId21"/>
-    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId22"/>
-    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId23"/>
-    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId24"/>
-    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId25"/>
-    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId26"/>
-    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId27"/>
-    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId28"/>
-    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId29"/>
-    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId30"/>
+    <sheet name="NoteNumberMissing" sheetId="37" r:id="rId4"/>
+    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId5"/>
+    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId6"/>
+    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId7"/>
+    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId8"/>
+    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId9"/>
+    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId10"/>
+    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId11"/>
+    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId12"/>
+    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId13"/>
+    <sheet name="SingleLineGroups" sheetId="10" r:id="rId14"/>
+    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId15"/>
+    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId16"/>
+    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId17"/>
+    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId18"/>
+    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId19"/>
+    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId20"/>
+    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId21"/>
+    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId22"/>
+    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId23"/>
+    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId24"/>
+    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId25"/>
+    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId26"/>
+    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId27"/>
+    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId28"/>
+    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId29"/>
+    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId30"/>
+    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId31"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -168,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="25">
   <si>
     <t>BBAS3</t>
   </si>
@@ -828,6 +829,258 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EC0A3F-FFB0-437C-B726-EA72E0B69675}">
+  <dimension ref="A1:AC7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="12"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="18"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="12">
+        <v>100</v>
+      </c>
+      <c r="E2" s="13">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="13">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="13">
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="13">
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
+      </c>
+      <c r="I2" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="13">
+        <v>0</v>
+      </c>
+      <c r="L2" s="13">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>39757</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1662</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12">
+        <v>200</v>
+      </c>
+      <c r="E3" s="13">
+        <v>25.19</v>
+      </c>
+      <c r="F3" s="13">
+        <f>D3*E3</f>
+        <v>5038</v>
+      </c>
+      <c r="G3" s="13">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.3854500000000001</v>
+      </c>
+      <c r="H3" s="13">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.35266000000000003</v>
+      </c>
+      <c r="I3" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="13">
+        <v>0</v>
+      </c>
+      <c r="L3" s="13">
+        <f t="shared" ref="L3:L4" si="2">F3+G3+H3+I3+J3</f>
+        <v>5056.5281099999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="12">
+        <v>1662</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="12">
+        <v>100</v>
+      </c>
+      <c r="E4" s="13">
+        <v>27.5</v>
+      </c>
+      <c r="F4" s="13">
+        <f>D4*E4</f>
+        <v>2750</v>
+      </c>
+      <c r="G4" s="13">
+        <f t="shared" si="0"/>
+        <v>0.75625000000000009</v>
+      </c>
+      <c r="H4" s="13">
+        <f t="shared" si="1"/>
+        <v>0.19250000000000003</v>
+      </c>
+      <c r="I4" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="13">
+        <v>0</v>
+      </c>
+      <c r="L4" s="13">
+        <f t="shared" si="2"/>
+        <v>2767.73875</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="F5" s="13">
+        <f t="shared" ref="F5:L5" si="3">SUM(F2:F4)</f>
+        <v>9322</v>
+      </c>
+      <c r="G5" s="13">
+        <f t="shared" si="3"/>
+        <v>2.5635500000000002</v>
+      </c>
+      <c r="H5" s="13">
+        <f t="shared" si="3"/>
+        <v>0.65254000000000012</v>
+      </c>
+      <c r="I5" s="13">
+        <f t="shared" si="3"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="13">
+        <f t="shared" si="3"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="13">
+        <f t="shared" si="3"/>
+        <v>9375.5860899999989</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -1414,7 +1667,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
@@ -1941,7 +2194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
@@ -2850,7 +3103,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -3106,7 +3359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7618D34E-0B33-4181-8E63-6765777C5B7E}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
@@ -3398,7 +3651,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19EF43A-AB48-4760-8CB3-D62FBA7ABFD8}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -3614,7 +3867,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -3830,7 +4083,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1583F5-F968-4E69-BCCF-4B8530FA0CCB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -4046,7 +4299,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -4337,445 +4590,6 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E6" s="21"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E3E40E-BCAE-41DB-80FC-C74D9CCDCD28}">
-  <dimension ref="A1:AC13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="9">
-        <v>200</v>
-      </c>
-      <c r="E2" s="8">
-        <v>40</v>
-      </c>
-      <c r="F2" s="8">
-        <f>D2*E2</f>
-        <v>8000</v>
-      </c>
-      <c r="G2" s="8">
-        <f>F2*0.0275%</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H2" s="8">
-        <f>F2*0.007%</f>
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="I2" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="8">
-        <v>0.19</v>
-      </c>
-      <c r="L2" s="8">
-        <f>F2-G2-H2-I2-K2</f>
-        <v>7981.06</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-    </row>
-    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B3" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9">
-        <v>200</v>
-      </c>
-      <c r="E3" s="8">
-        <v>34.479999999999997</v>
-      </c>
-      <c r="F3" s="8">
-        <f>D3*E3</f>
-        <v>6895.9999999999991</v>
-      </c>
-      <c r="G3" s="8">
-        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
-        <v>1.8963999999999999</v>
-      </c>
-      <c r="H3" s="8">
-        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
-        <v>0.48271999999999998</v>
-      </c>
-      <c r="I3" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="8">
-        <f>((F3 - G3 - H3 - I3 - J3) - (18.5 * D3)) * 0.005%</f>
-        <v>0.15884154399999997</v>
-      </c>
-      <c r="L3" s="8">
-        <f>F3-G3-H3-I3-K3</f>
-        <v>6877.4720384559996</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-    </row>
-    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="9">
-        <v>200</v>
-      </c>
-      <c r="E4" s="8">
-        <v>27.45</v>
-      </c>
-      <c r="F4" s="8">
-        <f>D4*E4</f>
-        <v>5490</v>
-      </c>
-      <c r="G4" s="8">
-        <f t="shared" si="0"/>
-        <v>1.5097500000000001</v>
-      </c>
-      <c r="H4" s="8">
-        <f t="shared" si="1"/>
-        <v>0.38430000000000003</v>
-      </c>
-      <c r="I4" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="8">
-        <f>((F4 - G4 - H4 - I4 - J4) - (22.3 * D4)) * 0.005%</f>
-        <v>5.0565797500000009E-2</v>
-      </c>
-      <c r="L4" s="8">
-        <f>F4-G4-H4-I4-K4</f>
-        <v>5472.0653842025004</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-    </row>
-    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="11">
-        <f t="shared" ref="F5:L5" si="2">SUM(F2:F4)</f>
-        <v>20386</v>
-      </c>
-      <c r="G5" s="11">
-        <f t="shared" si="2"/>
-        <v>5.6061500000000004</v>
-      </c>
-      <c r="H5" s="11">
-        <f t="shared" si="2"/>
-        <v>1.4270200000000002</v>
-      </c>
-      <c r="I5" s="11">
-        <f t="shared" si="2"/>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="11">
-        <f t="shared" si="2"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="11">
-        <f t="shared" si="2"/>
-        <v>0.39940734150000001</v>
-      </c>
-      <c r="L5" s="11">
-        <f t="shared" si="2"/>
-        <v>20330.597422658502</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="8"/>
-      <c r="AB5" s="8"/>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="L8" s="1">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E9" s="19">
-        <v>100</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2750</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.22</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0.74</v>
-      </c>
-      <c r="I9" s="1">
-        <v>15.99</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="K9" s="1">
-        <f>F9-G9-H9-I9-J9</f>
-        <v>2732.2500000000005</v>
-      </c>
-      <c r="L9" s="1">
-        <f>L8+K9</f>
-        <v>2732.2500000000005</v>
-      </c>
-      <c r="N9" s="19">
-        <f>N8+E9</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E10" s="19">
-        <v>200</v>
-      </c>
-      <c r="F10" s="1">
-        <v>5940</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0.47</v>
-      </c>
-      <c r="H10" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="I10" s="1">
-        <v>15.99</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="K10" s="1">
-        <f t="shared" ref="K10:K12" si="3">F10-G10-H10-I10-J10</f>
-        <v>5921.1399999999994</v>
-      </c>
-      <c r="L10" s="1">
-        <f>L9+K10</f>
-        <v>8653.39</v>
-      </c>
-      <c r="N10" s="19">
-        <f>N9+E10</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E11" s="19">
-        <v>-200</v>
-      </c>
-      <c r="F11" s="1">
-        <v>6630</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0.39</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1.89</v>
-      </c>
-      <c r="I11" s="1">
-        <v>15.99</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="K11" s="1">
-        <f t="shared" si="3"/>
-        <v>6610.9299999999994</v>
-      </c>
-      <c r="L11" s="1">
-        <f>L10+((L10/N10)*E11)</f>
-        <v>2884.4633333333331</v>
-      </c>
-      <c r="N11" s="19">
-        <f>N10+E11</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E12" s="19">
-        <v>200</v>
-      </c>
-      <c r="F12" s="1">
-        <v>6400</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0.38</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1.82</v>
-      </c>
-      <c r="I12" s="1">
-        <v>15.99</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="K12" s="1">
-        <f t="shared" si="3"/>
-        <v>6381.01</v>
-      </c>
-      <c r="L12" s="20">
-        <f>L11+K12</f>
-        <v>9265.4733333333334</v>
-      </c>
-      <c r="N12" s="21">
-        <f>N11+E12</f>
-        <v>300</v>
-      </c>
-      <c r="O12" s="1">
-        <f>L12/N12</f>
-        <v>30.884911111111112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E13" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -4929,6 +4743,445 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E3E40E-BCAE-41DB-80FC-C74D9CCDCD28}">
+  <dimension ref="A1:AC13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9">
+        <v>200</v>
+      </c>
+      <c r="E2" s="8">
+        <v>40</v>
+      </c>
+      <c r="F2" s="8">
+        <f>D2*E2</f>
+        <v>8000</v>
+      </c>
+      <c r="G2" s="8">
+        <f>F2*0.0275%</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H2" s="8">
+        <f>F2*0.007%</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I2" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="L2" s="8">
+        <f>F2-G2-H2-I2-K2</f>
+        <v>7981.06</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9">
+        <v>200</v>
+      </c>
+      <c r="E3" s="8">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3*E3</f>
+        <v>6895.9999999999991</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.8963999999999999</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.48271999999999998</v>
+      </c>
+      <c r="I3" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="8">
+        <f>((F3 - G3 - H3 - I3 - J3) - (18.5 * D3)) * 0.005%</f>
+        <v>0.15884154399999997</v>
+      </c>
+      <c r="L3" s="8">
+        <f>F3-G3-H3-I3-K3</f>
+        <v>6877.4720384559996</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="9">
+        <v>200</v>
+      </c>
+      <c r="E4" s="8">
+        <v>27.45</v>
+      </c>
+      <c r="F4" s="8">
+        <f>D4*E4</f>
+        <v>5490</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5097500000000001</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" si="1"/>
+        <v>0.38430000000000003</v>
+      </c>
+      <c r="I4" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="8">
+        <f>((F4 - G4 - H4 - I4 - J4) - (22.3 * D4)) * 0.005%</f>
+        <v>5.0565797500000009E-2</v>
+      </c>
+      <c r="L4" s="8">
+        <f>F4-G4-H4-I4-K4</f>
+        <v>5472.0653842025004</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="11">
+        <f t="shared" ref="F5:L5" si="2">SUM(F2:F4)</f>
+        <v>20386</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="2"/>
+        <v>5.6061500000000004</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="2"/>
+        <v>1.4270200000000002</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="2"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="2"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="2"/>
+        <v>0.39940734150000001</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="2"/>
+        <v>20330.597422658502</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E9" s="19">
+        <v>100</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2750</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="I9" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K9" s="1">
+        <f>F9-G9-H9-I9-J9</f>
+        <v>2732.2500000000005</v>
+      </c>
+      <c r="L9" s="1">
+        <f>L8+K9</f>
+        <v>2732.2500000000005</v>
+      </c>
+      <c r="N9" s="19">
+        <f>N8+E9</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E10" s="19">
+        <v>200</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5940</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.47</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I10" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" ref="K10:K12" si="3">F10-G10-H10-I10-J10</f>
+        <v>5921.1399999999994</v>
+      </c>
+      <c r="L10" s="1">
+        <f>L9+K10</f>
+        <v>8653.39</v>
+      </c>
+      <c r="N10" s="19">
+        <f>N9+E10</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E11" s="19">
+        <v>-200</v>
+      </c>
+      <c r="F11" s="1">
+        <v>6630</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1.89</v>
+      </c>
+      <c r="I11" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="3"/>
+        <v>6610.9299999999994</v>
+      </c>
+      <c r="L11" s="1">
+        <f>L10+((L10/N10)*E11)</f>
+        <v>2884.4633333333331</v>
+      </c>
+      <c r="N11" s="19">
+        <f>N10+E11</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E12" s="19">
+        <v>200</v>
+      </c>
+      <c r="F12" s="1">
+        <v>6400</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1.82</v>
+      </c>
+      <c r="I12" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="3"/>
+        <v>6381.01</v>
+      </c>
+      <c r="L12" s="20">
+        <f>L11+K12</f>
+        <v>9265.4733333333334</v>
+      </c>
+      <c r="N12" s="21">
+        <f>N11+E12</f>
+        <v>300</v>
+      </c>
+      <c r="O12" s="1">
+        <f>L12/N12</f>
+        <v>30.884911111111112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E13" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F402F95-319A-4797-B7E1-F3EB07A82FDD}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -5145,7 +5398,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A590E594-CB91-4439-95F2-7F159495761F}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -5362,7 +5615,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34F43A8-C89C-44C0-BF29-1F8134A0151F}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -5660,7 +5913,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5AE87-00E8-4CF9-A517-EB6C0CA40610}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -5876,7 +6129,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B51BEB4-905E-4036-959A-F9A0226AF070}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6093,7 +6346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B7349E-D984-4817-800E-2EB4836D5B5D}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6310,7 +6563,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA65F892-A6B4-4288-ADB5-125D04E295EB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6527,7 +6780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421F9D80-1D28-4F3C-95F7-8DE9883A26F0}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6744,7 +6997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D25BF0F-8645-49A4-A6C8-BE755BFA7BE7}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -7043,246 +7296,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4721B46-AB87-4CAA-ABF7-E48CFDA36C4A}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="2"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>42996</v>
-      </c>
-      <c r="B2" s="4">
-        <v>168102</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>23.65</v>
-      </c>
-      <c r="F2" s="3">
-        <f>D2*E2</f>
-        <v>9460</v>
-      </c>
-      <c r="G2" s="3">
-        <f t="shared" ref="G2:G3" si="0">F2*0.0275%</f>
-        <v>2.6015000000000001</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.47300000000000003</v>
-      </c>
-      <c r="I2" s="3">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="J2" s="3">
-        <f>I2*5%</f>
-        <v>0.12450000000000001</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>9465.6890000000003</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-    </row>
-    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>42996</v>
-      </c>
-      <c r="B3" s="9">
-        <v>168102</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="9">
-        <v>700</v>
-      </c>
-      <c r="E3" s="8">
-        <v>10.5</v>
-      </c>
-      <c r="F3" s="8">
-        <f>D3*E3</f>
-        <v>7350</v>
-      </c>
-      <c r="G3" s="8">
-        <f t="shared" si="0"/>
-        <v>2.0212500000000002</v>
-      </c>
-      <c r="H3" s="8">
-        <f>F3*0.005%</f>
-        <v>0.36749999999999999</v>
-      </c>
-      <c r="I3" s="8">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="J3" s="8">
-        <f>I3*5%</f>
-        <v>0.12450000000000001</v>
-      </c>
-      <c r="K3" s="8">
-        <v>0</v>
-      </c>
-      <c r="L3" s="8">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>7355.0032499999998</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7">
-        <f t="shared" ref="F4:K4" si="1">SUM(F2:F3)</f>
-        <v>16810</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" si="1"/>
-        <v>4.6227499999999999</v>
-      </c>
-      <c r="H4" s="7">
-        <f t="shared" si="1"/>
-        <v>0.84050000000000002</v>
-      </c>
-      <c r="I4" s="7">
-        <f t="shared" si="1"/>
-        <v>4.9800000000000004</v>
-      </c>
-      <c r="J4" s="7">
-        <f t="shared" si="1"/>
-        <v>0.24900000000000003</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="7">
-        <f>L3-L2</f>
-        <v>-2110.6857500000006</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9619B6EC-CCEF-49B4-8315-42E7841BC89B}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -7425,6 +7443,241 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4721B46-AB87-4CAA-ABF7-E48CFDA36C4A}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>42996</v>
+      </c>
+      <c r="B2" s="4">
+        <v>168102</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>23.65</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>9460</v>
+      </c>
+      <c r="G2" s="3">
+        <f t="shared" ref="G2:G3" si="0">F2*0.0275%</f>
+        <v>2.6015000000000001</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.47300000000000003</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="J2" s="3">
+        <f>I2*5%</f>
+        <v>0.12450000000000001</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>9465.6890000000003</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>42996</v>
+      </c>
+      <c r="B3" s="9">
+        <v>168102</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="9">
+        <v>700</v>
+      </c>
+      <c r="E3" s="8">
+        <v>10.5</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3*E3</f>
+        <v>7350</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" si="0"/>
+        <v>2.0212500000000002</v>
+      </c>
+      <c r="H3" s="8">
+        <f>F3*0.005%</f>
+        <v>0.36749999999999999</v>
+      </c>
+      <c r="I3" s="8">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="J3" s="8">
+        <f>I3*5%</f>
+        <v>0.12450000000000001</v>
+      </c>
+      <c r="K3" s="8">
+        <v>0</v>
+      </c>
+      <c r="L3" s="8">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>7355.0032499999998</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f t="shared" ref="F4:K4" si="1">SUM(F2:F3)</f>
+        <v>16810</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" si="1"/>
+        <v>4.6227499999999999</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="1"/>
+        <v>0.84050000000000002</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="1"/>
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="1"/>
+        <v>0.24900000000000003</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f>L3-L2</f>
+        <v>-2110.6857500000006</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF39107-DEBE-454A-A911-9FAC6360BB3B}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -7660,6 +7913,149 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4354C79-E6C9-44CE-9F1A-DAEDD0DC1366}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="18"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="24"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF98C6E-C61C-4098-8811-20C737B2746F}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -8246,7 +8642,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -8833,7 +9229,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F27D22B-36B9-402D-A19C-031FF2332945}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
@@ -9002,7 +9398,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7579CBF-C87A-40BF-91B5-CE83CDC20ECE}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9197,7 +9593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384BB7C-DF07-4187-ADF0-23E50C2BA287}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -9497,256 +9893,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EC0A3F-FFB0-437C-B726-EA72E0B69675}">
-  <dimension ref="A1:AC7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.140625" style="12"/>
-    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="18"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
-        <v>39757</v>
-      </c>
-      <c r="B2" s="12">
-        <v>1662</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="12">
-        <v>100</v>
-      </c>
-      <c r="E2" s="13">
-        <v>15.34</v>
-      </c>
-      <c r="F2" s="13">
-        <f>D2*E2</f>
-        <v>1534</v>
-      </c>
-      <c r="G2" s="13">
-        <f>F2*0.0275%</f>
-        <v>0.42185</v>
-      </c>
-      <c r="H2" s="13">
-        <f>F2*0.007%</f>
-        <v>0.10738000000000002</v>
-      </c>
-      <c r="I2" s="13">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="13">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="13">
-        <v>0</v>
-      </c>
-      <c r="L2" s="13">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>1551.3192299999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
-        <v>39757</v>
-      </c>
-      <c r="B3" s="12">
-        <v>1662</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="12">
-        <v>200</v>
-      </c>
-      <c r="E3" s="13">
-        <v>25.19</v>
-      </c>
-      <c r="F3" s="13">
-        <f>D3*E3</f>
-        <v>5038</v>
-      </c>
-      <c r="G3" s="13">
-        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
-        <v>1.3854500000000001</v>
-      </c>
-      <c r="H3" s="13">
-        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
-        <v>0.35266000000000003</v>
-      </c>
-      <c r="I3" s="13">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="13">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="13">
-        <v>0</v>
-      </c>
-      <c r="L3" s="13">
-        <f t="shared" ref="L3:L4" si="2">F3+G3+H3+I3+J3</f>
-        <v>5056.5281099999993</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
-        <v>39757</v>
-      </c>
-      <c r="B4" s="12">
-        <v>1662</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="12">
-        <v>100</v>
-      </c>
-      <c r="E4" s="13">
-        <v>27.5</v>
-      </c>
-      <c r="F4" s="13">
-        <f>D4*E4</f>
-        <v>2750</v>
-      </c>
-      <c r="G4" s="13">
-        <f t="shared" si="0"/>
-        <v>0.75625000000000009</v>
-      </c>
-      <c r="H4" s="13">
-        <f t="shared" si="1"/>
-        <v>0.19250000000000003</v>
-      </c>
-      <c r="I4" s="13">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="13">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="13">
-        <v>0</v>
-      </c>
-      <c r="L4" s="13">
-        <f t="shared" si="2"/>
-        <v>2767.73875</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="F5" s="13">
-        <f t="shared" ref="F5:L5" si="3">SUM(F2:F4)</f>
-        <v>9322</v>
-      </c>
-      <c r="G5" s="13">
-        <f t="shared" si="3"/>
-        <v>2.5635500000000002</v>
-      </c>
-      <c r="H5" s="13">
-        <f t="shared" si="3"/>
-        <v>0.65254000000000012</v>
-      </c>
-      <c r="I5" s="13">
-        <f t="shared" si="3"/>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="13">
-        <f t="shared" si="3"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L5" s="13">
-        <f t="shared" si="3"/>
-        <v>9375.5860899999989</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Prevents a 'BrokerageNotesWorksheetReader' from being created when a negative 'NoteNumber' is found.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,42 +8,43 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68CA0F0-AEDE-4109-8296-0F7DD7562FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF14D303-39D9-4D93-B011-AD0FA650F1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="2" activeTab="3" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="3" activeTab="4" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="NotUsed" sheetId="2" r:id="rId1"/>
     <sheet name="TradingDateMissing" sheetId="35" r:id="rId2"/>
     <sheet name="TradingDateBlack" sheetId="36" r:id="rId3"/>
     <sheet name="NoteNumberMissing" sheetId="37" r:id="rId4"/>
-    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId5"/>
-    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId6"/>
-    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId7"/>
-    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId8"/>
-    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId9"/>
-    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId10"/>
-    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId11"/>
-    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId12"/>
-    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId13"/>
-    <sheet name="SingleLineGroups" sheetId="10" r:id="rId14"/>
-    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId15"/>
-    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId16"/>
-    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId17"/>
-    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId18"/>
-    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId19"/>
-    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId20"/>
-    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId21"/>
-    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId22"/>
-    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId23"/>
-    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId24"/>
-    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId25"/>
-    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId26"/>
-    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId27"/>
-    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId28"/>
-    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId29"/>
-    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId30"/>
-    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId31"/>
+    <sheet name="NoteNumberNegative" sheetId="38" r:id="rId5"/>
+    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId6"/>
+    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId7"/>
+    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId8"/>
+    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId9"/>
+    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId10"/>
+    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId11"/>
+    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId12"/>
+    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId13"/>
+    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId14"/>
+    <sheet name="SingleLineGroups" sheetId="10" r:id="rId15"/>
+    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId16"/>
+    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId17"/>
+    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId18"/>
+    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId19"/>
+    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId20"/>
+    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId21"/>
+    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId22"/>
+    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId23"/>
+    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId24"/>
+    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId25"/>
+    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId26"/>
+    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId27"/>
+    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId28"/>
+    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId29"/>
+    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId30"/>
+    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId31"/>
+    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId32"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -169,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="25">
   <si>
     <t>BBAS3</t>
   </si>
@@ -829,6 +830,308 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384BB7C-DF07-4187-ADF0-23E50C2BA287}">
+  <dimension ref="A1:AC7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="1" sqref="B3 A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="12"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="18"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B3" s="22">
+        <v>1662</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>200</v>
+      </c>
+      <c r="E3" s="3">
+        <v>25.19</v>
+      </c>
+      <c r="F3" s="3">
+        <f>D3*E3</f>
+        <v>5038</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.3854500000000001</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.35266000000000003</v>
+      </c>
+      <c r="I3" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>5056.5281099999993</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4">
+        <v>100</v>
+      </c>
+      <c r="E4" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F4" s="3">
+        <f>D4*E4</f>
+        <v>2750</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.75625000000000009</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.19250000000000003</v>
+      </c>
+      <c r="I4" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <f>F4+G4+H4+I4+J4</f>
+        <v>2767.73875</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="7">
+        <f>-SUM(F2:F4)</f>
+        <v>-9322</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" ref="G5:K5" si="2">SUM(G2:G4)</f>
+        <v>2.5635500000000002</v>
+      </c>
+      <c r="H5" s="7">
+        <f t="shared" si="2"/>
+        <v>0.65254000000000012</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="shared" si="2"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" si="2"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="7">
+        <f>-SUM(L2:L4)</f>
+        <v>-9375.5860899999989</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EC0A3F-FFB0-437C-B726-EA72E0B69675}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -1080,7 +1383,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -1667,7 +1970,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
@@ -2194,7 +2497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
@@ -3103,7 +3406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -3359,7 +3662,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7618D34E-0B33-4181-8E63-6765777C5B7E}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
@@ -3651,7 +3954,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19EF43A-AB48-4760-8CB3-D62FBA7ABFD8}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -3867,7 +4170,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -4083,7 +4386,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1583F5-F968-4E69-BCCF-4B8530FA0CCB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -4296,305 +4599,6 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
-  <dimension ref="A1:AC6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="9">
-        <v>200</v>
-      </c>
-      <c r="E2" s="8">
-        <v>40</v>
-      </c>
-      <c r="F2" s="8">
-        <f>D2*E2</f>
-        <v>8000</v>
-      </c>
-      <c r="G2" s="8">
-        <f>F2*0.0275%</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H2" s="8">
-        <f>F2*0.007%</f>
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="I2" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="8">
-        <v>0.19</v>
-      </c>
-      <c r="L2" s="8">
-        <f>F2-G2-H2-I2-K2</f>
-        <v>7981.06</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-    </row>
-    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B3" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9">
-        <v>200</v>
-      </c>
-      <c r="E3" s="8">
-        <v>34.479999999999997</v>
-      </c>
-      <c r="F3" s="8">
-        <f>D3*E3</f>
-        <v>6895.9999999999991</v>
-      </c>
-      <c r="G3" s="8">
-        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
-        <v>1.8963999999999999</v>
-      </c>
-      <c r="H3" s="8">
-        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
-        <v>0.48271999999999998</v>
-      </c>
-      <c r="I3" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="8">
-        <f>((F3 - G3 - H3 - I3 - J3) - (18.5 * D3)) * 0.005%</f>
-        <v>0.15884154399999997</v>
-      </c>
-      <c r="L3" s="8">
-        <f>F3-G3-H3-I3-K3</f>
-        <v>6877.4720384559996</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-    </row>
-    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="9">
-        <v>200</v>
-      </c>
-      <c r="E4" s="8">
-        <v>27.45</v>
-      </c>
-      <c r="F4" s="8">
-        <f>D4*E4</f>
-        <v>5490</v>
-      </c>
-      <c r="G4" s="8">
-        <f t="shared" si="0"/>
-        <v>1.5097500000000001</v>
-      </c>
-      <c r="H4" s="8">
-        <f t="shared" si="1"/>
-        <v>0.38430000000000003</v>
-      </c>
-      <c r="I4" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="8">
-        <f>((F4 - G4 - H4 - I4 - J4) - (22.3 * D4)) * 0.005%</f>
-        <v>5.0565797500000009E-2</v>
-      </c>
-      <c r="L4" s="8">
-        <f>F4-G4-H4-I4-K4</f>
-        <v>5472.0653842025004</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-    </row>
-    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="11">
-        <f t="shared" ref="F5:L5" si="2">SUM(F2:F4)</f>
-        <v>20386</v>
-      </c>
-      <c r="G5" s="11">
-        <f t="shared" si="2"/>
-        <v>5.6061500000000004</v>
-      </c>
-      <c r="H5" s="11">
-        <f t="shared" si="2"/>
-        <v>1.4270200000000002</v>
-      </c>
-      <c r="I5" s="11">
-        <f t="shared" si="2"/>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="11">
-        <f t="shared" si="2"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="11">
-        <f t="shared" si="2"/>
-        <v>0.39940734150000001</v>
-      </c>
-      <c r="L5" s="11">
-        <f t="shared" si="2"/>
-        <v>20330.597422658502</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="8"/>
-      <c r="AB5" s="8"/>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E6" s="21"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4743,6 +4747,305 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
+  <dimension ref="A1:AC6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9">
+        <v>200</v>
+      </c>
+      <c r="E2" s="8">
+        <v>40</v>
+      </c>
+      <c r="F2" s="8">
+        <f>D2*E2</f>
+        <v>8000</v>
+      </c>
+      <c r="G2" s="8">
+        <f>F2*0.0275%</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H2" s="8">
+        <f>F2*0.007%</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I2" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="L2" s="8">
+        <f>F2-G2-H2-I2-K2</f>
+        <v>7981.06</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9">
+        <v>200</v>
+      </c>
+      <c r="E3" s="8">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3*E3</f>
+        <v>6895.9999999999991</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.8963999999999999</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.48271999999999998</v>
+      </c>
+      <c r="I3" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="8">
+        <f>((F3 - G3 - H3 - I3 - J3) - (18.5 * D3)) * 0.005%</f>
+        <v>0.15884154399999997</v>
+      </c>
+      <c r="L3" s="8">
+        <f>F3-G3-H3-I3-K3</f>
+        <v>6877.4720384559996</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="9">
+        <v>200</v>
+      </c>
+      <c r="E4" s="8">
+        <v>27.45</v>
+      </c>
+      <c r="F4" s="8">
+        <f>D4*E4</f>
+        <v>5490</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5097500000000001</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" si="1"/>
+        <v>0.38430000000000003</v>
+      </c>
+      <c r="I4" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="8">
+        <f>((F4 - G4 - H4 - I4 - J4) - (22.3 * D4)) * 0.005%</f>
+        <v>5.0565797500000009E-2</v>
+      </c>
+      <c r="L4" s="8">
+        <f>F4-G4-H4-I4-K4</f>
+        <v>5472.0653842025004</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="11">
+        <f t="shared" ref="F5:L5" si="2">SUM(F2:F4)</f>
+        <v>20386</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="2"/>
+        <v>5.6061500000000004</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="2"/>
+        <v>1.4270200000000002</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="2"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="2"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="2"/>
+        <v>0.39940734150000001</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="2"/>
+        <v>20330.597422658502</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E6" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E3E40E-BCAE-41DB-80FC-C74D9CCDCD28}">
   <dimension ref="A1:AC13"/>
   <sheetViews>
@@ -5181,7 +5484,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F402F95-319A-4797-B7E1-F3EB07A82FDD}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -5398,7 +5701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A590E594-CB91-4439-95F2-7F159495761F}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -5615,7 +5918,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34F43A8-C89C-44C0-BF29-1F8134A0151F}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -5913,7 +6216,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5AE87-00E8-4CF9-A517-EB6C0CA40610}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6129,7 +6432,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B51BEB4-905E-4036-959A-F9A0226AF070}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6346,7 +6649,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B7349E-D984-4817-800E-2EB4836D5B5D}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6563,7 +6866,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA65F892-A6B4-4288-ADB5-125D04E295EB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6780,7 +7083,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421F9D80-1D28-4F3C-95F7-8DE9883A26F0}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6990,305 +7293,6 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D25BF0F-8645-49A4-A6C8-BE755BFA7BE7}">
-  <dimension ref="A1:AC8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="9">
-        <v>200</v>
-      </c>
-      <c r="E2" s="8">
-        <v>35.15</v>
-      </c>
-      <c r="F2" s="8">
-        <f>D2*E2</f>
-        <v>7030</v>
-      </c>
-      <c r="G2" s="8">
-        <f>F2*0.0275%</f>
-        <v>1.9332500000000001</v>
-      </c>
-      <c r="H2" s="8">
-        <f>F2*0.007%</f>
-        <v>0.49210000000000004</v>
-      </c>
-      <c r="I2" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="8">
-        <f>((F2 - G2 - H2 - I2 - J2) - (30.88 * D2)) * 0.005%</f>
-        <v>4.173923249999998E-2</v>
-      </c>
-      <c r="L2" s="8">
-        <f t="shared" ref="L2:L4" si="0">F2-G2-H2-I2-J2</f>
-        <v>7010.7846499999996</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-    </row>
-    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B3" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="9">
-        <v>200</v>
-      </c>
-      <c r="E3" s="8">
-        <v>34.479999999999997</v>
-      </c>
-      <c r="F3" s="8">
-        <f>D3*E3</f>
-        <v>6895.9999999999991</v>
-      </c>
-      <c r="G3" s="8">
-        <f t="shared" ref="G3:G4" si="1">F3*0.0275%</f>
-        <v>1.8963999999999999</v>
-      </c>
-      <c r="H3" s="8">
-        <f t="shared" ref="H3:H4" si="2">F3*0.007%</f>
-        <v>0.48271999999999998</v>
-      </c>
-      <c r="I3" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="8">
-        <f>((F3 - G3 - H3 - I3 - J3) - (30.88 * D3)) * 0.005%</f>
-        <v>3.504154399999998E-2</v>
-      </c>
-      <c r="L3" s="8">
-        <f t="shared" si="0"/>
-        <v>6876.8308799999995</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-    </row>
-    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="9">
-        <v>200</v>
-      </c>
-      <c r="E4" s="8">
-        <v>31</v>
-      </c>
-      <c r="F4" s="8">
-        <f>D4*E4</f>
-        <v>6200</v>
-      </c>
-      <c r="G4" s="8">
-        <f t="shared" si="1"/>
-        <v>1.7050000000000001</v>
-      </c>
-      <c r="H4" s="8">
-        <f t="shared" si="2"/>
-        <v>0.43400000000000005</v>
-      </c>
-      <c r="I4" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="8">
-        <f>((F4 - G4 - H4 - I4 - J4) - (30.88 * D4)) * 0.005%</f>
-        <v>2.5354999999999567E-4</v>
-      </c>
-      <c r="L4" s="8">
-        <f t="shared" si="0"/>
-        <v>6181.0709999999999</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-    </row>
-    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="11">
-        <f t="shared" ref="F5:L5" si="3">SUM(F2:F4)</f>
-        <v>20126</v>
-      </c>
-      <c r="G5" s="11">
-        <f t="shared" si="3"/>
-        <v>5.5346500000000001</v>
-      </c>
-      <c r="H5" s="11">
-        <f t="shared" si="3"/>
-        <v>1.40882</v>
-      </c>
-      <c r="I5" s="11">
-        <f t="shared" si="3"/>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="11">
-        <f t="shared" si="3"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="11">
-        <f>SUM(K2:K4) - 0.03</f>
-        <v>4.7034326499999946E-2</v>
-      </c>
-      <c r="L5" s="11">
-        <f t="shared" si="3"/>
-        <v>20068.686529999999</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="8"/>
-      <c r="AB5" s="8"/>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E8" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -7443,6 +7447,305 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D25BF0F-8645-49A4-A6C8-BE755BFA7BE7}">
+  <dimension ref="A1:AC8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9">
+        <v>200</v>
+      </c>
+      <c r="E2" s="8">
+        <v>35.15</v>
+      </c>
+      <c r="F2" s="8">
+        <f>D2*E2</f>
+        <v>7030</v>
+      </c>
+      <c r="G2" s="8">
+        <f>F2*0.0275%</f>
+        <v>1.9332500000000001</v>
+      </c>
+      <c r="H2" s="8">
+        <f>F2*0.007%</f>
+        <v>0.49210000000000004</v>
+      </c>
+      <c r="I2" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="8">
+        <f>((F2 - G2 - H2 - I2 - J2) - (30.88 * D2)) * 0.005%</f>
+        <v>4.173923249999998E-2</v>
+      </c>
+      <c r="L2" s="8">
+        <f t="shared" ref="L2:L4" si="0">F2-G2-H2-I2-J2</f>
+        <v>7010.7846499999996</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9">
+        <v>200</v>
+      </c>
+      <c r="E3" s="8">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3*E3</f>
+        <v>6895.9999999999991</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" ref="G3:G4" si="1">F3*0.0275%</f>
+        <v>1.8963999999999999</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" ref="H3:H4" si="2">F3*0.007%</f>
+        <v>0.48271999999999998</v>
+      </c>
+      <c r="I3" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="8">
+        <f>((F3 - G3 - H3 - I3 - J3) - (30.88 * D3)) * 0.005%</f>
+        <v>3.504154399999998E-2</v>
+      </c>
+      <c r="L3" s="8">
+        <f t="shared" si="0"/>
+        <v>6876.8308799999995</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9">
+        <v>200</v>
+      </c>
+      <c r="E4" s="8">
+        <v>31</v>
+      </c>
+      <c r="F4" s="8">
+        <f>D4*E4</f>
+        <v>6200</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" si="1"/>
+        <v>1.7050000000000001</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" si="2"/>
+        <v>0.43400000000000005</v>
+      </c>
+      <c r="I4" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="8">
+        <f>((F4 - G4 - H4 - I4 - J4) - (30.88 * D4)) * 0.005%</f>
+        <v>2.5354999999999567E-4</v>
+      </c>
+      <c r="L4" s="8">
+        <f t="shared" si="0"/>
+        <v>6181.0709999999999</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="11">
+        <f t="shared" ref="F5:L5" si="3">SUM(F2:F4)</f>
+        <v>20126</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="3"/>
+        <v>5.5346500000000001</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="3"/>
+        <v>1.40882</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="3"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="3"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="11">
+        <f>SUM(K2:K4) - 0.03</f>
+        <v>4.7034326499999946E-2</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="3"/>
+        <v>20068.686529999999</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E8" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4721B46-AB87-4CAA-ABF7-E48CFDA36C4A}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -7677,7 +7980,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF39107-DEBE-454A-A911-9FAC6360BB3B}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -7914,6 +8217,149 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4354C79-E6C9-44CE-9F1A-DAEDD0DC1366}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="18"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="24"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE237FC-86A6-42F5-B3CD-F725B4DFF9E2}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -7999,6 +8445,9 @@
       <c r="A2" s="5">
         <v>39757</v>
       </c>
+      <c r="B2" s="4">
+        <v>-1662</v>
+      </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
@@ -8055,7 +8504,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF98C6E-C61C-4098-8811-20C737B2746F}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -8642,7 +9091,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -9229,7 +9678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F27D22B-36B9-402D-A19C-031FF2332945}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
@@ -9398,7 +9847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7579CBF-C87A-40BF-91B5-CE83CDC20ECE}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9591,306 +10040,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384BB7C-DF07-4187-ADF0-23E50C2BA287}">
-  <dimension ref="A1:AC7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="1" sqref="B3 A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.140625" style="12"/>
-    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="18"/>
-    </row>
-    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4">
-        <v>100</v>
-      </c>
-      <c r="E2" s="3">
-        <v>15.34</v>
-      </c>
-      <c r="F2" s="3">
-        <f>D2*E2</f>
-        <v>1534</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.0275%</f>
-        <v>0.42185</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.007%</f>
-        <v>0.10738000000000002</v>
-      </c>
-      <c r="I2" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>1551.3192299999998</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-    </row>
-    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B3" s="22">
-        <v>1662</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" s="3">
-        <v>25.19</v>
-      </c>
-      <c r="F3" s="3">
-        <f>D3*E3</f>
-        <v>5038</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
-        <v>1.3854500000000001</v>
-      </c>
-      <c r="H3" s="3">
-        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
-        <v>0.35266000000000003</v>
-      </c>
-      <c r="I3" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>5056.5281099999993</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4">
-        <v>100</v>
-      </c>
-      <c r="E4" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F4" s="3">
-        <f>D4*E4</f>
-        <v>2750</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" si="0"/>
-        <v>0.75625000000000009</v>
-      </c>
-      <c r="H4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.19250000000000003</v>
-      </c>
-      <c r="I4" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3">
-        <f>F4+G4+H4+I4+J4</f>
-        <v>2767.73875</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="7">
-        <f>-SUM(F2:F4)</f>
-        <v>-9322</v>
-      </c>
-      <c r="G5" s="7">
-        <f t="shared" ref="G5:K5" si="2">SUM(G2:G4)</f>
-        <v>2.5635500000000002</v>
-      </c>
-      <c r="H5" s="7">
-        <f t="shared" si="2"/>
-        <v>0.65254000000000012</v>
-      </c>
-      <c r="I5" s="7">
-        <f t="shared" si="2"/>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="7">
-        <f t="shared" si="2"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L5" s="7">
-        <f>-SUM(L2:L4)</f>
-        <v>-9375.5860899999989</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Prevents a 'BrokerageNotesWorksheetReader' from being created when a 'NoteNumber' contains extraneous characters that prevent it from being interpreted as an integer number.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF14D303-39D9-4D93-B011-AD0FA650F1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBC7861-DA02-4800-8B61-B975550058CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="3" activeTab="4" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="4" activeTab="5" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="NotUsed" sheetId="2" r:id="rId1"/>
@@ -18,33 +18,34 @@
     <sheet name="TradingDateBlack" sheetId="36" r:id="rId3"/>
     <sheet name="NoteNumberMissing" sheetId="37" r:id="rId4"/>
     <sheet name="NoteNumberNegative" sheetId="38" r:id="rId5"/>
-    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId6"/>
-    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId7"/>
-    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId8"/>
-    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId9"/>
-    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId10"/>
-    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId11"/>
-    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId12"/>
-    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId13"/>
-    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId14"/>
-    <sheet name="SingleLineGroups" sheetId="10" r:id="rId15"/>
-    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId16"/>
-    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId17"/>
-    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId18"/>
-    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId19"/>
-    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId20"/>
-    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId21"/>
-    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId22"/>
-    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId23"/>
-    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId24"/>
-    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId25"/>
-    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId26"/>
-    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId27"/>
-    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId28"/>
-    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId29"/>
-    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId30"/>
-    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId31"/>
-    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId32"/>
+    <sheet name="NoteNumberExtraneousCharacters" sheetId="39" r:id="rId6"/>
+    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId7"/>
+    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId8"/>
+    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId9"/>
+    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId10"/>
+    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId11"/>
+    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId12"/>
+    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId13"/>
+    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId14"/>
+    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId15"/>
+    <sheet name="SingleLineGroups" sheetId="10" r:id="rId16"/>
+    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId17"/>
+    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId18"/>
+    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId19"/>
+    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId20"/>
+    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId21"/>
+    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId22"/>
+    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId23"/>
+    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId24"/>
+    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId25"/>
+    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId26"/>
+    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId27"/>
+    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId28"/>
+    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId29"/>
+    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId30"/>
+    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId31"/>
+    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId32"/>
+    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId33"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -170,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="26">
   <si>
     <t>BBAS3</t>
   </si>
@@ -245,6 +246,9 @@
   </si>
   <si>
     <t>RAIL3</t>
+  </si>
+  <si>
+    <t>I662</t>
   </si>
 </sst>
 </file>
@@ -830,6 +834,201 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7579CBF-C87A-40BF-91B5-CE83CDC20ECE}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="F4" s="7">
+        <f>SUM(F1:F3)</f>
+        <v>22600</v>
+      </c>
+      <c r="G4" s="7">
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f>SUM(H1:H3)</f>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f>SUM(I1:I3)</f>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f>SUM(J1:J3)</f>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7">
+        <f>SUM(L1:L3)</f>
+        <v>22611.018699999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384BB7C-DF07-4187-ADF0-23E50C2BA287}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -1131,7 +1330,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EC0A3F-FFB0-437C-B726-EA72E0B69675}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -1383,7 +1582,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -1970,7 +2169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
@@ -2497,7 +2696,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
@@ -3406,7 +3605,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -3662,7 +3861,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7618D34E-0B33-4181-8E63-6765777C5B7E}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
@@ -3954,7 +4153,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19EF43A-AB48-4760-8CB3-D62FBA7ABFD8}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -4170,7 +4369,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -4366,222 +4565,6 @@
       <c r="L4" s="7">
         <f>-SUM(L2:L3)</f>
         <v>-22611.028699999995</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1583F5-F968-4E69-BCCF-4B8530FA0CCB}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B2" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
-        <v>11000</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.025%</f>
-        <v>2.75</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J2" s="3">
-        <v>0.12</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>11005.41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B3" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500</v>
-      </c>
-      <c r="E3" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" si="0"/>
-        <v>11600</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*0.025%</f>
-        <v>2.9</v>
-      </c>
-      <c r="H3" s="3">
-        <f>F3*0.005%</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" ref="J3" si="1">I3*6.5%</f>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>11605.599349999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7">
-        <f>-SUM(F2:F3)</f>
-        <v>-22600</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
-        <v>5.65</v>
-      </c>
-      <c r="H4" s="7">
-        <f t="shared" si="2"/>
-        <v>1.1300000000000001</v>
-      </c>
-      <c r="I4" s="7">
-        <f t="shared" si="2"/>
-        <v>3.98</v>
-      </c>
-      <c r="J4" s="7">
-        <f t="shared" si="2"/>
-        <v>0.24934999999999999</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="7">
-        <f>-SUM(L2:L3)</f>
-        <v>-22611.00935</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -4747,6 +4730,222 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1583F5-F968-4E69-BCCF-4B8530FA0CCB}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" ref="J3" si="1">I3*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.24934999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.00935</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -5045,7 +5244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E3E40E-BCAE-41DB-80FC-C74D9CCDCD28}">
   <dimension ref="A1:AC13"/>
   <sheetViews>
@@ -5484,7 +5683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F402F95-319A-4797-B7E1-F3EB07A82FDD}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -5701,7 +5900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A590E594-CB91-4439-95F2-7F159495761F}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -5918,7 +6117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34F43A8-C89C-44C0-BF29-1F8134A0151F}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -6216,7 +6415,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5AE87-00E8-4CF9-A517-EB6C0CA40610}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6432,7 +6631,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B51BEB4-905E-4036-959A-F9A0226AF070}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6649,7 +6848,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B7349E-D984-4817-800E-2EB4836D5B5D}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6866,7 +7065,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA65F892-A6B4-4288-ADB5-125D04E295EB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -7055,223 +7254,6 @@
       <c r="J4" s="7">
         <f t="shared" si="2"/>
         <v>0.25869999999999999</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="7">
-        <f>-SUM(L2:L3)</f>
-        <v>-22611.018699999997</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421F9D80-1D28-4F3C-95F7-8DE9883A26F0}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B2" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
-        <v>11000</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.025%</f>
-        <v>2.75</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>11005.419349999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B3" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500</v>
-      </c>
-      <c r="E3" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" si="0"/>
-        <v>11600</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*0.025%</f>
-        <v>2.9</v>
-      </c>
-      <c r="H3" s="3">
-        <f>F3*0.005%</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>11605.599349999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7">
-        <f>-SUM(F2:F3)</f>
-        <v>-22600</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
-        <v>5.65</v>
-      </c>
-      <c r="H4" s="7">
-        <f>SUM(H2:H3)</f>
-        <v>1.1300000000000001</v>
-      </c>
-      <c r="I4" s="7">
-        <f>SUM(I2:I3)</f>
-        <v>3.98</v>
-      </c>
-      <c r="J4" s="7">
-        <f>SUM(J2:J3) + 0.03</f>
-        <v>0.28869999999999996</v>
       </c>
       <c r="K4" s="7">
         <f t="shared" si="2"/>
@@ -7447,6 +7429,223 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421F9D80-1D28-4F3C-95F7-8DE9883A26F0}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f>SUM(H2:H3)</f>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f>SUM(I2:I3)</f>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f>SUM(J2:J3) + 0.03</f>
+        <v>0.28869999999999996</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.018699999997</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D25BF0F-8645-49A4-A6C8-BE755BFA7BE7}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -7745,7 +7944,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4721B46-AB87-4CAA-ABF7-E48CFDA36C4A}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -7980,7 +8179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF39107-DEBE-454A-A911-9FAC6360BB3B}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8362,6 +8561,152 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE237FC-86A6-42F5-B3CD-F725B4DFF9E2}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="18"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="24"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>-1662</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29FF2F8-FD89-4B31-BC92-2C175C3A29E3}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
@@ -8445,8 +8790,8 @@
       <c r="A2" s="5">
         <v>39757</v>
       </c>
-      <c r="B2" s="4">
-        <v>-1662</v>
+      <c r="B2" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -8504,7 +8849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF98C6E-C61C-4098-8811-20C737B2746F}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -9091,7 +9436,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -9678,7 +10023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F27D22B-36B9-402D-A19C-031FF2332945}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
@@ -9845,199 +10190,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7579CBF-C87A-40BF-91B5-CE83CDC20ECE}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B2" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
-        <v>11000</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.025%</f>
-        <v>2.75</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>11005.419349999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B3" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500</v>
-      </c>
-      <c r="E3" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" si="0"/>
-        <v>11600</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*0.025%</f>
-        <v>2.9</v>
-      </c>
-      <c r="H3" s="3">
-        <f>F3*0.005%</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>11605.599349999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="F4" s="7">
-        <f>SUM(F1:F3)</f>
-        <v>22600</v>
-      </c>
-      <c r="G4" s="7">
-        <v>5.65</v>
-      </c>
-      <c r="H4" s="7">
-        <f>SUM(H1:H3)</f>
-        <v>1.1300000000000001</v>
-      </c>
-      <c r="I4" s="7">
-        <f>SUM(I1:I3)</f>
-        <v>3.98</v>
-      </c>
-      <c r="J4" s="7">
-        <f>SUM(J1:J3)</f>
-        <v>0.25869999999999999</v>
-      </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7">
-        <f>SUM(L1:L3)</f>
-        <v>22611.018699999997</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Prevents a 'BrokerageNotesWorksheetReader' from being created when a 'NoteNumber' contains an invalid font color.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBC7861-DA02-4800-8B61-B975550058CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242DA4C0-597B-4474-B5D5-1F71EB0BEC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="4" activeTab="5" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="6" activeTab="6" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="NotUsed" sheetId="2" r:id="rId1"/>
@@ -19,33 +19,34 @@
     <sheet name="NoteNumberMissing" sheetId="37" r:id="rId4"/>
     <sheet name="NoteNumberNegative" sheetId="38" r:id="rId5"/>
     <sheet name="NoteNumberExtraneousCharacters" sheetId="39" r:id="rId6"/>
-    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId7"/>
-    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId8"/>
-    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId9"/>
-    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId10"/>
-    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId11"/>
-    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId12"/>
-    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId13"/>
-    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId14"/>
-    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId15"/>
-    <sheet name="SingleLineGroups" sheetId="10" r:id="rId16"/>
-    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId17"/>
-    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId18"/>
-    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId19"/>
-    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId20"/>
-    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId21"/>
-    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId22"/>
-    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId23"/>
-    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId24"/>
-    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId25"/>
-    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId26"/>
-    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId27"/>
-    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId28"/>
-    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId29"/>
-    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId30"/>
-    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId31"/>
-    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId32"/>
-    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId33"/>
+    <sheet name="NoteNumberBlack" sheetId="40" r:id="rId7"/>
+    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId8"/>
+    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId9"/>
+    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId10"/>
+    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId11"/>
+    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId12"/>
+    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId13"/>
+    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId14"/>
+    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId15"/>
+    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId16"/>
+    <sheet name="SingleLineGroups" sheetId="10" r:id="rId17"/>
+    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId18"/>
+    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId19"/>
+    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId20"/>
+    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId21"/>
+    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId22"/>
+    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId23"/>
+    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId24"/>
+    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId25"/>
+    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId26"/>
+    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId27"/>
+    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId28"/>
+    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId29"/>
+    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId30"/>
+    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId31"/>
+    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId32"/>
+    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId33"/>
+    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId34"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -171,7 +172,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="26">
   <si>
     <t>BBAS3</t>
   </si>
@@ -834,6 +835,175 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F27D22B-36B9-402D-A19C-031FF2332945}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7579CBF-C87A-40BF-91B5-CE83CDC20ECE}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -1028,7 +1198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384BB7C-DF07-4187-ADF0-23E50C2BA287}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -1330,7 +1500,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EC0A3F-FFB0-437C-B726-EA72E0B69675}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -1582,7 +1752,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -2169,7 +2339,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
@@ -2696,7 +2866,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
@@ -3605,7 +3775,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -3861,7 +4031,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7618D34E-0B33-4181-8E63-6765777C5B7E}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
@@ -4153,7 +4323,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19EF43A-AB48-4760-8CB3-D62FBA7ABFD8}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -4333,222 +4503,6 @@
       <c r="H4" s="7">
         <f t="shared" si="2"/>
         <v>1.1300000000000001</v>
-      </c>
-      <c r="I4" s="7">
-        <f t="shared" si="2"/>
-        <v>3.98</v>
-      </c>
-      <c r="J4" s="7">
-        <f t="shared" si="2"/>
-        <v>0.25869999999999999</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="7">
-        <f>-SUM(L2:L3)</f>
-        <v>-22611.028699999995</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B2" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
-        <v>11000</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.025%</f>
-        <v>2.75</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>11005.429349999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B3" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500</v>
-      </c>
-      <c r="E3" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" si="0"/>
-        <v>11600</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*0.025%</f>
-        <v>2.9</v>
-      </c>
-      <c r="H3" s="3">
-        <f>F3*0.005%</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>11605.599349999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7">
-        <f>-SUM(F2:F3)</f>
-        <v>-22600</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
-        <v>5.65</v>
-      </c>
-      <c r="H4" s="7">
-        <f t="shared" si="2"/>
-        <v>1.1400000000000001</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" si="2"/>
@@ -4730,6 +4684,222 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.429349999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1400000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.028699999995</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1583F5-F968-4E69-BCCF-4B8530FA0CCB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -4945,7 +5115,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -5244,7 +5414,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E3E40E-BCAE-41DB-80FC-C74D9CCDCD28}">
   <dimension ref="A1:AC13"/>
   <sheetViews>
@@ -5683,7 +5853,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F402F95-319A-4797-B7E1-F3EB07A82FDD}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -5900,7 +6070,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A590E594-CB91-4439-95F2-7F159495761F}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6117,7 +6287,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34F43A8-C89C-44C0-BF29-1F8134A0151F}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -6415,7 +6585,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5AE87-00E8-4CF9-A517-EB6C0CA40610}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6631,7 +6801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B51BEB4-905E-4036-959A-F9A0226AF070}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6848,7 +7018,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B7349E-D984-4817-800E-2EB4836D5B5D}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -7033,223 +7203,6 @@
       <c r="I4" s="7">
         <f t="shared" si="2"/>
         <v>3.98</v>
-      </c>
-      <c r="J4" s="7">
-        <f t="shared" si="2"/>
-        <v>0.25869999999999999</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="7">
-        <f>-SUM(L2:L3)</f>
-        <v>-22611.018699999997</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA65F892-A6B4-4288-ADB5-125D04E295EB}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B2" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
-        <v>11000</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.025%</f>
-        <v>2.75</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>11005.419349999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B3" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500</v>
-      </c>
-      <c r="E3" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" si="0"/>
-        <v>11600</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*0.025%</f>
-        <v>2.9</v>
-      </c>
-      <c r="H3" s="3">
-        <f>F3*0.005%</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>11605.599349999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7">
-        <f>-SUM(F2:F3)</f>
-        <v>-22600</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
-        <v>5.65</v>
-      </c>
-      <c r="H4" s="7">
-        <f>SUM(H2:H3)</f>
-        <v>1.1300000000000001</v>
-      </c>
-      <c r="I4" s="7">
-        <f>SUM(I2:I3) - 0.03</f>
-        <v>3.95</v>
       </c>
       <c r="J4" s="7">
         <f t="shared" si="2"/>
@@ -7429,6 +7382,223 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA65F892-A6B4-4288-ADB5-125D04E295EB}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f>SUM(H2:H3)</f>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f>SUM(I2:I3) - 0.03</f>
+        <v>3.95</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.018699999997</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421F9D80-1D28-4F3C-95F7-8DE9883A26F0}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -7645,7 +7815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D25BF0F-8645-49A4-A6C8-BE755BFA7BE7}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -7944,7 +8114,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4721B46-AB87-4CAA-ABF7-E48CFDA36C4A}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8179,7 +8349,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF39107-DEBE-454A-A911-9FAC6360BB3B}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8707,6 +8877,152 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29FF2F8-FD89-4B31-BC92-2C175C3A29E3}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="18"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="24"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD51868-72C8-4230-87D6-AB4CCC735441}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
@@ -8790,8 +9106,8 @@
       <c r="A2" s="5">
         <v>39757</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>25</v>
+      <c r="B2" s="18">
+        <v>1662</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -8849,7 +9165,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF98C6E-C61C-4098-8811-20C737B2746F}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -9436,7 +9752,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -10021,173 +10337,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F27D22B-36B9-402D-A19C-031FF2332945}">
-  <dimension ref="A1:AC3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B2" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
-        <v>11000</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.025%</f>
-        <v>2.75</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>11005.419349999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B3" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500</v>
-      </c>
-      <c r="E3" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" si="0"/>
-        <v>11600</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*0.025%</f>
-        <v>2.9</v>
-      </c>
-      <c r="H3" s="3">
-        <f>F3*0.005%</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>11605.599349999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Prevents a 'BrokerageNotesWorksheetReader' from being created when a 'Ticker' is missing.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242DA4C0-597B-4474-B5D5-1F71EB0BEC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553E1067-1EA1-4052-AA3C-E69D7E7B9F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="6" activeTab="6" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="6" activeTab="7" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="NotUsed" sheetId="2" r:id="rId1"/>
@@ -20,33 +20,34 @@
     <sheet name="NoteNumberNegative" sheetId="38" r:id="rId5"/>
     <sheet name="NoteNumberExtraneousCharacters" sheetId="39" r:id="rId6"/>
     <sheet name="NoteNumberBlack" sheetId="40" r:id="rId7"/>
-    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId8"/>
-    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId9"/>
-    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId10"/>
-    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId11"/>
-    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId12"/>
-    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId13"/>
-    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId14"/>
-    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId15"/>
-    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId16"/>
-    <sheet name="SingleLineGroups" sheetId="10" r:id="rId17"/>
-    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId18"/>
-    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId19"/>
-    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId20"/>
-    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId21"/>
-    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId22"/>
-    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId23"/>
-    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId24"/>
-    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId25"/>
-    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId26"/>
-    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId27"/>
-    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId28"/>
-    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId29"/>
-    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId30"/>
-    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId31"/>
-    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId32"/>
-    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId33"/>
-    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId34"/>
+    <sheet name="TickerMissing" sheetId="41" r:id="rId8"/>
+    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId9"/>
+    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId10"/>
+    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId11"/>
+    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId12"/>
+    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId13"/>
+    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId14"/>
+    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId15"/>
+    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId16"/>
+    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId17"/>
+    <sheet name="SingleLineGroups" sheetId="10" r:id="rId18"/>
+    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId19"/>
+    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId20"/>
+    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId21"/>
+    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId22"/>
+    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId23"/>
+    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId24"/>
+    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId25"/>
+    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId26"/>
+    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId27"/>
+    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId28"/>
+    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId29"/>
+    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId30"/>
+    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId31"/>
+    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId32"/>
+    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId33"/>
+    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId34"/>
+    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId35"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -172,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="26">
   <si>
     <t>BBAS3</t>
   </si>
@@ -835,6 +836,593 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
+  <dimension ref="A1:AC14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="12"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="18"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1663</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>200</v>
+      </c>
+      <c r="E3" s="3">
+        <v>25.19</v>
+      </c>
+      <c r="F3" s="3">
+        <f>D3*E3</f>
+        <v>5038</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.3854500000000001</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.35266000000000003</v>
+      </c>
+      <c r="I3" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f t="shared" ref="L3:L4" si="2">F3+G3+H3+I3+J3</f>
+        <v>5056.5281099999993</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4">
+        <v>100</v>
+      </c>
+      <c r="E4" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F4" s="3">
+        <f>D4*E4</f>
+        <v>2750</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.75625000000000009</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.19250000000000003</v>
+      </c>
+      <c r="I4" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" si="2"/>
+        <v>2767.73875</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3">
+        <f>-SUM(F2:F4)</f>
+        <v>-9322</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" ref="G5:K5" si="3">SUM(G2:G4)</f>
+        <v>2.5635500000000002</v>
+      </c>
+      <c r="H5" s="3">
+        <f t="shared" si="3"/>
+        <v>0.65254000000000012</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="3"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="3"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <f>-SUM(L2:L4)</f>
+        <v>-9375.5860899999989</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+    </row>
+    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="6"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+    </row>
+    <row r="7" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>39758</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1344</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>100</v>
+      </c>
+      <c r="E7" s="3">
+        <v>15.2</v>
+      </c>
+      <c r="F7" s="3">
+        <f>D7*E7</f>
+        <v>1520</v>
+      </c>
+      <c r="G7" s="3">
+        <f>F7*0.0275%</f>
+        <v>0.41800000000000004</v>
+      </c>
+      <c r="H7" s="3">
+        <f>F7*0.007%</f>
+        <v>0.10640000000000001</v>
+      </c>
+      <c r="I7" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <f>F7+G7+H7+I7+J7</f>
+        <v>1537.3143999999998</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+    </row>
+    <row r="8" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>39758</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1344</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4">
+        <v>100</v>
+      </c>
+      <c r="E8" s="3">
+        <v>7.69</v>
+      </c>
+      <c r="F8" s="3">
+        <f>D8*E8</f>
+        <v>769</v>
+      </c>
+      <c r="G8" s="3">
+        <f>F8*0.0275%</f>
+        <v>0.21147500000000002</v>
+      </c>
+      <c r="H8" s="3">
+        <f>F8*0.007%</f>
+        <v>5.3830000000000003E-2</v>
+      </c>
+      <c r="I8" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <f>F8+G8+H8+I8+J8</f>
+        <v>786.05530499999986</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+    </row>
+    <row r="9" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <f>-SUM(F7:F8)</f>
+        <v>-2289</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" ref="G9:K9" si="4">SUM(G7:G8)</f>
+        <v>0.62947500000000001</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="4"/>
+        <v>0.16023000000000001</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="4"/>
+        <v>31.98</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="4"/>
+        <v>1.6</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <f>-SUM(L7:L8)</f>
+        <v>-2323.3697049999996</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+    </row>
+    <row r="11" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>39849</v>
+      </c>
+      <c r="B11" s="9">
+        <v>1319</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="9">
+        <v>100</v>
+      </c>
+      <c r="E11" s="8">
+        <v>31.5</v>
+      </c>
+      <c r="F11" s="8">
+        <f>D11*E11</f>
+        <v>3150</v>
+      </c>
+      <c r="G11" s="8">
+        <f>F11*0.0275%</f>
+        <v>0.86625000000000008</v>
+      </c>
+      <c r="H11" s="8">
+        <f>F11*0.007%</f>
+        <v>0.22050000000000003</v>
+      </c>
+      <c r="I11" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J11" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K11" s="8">
+        <v>0</v>
+      </c>
+      <c r="L11" s="8">
+        <f>F11-G11-H11-I11-J11</f>
+        <v>3132.1232500000001</v>
+      </c>
+      <c r="M11" s="6"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+    </row>
+    <row r="13" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>39853</v>
+      </c>
+      <c r="B13" s="9">
+        <v>1362</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="9">
+        <v>100</v>
+      </c>
+      <c r="E13" s="8">
+        <v>31.5</v>
+      </c>
+      <c r="F13" s="8">
+        <f>D13*E13</f>
+        <v>3150</v>
+      </c>
+      <c r="G13" s="8">
+        <f>F13*0.0275%</f>
+        <v>0.86625000000000008</v>
+      </c>
+      <c r="H13" s="8">
+        <f>F13*0.007%</f>
+        <v>0.22050000000000003</v>
+      </c>
+      <c r="I13" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K13" s="8">
+        <v>0</v>
+      </c>
+      <c r="L13" s="8">
+        <f>F13-G13-H13-I13-J13</f>
+        <v>3132.1232500000001</v>
+      </c>
+      <c r="M13" s="6"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F27D22B-36B9-402D-A19C-031FF2332945}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
@@ -1003,7 +1591,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7579CBF-C87A-40BF-91B5-CE83CDC20ECE}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -1198,7 +1786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384BB7C-DF07-4187-ADF0-23E50C2BA287}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -1500,7 +2088,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EC0A3F-FFB0-437C-B726-EA72E0B69675}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -1752,7 +2340,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -2339,7 +2927,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
@@ -2866,7 +3454,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
@@ -3775,7 +4363,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -4031,7 +4619,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7618D34E-0B33-4181-8E63-6765777C5B7E}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
@@ -4316,222 +4904,6 @@
       <c r="Z5" s="8"/>
       <c r="AA5" s="8"/>
       <c r="AB5" s="8"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19EF43A-AB48-4760-8CB3-D62FBA7ABFD8}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B2" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
-        <v>11000</v>
-      </c>
-      <c r="G2" s="3">
-        <v>2.76</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>11005.429349999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B3" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500</v>
-      </c>
-      <c r="E3" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" si="0"/>
-        <v>11600</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*0.025%</f>
-        <v>2.9</v>
-      </c>
-      <c r="H3" s="3">
-        <f>F3*0.005%</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>11605.599349999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7">
-        <f>-SUM(F2:F3)</f>
-        <v>-22600</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
-        <v>5.66</v>
-      </c>
-      <c r="H4" s="7">
-        <f t="shared" si="2"/>
-        <v>1.1300000000000001</v>
-      </c>
-      <c r="I4" s="7">
-        <f t="shared" si="2"/>
-        <v>3.98</v>
-      </c>
-      <c r="J4" s="7">
-        <f t="shared" si="2"/>
-        <v>0.25869999999999999</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="7">
-        <f>-SUM(L2:L3)</f>
-        <v>-22611.028699999995</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -4684,6 +5056,222 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19EF43A-AB48-4760-8CB3-D62FBA7ABFD8}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <v>2.76</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.429349999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
+        <v>5.66</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.028699999995</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -4899,7 +5487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1583F5-F968-4E69-BCCF-4B8530FA0CCB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -5115,7 +5703,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -5414,7 +6002,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E3E40E-BCAE-41DB-80FC-C74D9CCDCD28}">
   <dimension ref="A1:AC13"/>
   <sheetViews>
@@ -5853,7 +6441,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F402F95-319A-4797-B7E1-F3EB07A82FDD}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6070,7 +6658,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A590E594-CB91-4439-95F2-7F159495761F}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6287,7 +6875,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34F43A8-C89C-44C0-BF29-1F8134A0151F}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -6585,7 +7173,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5AE87-00E8-4CF9-A517-EB6C0CA40610}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6801,7 +7389,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B51BEB4-905E-4036-959A-F9A0226AF070}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6982,223 +7570,6 @@
       <c r="H4" s="7">
         <f t="shared" ref="H4:K4" si="2">SUM(H2:H3)</f>
         <v>1.1300000000000001</v>
-      </c>
-      <c r="I4" s="7">
-        <f t="shared" si="2"/>
-        <v>3.98</v>
-      </c>
-      <c r="J4" s="7">
-        <f t="shared" si="2"/>
-        <v>0.25869999999999999</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="7">
-        <f>-SUM(L2:L3)</f>
-        <v>-22611.018699999997</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B7349E-D984-4817-800E-2EB4836D5B5D}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B2" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
-        <v>11000</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.025%</f>
-        <v>2.75</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>11005.419349999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B3" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500</v>
-      </c>
-      <c r="E3" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" si="0"/>
-        <v>11600</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*0.025%</f>
-        <v>2.9</v>
-      </c>
-      <c r="H3" s="3">
-        <f>F3*0.005%</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>11605.599349999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7">
-        <f>-SUM(F2:F3)</f>
-        <v>-22600</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
-        <v>5.65</v>
-      </c>
-      <c r="H4" s="7">
-        <f>SUM(H2:H3) - 0.03</f>
-        <v>1.1000000000000001</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" si="2"/>
@@ -7382,6 +7753,223 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B7349E-D984-4817-800E-2EB4836D5B5D}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f>SUM(H2:H3) - 0.03</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.018699999997</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA65F892-A6B4-4288-ADB5-125D04E295EB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -7598,7 +8186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421F9D80-1D28-4F3C-95F7-8DE9883A26F0}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -7815,7 +8403,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D25BF0F-8645-49A4-A6C8-BE755BFA7BE7}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -8114,7 +8702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4721B46-AB87-4CAA-ABF7-E48CFDA36C4A}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8349,7 +8937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF39107-DEBE-454A-A911-9FAC6360BB3B}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9023,7 +9611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD51868-72C8-4230-87D6-AB4CCC735441}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
@@ -9166,6 +9754,149 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A3DE2F6-22BE-4056-9BC8-1D497B09969E}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="18"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="24"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF98C6E-C61C-4098-8811-20C737B2746F}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -9750,591 +10481,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
-  <dimension ref="A1:AC14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.140625" style="12"/>
-    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="18"/>
-    </row>
-    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4">
-        <v>100</v>
-      </c>
-      <c r="E2" s="3">
-        <v>15.34</v>
-      </c>
-      <c r="F2" s="3">
-        <f>D2*E2</f>
-        <v>1534</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.0275%</f>
-        <v>0.42185</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.007%</f>
-        <v>0.10738000000000002</v>
-      </c>
-      <c r="I2" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>1551.3192299999998</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-    </row>
-    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1663</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" s="3">
-        <v>25.19</v>
-      </c>
-      <c r="F3" s="3">
-        <f>D3*E3</f>
-        <v>5038</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
-        <v>1.3854500000000001</v>
-      </c>
-      <c r="H3" s="3">
-        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
-        <v>0.35266000000000003</v>
-      </c>
-      <c r="I3" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f t="shared" ref="L3:L4" si="2">F3+G3+H3+I3+J3</f>
-        <v>5056.5281099999993</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4">
-        <v>100</v>
-      </c>
-      <c r="E4" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F4" s="3">
-        <f>D4*E4</f>
-        <v>2750</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" si="0"/>
-        <v>0.75625000000000009</v>
-      </c>
-      <c r="H4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.19250000000000003</v>
-      </c>
-      <c r="I4" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3">
-        <f t="shared" si="2"/>
-        <v>2767.73875</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3">
-        <f>-SUM(F2:F4)</f>
-        <v>-9322</v>
-      </c>
-      <c r="G5" s="3">
-        <f t="shared" ref="G5:K5" si="3">SUM(G2:G4)</f>
-        <v>2.5635500000000002</v>
-      </c>
-      <c r="H5" s="3">
-        <f t="shared" si="3"/>
-        <v>0.65254000000000012</v>
-      </c>
-      <c r="I5" s="3">
-        <f t="shared" si="3"/>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="3">
-        <f t="shared" si="3"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L5" s="3">
-        <f>-SUM(L2:L4)</f>
-        <v>-9375.5860899999989</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-    </row>
-    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="6"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-    </row>
-    <row r="7" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>100</v>
-      </c>
-      <c r="E7" s="3">
-        <v>15.2</v>
-      </c>
-      <c r="F7" s="3">
-        <f>D7*E7</f>
-        <v>1520</v>
-      </c>
-      <c r="G7" s="3">
-        <f>F7*0.0275%</f>
-        <v>0.41800000000000004</v>
-      </c>
-      <c r="H7" s="3">
-        <f>F7*0.007%</f>
-        <v>0.10640000000000001</v>
-      </c>
-      <c r="I7" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K7" s="3">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3">
-        <f>F7+G7+H7+I7+J7</f>
-        <v>1537.3143999999998</v>
-      </c>
-      <c r="M7" s="6"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-    </row>
-    <row r="8" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="4">
-        <v>100</v>
-      </c>
-      <c r="E8" s="3">
-        <v>7.69</v>
-      </c>
-      <c r="F8" s="3">
-        <f>D8*E8</f>
-        <v>769</v>
-      </c>
-      <c r="G8" s="3">
-        <f>F8*0.0275%</f>
-        <v>0.21147500000000002</v>
-      </c>
-      <c r="H8" s="3">
-        <f>F8*0.007%</f>
-        <v>5.3830000000000003E-2</v>
-      </c>
-      <c r="I8" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3">
-        <f>F8+G8+H8+I8+J8</f>
-        <v>786.05530499999986</v>
-      </c>
-      <c r="M8" s="6"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-    </row>
-    <row r="9" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3">
-        <f>-SUM(F7:F8)</f>
-        <v>-2289</v>
-      </c>
-      <c r="G9" s="3">
-        <f t="shared" ref="G9:K9" si="4">SUM(G7:G8)</f>
-        <v>0.62947500000000001</v>
-      </c>
-      <c r="H9" s="3">
-        <f t="shared" si="4"/>
-        <v>0.16023000000000001</v>
-      </c>
-      <c r="I9" s="3">
-        <f t="shared" si="4"/>
-        <v>31.98</v>
-      </c>
-      <c r="J9" s="3">
-        <f t="shared" si="4"/>
-        <v>1.6</v>
-      </c>
-      <c r="K9" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L9" s="3">
-        <f>-SUM(L7:L8)</f>
-        <v>-2323.3697049999996</v>
-      </c>
-      <c r="M9" s="6"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-    </row>
-    <row r="11" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
-        <v>39849</v>
-      </c>
-      <c r="B11" s="9">
-        <v>1319</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="9">
-        <v>100</v>
-      </c>
-      <c r="E11" s="8">
-        <v>31.5</v>
-      </c>
-      <c r="F11" s="8">
-        <f>D11*E11</f>
-        <v>3150</v>
-      </c>
-      <c r="G11" s="8">
-        <f>F11*0.0275%</f>
-        <v>0.86625000000000008</v>
-      </c>
-      <c r="H11" s="8">
-        <f>F11*0.007%</f>
-        <v>0.22050000000000003</v>
-      </c>
-      <c r="I11" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J11" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K11" s="8">
-        <v>0</v>
-      </c>
-      <c r="L11" s="8">
-        <f>F11-G11-H11-I11-J11</f>
-        <v>3132.1232500000001</v>
-      </c>
-      <c r="M11" s="6"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
-      <c r="AA11" s="8"/>
-      <c r="AB11" s="8"/>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-    </row>
-    <row r="13" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
-        <v>39853</v>
-      </c>
-      <c r="B13" s="9">
-        <v>1362</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="9">
-        <v>100</v>
-      </c>
-      <c r="E13" s="8">
-        <v>31.5</v>
-      </c>
-      <c r="F13" s="8">
-        <f>D13*E13</f>
-        <v>3150</v>
-      </c>
-      <c r="G13" s="8">
-        <f>F13*0.0275%</f>
-        <v>0.86625000000000008</v>
-      </c>
-      <c r="H13" s="8">
-        <f>F13*0.007%</f>
-        <v>0.22050000000000003</v>
-      </c>
-      <c r="I13" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J13" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K13" s="8">
-        <v>0</v>
-      </c>
-      <c r="L13" s="8">
-        <f>F13-G13-H13-I13-J13</f>
-        <v>3132.1232500000001</v>
-      </c>
-      <c r="M13" s="6"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="8"/>
-      <c r="AA13" s="8"/>
-      <c r="AB13" s="8"/>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Prevents a 'BrokerageNotesWorksheetReader' from being created when a 'Ticker' has an invalid font color.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553E1067-1EA1-4052-AA3C-E69D7E7B9F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FD5EC5-FB5B-496C-8F96-F85B4763338C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="6" activeTab="7" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="6" activeTab="8" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="NotUsed" sheetId="2" r:id="rId1"/>
@@ -21,33 +21,34 @@
     <sheet name="NoteNumberExtraneousCharacters" sheetId="39" r:id="rId6"/>
     <sheet name="NoteNumberBlack" sheetId="40" r:id="rId7"/>
     <sheet name="TickerMissing" sheetId="41" r:id="rId8"/>
-    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId9"/>
-    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId10"/>
-    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId11"/>
-    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId12"/>
-    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId13"/>
-    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId14"/>
-    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId15"/>
-    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId16"/>
-    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId17"/>
-    <sheet name="SingleLineGroups" sheetId="10" r:id="rId18"/>
-    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId19"/>
-    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId20"/>
-    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId21"/>
-    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId22"/>
-    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId23"/>
-    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId24"/>
-    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId25"/>
-    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId26"/>
-    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId27"/>
-    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId28"/>
-    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId29"/>
-    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId30"/>
-    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId31"/>
-    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId32"/>
-    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId33"/>
-    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId34"/>
-    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId35"/>
+    <sheet name="TickerBlack" sheetId="42" r:id="rId9"/>
+    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId10"/>
+    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId11"/>
+    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId12"/>
+    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId13"/>
+    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId14"/>
+    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId15"/>
+    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId16"/>
+    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId17"/>
+    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId18"/>
+    <sheet name="SingleLineGroups" sheetId="10" r:id="rId19"/>
+    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId20"/>
+    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId21"/>
+    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId22"/>
+    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId23"/>
+    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId24"/>
+    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId25"/>
+    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId26"/>
+    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId27"/>
+    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId28"/>
+    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId29"/>
+    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId30"/>
+    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId31"/>
+    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId32"/>
+    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId33"/>
+    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId34"/>
+    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId35"/>
+    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId36"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -173,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="26">
   <si>
     <t>BBAS3</t>
   </si>
@@ -836,6 +837,593 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF98C6E-C61C-4098-8811-20C737B2746F}">
+  <dimension ref="A1:AC14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="12"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="18"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>39758</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>200</v>
+      </c>
+      <c r="E3" s="3">
+        <v>25.19</v>
+      </c>
+      <c r="F3" s="3">
+        <f>D3*E3</f>
+        <v>5038</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.3854500000000001</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.35266000000000003</v>
+      </c>
+      <c r="I3" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f t="shared" ref="L3:L4" si="2">F3+G3+H3+I3+J3</f>
+        <v>5056.5281099999993</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4">
+        <v>100</v>
+      </c>
+      <c r="E4" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F4" s="3">
+        <f>D4*E4</f>
+        <v>2750</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.75625000000000009</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.19250000000000003</v>
+      </c>
+      <c r="I4" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" si="2"/>
+        <v>2767.73875</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3">
+        <f>-SUM(F2:F4)</f>
+        <v>-9322</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" ref="G5:K5" si="3">SUM(G2:G4)</f>
+        <v>2.5635500000000002</v>
+      </c>
+      <c r="H5" s="3">
+        <f t="shared" si="3"/>
+        <v>0.65254000000000012</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="3"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="3"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <f>-SUM(L2:L4)</f>
+        <v>-9375.5860899999989</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+    </row>
+    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="6"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+    </row>
+    <row r="7" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>39758</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1344</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>100</v>
+      </c>
+      <c r="E7" s="3">
+        <v>15.2</v>
+      </c>
+      <c r="F7" s="3">
+        <f>D7*E7</f>
+        <v>1520</v>
+      </c>
+      <c r="G7" s="3">
+        <f>F7*0.0275%</f>
+        <v>0.41800000000000004</v>
+      </c>
+      <c r="H7" s="3">
+        <f>F7*0.007%</f>
+        <v>0.10640000000000001</v>
+      </c>
+      <c r="I7" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <f>F7+G7+H7+I7+J7</f>
+        <v>1537.3143999999998</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+    </row>
+    <row r="8" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>39758</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1344</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4">
+        <v>100</v>
+      </c>
+      <c r="E8" s="3">
+        <v>7.69</v>
+      </c>
+      <c r="F8" s="3">
+        <f>D8*E8</f>
+        <v>769</v>
+      </c>
+      <c r="G8" s="3">
+        <f>F8*0.0275%</f>
+        <v>0.21147500000000002</v>
+      </c>
+      <c r="H8" s="3">
+        <f>F8*0.007%</f>
+        <v>5.3830000000000003E-2</v>
+      </c>
+      <c r="I8" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <f>F8+G8+H8+I8+J8</f>
+        <v>786.05530499999986</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+    </row>
+    <row r="9" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <f>-SUM(F7:F8)</f>
+        <v>-2289</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" ref="G9:K9" si="4">SUM(G7:G8)</f>
+        <v>0.62947500000000001</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="4"/>
+        <v>0.16023000000000001</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="4"/>
+        <v>31.98</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="4"/>
+        <v>1.6</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <f>-SUM(L7:L8)</f>
+        <v>-2323.3697049999996</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+    </row>
+    <row r="11" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>39849</v>
+      </c>
+      <c r="B11" s="9">
+        <v>1319</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="9">
+        <v>100</v>
+      </c>
+      <c r="E11" s="8">
+        <v>31.5</v>
+      </c>
+      <c r="F11" s="8">
+        <f>D11*E11</f>
+        <v>3150</v>
+      </c>
+      <c r="G11" s="8">
+        <f>F11*0.0275%</f>
+        <v>0.86625000000000008</v>
+      </c>
+      <c r="H11" s="8">
+        <f>F11*0.007%</f>
+        <v>0.22050000000000003</v>
+      </c>
+      <c r="I11" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J11" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K11" s="8">
+        <v>0</v>
+      </c>
+      <c r="L11" s="8">
+        <f>F11-G11-H11-I11-J11</f>
+        <v>3132.1232500000001</v>
+      </c>
+      <c r="M11" s="6"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+    </row>
+    <row r="13" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>39853</v>
+      </c>
+      <c r="B13" s="9">
+        <v>1362</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="9">
+        <v>100</v>
+      </c>
+      <c r="E13" s="8">
+        <v>31.5</v>
+      </c>
+      <c r="F13" s="8">
+        <f>D13*E13</f>
+        <v>3150</v>
+      </c>
+      <c r="G13" s="8">
+        <f>F13*0.0275%</f>
+        <v>0.86625000000000008</v>
+      </c>
+      <c r="H13" s="8">
+        <f>F13*0.007%</f>
+        <v>0.22050000000000003</v>
+      </c>
+      <c r="I13" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K13" s="8">
+        <v>0</v>
+      </c>
+      <c r="L13" s="8">
+        <f>F13-G13-H13-I13-J13</f>
+        <v>3132.1232500000001</v>
+      </c>
+      <c r="M13" s="6"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -1422,7 +2010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F27D22B-36B9-402D-A19C-031FF2332945}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
@@ -1591,7 +2179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7579CBF-C87A-40BF-91B5-CE83CDC20ECE}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -1786,7 +2374,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384BB7C-DF07-4187-ADF0-23E50C2BA287}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -2088,7 +2676,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EC0A3F-FFB0-437C-B726-EA72E0B69675}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -2340,7 +2928,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -2927,7 +3515,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
@@ -3454,7 +4042,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
@@ -4363,7 +4951,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -4616,298 +5204,6 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7618D34E-0B33-4181-8E63-6765777C5B7E}">
-  <dimension ref="A1:AC5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="9">
-        <v>200</v>
-      </c>
-      <c r="E2" s="8">
-        <v>35.15</v>
-      </c>
-      <c r="F2" s="8">
-        <v>7030.01</v>
-      </c>
-      <c r="G2" s="8">
-        <f>1.16*(F2/SUM(F2:F4))</f>
-        <v>0.42000450143979118</v>
-      </c>
-      <c r="H2" s="8">
-        <f>5.53*(F2/SUM(F2:F4))</f>
-        <v>2.0022628387603842</v>
-      </c>
-      <c r="I2" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="8">
-        <v>0</v>
-      </c>
-      <c r="L2" s="8">
-        <f>F2-G2-H2-I2-K2</f>
-        <v>7011.5977326598004</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-    </row>
-    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B3" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9">
-        <v>200</v>
-      </c>
-      <c r="E3" s="8">
-        <v>34.479999999999997</v>
-      </c>
-      <c r="F3" s="8">
-        <f>D3*E3</f>
-        <v>6895.9999999999991</v>
-      </c>
-      <c r="G3" s="8">
-        <f>1.16*(F3/SUM(F2:F4))</f>
-        <v>0.41199813967957366</v>
-      </c>
-      <c r="H3" s="8">
-        <f>5.53*(F3/SUM(F2:F4))</f>
-        <v>1.9640945796793472</v>
-      </c>
-      <c r="I3" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="8">
-        <v>0</v>
-      </c>
-      <c r="L3" s="8">
-        <f>F3-G3-H3-I3-K3</f>
-        <v>6877.6339072806404</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-    </row>
-    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="9">
-        <v>200</v>
-      </c>
-      <c r="E4" s="8">
-        <v>27.45</v>
-      </c>
-      <c r="F4" s="8">
-        <f>D4*E4</f>
-        <v>5490</v>
-      </c>
-      <c r="G4" s="8">
-        <f>1.16*(F4/SUM(F2:F4))</f>
-        <v>0.32799735888063514</v>
-      </c>
-      <c r="H4" s="8">
-        <f>5.53*(F4/SUM(F2:F4))</f>
-        <v>1.5636425815602693</v>
-      </c>
-      <c r="I4" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="8">
-        <v>0</v>
-      </c>
-      <c r="L4" s="8">
-        <f>F4-G4-H4-I4-K4</f>
-        <v>5472.1183600595596</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-    </row>
-    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="11">
-        <f t="shared" ref="F5:L5" si="0">SUM(F2:F4)</f>
-        <v>19416.009999999998</v>
-      </c>
-      <c r="G5" s="11">
-        <f t="shared" si="0"/>
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="H5" s="11">
-        <f t="shared" si="0"/>
-        <v>5.53</v>
-      </c>
-      <c r="I5" s="11">
-        <f t="shared" si="0"/>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="11">
-        <f t="shared" si="0"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L5" s="11">
-        <f t="shared" si="0"/>
-        <v>19361.349999999999</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="8"/>
-      <c r="AB5" s="8"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5056,6 +5352,298 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7618D34E-0B33-4181-8E63-6765777C5B7E}">
+  <dimension ref="A1:AC5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9">
+        <v>200</v>
+      </c>
+      <c r="E2" s="8">
+        <v>35.15</v>
+      </c>
+      <c r="F2" s="8">
+        <v>7030.01</v>
+      </c>
+      <c r="G2" s="8">
+        <f>1.16*(F2/SUM(F2:F4))</f>
+        <v>0.42000450143979118</v>
+      </c>
+      <c r="H2" s="8">
+        <f>5.53*(F2/SUM(F2:F4))</f>
+        <v>2.0022628387603842</v>
+      </c>
+      <c r="I2" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0</v>
+      </c>
+      <c r="L2" s="8">
+        <f>F2-G2-H2-I2-K2</f>
+        <v>7011.5977326598004</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9">
+        <v>200</v>
+      </c>
+      <c r="E3" s="8">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3*E3</f>
+        <v>6895.9999999999991</v>
+      </c>
+      <c r="G3" s="8">
+        <f>1.16*(F3/SUM(F2:F4))</f>
+        <v>0.41199813967957366</v>
+      </c>
+      <c r="H3" s="8">
+        <f>5.53*(F3/SUM(F2:F4))</f>
+        <v>1.9640945796793472</v>
+      </c>
+      <c r="I3" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="8">
+        <v>0</v>
+      </c>
+      <c r="L3" s="8">
+        <f>F3-G3-H3-I3-K3</f>
+        <v>6877.6339072806404</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="9">
+        <v>200</v>
+      </c>
+      <c r="E4" s="8">
+        <v>27.45</v>
+      </c>
+      <c r="F4" s="8">
+        <f>D4*E4</f>
+        <v>5490</v>
+      </c>
+      <c r="G4" s="8">
+        <f>1.16*(F4/SUM(F2:F4))</f>
+        <v>0.32799735888063514</v>
+      </c>
+      <c r="H4" s="8">
+        <f>5.53*(F4/SUM(F2:F4))</f>
+        <v>1.5636425815602693</v>
+      </c>
+      <c r="I4" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="8">
+        <v>0</v>
+      </c>
+      <c r="L4" s="8">
+        <f>F4-G4-H4-I4-K4</f>
+        <v>5472.1183600595596</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="11">
+        <f t="shared" ref="F5:L5" si="0">SUM(F2:F4)</f>
+        <v>19416.009999999998</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="0"/>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="0"/>
+        <v>5.53</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="0"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="0"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="0"/>
+        <v>19361.349999999999</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19EF43A-AB48-4760-8CB3-D62FBA7ABFD8}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -5271,7 +5859,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -5487,7 +6075,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1583F5-F968-4E69-BCCF-4B8530FA0CCB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -5703,7 +6291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -6002,7 +6590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E3E40E-BCAE-41DB-80FC-C74D9CCDCD28}">
   <dimension ref="A1:AC13"/>
   <sheetViews>
@@ -6441,7 +7029,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F402F95-319A-4797-B7E1-F3EB07A82FDD}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6658,7 +7246,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A590E594-CB91-4439-95F2-7F159495761F}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6875,7 +7463,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34F43A8-C89C-44C0-BF29-1F8134A0151F}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -7173,7 +7761,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5AE87-00E8-4CF9-A517-EB6C0CA40610}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -7369,223 +7957,6 @@
       <c r="L4" s="7">
         <f>-SUM(L2:L3)</f>
         <v>-22611.049350000001</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B51BEB4-905E-4036-959A-F9A0226AF070}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B2" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
-        <v>11000</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.025%</f>
-        <v>2.75</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>11005.419349999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B3" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500</v>
-      </c>
-      <c r="E3" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" si="0"/>
-        <v>11600</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*0.025%</f>
-        <v>2.9</v>
-      </c>
-      <c r="H3" s="3">
-        <f>F3*0.005%</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>11605.599349999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7">
-        <f>-SUM(F2:F3)</f>
-        <v>-22600</v>
-      </c>
-      <c r="G4" s="7">
-        <f>SUM(G2:G3) + 0.03</f>
-        <v>5.6800000000000006</v>
-      </c>
-      <c r="H4" s="7">
-        <f t="shared" ref="H4:K4" si="2">SUM(H2:H3)</f>
-        <v>1.1300000000000001</v>
-      </c>
-      <c r="I4" s="7">
-        <f t="shared" si="2"/>
-        <v>3.98</v>
-      </c>
-      <c r="J4" s="7">
-        <f t="shared" si="2"/>
-        <v>0.25869999999999999</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="7">
-        <f>-SUM(L2:L3)</f>
-        <v>-22611.018699999997</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -7753,6 +8124,223 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B51BEB4-905E-4036-959A-F9A0226AF070}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f>SUM(G2:G3) + 0.03</f>
+        <v>5.6800000000000006</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" ref="H4:K4" si="2">SUM(H2:H3)</f>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.018699999997</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B7349E-D984-4817-800E-2EB4836D5B5D}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -7969,7 +8557,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA65F892-A6B4-4288-ADB5-125D04E295EB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8186,7 +8774,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421F9D80-1D28-4F3C-95F7-8DE9883A26F0}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8403,7 +8991,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D25BF0F-8645-49A4-A6C8-BE755BFA7BE7}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -8702,7 +9290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4721B46-AB87-4CAA-ABF7-E48CFDA36C4A}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8937,7 +9525,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF39107-DEBE-454A-A911-9FAC6360BB3B}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9757,6 +10345,149 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A3DE2F6-22BE-4056-9BC8-1D497B09969E}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="18"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="24"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115D998F-F972-4A55-98C2-51ABEC82B597}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
@@ -9843,6 +10574,9 @@
       <c r="B2" s="4">
         <v>1662</v>
       </c>
+      <c r="C2" s="18" t="s">
+        <v>2</v>
+      </c>
       <c r="D2" s="4">
         <v>100</v>
       </c>
@@ -9894,591 +10628,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF98C6E-C61C-4098-8811-20C737B2746F}">
-  <dimension ref="A1:AC14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.140625" style="12"/>
-    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="18"/>
-    </row>
-    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4">
-        <v>100</v>
-      </c>
-      <c r="E2" s="3">
-        <v>15.34</v>
-      </c>
-      <c r="F2" s="3">
-        <f>D2*E2</f>
-        <v>1534</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.0275%</f>
-        <v>0.42185</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.007%</f>
-        <v>0.10738000000000002</v>
-      </c>
-      <c r="I2" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>1551.3192299999998</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-    </row>
-    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" s="3">
-        <v>25.19</v>
-      </c>
-      <c r="F3" s="3">
-        <f>D3*E3</f>
-        <v>5038</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
-        <v>1.3854500000000001</v>
-      </c>
-      <c r="H3" s="3">
-        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
-        <v>0.35266000000000003</v>
-      </c>
-      <c r="I3" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f t="shared" ref="L3:L4" si="2">F3+G3+H3+I3+J3</f>
-        <v>5056.5281099999993</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4">
-        <v>100</v>
-      </c>
-      <c r="E4" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F4" s="3">
-        <f>D4*E4</f>
-        <v>2750</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" si="0"/>
-        <v>0.75625000000000009</v>
-      </c>
-      <c r="H4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.19250000000000003</v>
-      </c>
-      <c r="I4" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3">
-        <f t="shared" si="2"/>
-        <v>2767.73875</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3">
-        <f>-SUM(F2:F4)</f>
-        <v>-9322</v>
-      </c>
-      <c r="G5" s="3">
-        <f t="shared" ref="G5:K5" si="3">SUM(G2:G4)</f>
-        <v>2.5635500000000002</v>
-      </c>
-      <c r="H5" s="3">
-        <f t="shared" si="3"/>
-        <v>0.65254000000000012</v>
-      </c>
-      <c r="I5" s="3">
-        <f t="shared" si="3"/>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="3">
-        <f t="shared" si="3"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L5" s="3">
-        <f>-SUM(L2:L4)</f>
-        <v>-9375.5860899999989</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-    </row>
-    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="6"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-    </row>
-    <row r="7" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>100</v>
-      </c>
-      <c r="E7" s="3">
-        <v>15.2</v>
-      </c>
-      <c r="F7" s="3">
-        <f>D7*E7</f>
-        <v>1520</v>
-      </c>
-      <c r="G7" s="3">
-        <f>F7*0.0275%</f>
-        <v>0.41800000000000004</v>
-      </c>
-      <c r="H7" s="3">
-        <f>F7*0.007%</f>
-        <v>0.10640000000000001</v>
-      </c>
-      <c r="I7" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K7" s="3">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3">
-        <f>F7+G7+H7+I7+J7</f>
-        <v>1537.3143999999998</v>
-      </c>
-      <c r="M7" s="6"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-    </row>
-    <row r="8" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="4">
-        <v>100</v>
-      </c>
-      <c r="E8" s="3">
-        <v>7.69</v>
-      </c>
-      <c r="F8" s="3">
-        <f>D8*E8</f>
-        <v>769</v>
-      </c>
-      <c r="G8" s="3">
-        <f>F8*0.0275%</f>
-        <v>0.21147500000000002</v>
-      </c>
-      <c r="H8" s="3">
-        <f>F8*0.007%</f>
-        <v>5.3830000000000003E-2</v>
-      </c>
-      <c r="I8" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3">
-        <f>F8+G8+H8+I8+J8</f>
-        <v>786.05530499999986</v>
-      </c>
-      <c r="M8" s="6"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-    </row>
-    <row r="9" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3">
-        <f>-SUM(F7:F8)</f>
-        <v>-2289</v>
-      </c>
-      <c r="G9" s="3">
-        <f t="shared" ref="G9:K9" si="4">SUM(G7:G8)</f>
-        <v>0.62947500000000001</v>
-      </c>
-      <c r="H9" s="3">
-        <f t="shared" si="4"/>
-        <v>0.16023000000000001</v>
-      </c>
-      <c r="I9" s="3">
-        <f t="shared" si="4"/>
-        <v>31.98</v>
-      </c>
-      <c r="J9" s="3">
-        <f t="shared" si="4"/>
-        <v>1.6</v>
-      </c>
-      <c r="K9" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L9" s="3">
-        <f>-SUM(L7:L8)</f>
-        <v>-2323.3697049999996</v>
-      </c>
-      <c r="M9" s="6"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-    </row>
-    <row r="11" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
-        <v>39849</v>
-      </c>
-      <c r="B11" s="9">
-        <v>1319</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="9">
-        <v>100</v>
-      </c>
-      <c r="E11" s="8">
-        <v>31.5</v>
-      </c>
-      <c r="F11" s="8">
-        <f>D11*E11</f>
-        <v>3150</v>
-      </c>
-      <c r="G11" s="8">
-        <f>F11*0.0275%</f>
-        <v>0.86625000000000008</v>
-      </c>
-      <c r="H11" s="8">
-        <f>F11*0.007%</f>
-        <v>0.22050000000000003</v>
-      </c>
-      <c r="I11" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J11" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K11" s="8">
-        <v>0</v>
-      </c>
-      <c r="L11" s="8">
-        <f>F11-G11-H11-I11-J11</f>
-        <v>3132.1232500000001</v>
-      </c>
-      <c r="M11" s="6"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
-      <c r="AA11" s="8"/>
-      <c r="AB11" s="8"/>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-    </row>
-    <row r="13" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
-        <v>39853</v>
-      </c>
-      <c r="B13" s="9">
-        <v>1362</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="9">
-        <v>100</v>
-      </c>
-      <c r="E13" s="8">
-        <v>31.5</v>
-      </c>
-      <c r="F13" s="8">
-        <f>D13*E13</f>
-        <v>3150</v>
-      </c>
-      <c r="G13" s="8">
-        <f>F13*0.0275%</f>
-        <v>0.86625000000000008</v>
-      </c>
-      <c r="H13" s="8">
-        <f>F13*0.007%</f>
-        <v>0.22050000000000003</v>
-      </c>
-      <c r="I13" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J13" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K13" s="8">
-        <v>0</v>
-      </c>
-      <c r="L13" s="8">
-        <f>F13-G13-H13-I13-J13</f>
-        <v>3132.1232500000001</v>
-      </c>
-      <c r="M13" s="6"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="8"/>
-      <c r="AA13" s="8"/>
-      <c r="AB13" s="8"/>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Prevents a 'BrokerageNotesWorksheetReader' from being created when a 'Qty' is missing.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FD5EC5-FB5B-496C-8F96-F85B4763338C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3C49A4-A46C-4A09-82D9-0FF6EEFE02FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="6" activeTab="8" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="9" activeTab="9" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="NotUsed" sheetId="2" r:id="rId1"/>
@@ -22,33 +22,34 @@
     <sheet name="NoteNumberBlack" sheetId="40" r:id="rId7"/>
     <sheet name="TickerMissing" sheetId="41" r:id="rId8"/>
     <sheet name="TickerBlack" sheetId="42" r:id="rId9"/>
-    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId10"/>
-    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId11"/>
-    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId12"/>
-    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId13"/>
-    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId14"/>
-    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId15"/>
-    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId16"/>
-    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId17"/>
-    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId18"/>
-    <sheet name="SingleLineGroups" sheetId="10" r:id="rId19"/>
-    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId20"/>
-    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId21"/>
-    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId22"/>
-    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId23"/>
-    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId24"/>
-    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId25"/>
-    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId26"/>
-    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId27"/>
-    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId28"/>
-    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId29"/>
-    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId30"/>
-    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId31"/>
-    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId32"/>
-    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId33"/>
-    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId34"/>
-    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId35"/>
-    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId36"/>
+    <sheet name="QtyMissing" sheetId="43" r:id="rId10"/>
+    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId11"/>
+    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId12"/>
+    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId13"/>
+    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId14"/>
+    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId15"/>
+    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId16"/>
+    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId17"/>
+    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId18"/>
+    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId19"/>
+    <sheet name="SingleLineGroups" sheetId="10" r:id="rId20"/>
+    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId21"/>
+    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId22"/>
+    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId23"/>
+    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId24"/>
+    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId25"/>
+    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId26"/>
+    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId27"/>
+    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId28"/>
+    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId29"/>
+    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId30"/>
+    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId31"/>
+    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId32"/>
+    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId33"/>
+    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId34"/>
+    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId35"/>
+    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId36"/>
+    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId37"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -174,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="26">
   <si>
     <t>BBAS3</t>
   </si>
@@ -837,6 +838,149 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59782B83-4946-4BE6-BF65-B7005D7A9C90}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="18"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="24"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>16.79</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF98C6E-C61C-4098-8811-20C737B2746F}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -1423,7 +1567,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -2010,7 +2154,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F27D22B-36B9-402D-A19C-031FF2332945}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
@@ -2179,7 +2323,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7579CBF-C87A-40BF-91B5-CE83CDC20ECE}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -2374,7 +2518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384BB7C-DF07-4187-ADF0-23E50C2BA287}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -2676,7 +2820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EC0A3F-FFB0-437C-B726-EA72E0B69675}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -2928,7 +3072,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -3515,7 +3659,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
@@ -4042,7 +4186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
@@ -4948,262 +5092,6 @@
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
-  <dimension ref="A1:AC6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A6" activeCellId="2" sqref="A2:XFD2 A4:XFD4 A6:XFD6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>39959</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1430</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="9">
-        <v>200</v>
-      </c>
-      <c r="E2" s="8">
-        <v>23.4</v>
-      </c>
-      <c r="F2" s="8">
-        <f>D2*E2</f>
-        <v>4680</v>
-      </c>
-      <c r="G2" s="8">
-        <f>F2*0.0275%</f>
-        <v>1.2870000000000001</v>
-      </c>
-      <c r="H2" s="8">
-        <f>F2*0.007%</f>
-        <v>0.32760000000000006</v>
-      </c>
-      <c r="I2" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="8">
-        <v>0.23</v>
-      </c>
-      <c r="L2" s="8">
-        <f>F2-G2-H2-I2-J2</f>
-        <v>4661.5954000000002</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>39960</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1681</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="9">
-        <v>200</v>
-      </c>
-      <c r="E4" s="8">
-        <v>34.04</v>
-      </c>
-      <c r="F4" s="8">
-        <f>D4*E4</f>
-        <v>6808</v>
-      </c>
-      <c r="G4" s="8">
-        <f>F4*0.0275%</f>
-        <v>1.8722000000000001</v>
-      </c>
-      <c r="H4" s="8">
-        <f>F4*0.007%</f>
-        <v>0.47656000000000004</v>
-      </c>
-      <c r="I4" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="8">
-        <v>0.34</v>
-      </c>
-      <c r="L4" s="8">
-        <f>F4-G4-H4-I4-J4</f>
-        <v>6788.8612400000002</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>39961</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1246</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1000</v>
-      </c>
-      <c r="E6" s="3">
-        <v>3.31</v>
-      </c>
-      <c r="F6" s="3">
-        <f>D6*E6</f>
-        <v>3310</v>
-      </c>
-      <c r="G6" s="3">
-        <f>F6*0.0275%</f>
-        <v>0.91025</v>
-      </c>
-      <c r="H6" s="3">
-        <f>F6*0.007%</f>
-        <v>0.23170000000000002</v>
-      </c>
-      <c r="I6" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3">
-        <f>F6+G6+H6+I6+J6</f>
-        <v>3327.9319499999997</v>
-      </c>
-      <c r="M6" s="6"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5352,6 +5240,262 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
+  <dimension ref="A1:AC6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="A6" activeCellId="2" sqref="A2:XFD2 A4:XFD4 A6:XFD6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>39959</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1430</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="9">
+        <v>200</v>
+      </c>
+      <c r="E2" s="8">
+        <v>23.4</v>
+      </c>
+      <c r="F2" s="8">
+        <f>D2*E2</f>
+        <v>4680</v>
+      </c>
+      <c r="G2" s="8">
+        <f>F2*0.0275%</f>
+        <v>1.2870000000000001</v>
+      </c>
+      <c r="H2" s="8">
+        <f>F2*0.007%</f>
+        <v>0.32760000000000006</v>
+      </c>
+      <c r="I2" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="L2" s="8">
+        <f>F2-G2-H2-I2-J2</f>
+        <v>4661.5954000000002</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>39960</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1681</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9">
+        <v>200</v>
+      </c>
+      <c r="E4" s="8">
+        <v>34.04</v>
+      </c>
+      <c r="F4" s="8">
+        <f>D4*E4</f>
+        <v>6808</v>
+      </c>
+      <c r="G4" s="8">
+        <f>F4*0.0275%</f>
+        <v>1.8722000000000001</v>
+      </c>
+      <c r="H4" s="8">
+        <f>F4*0.007%</f>
+        <v>0.47656000000000004</v>
+      </c>
+      <c r="I4" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="8">
+        <v>0.34</v>
+      </c>
+      <c r="L4" s="8">
+        <f>F4-G4-H4-I4-J4</f>
+        <v>6788.8612400000002</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>39961</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1246</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E6" s="3">
+        <v>3.31</v>
+      </c>
+      <c r="F6" s="3">
+        <f>D6*E6</f>
+        <v>3310</v>
+      </c>
+      <c r="G6" s="3">
+        <f>F6*0.0275%</f>
+        <v>0.91025</v>
+      </c>
+      <c r="H6" s="3">
+        <f>F6*0.007%</f>
+        <v>0.23170000000000002</v>
+      </c>
+      <c r="I6" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3">
+        <f>F6+G6+H6+I6+J6</f>
+        <v>3327.9319499999997</v>
+      </c>
+      <c r="M6" s="6"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7618D34E-0B33-4181-8E63-6765777C5B7E}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
@@ -5643,7 +5787,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19EF43A-AB48-4760-8CB3-D62FBA7ABFD8}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -5859,7 +6003,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6075,7 +6219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1583F5-F968-4E69-BCCF-4B8530FA0CCB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6291,7 +6435,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -6590,7 +6734,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E3E40E-BCAE-41DB-80FC-C74D9CCDCD28}">
   <dimension ref="A1:AC13"/>
   <sheetViews>
@@ -7029,7 +7173,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F402F95-319A-4797-B7E1-F3EB07A82FDD}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -7246,7 +7390,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A590E594-CB91-4439-95F2-7F159495761F}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -7463,7 +7607,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34F43A8-C89C-44C0-BF29-1F8134A0151F}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -7754,222 +7898,6 @@
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E8" s="21"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5AE87-00E8-4CF9-A517-EB6C0CA40610}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B2" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
-        <v>11000</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.025%</f>
-        <v>2.75</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <v>11005.45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B3" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500</v>
-      </c>
-      <c r="E3" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" si="0"/>
-        <v>11600</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*0.025%</f>
-        <v>2.9</v>
-      </c>
-      <c r="H3" s="3">
-        <f>F3*0.005%</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>11605.599349999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7">
-        <f>-SUM(F2:F3)</f>
-        <v>-22600</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
-        <v>5.65</v>
-      </c>
-      <c r="H4" s="7">
-        <f t="shared" si="2"/>
-        <v>1.1300000000000001</v>
-      </c>
-      <c r="I4" s="7">
-        <f t="shared" si="2"/>
-        <v>3.98</v>
-      </c>
-      <c r="J4" s="7">
-        <f t="shared" si="2"/>
-        <v>0.25869999999999999</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="7">
-        <f>-SUM(L2:L3)</f>
-        <v>-22611.049350000001</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -8124,6 +8052,222 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5AE87-00E8-4CF9-A517-EB6C0CA40610}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <v>11005.45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.049350000001</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B51BEB4-905E-4036-959A-F9A0226AF070}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8340,7 +8484,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B7349E-D984-4817-800E-2EB4836D5B5D}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8557,7 +8701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA65F892-A6B4-4288-ADB5-125D04E295EB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8774,7 +8918,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421F9D80-1D28-4F3C-95F7-8DE9883A26F0}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8991,7 +9135,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D25BF0F-8645-49A4-A6C8-BE755BFA7BE7}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -9290,7 +9434,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4721B46-AB87-4CAA-ABF7-E48CFDA36C4A}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9525,7 +9669,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF39107-DEBE-454A-A911-9FAC6360BB3B}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -10488,7 +10632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115D998F-F972-4A55-98C2-51ABEC82B597}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>

</xml_diff>

<commit_message>
Prevents a 'BrokerageNotesWorksheetReader' from being created when a negative 'Qty' is found.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3C49A4-A46C-4A09-82D9-0FF6EEFE02FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F7A998-4FD8-4EF6-94D2-8F2FF288C56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="9" activeTab="9" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="9" activeTab="10" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="NotUsed" sheetId="2" r:id="rId1"/>
@@ -23,33 +23,34 @@
     <sheet name="TickerMissing" sheetId="41" r:id="rId8"/>
     <sheet name="TickerBlack" sheetId="42" r:id="rId9"/>
     <sheet name="QtyMissing" sheetId="43" r:id="rId10"/>
-    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId11"/>
-    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId12"/>
-    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId13"/>
-    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId14"/>
-    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId15"/>
-    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId16"/>
-    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId17"/>
-    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId18"/>
-    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId19"/>
-    <sheet name="SingleLineGroups" sheetId="10" r:id="rId20"/>
-    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId21"/>
-    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId22"/>
-    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId23"/>
-    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId24"/>
-    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId25"/>
-    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId26"/>
-    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId27"/>
-    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId28"/>
-    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId29"/>
-    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId30"/>
-    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId31"/>
-    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId32"/>
-    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId33"/>
-    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId34"/>
-    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId35"/>
-    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId36"/>
-    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId37"/>
+    <sheet name="QtyNegative" sheetId="44" r:id="rId11"/>
+    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId12"/>
+    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId13"/>
+    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId14"/>
+    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId15"/>
+    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId16"/>
+    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId17"/>
+    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId18"/>
+    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId19"/>
+    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId20"/>
+    <sheet name="SingleLineGroups" sheetId="10" r:id="rId21"/>
+    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId22"/>
+    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId23"/>
+    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId24"/>
+    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId25"/>
+    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId26"/>
+    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId27"/>
+    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId28"/>
+    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId29"/>
+    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId30"/>
+    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId31"/>
+    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId32"/>
+    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId33"/>
+    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId34"/>
+    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId35"/>
+    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId36"/>
+    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId37"/>
+    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId38"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -175,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="26">
   <si>
     <t>BBAS3</t>
   </si>
@@ -841,6 +842,149 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59782B83-4946-4BE6-BF65-B7005D7A9C90}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="18"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="24"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>16.79</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B230233-E9C7-4B69-BCD8-56729CA32643}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
@@ -930,20 +1074,23 @@
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="D2" s="4">
+        <v>-100</v>
+      </c>
       <c r="E2" s="3">
         <v>15.34</v>
       </c>
       <c r="F2" s="3">
         <f>D2*E2</f>
-        <v>0</v>
+        <v>-1534</v>
       </c>
       <c r="G2" s="3">
         <f>F2*0.0275%</f>
-        <v>0</v>
+        <v>-0.42185</v>
       </c>
       <c r="H2" s="3">
         <f>F2*0.007%</f>
-        <v>0</v>
+        <v>-0.10738000000000002</v>
       </c>
       <c r="I2" s="3">
         <v>15.99</v>
@@ -956,7 +1103,7 @@
       </c>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2+J2</f>
-        <v>16.79</v>
+        <v>-1517.7392299999999</v>
       </c>
       <c r="M2" s="6"/>
       <c r="R2" s="3"/>
@@ -980,7 +1127,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF98C6E-C61C-4098-8811-20C737B2746F}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -1567,7 +1714,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -2154,7 +2301,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F27D22B-36B9-402D-A19C-031FF2332945}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
@@ -2323,7 +2470,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7579CBF-C87A-40BF-91B5-CE83CDC20ECE}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -2518,7 +2665,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384BB7C-DF07-4187-ADF0-23E50C2BA287}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -2820,7 +2967,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EC0A3F-FFB0-437C-B726-EA72E0B69675}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -3072,7 +3219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -3659,7 +3806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
@@ -4181,915 +4328,6 @@
       <c r="A11" s="15"/>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
-  <dimension ref="A1:AC19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="1" sqref="A2:XFD2 A12:XFD12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4">
-        <v>100</v>
-      </c>
-      <c r="E2" s="3">
-        <v>15.34</v>
-      </c>
-      <c r="F2" s="3">
-        <f>D2*E2</f>
-        <v>1534</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.0275%</f>
-        <v>0.42185</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.007%</f>
-        <v>0.10738000000000002</v>
-      </c>
-      <c r="I2" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>1551.3192299999998</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-    </row>
-    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" s="3">
-        <v>25.19</v>
-      </c>
-      <c r="F3" s="3">
-        <f>D3*E3</f>
-        <v>5038</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
-        <v>1.3854500000000001</v>
-      </c>
-      <c r="H3" s="3">
-        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
-        <v>0.35266000000000003</v>
-      </c>
-      <c r="I3" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>5056.5281099999993</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4">
-        <v>100</v>
-      </c>
-      <c r="E4" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F4" s="3">
-        <f>D4*E4</f>
-        <v>2750</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" si="0"/>
-        <v>0.75625000000000009</v>
-      </c>
-      <c r="H4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.19250000000000003</v>
-      </c>
-      <c r="I4" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3">
-        <f>F4+G4+H4+I4+J4</f>
-        <v>2767.73875</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="7">
-        <f>-SUM(F2:F4)</f>
-        <v>-9322</v>
-      </c>
-      <c r="G5" s="7">
-        <f t="shared" ref="G5:K5" si="2">SUM(G2:G4)</f>
-        <v>2.5635500000000002</v>
-      </c>
-      <c r="H5" s="7">
-        <f t="shared" si="2"/>
-        <v>0.65254000000000012</v>
-      </c>
-      <c r="I5" s="7">
-        <f t="shared" si="2"/>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="7">
-        <f t="shared" si="2"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L5" s="7">
-        <f>-SUM(L2:L4)</f>
-        <v>-9375.5860899999989</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-    </row>
-    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="6"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-    </row>
-    <row r="7" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="4">
-        <v>100</v>
-      </c>
-      <c r="E7" s="3">
-        <v>2.68</v>
-      </c>
-      <c r="F7" s="3">
-        <f>D7*E7</f>
-        <v>268</v>
-      </c>
-      <c r="G7" s="3">
-        <f>F7*0.0275%</f>
-        <v>7.3700000000000002E-2</v>
-      </c>
-      <c r="H7" s="3">
-        <f>F7*0.007%</f>
-        <v>1.8760000000000002E-2</v>
-      </c>
-      <c r="I7" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K7" s="3">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3">
-        <f>F7+G7+H7+I7+J7</f>
-        <v>284.88245999999998</v>
-      </c>
-      <c r="M7" s="6"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-    </row>
-    <row r="8" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>100</v>
-      </c>
-      <c r="E8" s="3">
-        <v>15.2</v>
-      </c>
-      <c r="F8" s="3">
-        <f>D8*E8</f>
-        <v>1520</v>
-      </c>
-      <c r="G8" s="3">
-        <f t="shared" ref="G8:G9" si="3">F8*0.0275%</f>
-        <v>0.41800000000000004</v>
-      </c>
-      <c r="H8" s="3">
-        <f t="shared" ref="H8:H9" si="4">F8*0.007%</f>
-        <v>0.10640000000000001</v>
-      </c>
-      <c r="I8" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3">
-        <f>F8+G8+H8+I8+J8</f>
-        <v>1537.3143999999998</v>
-      </c>
-      <c r="M8" s="6"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-    </row>
-    <row r="9" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B9" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="4">
-        <v>100</v>
-      </c>
-      <c r="E9" s="3">
-        <v>7.69</v>
-      </c>
-      <c r="F9" s="3">
-        <f>D9*E9</f>
-        <v>769</v>
-      </c>
-      <c r="G9" s="3">
-        <f t="shared" si="3"/>
-        <v>0.21147500000000002</v>
-      </c>
-      <c r="H9" s="3">
-        <f t="shared" si="4"/>
-        <v>5.3830000000000003E-2</v>
-      </c>
-      <c r="I9" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3">
-        <f>F9+G9+H9+I9+J9</f>
-        <v>786.05530499999986</v>
-      </c>
-      <c r="M9" s="6"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-    </row>
-    <row r="10" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="7">
-        <f>-SUM(F7:F9)</f>
-        <v>-2557</v>
-      </c>
-      <c r="G10" s="7">
-        <f t="shared" ref="G10:K10" si="5">SUM(G7:G9)</f>
-        <v>0.70317500000000011</v>
-      </c>
-      <c r="H10" s="7">
-        <f t="shared" si="5"/>
-        <v>0.17899000000000004</v>
-      </c>
-      <c r="I10" s="7">
-        <f t="shared" si="5"/>
-        <v>47.97</v>
-      </c>
-      <c r="J10" s="7">
-        <f t="shared" si="5"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K10" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L10" s="7">
-        <f>-SUM(L7:L9)</f>
-        <v>-2608.2521649999999</v>
-      </c>
-      <c r="M10" s="6"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
-      <c r="AB10" s="3"/>
-    </row>
-    <row r="11" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="6"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="3"/>
-      <c r="AB11" s="3"/>
-    </row>
-    <row r="12" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B12" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="9">
-        <v>200</v>
-      </c>
-      <c r="E12" s="8">
-        <v>35.15</v>
-      </c>
-      <c r="F12" s="8">
-        <f>D12*E12</f>
-        <v>7030</v>
-      </c>
-      <c r="G12" s="8">
-        <f>F12*0.0275%</f>
-        <v>1.9332500000000001</v>
-      </c>
-      <c r="H12" s="8">
-        <f>F12*0.007%</f>
-        <v>0.49210000000000004</v>
-      </c>
-      <c r="I12" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J12" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K12" s="8">
-        <f>((F12 - G12 - H12 - I12 - J12) - (30.88 * D12)) * 0.005%</f>
-        <v>4.173923249999998E-2</v>
-      </c>
-      <c r="L12" s="8">
-        <f>F12-G12-H12-I12-J12</f>
-        <v>7010.7846499999996</v>
-      </c>
-      <c r="M12" s="6"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="8"/>
-      <c r="X12" s="8"/>
-      <c r="Y12" s="8"/>
-      <c r="Z12" s="8"/>
-      <c r="AA12" s="8"/>
-      <c r="AB12" s="8"/>
-    </row>
-    <row r="13" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B13" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="9">
-        <v>200</v>
-      </c>
-      <c r="E13" s="8">
-        <v>34.479999999999997</v>
-      </c>
-      <c r="F13" s="8">
-        <f>D13*E13</f>
-        <v>6895.9999999999991</v>
-      </c>
-      <c r="G13" s="8">
-        <f t="shared" ref="G13:G14" si="6">F13*0.0275%</f>
-        <v>1.8963999999999999</v>
-      </c>
-      <c r="H13" s="8">
-        <f t="shared" ref="H13:H14" si="7">F13*0.007%</f>
-        <v>0.48271999999999998</v>
-      </c>
-      <c r="I13" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J13" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K13" s="8">
-        <f>((F13 - G13 - H13 - I13 - J13) - (30.88 * D13)) * 0.005%</f>
-        <v>3.504154399999998E-2</v>
-      </c>
-      <c r="L13" s="8">
-        <f t="shared" ref="L13:L14" si="8">F13-G13-H13-I13-J13</f>
-        <v>6876.8308799999995</v>
-      </c>
-      <c r="M13" s="6"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="8"/>
-      <c r="AA13" s="8"/>
-      <c r="AB13" s="8"/>
-    </row>
-    <row r="14" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B14" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="9">
-        <v>200</v>
-      </c>
-      <c r="E14" s="8">
-        <v>31</v>
-      </c>
-      <c r="F14" s="8">
-        <f>D14*E14</f>
-        <v>6200</v>
-      </c>
-      <c r="G14" s="8">
-        <f t="shared" si="6"/>
-        <v>1.7050000000000001</v>
-      </c>
-      <c r="H14" s="8">
-        <f t="shared" si="7"/>
-        <v>0.43400000000000005</v>
-      </c>
-      <c r="I14" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J14" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K14" s="8">
-        <f>((F14 - G14 - H14 - I14 - J14) - (30.88 * D14)) * 0.005%</f>
-        <v>2.5354999999999567E-4</v>
-      </c>
-      <c r="L14" s="8">
-        <f t="shared" si="8"/>
-        <v>6181.0709999999999</v>
-      </c>
-      <c r="M14" s="6"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="8"/>
-      <c r="AA14" s="8"/>
-      <c r="AB14" s="8"/>
-    </row>
-    <row r="15" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="11">
-        <f t="shared" ref="F15:L15" si="9">SUM(F12:F14)</f>
-        <v>20126</v>
-      </c>
-      <c r="G15" s="11">
-        <f t="shared" si="9"/>
-        <v>5.5346500000000001</v>
-      </c>
-      <c r="H15" s="11">
-        <f t="shared" si="9"/>
-        <v>1.40882</v>
-      </c>
-      <c r="I15" s="11">
-        <f t="shared" si="9"/>
-        <v>47.97</v>
-      </c>
-      <c r="J15" s="11">
-        <f t="shared" si="9"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K15" s="11">
-        <f t="shared" si="9"/>
-        <v>7.7034326499999944E-2</v>
-      </c>
-      <c r="L15" s="11">
-        <f t="shared" si="9"/>
-        <v>20068.686529999999</v>
-      </c>
-      <c r="M15" s="6"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="8"/>
-      <c r="Z15" s="8"/>
-      <c r="AA15" s="8"/>
-      <c r="AB15" s="8"/>
-    </row>
-    <row r="17" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
-        <v>40158</v>
-      </c>
-      <c r="B17" s="9">
-        <v>1171</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="9">
-        <v>500</v>
-      </c>
-      <c r="E17" s="8">
-        <v>31</v>
-      </c>
-      <c r="F17" s="8">
-        <f>D17*E17</f>
-        <v>15500</v>
-      </c>
-      <c r="G17" s="8">
-        <f>F17*0.0275%</f>
-        <v>4.2625000000000002</v>
-      </c>
-      <c r="H17" s="8">
-        <f>F17*0.007%</f>
-        <v>1.0850000000000002</v>
-      </c>
-      <c r="I17" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J17" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K17" s="8">
-        <f>((F17 - G17 - H17 - I17 - J17) - (30.88 * D17)) * 0.005%</f>
-        <v>1.8931250000000547E-3</v>
-      </c>
-      <c r="L17" s="8">
-        <f>F17-G17-H17-I17-J17</f>
-        <v>15477.862500000001</v>
-      </c>
-      <c r="M17" s="6"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="8"/>
-      <c r="Z17" s="8"/>
-      <c r="AA17" s="8"/>
-      <c r="AB17" s="8"/>
-    </row>
-    <row r="18" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>40158</v>
-      </c>
-      <c r="B18" s="9">
-        <v>1171</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="9">
-        <v>1000</v>
-      </c>
-      <c r="E18" s="8">
-        <v>31</v>
-      </c>
-      <c r="F18" s="8">
-        <f>D18*E18</f>
-        <v>31000</v>
-      </c>
-      <c r="G18" s="8">
-        <f>F18*0.0275%</f>
-        <v>8.5250000000000004</v>
-      </c>
-      <c r="H18" s="8">
-        <f>F18*0.007%</f>
-        <v>2.1700000000000004</v>
-      </c>
-      <c r="I18" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J18" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K18" s="8">
-        <f>((F18 - G18 - H18 - I18 - J18) - (30.88 * D18)) * 0.005%</f>
-        <v>4.625749999999971E-3</v>
-      </c>
-      <c r="L18" s="8">
-        <f>F18-G18-H18-I18-J18</f>
-        <v>30972.514999999999</v>
-      </c>
-      <c r="M18" s="6"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="8"/>
-      <c r="X18" s="8"/>
-      <c r="Y18" s="8"/>
-      <c r="Z18" s="8"/>
-      <c r="AA18" s="8"/>
-      <c r="AB18" s="8"/>
-    </row>
-    <row r="19" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="11">
-        <f t="shared" ref="F19:L19" si="10">SUM(F17:F18)</f>
-        <v>46500</v>
-      </c>
-      <c r="G19" s="11">
-        <f t="shared" si="10"/>
-        <v>12.787500000000001</v>
-      </c>
-      <c r="H19" s="11">
-        <f t="shared" si="10"/>
-        <v>3.2550000000000008</v>
-      </c>
-      <c r="I19" s="11">
-        <f t="shared" si="10"/>
-        <v>31.98</v>
-      </c>
-      <c r="J19" s="11">
-        <f t="shared" si="10"/>
-        <v>1.6</v>
-      </c>
-      <c r="K19" s="11">
-        <f t="shared" si="10"/>
-        <v>6.5188750000000255E-3</v>
-      </c>
-      <c r="L19" s="11">
-        <f t="shared" si="10"/>
-        <v>46450.377500000002</v>
-      </c>
-      <c r="M19" s="6"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="8"/>
-      <c r="V19" s="8"/>
-      <c r="W19" s="8"/>
-      <c r="X19" s="8"/>
-      <c r="Y19" s="8"/>
-      <c r="Z19" s="8"/>
-      <c r="AA19" s="8"/>
-      <c r="AB19" s="8"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5240,6 +4478,915 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
+  <dimension ref="A1:AC19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="1" sqref="A2:XFD2 A12:XFD12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>200</v>
+      </c>
+      <c r="E3" s="3">
+        <v>25.19</v>
+      </c>
+      <c r="F3" s="3">
+        <f>D3*E3</f>
+        <v>5038</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.3854500000000001</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.35266000000000003</v>
+      </c>
+      <c r="I3" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>5056.5281099999993</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4">
+        <v>100</v>
+      </c>
+      <c r="E4" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F4" s="3">
+        <f>D4*E4</f>
+        <v>2750</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.75625000000000009</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.19250000000000003</v>
+      </c>
+      <c r="I4" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <f>F4+G4+H4+I4+J4</f>
+        <v>2767.73875</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="7">
+        <f>-SUM(F2:F4)</f>
+        <v>-9322</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" ref="G5:K5" si="2">SUM(G2:G4)</f>
+        <v>2.5635500000000002</v>
+      </c>
+      <c r="H5" s="7">
+        <f t="shared" si="2"/>
+        <v>0.65254000000000012</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="shared" si="2"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" si="2"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="7">
+        <f>-SUM(L2:L4)</f>
+        <v>-9375.5860899999989</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+    </row>
+    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="6"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+    </row>
+    <row r="7" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>39758</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1344</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4">
+        <v>100</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2.68</v>
+      </c>
+      <c r="F7" s="3">
+        <f>D7*E7</f>
+        <v>268</v>
+      </c>
+      <c r="G7" s="3">
+        <f>F7*0.0275%</f>
+        <v>7.3700000000000002E-2</v>
+      </c>
+      <c r="H7" s="3">
+        <f>F7*0.007%</f>
+        <v>1.8760000000000002E-2</v>
+      </c>
+      <c r="I7" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <f>F7+G7+H7+I7+J7</f>
+        <v>284.88245999999998</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+    </row>
+    <row r="8" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>39758</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1344</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>100</v>
+      </c>
+      <c r="E8" s="3">
+        <v>15.2</v>
+      </c>
+      <c r="F8" s="3">
+        <f>D8*E8</f>
+        <v>1520</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" ref="G8:G9" si="3">F8*0.0275%</f>
+        <v>0.41800000000000004</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" ref="H8:H9" si="4">F8*0.007%</f>
+        <v>0.10640000000000001</v>
+      </c>
+      <c r="I8" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <f>F8+G8+H8+I8+J8</f>
+        <v>1537.3143999999998</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+    </row>
+    <row r="9" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>39758</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1344</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4">
+        <v>100</v>
+      </c>
+      <c r="E9" s="3">
+        <v>7.69</v>
+      </c>
+      <c r="F9" s="3">
+        <f>D9*E9</f>
+        <v>769</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="3"/>
+        <v>0.21147500000000002</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="4"/>
+        <v>5.3830000000000003E-2</v>
+      </c>
+      <c r="I9" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <f>F9+G9+H9+I9+J9</f>
+        <v>786.05530499999986</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+    </row>
+    <row r="10" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="7">
+        <f>-SUM(F7:F9)</f>
+        <v>-2557</v>
+      </c>
+      <c r="G10" s="7">
+        <f t="shared" ref="G10:K10" si="5">SUM(G7:G9)</f>
+        <v>0.70317500000000011</v>
+      </c>
+      <c r="H10" s="7">
+        <f t="shared" si="5"/>
+        <v>0.17899000000000004</v>
+      </c>
+      <c r="I10" s="7">
+        <f t="shared" si="5"/>
+        <v>47.97</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="5"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="7">
+        <f>-SUM(L7:L9)</f>
+        <v>-2608.2521649999999</v>
+      </c>
+      <c r="M10" s="6"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+    </row>
+    <row r="11" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="6"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+    </row>
+    <row r="12" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B12" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="9">
+        <v>200</v>
+      </c>
+      <c r="E12" s="8">
+        <v>35.15</v>
+      </c>
+      <c r="F12" s="8">
+        <f>D12*E12</f>
+        <v>7030</v>
+      </c>
+      <c r="G12" s="8">
+        <f>F12*0.0275%</f>
+        <v>1.9332500000000001</v>
+      </c>
+      <c r="H12" s="8">
+        <f>F12*0.007%</f>
+        <v>0.49210000000000004</v>
+      </c>
+      <c r="I12" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K12" s="8">
+        <f>((F12 - G12 - H12 - I12 - J12) - (30.88 * D12)) * 0.005%</f>
+        <v>4.173923249999998E-2</v>
+      </c>
+      <c r="L12" s="8">
+        <f>F12-G12-H12-I12-J12</f>
+        <v>7010.7846499999996</v>
+      </c>
+      <c r="M12" s="6"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="8"/>
+    </row>
+    <row r="13" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B13" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="9">
+        <v>200</v>
+      </c>
+      <c r="E13" s="8">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="F13" s="8">
+        <f>D13*E13</f>
+        <v>6895.9999999999991</v>
+      </c>
+      <c r="G13" s="8">
+        <f t="shared" ref="G13:G14" si="6">F13*0.0275%</f>
+        <v>1.8963999999999999</v>
+      </c>
+      <c r="H13" s="8">
+        <f t="shared" ref="H13:H14" si="7">F13*0.007%</f>
+        <v>0.48271999999999998</v>
+      </c>
+      <c r="I13" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K13" s="8">
+        <f>((F13 - G13 - H13 - I13 - J13) - (30.88 * D13)) * 0.005%</f>
+        <v>3.504154399999998E-2</v>
+      </c>
+      <c r="L13" s="8">
+        <f t="shared" ref="L13:L14" si="8">F13-G13-H13-I13-J13</f>
+        <v>6876.8308799999995</v>
+      </c>
+      <c r="M13" s="6"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
+    </row>
+    <row r="14" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="9">
+        <v>200</v>
+      </c>
+      <c r="E14" s="8">
+        <v>31</v>
+      </c>
+      <c r="F14" s="8">
+        <f>D14*E14</f>
+        <v>6200</v>
+      </c>
+      <c r="G14" s="8">
+        <f t="shared" si="6"/>
+        <v>1.7050000000000001</v>
+      </c>
+      <c r="H14" s="8">
+        <f t="shared" si="7"/>
+        <v>0.43400000000000005</v>
+      </c>
+      <c r="I14" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J14" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K14" s="8">
+        <f>((F14 - G14 - H14 - I14 - J14) - (30.88 * D14)) * 0.005%</f>
+        <v>2.5354999999999567E-4</v>
+      </c>
+      <c r="L14" s="8">
+        <f t="shared" si="8"/>
+        <v>6181.0709999999999</v>
+      </c>
+      <c r="M14" s="6"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
+    </row>
+    <row r="15" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="11">
+        <f t="shared" ref="F15:L15" si="9">SUM(F12:F14)</f>
+        <v>20126</v>
+      </c>
+      <c r="G15" s="11">
+        <f t="shared" si="9"/>
+        <v>5.5346500000000001</v>
+      </c>
+      <c r="H15" s="11">
+        <f t="shared" si="9"/>
+        <v>1.40882</v>
+      </c>
+      <c r="I15" s="11">
+        <f t="shared" si="9"/>
+        <v>47.97</v>
+      </c>
+      <c r="J15" s="11">
+        <f t="shared" si="9"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K15" s="11">
+        <f t="shared" si="9"/>
+        <v>7.7034326499999944E-2</v>
+      </c>
+      <c r="L15" s="11">
+        <f t="shared" si="9"/>
+        <v>20068.686529999999</v>
+      </c>
+      <c r="M15" s="6"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="8"/>
+      <c r="AA15" s="8"/>
+      <c r="AB15" s="8"/>
+    </row>
+    <row r="17" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>40158</v>
+      </c>
+      <c r="B17" s="9">
+        <v>1171</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="9">
+        <v>500</v>
+      </c>
+      <c r="E17" s="8">
+        <v>31</v>
+      </c>
+      <c r="F17" s="8">
+        <f>D17*E17</f>
+        <v>15500</v>
+      </c>
+      <c r="G17" s="8">
+        <f>F17*0.0275%</f>
+        <v>4.2625000000000002</v>
+      </c>
+      <c r="H17" s="8">
+        <f>F17*0.007%</f>
+        <v>1.0850000000000002</v>
+      </c>
+      <c r="I17" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K17" s="8">
+        <f>((F17 - G17 - H17 - I17 - J17) - (30.88 * D17)) * 0.005%</f>
+        <v>1.8931250000000547E-3</v>
+      </c>
+      <c r="L17" s="8">
+        <f>F17-G17-H17-I17-J17</f>
+        <v>15477.862500000001</v>
+      </c>
+      <c r="M17" s="6"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="8"/>
+      <c r="AA17" s="8"/>
+      <c r="AB17" s="8"/>
+    </row>
+    <row r="18" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>40158</v>
+      </c>
+      <c r="B18" s="9">
+        <v>1171</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="9">
+        <v>1000</v>
+      </c>
+      <c r="E18" s="8">
+        <v>31</v>
+      </c>
+      <c r="F18" s="8">
+        <f>D18*E18</f>
+        <v>31000</v>
+      </c>
+      <c r="G18" s="8">
+        <f>F18*0.0275%</f>
+        <v>8.5250000000000004</v>
+      </c>
+      <c r="H18" s="8">
+        <f>F18*0.007%</f>
+        <v>2.1700000000000004</v>
+      </c>
+      <c r="I18" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J18" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K18" s="8">
+        <f>((F18 - G18 - H18 - I18 - J18) - (30.88 * D18)) * 0.005%</f>
+        <v>4.625749999999971E-3</v>
+      </c>
+      <c r="L18" s="8">
+        <f>F18-G18-H18-I18-J18</f>
+        <v>30972.514999999999</v>
+      </c>
+      <c r="M18" s="6"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+      <c r="Y18" s="8"/>
+      <c r="Z18" s="8"/>
+      <c r="AA18" s="8"/>
+      <c r="AB18" s="8"/>
+    </row>
+    <row r="19" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="11">
+        <f t="shared" ref="F19:L19" si="10">SUM(F17:F18)</f>
+        <v>46500</v>
+      </c>
+      <c r="G19" s="11">
+        <f t="shared" si="10"/>
+        <v>12.787500000000001</v>
+      </c>
+      <c r="H19" s="11">
+        <f t="shared" si="10"/>
+        <v>3.2550000000000008</v>
+      </c>
+      <c r="I19" s="11">
+        <f t="shared" si="10"/>
+        <v>31.98</v>
+      </c>
+      <c r="J19" s="11">
+        <f t="shared" si="10"/>
+        <v>1.6</v>
+      </c>
+      <c r="K19" s="11">
+        <f t="shared" si="10"/>
+        <v>6.5188750000000255E-3</v>
+      </c>
+      <c r="L19" s="11">
+        <f t="shared" si="10"/>
+        <v>46450.377500000002</v>
+      </c>
+      <c r="M19" s="6"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+      <c r="Y19" s="8"/>
+      <c r="Z19" s="8"/>
+      <c r="AA19" s="8"/>
+      <c r="AB19" s="8"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -5495,7 +5642,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7618D34E-0B33-4181-8E63-6765777C5B7E}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
@@ -5787,7 +5934,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19EF43A-AB48-4760-8CB3-D62FBA7ABFD8}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6003,7 +6150,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6219,7 +6366,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1583F5-F968-4E69-BCCF-4B8530FA0CCB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6435,7 +6582,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -6734,7 +6881,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E3E40E-BCAE-41DB-80FC-C74D9CCDCD28}">
   <dimension ref="A1:AC13"/>
   <sheetViews>
@@ -7173,7 +7320,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F402F95-319A-4797-B7E1-F3EB07A82FDD}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -7390,7 +7537,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A590E594-CB91-4439-95F2-7F159495761F}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -7600,304 +7747,6 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34F43A8-C89C-44C0-BF29-1F8134A0151F}">
-  <dimension ref="A1:AC8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="9">
-        <v>200</v>
-      </c>
-      <c r="E2" s="8">
-        <v>35.15</v>
-      </c>
-      <c r="F2" s="8">
-        <f>D2*E2</f>
-        <v>7030</v>
-      </c>
-      <c r="G2" s="8">
-        <f>F2*0.0275%</f>
-        <v>1.9332500000000001</v>
-      </c>
-      <c r="H2" s="8">
-        <f>F2*0.007%</f>
-        <v>0.49210000000000004</v>
-      </c>
-      <c r="I2" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="8">
-        <f>((F2 - G2 - H2 - I2 - J2) - (30.88 * D2)) * 0.005%</f>
-        <v>4.173923249999998E-2</v>
-      </c>
-      <c r="L2" s="8">
-        <v>7010.81</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-    </row>
-    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B3" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="9">
-        <v>200</v>
-      </c>
-      <c r="E3" s="8">
-        <v>34.479999999999997</v>
-      </c>
-      <c r="F3" s="8">
-        <f>D3*E3</f>
-        <v>6895.9999999999991</v>
-      </c>
-      <c r="G3" s="8">
-        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
-        <v>1.8963999999999999</v>
-      </c>
-      <c r="H3" s="8">
-        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
-        <v>0.48271999999999998</v>
-      </c>
-      <c r="I3" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="8">
-        <f>((F3 - G3 - H3 - I3 - J3) - (30.88 * D3)) * 0.005%</f>
-        <v>3.504154399999998E-2</v>
-      </c>
-      <c r="L3" s="8">
-        <f t="shared" ref="L3:L4" si="2">F3-G3-H3-I3-J3</f>
-        <v>6876.8308799999995</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-    </row>
-    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="9">
-        <v>200</v>
-      </c>
-      <c r="E4" s="8">
-        <v>31</v>
-      </c>
-      <c r="F4" s="8">
-        <f>D4*E4</f>
-        <v>6200</v>
-      </c>
-      <c r="G4" s="8">
-        <f t="shared" si="0"/>
-        <v>1.7050000000000001</v>
-      </c>
-      <c r="H4" s="8">
-        <f t="shared" si="1"/>
-        <v>0.43400000000000005</v>
-      </c>
-      <c r="I4" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="8">
-        <f>((F4 - G4 - H4 - I4 - J4) - (30.88 * D4)) * 0.005%</f>
-        <v>2.5354999999999567E-4</v>
-      </c>
-      <c r="L4" s="8">
-        <f t="shared" si="2"/>
-        <v>6181.0709999999999</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-    </row>
-    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="11">
-        <f t="shared" ref="F5:L5" si="3">SUM(F2:F4)</f>
-        <v>20126</v>
-      </c>
-      <c r="G5" s="11">
-        <f t="shared" si="3"/>
-        <v>5.5346500000000001</v>
-      </c>
-      <c r="H5" s="11">
-        <f t="shared" si="3"/>
-        <v>1.40882</v>
-      </c>
-      <c r="I5" s="11">
-        <f t="shared" si="3"/>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="11">
-        <f t="shared" si="3"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="11">
-        <f t="shared" si="3"/>
-        <v>7.7034326499999944E-2</v>
-      </c>
-      <c r="L5" s="11">
-        <f t="shared" si="3"/>
-        <v>20068.711879999999</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="8"/>
-      <c r="AB5" s="8"/>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E8" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -8052,6 +7901,304 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34F43A8-C89C-44C0-BF29-1F8134A0151F}">
+  <dimension ref="A1:AC8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9">
+        <v>200</v>
+      </c>
+      <c r="E2" s="8">
+        <v>35.15</v>
+      </c>
+      <c r="F2" s="8">
+        <f>D2*E2</f>
+        <v>7030</v>
+      </c>
+      <c r="G2" s="8">
+        <f>F2*0.0275%</f>
+        <v>1.9332500000000001</v>
+      </c>
+      <c r="H2" s="8">
+        <f>F2*0.007%</f>
+        <v>0.49210000000000004</v>
+      </c>
+      <c r="I2" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="8">
+        <f>((F2 - G2 - H2 - I2 - J2) - (30.88 * D2)) * 0.005%</f>
+        <v>4.173923249999998E-2</v>
+      </c>
+      <c r="L2" s="8">
+        <v>7010.81</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9">
+        <v>200</v>
+      </c>
+      <c r="E3" s="8">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3*E3</f>
+        <v>6895.9999999999991</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.8963999999999999</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.48271999999999998</v>
+      </c>
+      <c r="I3" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="8">
+        <f>((F3 - G3 - H3 - I3 - J3) - (30.88 * D3)) * 0.005%</f>
+        <v>3.504154399999998E-2</v>
+      </c>
+      <c r="L3" s="8">
+        <f t="shared" ref="L3:L4" si="2">F3-G3-H3-I3-J3</f>
+        <v>6876.8308799999995</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9">
+        <v>200</v>
+      </c>
+      <c r="E4" s="8">
+        <v>31</v>
+      </c>
+      <c r="F4" s="8">
+        <f>D4*E4</f>
+        <v>6200</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" si="0"/>
+        <v>1.7050000000000001</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" si="1"/>
+        <v>0.43400000000000005</v>
+      </c>
+      <c r="I4" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="8">
+        <f>((F4 - G4 - H4 - I4 - J4) - (30.88 * D4)) * 0.005%</f>
+        <v>2.5354999999999567E-4</v>
+      </c>
+      <c r="L4" s="8">
+        <f t="shared" si="2"/>
+        <v>6181.0709999999999</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="11">
+        <f t="shared" ref="F5:L5" si="3">SUM(F2:F4)</f>
+        <v>20126</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="3"/>
+        <v>5.5346500000000001</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="3"/>
+        <v>1.40882</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="3"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="3"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="3"/>
+        <v>7.7034326499999944E-2</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="3"/>
+        <v>20068.711879999999</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E8" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5AE87-00E8-4CF9-A517-EB6C0CA40610}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8267,7 +8414,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B51BEB4-905E-4036-959A-F9A0226AF070}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8484,7 +8631,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B7349E-D984-4817-800E-2EB4836D5B5D}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8701,7 +8848,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA65F892-A6B4-4288-ADB5-125D04E295EB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8918,7 +9065,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421F9D80-1D28-4F3C-95F7-8DE9883A26F0}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9135,7 +9282,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D25BF0F-8645-49A4-A6C8-BE755BFA7BE7}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -9434,7 +9581,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4721B46-AB87-4CAA-ABF7-E48CFDA36C4A}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9669,7 +9816,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF39107-DEBE-454A-A911-9FAC6360BB3B}">
   <dimension ref="A1:AC4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Prevents a 'BrokerageNotesWorksheetReader' from being created when a 'Qty' contains extraneous characters that prevent it from being interpreted as an integer number.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F7A998-4FD8-4EF6-94D2-8F2FF288C56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B741839-01C0-4763-B048-281E1D9D359B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="9" activeTab="10" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="9" activeTab="11" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="NotUsed" sheetId="2" r:id="rId1"/>
@@ -24,33 +24,34 @@
     <sheet name="TickerBlack" sheetId="42" r:id="rId9"/>
     <sheet name="QtyMissing" sheetId="43" r:id="rId10"/>
     <sheet name="QtyNegative" sheetId="44" r:id="rId11"/>
-    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId12"/>
-    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId13"/>
-    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId14"/>
-    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId15"/>
-    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId16"/>
-    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId17"/>
-    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId18"/>
-    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId19"/>
-    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId20"/>
-    <sheet name="SingleLineGroups" sheetId="10" r:id="rId21"/>
-    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId22"/>
-    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId23"/>
-    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId24"/>
-    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId25"/>
-    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId26"/>
-    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId27"/>
-    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId28"/>
-    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId29"/>
-    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId30"/>
-    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId31"/>
-    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId32"/>
-    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId33"/>
-    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId34"/>
-    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId35"/>
-    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId36"/>
-    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId37"/>
-    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId38"/>
+    <sheet name="QtyExtraneousCharacters" sheetId="45" r:id="rId12"/>
+    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId13"/>
+    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId14"/>
+    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId15"/>
+    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId16"/>
+    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId17"/>
+    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId18"/>
+    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId19"/>
+    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId20"/>
+    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId21"/>
+    <sheet name="SingleLineGroups" sheetId="10" r:id="rId22"/>
+    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId23"/>
+    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId24"/>
+    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId25"/>
+    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId26"/>
+    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId27"/>
+    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId28"/>
+    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId29"/>
+    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId30"/>
+    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId31"/>
+    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId32"/>
+    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId33"/>
+    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId34"/>
+    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId35"/>
+    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId36"/>
+    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId37"/>
+    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId38"/>
+    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId39"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -176,7 +177,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="27">
   <si>
     <t>BBAS3</t>
   </si>
@@ -254,6 +255,9 @@
   </si>
   <si>
     <t>I662</t>
+  </si>
+  <si>
+    <t>l00</t>
   </si>
 </sst>
 </file>
@@ -985,6 +989,152 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B230233-E9C7-4B69-BCD8-56729CA32643}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="18"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="24"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>-100</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>-1534</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>-0.42185</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>-0.10738000000000002</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>-1517.7392299999999</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20115EB7-321C-4C2E-93B6-FB82C1A7BA88}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
@@ -1074,23 +1224,23 @@
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4">
-        <v>-100</v>
+      <c r="D2" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="E2" s="3">
         <v>15.34</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="3" t="e">
         <f>D2*E2</f>
-        <v>-1534</v>
-      </c>
-      <c r="G2" s="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G2" s="3" t="e">
         <f>F2*0.0275%</f>
-        <v>-0.42185</v>
-      </c>
-      <c r="H2" s="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H2" s="3" t="e">
         <f>F2*0.007%</f>
-        <v>-0.10738000000000002</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I2" s="3">
         <v>15.99</v>
@@ -1101,9 +1251,9 @@
       <c r="K2" s="3">
         <v>0</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="3" t="e">
         <f>F2+G2+H2+I2+J2</f>
-        <v>-1517.7392299999999</v>
+        <v>#VALUE!</v>
       </c>
       <c r="M2" s="6"/>
       <c r="R2" s="3"/>
@@ -1127,7 +1277,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF98C6E-C61C-4098-8811-20C737B2746F}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -1714,7 +1864,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -2301,7 +2451,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F27D22B-36B9-402D-A19C-031FF2332945}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
@@ -2470,7 +2620,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7579CBF-C87A-40BF-91B5-CE83CDC20ECE}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -2665,7 +2815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384BB7C-DF07-4187-ADF0-23E50C2BA287}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -2967,7 +3117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EC0A3F-FFB0-437C-B726-EA72E0B69675}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -3219,7 +3369,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -3799,533 +3949,6 @@
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
-  <dimension ref="A1:AC11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A10" activeCellId="1" sqref="A5:XFD5 A10:XFD10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.140625" style="12"/>
-    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="18"/>
-    </row>
-    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4">
-        <v>100</v>
-      </c>
-      <c r="E2" s="3">
-        <v>15.34</v>
-      </c>
-      <c r="F2" s="3">
-        <f>D2*E2</f>
-        <v>1534</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.0275%</f>
-        <v>0.42185</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.007%</f>
-        <v>0.10738000000000002</v>
-      </c>
-      <c r="I2" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>1551.3192299999998</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-    </row>
-    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" s="3">
-        <v>25.19</v>
-      </c>
-      <c r="F3" s="3">
-        <f>D3*E3</f>
-        <v>5038</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
-        <v>1.3854500000000001</v>
-      </c>
-      <c r="H3" s="3">
-        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
-        <v>0.35266000000000003</v>
-      </c>
-      <c r="I3" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>5056.5281099999993</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4">
-        <v>100</v>
-      </c>
-      <c r="E4" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F4" s="3">
-        <f>D4*E4</f>
-        <v>2750</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" si="0"/>
-        <v>0.75625000000000009</v>
-      </c>
-      <c r="H4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.19250000000000003</v>
-      </c>
-      <c r="I4" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3">
-        <f>F4+G4+H4+I4+J4</f>
-        <v>2767.73875</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="7">
-        <f>-SUM(F2:F4)</f>
-        <v>-9322</v>
-      </c>
-      <c r="G5" s="7">
-        <f t="shared" ref="G5:K5" si="2">SUM(G2:G4)</f>
-        <v>2.5635500000000002</v>
-      </c>
-      <c r="H5" s="7">
-        <f t="shared" si="2"/>
-        <v>0.65254000000000012</v>
-      </c>
-      <c r="I5" s="7">
-        <f t="shared" si="2"/>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="7">
-        <f t="shared" si="2"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L5" s="7">
-        <f>-SUM(L2:L4)</f>
-        <v>-9375.5860899999989</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-    </row>
-    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="6"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-    </row>
-    <row r="7" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="4">
-        <v>100</v>
-      </c>
-      <c r="E7" s="3">
-        <v>2.68</v>
-      </c>
-      <c r="F7" s="3">
-        <f>D7*E7</f>
-        <v>268</v>
-      </c>
-      <c r="G7" s="3">
-        <f>F7*0.0275%</f>
-        <v>7.3700000000000002E-2</v>
-      </c>
-      <c r="H7" s="3">
-        <f>F7*0.007%</f>
-        <v>1.8760000000000002E-2</v>
-      </c>
-      <c r="I7" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K7" s="3">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3">
-        <f>F7+G7+H7+I7+J7</f>
-        <v>284.88245999999998</v>
-      </c>
-      <c r="M7" s="6"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-    </row>
-    <row r="8" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>100</v>
-      </c>
-      <c r="E8" s="3">
-        <v>15.2</v>
-      </c>
-      <c r="F8" s="3">
-        <f>D8*E8</f>
-        <v>1520</v>
-      </c>
-      <c r="G8" s="3">
-        <f t="shared" ref="G8:G9" si="3">F8*0.0275%</f>
-        <v>0.41800000000000004</v>
-      </c>
-      <c r="H8" s="3">
-        <f t="shared" ref="H8:H9" si="4">F8*0.007%</f>
-        <v>0.10640000000000001</v>
-      </c>
-      <c r="I8" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3">
-        <f>F8+G8+H8+I8+J8</f>
-        <v>1537.3143999999998</v>
-      </c>
-      <c r="M8" s="6"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-    </row>
-    <row r="9" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B9" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="4">
-        <v>100</v>
-      </c>
-      <c r="E9" s="3">
-        <v>7.69</v>
-      </c>
-      <c r="F9" s="3">
-        <f>D9*E9</f>
-        <v>769</v>
-      </c>
-      <c r="G9" s="3">
-        <f t="shared" si="3"/>
-        <v>0.21147500000000002</v>
-      </c>
-      <c r="H9" s="3">
-        <f t="shared" si="4"/>
-        <v>5.3830000000000003E-2</v>
-      </c>
-      <c r="I9" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3">
-        <f>F9+G9+H9+I9+J9</f>
-        <v>786.05530499999986</v>
-      </c>
-      <c r="M9" s="6"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-    </row>
-    <row r="10" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="7">
-        <f>-SUM(F7:F9)</f>
-        <v>-2557</v>
-      </c>
-      <c r="G10" s="7">
-        <f t="shared" ref="G10:K10" si="5">SUM(G7:G9)</f>
-        <v>0.70317500000000011</v>
-      </c>
-      <c r="H10" s="7">
-        <f t="shared" si="5"/>
-        <v>0.17899000000000004</v>
-      </c>
-      <c r="I10" s="7">
-        <f t="shared" si="5"/>
-        <v>47.97</v>
-      </c>
-      <c r="J10" s="7">
-        <f t="shared" si="5"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K10" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L10" s="7">
-        <f>-SUM(L7:L9)</f>
-        <v>-2608.2521649999999</v>
-      </c>
-      <c r="M10" s="6"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
-      <c r="AB10" s="3"/>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -4478,6 +4101,533 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
+  <dimension ref="A1:AC11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="1" sqref="A5:XFD5 A10:XFD10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="12"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="18"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>200</v>
+      </c>
+      <c r="E3" s="3">
+        <v>25.19</v>
+      </c>
+      <c r="F3" s="3">
+        <f>D3*E3</f>
+        <v>5038</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.3854500000000001</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.35266000000000003</v>
+      </c>
+      <c r="I3" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>5056.5281099999993</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4">
+        <v>100</v>
+      </c>
+      <c r="E4" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F4" s="3">
+        <f>D4*E4</f>
+        <v>2750</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.75625000000000009</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.19250000000000003</v>
+      </c>
+      <c r="I4" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <f>F4+G4+H4+I4+J4</f>
+        <v>2767.73875</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="7">
+        <f>-SUM(F2:F4)</f>
+        <v>-9322</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" ref="G5:K5" si="2">SUM(G2:G4)</f>
+        <v>2.5635500000000002</v>
+      </c>
+      <c r="H5" s="7">
+        <f t="shared" si="2"/>
+        <v>0.65254000000000012</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="shared" si="2"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" si="2"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="7">
+        <f>-SUM(L2:L4)</f>
+        <v>-9375.5860899999989</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+    </row>
+    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="6"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+    </row>
+    <row r="7" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>39758</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1344</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4">
+        <v>100</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2.68</v>
+      </c>
+      <c r="F7" s="3">
+        <f>D7*E7</f>
+        <v>268</v>
+      </c>
+      <c r="G7" s="3">
+        <f>F7*0.0275%</f>
+        <v>7.3700000000000002E-2</v>
+      </c>
+      <c r="H7" s="3">
+        <f>F7*0.007%</f>
+        <v>1.8760000000000002E-2</v>
+      </c>
+      <c r="I7" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <f>F7+G7+H7+I7+J7</f>
+        <v>284.88245999999998</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+    </row>
+    <row r="8" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>39758</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1344</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>100</v>
+      </c>
+      <c r="E8" s="3">
+        <v>15.2</v>
+      </c>
+      <c r="F8" s="3">
+        <f>D8*E8</f>
+        <v>1520</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" ref="G8:G9" si="3">F8*0.0275%</f>
+        <v>0.41800000000000004</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" ref="H8:H9" si="4">F8*0.007%</f>
+        <v>0.10640000000000001</v>
+      </c>
+      <c r="I8" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <f>F8+G8+H8+I8+J8</f>
+        <v>1537.3143999999998</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+    </row>
+    <row r="9" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>39758</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1344</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4">
+        <v>100</v>
+      </c>
+      <c r="E9" s="3">
+        <v>7.69</v>
+      </c>
+      <c r="F9" s="3">
+        <f>D9*E9</f>
+        <v>769</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="3"/>
+        <v>0.21147500000000002</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="4"/>
+        <v>5.3830000000000003E-2</v>
+      </c>
+      <c r="I9" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <f>F9+G9+H9+I9+J9</f>
+        <v>786.05530499999986</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+    </row>
+    <row r="10" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="7">
+        <f>-SUM(F7:F9)</f>
+        <v>-2557</v>
+      </c>
+      <c r="G10" s="7">
+        <f t="shared" ref="G10:K10" si="5">SUM(G7:G9)</f>
+        <v>0.70317500000000011</v>
+      </c>
+      <c r="H10" s="7">
+        <f t="shared" si="5"/>
+        <v>0.17899000000000004</v>
+      </c>
+      <c r="I10" s="7">
+        <f t="shared" si="5"/>
+        <v>47.97</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="5"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="7">
+        <f>-SUM(L7:L9)</f>
+        <v>-2608.2521649999999</v>
+      </c>
+      <c r="M10" s="6"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
@@ -5386,7 +5536,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -5642,7 +5792,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7618D34E-0B33-4181-8E63-6765777C5B7E}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
@@ -5934,7 +6084,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19EF43A-AB48-4760-8CB3-D62FBA7ABFD8}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6150,7 +6300,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6366,7 +6516,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1583F5-F968-4E69-BCCF-4B8530FA0CCB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6582,7 +6732,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -6881,7 +7031,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E3E40E-BCAE-41DB-80FC-C74D9CCDCD28}">
   <dimension ref="A1:AC13"/>
   <sheetViews>
@@ -7320,7 +7470,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F402F95-319A-4797-B7E1-F3EB07A82FDD}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -7513,223 +7663,6 @@
       <c r="K4" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="L4" s="7">
-        <f>-SUM(L2:L3)</f>
-        <v>-22611.018699999997</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A590E594-CB91-4439-95F2-7F159495761F}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B2" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
-        <v>11000</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.025%</f>
-        <v>2.75</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>11005.419349999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B3" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500</v>
-      </c>
-      <c r="E3" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" si="0"/>
-        <v>11600</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*0.025%</f>
-        <v>2.9</v>
-      </c>
-      <c r="H3" s="3">
-        <f>F3*0.005%</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>11605.599349999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7">
-        <f>-SUM(F2:F3)</f>
-        <v>-22600</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
-        <v>5.65</v>
-      </c>
-      <c r="H4" s="7">
-        <f t="shared" si="2"/>
-        <v>1.1300000000000001</v>
-      </c>
-      <c r="I4" s="7">
-        <f t="shared" si="2"/>
-        <v>3.98</v>
-      </c>
-      <c r="J4" s="7">
-        <f t="shared" si="2"/>
-        <v>0.25869999999999999</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="2"/>
-        <v>0.01</v>
       </c>
       <c r="L4" s="7">
         <f>-SUM(L2:L3)</f>
@@ -7901,6 +7834,223 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A590E594-CB91-4439-95F2-7F159495761F}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="L4" s="7">
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.018699999997</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34F43A8-C89C-44C0-BF29-1F8134A0151F}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -8198,7 +8348,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5AE87-00E8-4CF9-A517-EB6C0CA40610}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8414,7 +8564,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B51BEB4-905E-4036-959A-F9A0226AF070}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8631,7 +8781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B7349E-D984-4817-800E-2EB4836D5B5D}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8848,7 +8998,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA65F892-A6B4-4288-ADB5-125D04E295EB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9065,7 +9215,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421F9D80-1D28-4F3C-95F7-8DE9883A26F0}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9282,7 +9432,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D25BF0F-8645-49A4-A6C8-BE755BFA7BE7}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -9581,7 +9731,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4721B46-AB87-4CAA-ABF7-E48CFDA36C4A}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9816,7 +9966,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF39107-DEBE-454A-A911-9FAC6360BB3B}">
   <dimension ref="A1:AC4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Prevents a 'BrokerageNotesWorksheetReader' from being created when a 'Qty' has an invalid font color.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B741839-01C0-4763-B048-281E1D9D359B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740F4FF7-2CA2-41E7-AF99-4A9702AC0ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="9" activeTab="11" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="11" activeTab="12" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="NotUsed" sheetId="2" r:id="rId1"/>
@@ -25,33 +25,34 @@
     <sheet name="QtyMissing" sheetId="43" r:id="rId10"/>
     <sheet name="QtyNegative" sheetId="44" r:id="rId11"/>
     <sheet name="QtyExtraneousCharacters" sheetId="45" r:id="rId12"/>
-    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId13"/>
-    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId14"/>
-    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId15"/>
-    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId16"/>
-    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId17"/>
-    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId18"/>
-    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId19"/>
-    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId20"/>
-    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId21"/>
-    <sheet name="SingleLineGroups" sheetId="10" r:id="rId22"/>
-    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId23"/>
-    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId24"/>
-    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId25"/>
-    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId26"/>
-    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId27"/>
-    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId28"/>
-    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId29"/>
-    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId30"/>
-    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId31"/>
-    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId32"/>
-    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId33"/>
-    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId34"/>
-    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId35"/>
-    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId36"/>
-    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId37"/>
-    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId38"/>
-    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId39"/>
+    <sheet name="QtyBlack" sheetId="46" r:id="rId13"/>
+    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId14"/>
+    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId15"/>
+    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId16"/>
+    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId17"/>
+    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId18"/>
+    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId19"/>
+    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId20"/>
+    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId21"/>
+    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId22"/>
+    <sheet name="SingleLineGroups" sheetId="10" r:id="rId23"/>
+    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId24"/>
+    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId25"/>
+    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId26"/>
+    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId27"/>
+    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId28"/>
+    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId29"/>
+    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId30"/>
+    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId31"/>
+    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId32"/>
+    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId33"/>
+    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId34"/>
+    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId35"/>
+    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId36"/>
+    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId37"/>
+    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId38"/>
+    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId39"/>
+    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId40"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -177,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="27">
   <si>
     <t>BBAS3</t>
   </si>
@@ -1135,6 +1136,152 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20115EB7-321C-4C2E-93B6-FB82C1A7BA88}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="18"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="24"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3" t="e">
+        <f>D2*E2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G2" s="3" t="e">
+        <f>F2*0.0275%</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H2" s="3" t="e">
+        <f>F2*0.007%</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3" t="e">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{551AE2BD-7789-484D-9349-B1B4575C7D73}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
@@ -1224,23 +1371,23 @@
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>26</v>
+      <c r="D2" s="18">
+        <v>100</v>
       </c>
       <c r="E2" s="3">
         <v>15.34</v>
       </c>
-      <c r="F2" s="3" t="e">
+      <c r="F2" s="3">
         <f>D2*E2</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G2" s="3" t="e">
+        <v>1534</v>
+      </c>
+      <c r="G2" s="3">
         <f>F2*0.0275%</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H2" s="3" t="e">
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="3">
         <f>F2*0.007%</f>
-        <v>#VALUE!</v>
+        <v>0.10738000000000002</v>
       </c>
       <c r="I2" s="3">
         <v>15.99</v>
@@ -1251,9 +1398,9 @@
       <c r="K2" s="3">
         <v>0</v>
       </c>
-      <c r="L2" s="3" t="e">
+      <c r="L2" s="3">
         <f>F2+G2+H2+I2+J2</f>
-        <v>#VALUE!</v>
+        <v>1551.3192299999998</v>
       </c>
       <c r="M2" s="6"/>
       <c r="R2" s="3"/>
@@ -1277,7 +1424,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF98C6E-C61C-4098-8811-20C737B2746F}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -1864,7 +2011,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -2451,7 +2598,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F27D22B-36B9-402D-A19C-031FF2332945}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
@@ -2620,7 +2767,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7579CBF-C87A-40BF-91B5-CE83CDC20ECE}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -2815,7 +2962,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384BB7C-DF07-4187-ADF0-23E50C2BA287}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -3117,7 +3264,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EC0A3F-FFB0-437C-B726-EA72E0B69675}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -3362,593 +3509,6 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
-  <dimension ref="A1:AC14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.140625" style="12"/>
-    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="18"/>
-    </row>
-    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4">
-        <v>100</v>
-      </c>
-      <c r="E2" s="3">
-        <v>15.34</v>
-      </c>
-      <c r="F2" s="3">
-        <f>D2*E2</f>
-        <v>1534</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.0275%</f>
-        <v>0.42185</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.007%</f>
-        <v>0.10738000000000002</v>
-      </c>
-      <c r="I2" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>1551.3192299999998</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-    </row>
-    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" s="3">
-        <v>25.19</v>
-      </c>
-      <c r="F3" s="3">
-        <f>D3*E3</f>
-        <v>5038</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
-        <v>1.3854500000000001</v>
-      </c>
-      <c r="H3" s="3">
-        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
-        <v>0.35266000000000003</v>
-      </c>
-      <c r="I3" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f t="shared" ref="L3:L4" si="2">F3+G3+H3+I3+J3</f>
-        <v>5056.5281099999993</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4">
-        <v>100</v>
-      </c>
-      <c r="E4" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F4" s="3">
-        <f>D4*E4</f>
-        <v>2750</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" si="0"/>
-        <v>0.75625000000000009</v>
-      </c>
-      <c r="H4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.19250000000000003</v>
-      </c>
-      <c r="I4" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3">
-        <f t="shared" si="2"/>
-        <v>2767.73875</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3">
-        <f>-SUM(F2:F4)</f>
-        <v>-9322</v>
-      </c>
-      <c r="G5" s="3">
-        <f t="shared" ref="G5:K5" si="3">SUM(G2:G4)</f>
-        <v>2.5635500000000002</v>
-      </c>
-      <c r="H5" s="3">
-        <f t="shared" si="3"/>
-        <v>0.65254000000000012</v>
-      </c>
-      <c r="I5" s="3">
-        <f t="shared" si="3"/>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="3">
-        <f t="shared" si="3"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L5" s="3">
-        <f>-SUM(L2:L4)</f>
-        <v>-9375.5860899999989</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-    </row>
-    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="6"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-    </row>
-    <row r="7" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>100</v>
-      </c>
-      <c r="E7" s="3">
-        <v>15.2</v>
-      </c>
-      <c r="F7" s="3">
-        <f>D7*E7</f>
-        <v>1520</v>
-      </c>
-      <c r="G7" s="3">
-        <f>F7*0.0275%</f>
-        <v>0.41800000000000004</v>
-      </c>
-      <c r="H7" s="3">
-        <f>F7*0.007%</f>
-        <v>0.10640000000000001</v>
-      </c>
-      <c r="I7" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K7" s="3">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3">
-        <f>F7+G7+H7+I7+J7</f>
-        <v>1537.3143999999998</v>
-      </c>
-      <c r="M7" s="6"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-    </row>
-    <row r="8" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="4">
-        <v>100</v>
-      </c>
-      <c r="E8" s="3">
-        <v>7.69</v>
-      </c>
-      <c r="F8" s="3">
-        <f>D8*E8</f>
-        <v>769</v>
-      </c>
-      <c r="G8" s="3">
-        <f>F8*0.0275%</f>
-        <v>0.21147500000000002</v>
-      </c>
-      <c r="H8" s="3">
-        <f>F8*0.007%</f>
-        <v>5.3830000000000003E-2</v>
-      </c>
-      <c r="I8" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3">
-        <f>F8+G8+H8+I8+J8</f>
-        <v>786.05530499999986</v>
-      </c>
-      <c r="M8" s="6"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-    </row>
-    <row r="9" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3">
-        <f>-SUM(F7:F8)</f>
-        <v>-2289</v>
-      </c>
-      <c r="G9" s="3">
-        <f t="shared" ref="G9:K9" si="4">SUM(G7:G8)</f>
-        <v>0.62947500000000001</v>
-      </c>
-      <c r="H9" s="3">
-        <f t="shared" si="4"/>
-        <v>0.16023000000000001</v>
-      </c>
-      <c r="I9" s="3">
-        <f t="shared" si="4"/>
-        <v>31.98</v>
-      </c>
-      <c r="J9" s="3">
-        <f t="shared" si="4"/>
-        <v>1.6</v>
-      </c>
-      <c r="K9" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L9" s="3">
-        <f>-SUM(L7:L8)</f>
-        <v>-2323.3697049999996</v>
-      </c>
-      <c r="M9" s="6"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-    </row>
-    <row r="11" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
-        <v>39849</v>
-      </c>
-      <c r="B11" s="9">
-        <v>1319</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="9">
-        <v>100</v>
-      </c>
-      <c r="E11" s="8">
-        <v>31.5</v>
-      </c>
-      <c r="F11" s="8">
-        <f>D11*E11</f>
-        <v>3150</v>
-      </c>
-      <c r="G11" s="8">
-        <f>F11*0.0275%</f>
-        <v>0.86625000000000008</v>
-      </c>
-      <c r="H11" s="8">
-        <f>F11*0.007%</f>
-        <v>0.22050000000000003</v>
-      </c>
-      <c r="I11" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J11" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K11" s="8">
-        <v>0</v>
-      </c>
-      <c r="L11" s="8">
-        <f>F11-G11-H11-I11-J11</f>
-        <v>3132.1232500000001</v>
-      </c>
-      <c r="M11" s="6"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
-      <c r="AA11" s="8"/>
-      <c r="AB11" s="8"/>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-    </row>
-    <row r="13" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
-        <v>39853</v>
-      </c>
-      <c r="B13" s="9">
-        <v>1362</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="9">
-        <v>100</v>
-      </c>
-      <c r="E13" s="8">
-        <v>31.5</v>
-      </c>
-      <c r="F13" s="8">
-        <f>D13*E13</f>
-        <v>3150</v>
-      </c>
-      <c r="G13" s="8">
-        <f>F13*0.0275%</f>
-        <v>0.86625000000000008</v>
-      </c>
-      <c r="H13" s="8">
-        <f>F13*0.007%</f>
-        <v>0.22050000000000003</v>
-      </c>
-      <c r="I13" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J13" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K13" s="8">
-        <v>0</v>
-      </c>
-      <c r="L13" s="8">
-        <f>F13-G13-H13-I13-J13</f>
-        <v>3132.1232500000001</v>
-      </c>
-      <c r="M13" s="6"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="8"/>
-      <c r="AA13" s="8"/>
-      <c r="AB13" s="8"/>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -4101,6 +3661,593 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
+  <dimension ref="A1:AC14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="12"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="18"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>200</v>
+      </c>
+      <c r="E3" s="3">
+        <v>25.19</v>
+      </c>
+      <c r="F3" s="3">
+        <f>D3*E3</f>
+        <v>5038</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.3854500000000001</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.35266000000000003</v>
+      </c>
+      <c r="I3" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f t="shared" ref="L3:L4" si="2">F3+G3+H3+I3+J3</f>
+        <v>5056.5281099999993</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4">
+        <v>100</v>
+      </c>
+      <c r="E4" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F4" s="3">
+        <f>D4*E4</f>
+        <v>2750</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.75625000000000009</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.19250000000000003</v>
+      </c>
+      <c r="I4" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" si="2"/>
+        <v>2767.73875</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3">
+        <f>-SUM(F2:F4)</f>
+        <v>-9322</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" ref="G5:K5" si="3">SUM(G2:G4)</f>
+        <v>2.5635500000000002</v>
+      </c>
+      <c r="H5" s="3">
+        <f t="shared" si="3"/>
+        <v>0.65254000000000012</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="3"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="3"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <f>-SUM(L2:L4)</f>
+        <v>-9375.5860899999989</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+    </row>
+    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="6"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+    </row>
+    <row r="7" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>39758</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1344</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>100</v>
+      </c>
+      <c r="E7" s="3">
+        <v>15.2</v>
+      </c>
+      <c r="F7" s="3">
+        <f>D7*E7</f>
+        <v>1520</v>
+      </c>
+      <c r="G7" s="3">
+        <f>F7*0.0275%</f>
+        <v>0.41800000000000004</v>
+      </c>
+      <c r="H7" s="3">
+        <f>F7*0.007%</f>
+        <v>0.10640000000000001</v>
+      </c>
+      <c r="I7" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <f>F7+G7+H7+I7+J7</f>
+        <v>1537.3143999999998</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+    </row>
+    <row r="8" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>39758</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1344</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4">
+        <v>100</v>
+      </c>
+      <c r="E8" s="3">
+        <v>7.69</v>
+      </c>
+      <c r="F8" s="3">
+        <f>D8*E8</f>
+        <v>769</v>
+      </c>
+      <c r="G8" s="3">
+        <f>F8*0.0275%</f>
+        <v>0.21147500000000002</v>
+      </c>
+      <c r="H8" s="3">
+        <f>F8*0.007%</f>
+        <v>5.3830000000000003E-2</v>
+      </c>
+      <c r="I8" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <f>F8+G8+H8+I8+J8</f>
+        <v>786.05530499999986</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+    </row>
+    <row r="9" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <f>-SUM(F7:F8)</f>
+        <v>-2289</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" ref="G9:K9" si="4">SUM(G7:G8)</f>
+        <v>0.62947500000000001</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="4"/>
+        <v>0.16023000000000001</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="4"/>
+        <v>31.98</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="4"/>
+        <v>1.6</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <f>-SUM(L7:L8)</f>
+        <v>-2323.3697049999996</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+    </row>
+    <row r="11" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>39849</v>
+      </c>
+      <c r="B11" s="9">
+        <v>1319</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="9">
+        <v>100</v>
+      </c>
+      <c r="E11" s="8">
+        <v>31.5</v>
+      </c>
+      <c r="F11" s="8">
+        <f>D11*E11</f>
+        <v>3150</v>
+      </c>
+      <c r="G11" s="8">
+        <f>F11*0.0275%</f>
+        <v>0.86625000000000008</v>
+      </c>
+      <c r="H11" s="8">
+        <f>F11*0.007%</f>
+        <v>0.22050000000000003</v>
+      </c>
+      <c r="I11" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J11" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K11" s="8">
+        <v>0</v>
+      </c>
+      <c r="L11" s="8">
+        <f>F11-G11-H11-I11-J11</f>
+        <v>3132.1232500000001</v>
+      </c>
+      <c r="M11" s="6"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+    </row>
+    <row r="13" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>39853</v>
+      </c>
+      <c r="B13" s="9">
+        <v>1362</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="9">
+        <v>100</v>
+      </c>
+      <c r="E13" s="8">
+        <v>31.5</v>
+      </c>
+      <c r="F13" s="8">
+        <f>D13*E13</f>
+        <v>3150</v>
+      </c>
+      <c r="G13" s="8">
+        <f>F13*0.0275%</f>
+        <v>0.86625000000000008</v>
+      </c>
+      <c r="H13" s="8">
+        <f>F13*0.007%</f>
+        <v>0.22050000000000003</v>
+      </c>
+      <c r="I13" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K13" s="8">
+        <v>0</v>
+      </c>
+      <c r="L13" s="8">
+        <f>F13-G13-H13-I13-J13</f>
+        <v>3132.1232500000001</v>
+      </c>
+      <c r="M13" s="6"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
@@ -4627,7 +4774,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
@@ -5536,7 +5683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -5792,7 +5939,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7618D34E-0B33-4181-8E63-6765777C5B7E}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
@@ -6084,7 +6231,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19EF43A-AB48-4760-8CB3-D62FBA7ABFD8}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6300,7 +6447,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6516,7 +6663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1583F5-F968-4E69-BCCF-4B8530FA0CCB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6732,7 +6879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -7031,7 +7178,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E3E40E-BCAE-41DB-80FC-C74D9CCDCD28}">
   <dimension ref="A1:AC13"/>
   <sheetViews>
@@ -7467,223 +7614,6 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F402F95-319A-4797-B7E1-F3EB07A82FDD}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B2" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
-        <v>11000</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.025%</f>
-        <v>2.75</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K2" s="23">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>11005.419349999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B3" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500</v>
-      </c>
-      <c r="E3" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" si="0"/>
-        <v>11600</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*0.025%</f>
-        <v>2.9</v>
-      </c>
-      <c r="H3" s="3">
-        <f>F3*0.005%</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>11605.599349999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7">
-        <f>-SUM(F2:F3)</f>
-        <v>-22600</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
-        <v>5.65</v>
-      </c>
-      <c r="H4" s="7">
-        <f t="shared" si="2"/>
-        <v>1.1300000000000001</v>
-      </c>
-      <c r="I4" s="7">
-        <f t="shared" si="2"/>
-        <v>3.98</v>
-      </c>
-      <c r="J4" s="7">
-        <f t="shared" si="2"/>
-        <v>0.25869999999999999</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="7">
-        <f>-SUM(L2:L3)</f>
-        <v>-22611.018699999997</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7834,6 +7764,223 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F402F95-319A-4797-B7E1-F3EB07A82FDD}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="23">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.018699999997</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A590E594-CB91-4439-95F2-7F159495761F}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8050,7 +8197,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34F43A8-C89C-44C0-BF29-1F8134A0151F}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -8348,7 +8495,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5AE87-00E8-4CF9-A517-EB6C0CA40610}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8564,7 +8711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B51BEB4-905E-4036-959A-F9A0226AF070}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8781,7 +8928,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B7349E-D984-4817-800E-2EB4836D5B5D}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8998,7 +9145,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA65F892-A6B4-4288-ADB5-125D04E295EB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9215,7 +9362,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421F9D80-1D28-4F3C-95F7-8DE9883A26F0}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9432,7 +9579,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D25BF0F-8645-49A4-A6C8-BE755BFA7BE7}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -9731,7 +9878,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4721B46-AB87-4CAA-ABF7-E48CFDA36C4A}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9947,241 +10094,6 @@
       <c r="L4" s="7">
         <f>L3-L2</f>
         <v>-2110.6857500000006</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF39107-DEBE-454A-A911-9FAC6360BB3B}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="2"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>42996</v>
-      </c>
-      <c r="B2" s="4">
-        <v>168102</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>23.65</v>
-      </c>
-      <c r="F2" s="3">
-        <f>D2*E2</f>
-        <v>9460</v>
-      </c>
-      <c r="G2" s="3">
-        <f t="shared" ref="G2:G3" si="0">F2*0.0275%</f>
-        <v>2.6015000000000001</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.47300000000000003</v>
-      </c>
-      <c r="I2" s="3">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="J2" s="3">
-        <f>I2*5%</f>
-        <v>0.12450000000000001</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>9465.6890000000003</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-    </row>
-    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>42996</v>
-      </c>
-      <c r="B3" s="9">
-        <v>168102</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="9">
-        <v>700</v>
-      </c>
-      <c r="E3" s="8">
-        <v>10.5</v>
-      </c>
-      <c r="F3" s="8">
-        <f>D3*E3</f>
-        <v>7350</v>
-      </c>
-      <c r="G3" s="8">
-        <f t="shared" si="0"/>
-        <v>2.0212500000000002</v>
-      </c>
-      <c r="H3" s="8">
-        <f>F3*0.005%</f>
-        <v>0.36749999999999999</v>
-      </c>
-      <c r="I3" s="8">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="J3" s="8">
-        <f>I3*5%</f>
-        <v>0.12450000000000001</v>
-      </c>
-      <c r="K3" s="8">
-        <v>0</v>
-      </c>
-      <c r="L3" s="8">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>7355.0032499999998</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7">
-        <f>F3-F2</f>
-        <v>-2110</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" ref="G4:L4" si="1">SUM(G2:G3)</f>
-        <v>4.6227499999999999</v>
-      </c>
-      <c r="H4" s="7">
-        <f t="shared" si="1"/>
-        <v>0.84050000000000002</v>
-      </c>
-      <c r="I4" s="7">
-        <f t="shared" si="1"/>
-        <v>4.9800000000000004</v>
-      </c>
-      <c r="J4" s="7">
-        <f t="shared" si="1"/>
-        <v>0.24900000000000003</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="7">
-        <f t="shared" si="1"/>
-        <v>16820.69225</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -10341,6 +10253,241 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF39107-DEBE-454A-A911-9FAC6360BB3B}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>42996</v>
+      </c>
+      <c r="B2" s="4">
+        <v>168102</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>23.65</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>9460</v>
+      </c>
+      <c r="G2" s="3">
+        <f t="shared" ref="G2:G3" si="0">F2*0.0275%</f>
+        <v>2.6015000000000001</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.47300000000000003</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="J2" s="3">
+        <f>I2*5%</f>
+        <v>0.12450000000000001</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>9465.6890000000003</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>42996</v>
+      </c>
+      <c r="B3" s="9">
+        <v>168102</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="9">
+        <v>700</v>
+      </c>
+      <c r="E3" s="8">
+        <v>10.5</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3*E3</f>
+        <v>7350</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" si="0"/>
+        <v>2.0212500000000002</v>
+      </c>
+      <c r="H3" s="8">
+        <f>F3*0.005%</f>
+        <v>0.36749999999999999</v>
+      </c>
+      <c r="I3" s="8">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="J3" s="8">
+        <f>I3*5%</f>
+        <v>0.12450000000000001</v>
+      </c>
+      <c r="K3" s="8">
+        <v>0</v>
+      </c>
+      <c r="L3" s="8">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>7355.0032499999998</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>F3-F2</f>
+        <v>-2110</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:L4" si="1">SUM(G2:G3)</f>
+        <v>4.6227499999999999</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="1"/>
+        <v>0.84050000000000002</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="1"/>
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="1"/>
+        <v>0.24900000000000003</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="1"/>
+        <v>16820.69225</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Prevents a 'BrokerageNotesWorksheetReader' from being created when a 'Price' is missing.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740F4FF7-2CA2-41E7-AF99-4A9702AC0ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A8B2B2-9456-4EEE-832A-4B5C8AB9915B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="11" activeTab="12" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="11" activeTab="13" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="NotUsed" sheetId="2" r:id="rId1"/>
@@ -26,33 +26,34 @@
     <sheet name="QtyNegative" sheetId="44" r:id="rId11"/>
     <sheet name="QtyExtraneousCharacters" sheetId="45" r:id="rId12"/>
     <sheet name="QtyBlack" sheetId="46" r:id="rId13"/>
-    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId14"/>
-    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId15"/>
-    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId16"/>
-    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId17"/>
-    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId18"/>
-    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId19"/>
-    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId20"/>
-    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId21"/>
-    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId22"/>
-    <sheet name="SingleLineGroups" sheetId="10" r:id="rId23"/>
-    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId24"/>
-    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId25"/>
-    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId26"/>
-    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId27"/>
-    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId28"/>
-    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId29"/>
-    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId30"/>
-    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId31"/>
-    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId32"/>
-    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId33"/>
-    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId34"/>
-    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId35"/>
-    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId36"/>
-    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId37"/>
-    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId38"/>
-    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId39"/>
-    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId40"/>
+    <sheet name="PriceMissing" sheetId="47" r:id="rId14"/>
+    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId15"/>
+    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId16"/>
+    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId17"/>
+    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId18"/>
+    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId19"/>
+    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId20"/>
+    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId21"/>
+    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId22"/>
+    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId23"/>
+    <sheet name="SingleLineGroups" sheetId="10" r:id="rId24"/>
+    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId25"/>
+    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId26"/>
+    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId27"/>
+    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId28"/>
+    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId29"/>
+    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId30"/>
+    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId31"/>
+    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId32"/>
+    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId33"/>
+    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId34"/>
+    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId35"/>
+    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId36"/>
+    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId37"/>
+    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId38"/>
+    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId39"/>
+    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId40"/>
+    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId41"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -178,7 +179,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="27">
   <si>
     <t>BBAS3</t>
   </si>
@@ -1282,7 +1283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{551AE2BD-7789-484D-9349-B1B4575C7D73}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
@@ -1425,6 +1426,150 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EAB37C1-DC87-4BE0-9B0C-DB97F9056CC1}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="18"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="24"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>16.79</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF98C6E-C61C-4098-8811-20C737B2746F}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -2011,7 +2156,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -2598,7 +2743,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F27D22B-36B9-402D-A19C-031FF2332945}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
@@ -2767,7 +2912,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7579CBF-C87A-40BF-91B5-CE83CDC20ECE}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -2962,7 +3107,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384BB7C-DF07-4187-ADF0-23E50C2BA287}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -3251,258 +3396,6 @@
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EC0A3F-FFB0-437C-B726-EA72E0B69675}">
-  <dimension ref="A1:AC7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.140625" style="12"/>
-    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="18"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
-        <v>39757</v>
-      </c>
-      <c r="B2" s="12">
-        <v>1662</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="12">
-        <v>100</v>
-      </c>
-      <c r="E2" s="13">
-        <v>15.34</v>
-      </c>
-      <c r="F2" s="13">
-        <f>D2*E2</f>
-        <v>1534</v>
-      </c>
-      <c r="G2" s="13">
-        <f>F2*0.0275%</f>
-        <v>0.42185</v>
-      </c>
-      <c r="H2" s="13">
-        <f>F2*0.007%</f>
-        <v>0.10738000000000002</v>
-      </c>
-      <c r="I2" s="13">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="13">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="13">
-        <v>0</v>
-      </c>
-      <c r="L2" s="13">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>1551.3192299999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
-        <v>39757</v>
-      </c>
-      <c r="B3" s="12">
-        <v>1662</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="12">
-        <v>200</v>
-      </c>
-      <c r="E3" s="13">
-        <v>25.19</v>
-      </c>
-      <c r="F3" s="13">
-        <f>D3*E3</f>
-        <v>5038</v>
-      </c>
-      <c r="G3" s="13">
-        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
-        <v>1.3854500000000001</v>
-      </c>
-      <c r="H3" s="13">
-        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
-        <v>0.35266000000000003</v>
-      </c>
-      <c r="I3" s="13">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="13">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="13">
-        <v>0</v>
-      </c>
-      <c r="L3" s="13">
-        <f t="shared" ref="L3:L4" si="2">F3+G3+H3+I3+J3</f>
-        <v>5056.5281099999993</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
-        <v>39757</v>
-      </c>
-      <c r="B4" s="12">
-        <v>1662</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="12">
-        <v>100</v>
-      </c>
-      <c r="E4" s="13">
-        <v>27.5</v>
-      </c>
-      <c r="F4" s="13">
-        <f>D4*E4</f>
-        <v>2750</v>
-      </c>
-      <c r="G4" s="13">
-        <f t="shared" si="0"/>
-        <v>0.75625000000000009</v>
-      </c>
-      <c r="H4" s="13">
-        <f t="shared" si="1"/>
-        <v>0.19250000000000003</v>
-      </c>
-      <c r="I4" s="13">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="13">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="13">
-        <v>0</v>
-      </c>
-      <c r="L4" s="13">
-        <f t="shared" si="2"/>
-        <v>2767.73875</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="F5" s="13">
-        <f t="shared" ref="F5:L5" si="3">SUM(F2:F4)</f>
-        <v>9322</v>
-      </c>
-      <c r="G5" s="13">
-        <f t="shared" si="3"/>
-        <v>2.5635500000000002</v>
-      </c>
-      <c r="H5" s="13">
-        <f t="shared" si="3"/>
-        <v>0.65254000000000012</v>
-      </c>
-      <c r="I5" s="13">
-        <f t="shared" si="3"/>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="13">
-        <f t="shared" si="3"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L5" s="13">
-        <f t="shared" si="3"/>
-        <v>9375.5860899999989</v>
-      </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
@@ -3661,6 +3554,258 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EC0A3F-FFB0-437C-B726-EA72E0B69675}">
+  <dimension ref="A1:AC7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="12"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="18"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="12">
+        <v>100</v>
+      </c>
+      <c r="E2" s="13">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="13">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="13">
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="13">
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
+      </c>
+      <c r="I2" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="13">
+        <v>0</v>
+      </c>
+      <c r="L2" s="13">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>39757</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1662</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12">
+        <v>200</v>
+      </c>
+      <c r="E3" s="13">
+        <v>25.19</v>
+      </c>
+      <c r="F3" s="13">
+        <f>D3*E3</f>
+        <v>5038</v>
+      </c>
+      <c r="G3" s="13">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.3854500000000001</v>
+      </c>
+      <c r="H3" s="13">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.35266000000000003</v>
+      </c>
+      <c r="I3" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="13">
+        <v>0</v>
+      </c>
+      <c r="L3" s="13">
+        <f t="shared" ref="L3:L4" si="2">F3+G3+H3+I3+J3</f>
+        <v>5056.5281099999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="12">
+        <v>1662</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="12">
+        <v>100</v>
+      </c>
+      <c r="E4" s="13">
+        <v>27.5</v>
+      </c>
+      <c r="F4" s="13">
+        <f>D4*E4</f>
+        <v>2750</v>
+      </c>
+      <c r="G4" s="13">
+        <f t="shared" si="0"/>
+        <v>0.75625000000000009</v>
+      </c>
+      <c r="H4" s="13">
+        <f t="shared" si="1"/>
+        <v>0.19250000000000003</v>
+      </c>
+      <c r="I4" s="13">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="13">
+        <v>0</v>
+      </c>
+      <c r="L4" s="13">
+        <f t="shared" si="2"/>
+        <v>2767.73875</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="F5" s="13">
+        <f t="shared" ref="F5:L5" si="3">SUM(F2:F4)</f>
+        <v>9322</v>
+      </c>
+      <c r="G5" s="13">
+        <f t="shared" si="3"/>
+        <v>2.5635500000000002</v>
+      </c>
+      <c r="H5" s="13">
+        <f t="shared" si="3"/>
+        <v>0.65254000000000012</v>
+      </c>
+      <c r="I5" s="13">
+        <f t="shared" si="3"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="13">
+        <f t="shared" si="3"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="13">
+        <f t="shared" si="3"/>
+        <v>9375.5860899999989</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -4247,7 +4392,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
@@ -4774,7 +4919,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
@@ -5683,7 +5828,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -5939,7 +6084,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7618D34E-0B33-4181-8E63-6765777C5B7E}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
@@ -6231,7 +6376,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19EF43A-AB48-4760-8CB3-D62FBA7ABFD8}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6447,7 +6592,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6663,7 +6808,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1583F5-F968-4E69-BCCF-4B8530FA0CCB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6879,7 +7024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -7170,445 +7315,6 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E6" s="21"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E3E40E-BCAE-41DB-80FC-C74D9CCDCD28}">
-  <dimension ref="A1:AC13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="9">
-        <v>200</v>
-      </c>
-      <c r="E2" s="8">
-        <v>40</v>
-      </c>
-      <c r="F2" s="8">
-        <f>D2*E2</f>
-        <v>8000</v>
-      </c>
-      <c r="G2" s="8">
-        <f>F2*0.0275%</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H2" s="8">
-        <f>F2*0.007%</f>
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="I2" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="8">
-        <v>0.19</v>
-      </c>
-      <c r="L2" s="8">
-        <f>F2-G2-H2-I2-K2</f>
-        <v>7981.06</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-    </row>
-    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B3" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9">
-        <v>200</v>
-      </c>
-      <c r="E3" s="8">
-        <v>34.479999999999997</v>
-      </c>
-      <c r="F3" s="8">
-        <f>D3*E3</f>
-        <v>6895.9999999999991</v>
-      </c>
-      <c r="G3" s="8">
-        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
-        <v>1.8963999999999999</v>
-      </c>
-      <c r="H3" s="8">
-        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
-        <v>0.48271999999999998</v>
-      </c>
-      <c r="I3" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="8">
-        <f>((F3 - G3 - H3 - I3 - J3) - (18.5 * D3)) * 0.005%</f>
-        <v>0.15884154399999997</v>
-      </c>
-      <c r="L3" s="8">
-        <f>F3-G3-H3-I3-K3</f>
-        <v>6877.4720384559996</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-    </row>
-    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="9">
-        <v>200</v>
-      </c>
-      <c r="E4" s="8">
-        <v>27.45</v>
-      </c>
-      <c r="F4" s="8">
-        <f>D4*E4</f>
-        <v>5490</v>
-      </c>
-      <c r="G4" s="8">
-        <f t="shared" si="0"/>
-        <v>1.5097500000000001</v>
-      </c>
-      <c r="H4" s="8">
-        <f t="shared" si="1"/>
-        <v>0.38430000000000003</v>
-      </c>
-      <c r="I4" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="8">
-        <f>((F4 - G4 - H4 - I4 - J4) - (22.3 * D4)) * 0.005%</f>
-        <v>5.0565797500000009E-2</v>
-      </c>
-      <c r="L4" s="8">
-        <f>F4-G4-H4-I4-K4</f>
-        <v>5472.0653842025004</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-    </row>
-    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="11">
-        <f t="shared" ref="F5:L5" si="2">SUM(F2:F4)</f>
-        <v>20386</v>
-      </c>
-      <c r="G5" s="11">
-        <f t="shared" si="2"/>
-        <v>5.6061500000000004</v>
-      </c>
-      <c r="H5" s="11">
-        <f t="shared" si="2"/>
-        <v>1.4270200000000002</v>
-      </c>
-      <c r="I5" s="11">
-        <f t="shared" si="2"/>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="11">
-        <f t="shared" si="2"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="11">
-        <f t="shared" si="2"/>
-        <v>0.39940734150000001</v>
-      </c>
-      <c r="L5" s="11">
-        <f t="shared" si="2"/>
-        <v>20330.597422658502</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="8"/>
-      <c r="AB5" s="8"/>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="L8" s="1">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E9" s="19">
-        <v>100</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2750</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.22</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0.74</v>
-      </c>
-      <c r="I9" s="1">
-        <v>15.99</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="K9" s="1">
-        <f>F9-G9-H9-I9-J9</f>
-        <v>2732.2500000000005</v>
-      </c>
-      <c r="L9" s="1">
-        <f>L8+K9</f>
-        <v>2732.2500000000005</v>
-      </c>
-      <c r="N9" s="19">
-        <f>N8+E9</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E10" s="19">
-        <v>200</v>
-      </c>
-      <c r="F10" s="1">
-        <v>5940</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0.47</v>
-      </c>
-      <c r="H10" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="I10" s="1">
-        <v>15.99</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="K10" s="1">
-        <f t="shared" ref="K10:K12" si="3">F10-G10-H10-I10-J10</f>
-        <v>5921.1399999999994</v>
-      </c>
-      <c r="L10" s="1">
-        <f>L9+K10</f>
-        <v>8653.39</v>
-      </c>
-      <c r="N10" s="19">
-        <f>N9+E10</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E11" s="19">
-        <v>-200</v>
-      </c>
-      <c r="F11" s="1">
-        <v>6630</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0.39</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1.89</v>
-      </c>
-      <c r="I11" s="1">
-        <v>15.99</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="K11" s="1">
-        <f t="shared" si="3"/>
-        <v>6610.9299999999994</v>
-      </c>
-      <c r="L11" s="1">
-        <f>L10+((L10/N10)*E11)</f>
-        <v>2884.4633333333331</v>
-      </c>
-      <c r="N11" s="19">
-        <f>N10+E11</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E12" s="19">
-        <v>200</v>
-      </c>
-      <c r="F12" s="1">
-        <v>6400</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0.38</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1.82</v>
-      </c>
-      <c r="I12" s="1">
-        <v>15.99</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="K12" s="1">
-        <f t="shared" si="3"/>
-        <v>6381.01</v>
-      </c>
-      <c r="L12" s="20">
-        <f>L11+K12</f>
-        <v>9265.4733333333334</v>
-      </c>
-      <c r="N12" s="21">
-        <f>N11+E12</f>
-        <v>300</v>
-      </c>
-      <c r="O12" s="1">
-        <f>L12/N12</f>
-        <v>30.884911111111112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E13" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -7764,6 +7470,445 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E3E40E-BCAE-41DB-80FC-C74D9CCDCD28}">
+  <dimension ref="A1:AC13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9">
+        <v>200</v>
+      </c>
+      <c r="E2" s="8">
+        <v>40</v>
+      </c>
+      <c r="F2" s="8">
+        <f>D2*E2</f>
+        <v>8000</v>
+      </c>
+      <c r="G2" s="8">
+        <f>F2*0.0275%</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H2" s="8">
+        <f>F2*0.007%</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I2" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="L2" s="8">
+        <f>F2-G2-H2-I2-K2</f>
+        <v>7981.06</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9">
+        <v>200</v>
+      </c>
+      <c r="E3" s="8">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3*E3</f>
+        <v>6895.9999999999991</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.8963999999999999</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.48271999999999998</v>
+      </c>
+      <c r="I3" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="8">
+        <f>((F3 - G3 - H3 - I3 - J3) - (18.5 * D3)) * 0.005%</f>
+        <v>0.15884154399999997</v>
+      </c>
+      <c r="L3" s="8">
+        <f>F3-G3-H3-I3-K3</f>
+        <v>6877.4720384559996</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="9">
+        <v>200</v>
+      </c>
+      <c r="E4" s="8">
+        <v>27.45</v>
+      </c>
+      <c r="F4" s="8">
+        <f>D4*E4</f>
+        <v>5490</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5097500000000001</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" si="1"/>
+        <v>0.38430000000000003</v>
+      </c>
+      <c r="I4" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="8">
+        <f>((F4 - G4 - H4 - I4 - J4) - (22.3 * D4)) * 0.005%</f>
+        <v>5.0565797500000009E-2</v>
+      </c>
+      <c r="L4" s="8">
+        <f>F4-G4-H4-I4-K4</f>
+        <v>5472.0653842025004</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="11">
+        <f t="shared" ref="F5:L5" si="2">SUM(F2:F4)</f>
+        <v>20386</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="2"/>
+        <v>5.6061500000000004</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="2"/>
+        <v>1.4270200000000002</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="2"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="2"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="2"/>
+        <v>0.39940734150000001</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="2"/>
+        <v>20330.597422658502</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E9" s="19">
+        <v>100</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2750</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="I9" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K9" s="1">
+        <f>F9-G9-H9-I9-J9</f>
+        <v>2732.2500000000005</v>
+      </c>
+      <c r="L9" s="1">
+        <f>L8+K9</f>
+        <v>2732.2500000000005</v>
+      </c>
+      <c r="N9" s="19">
+        <f>N8+E9</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E10" s="19">
+        <v>200</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5940</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.47</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I10" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" ref="K10:K12" si="3">F10-G10-H10-I10-J10</f>
+        <v>5921.1399999999994</v>
+      </c>
+      <c r="L10" s="1">
+        <f>L9+K10</f>
+        <v>8653.39</v>
+      </c>
+      <c r="N10" s="19">
+        <f>N9+E10</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E11" s="19">
+        <v>-200</v>
+      </c>
+      <c r="F11" s="1">
+        <v>6630</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1.89</v>
+      </c>
+      <c r="I11" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="3"/>
+        <v>6610.9299999999994</v>
+      </c>
+      <c r="L11" s="1">
+        <f>L10+((L10/N10)*E11)</f>
+        <v>2884.4633333333331</v>
+      </c>
+      <c r="N11" s="19">
+        <f>N10+E11</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E12" s="19">
+        <v>200</v>
+      </c>
+      <c r="F12" s="1">
+        <v>6400</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1.82</v>
+      </c>
+      <c r="I12" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="3"/>
+        <v>6381.01</v>
+      </c>
+      <c r="L12" s="20">
+        <f>L11+K12</f>
+        <v>9265.4733333333334</v>
+      </c>
+      <c r="N12" s="21">
+        <f>N11+E12</f>
+        <v>300</v>
+      </c>
+      <c r="O12" s="1">
+        <f>L12/N12</f>
+        <v>30.884911111111112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E13" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F402F95-319A-4797-B7E1-F3EB07A82FDD}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -7980,7 +8125,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A590E594-CB91-4439-95F2-7F159495761F}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8197,7 +8342,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34F43A8-C89C-44C0-BF29-1F8134A0151F}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -8495,7 +8640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5AE87-00E8-4CF9-A517-EB6C0CA40610}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8711,7 +8856,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B51BEB4-905E-4036-959A-F9A0226AF070}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8928,7 +9073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B7349E-D984-4817-800E-2EB4836D5B5D}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9145,7 +9290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA65F892-A6B4-4288-ADB5-125D04E295EB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9362,7 +9507,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421F9D80-1D28-4F3C-95F7-8DE9883A26F0}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9579,7 +9724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D25BF0F-8645-49A4-A6C8-BE755BFA7BE7}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -9875,241 +10020,6 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4721B46-AB87-4CAA-ABF7-E48CFDA36C4A}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="2"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>42996</v>
-      </c>
-      <c r="B2" s="4">
-        <v>168102</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>23.65</v>
-      </c>
-      <c r="F2" s="3">
-        <f>D2*E2</f>
-        <v>9460</v>
-      </c>
-      <c r="G2" s="3">
-        <f t="shared" ref="G2:G3" si="0">F2*0.0275%</f>
-        <v>2.6015000000000001</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.47300000000000003</v>
-      </c>
-      <c r="I2" s="3">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="J2" s="3">
-        <f>I2*5%</f>
-        <v>0.12450000000000001</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>9465.6890000000003</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-    </row>
-    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>42996</v>
-      </c>
-      <c r="B3" s="9">
-        <v>168102</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="9">
-        <v>700</v>
-      </c>
-      <c r="E3" s="8">
-        <v>10.5</v>
-      </c>
-      <c r="F3" s="8">
-        <f>D3*E3</f>
-        <v>7350</v>
-      </c>
-      <c r="G3" s="8">
-        <f t="shared" si="0"/>
-        <v>2.0212500000000002</v>
-      </c>
-      <c r="H3" s="8">
-        <f>F3*0.005%</f>
-        <v>0.36749999999999999</v>
-      </c>
-      <c r="I3" s="8">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="J3" s="8">
-        <f>I3*5%</f>
-        <v>0.12450000000000001</v>
-      </c>
-      <c r="K3" s="8">
-        <v>0</v>
-      </c>
-      <c r="L3" s="8">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>7355.0032499999998</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7">
-        <f t="shared" ref="F4:K4" si="1">SUM(F2:F3)</f>
-        <v>16810</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" si="1"/>
-        <v>4.6227499999999999</v>
-      </c>
-      <c r="H4" s="7">
-        <f t="shared" si="1"/>
-        <v>0.84050000000000002</v>
-      </c>
-      <c r="I4" s="7">
-        <f t="shared" si="1"/>
-        <v>4.9800000000000004</v>
-      </c>
-      <c r="J4" s="7">
-        <f t="shared" si="1"/>
-        <v>0.24900000000000003</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="7">
-        <f>L3-L2</f>
-        <v>-2110.6857500000006</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -10257,6 +10167,241 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4721B46-AB87-4CAA-ABF7-E48CFDA36C4A}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>42996</v>
+      </c>
+      <c r="B2" s="4">
+        <v>168102</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>23.65</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>9460</v>
+      </c>
+      <c r="G2" s="3">
+        <f t="shared" ref="G2:G3" si="0">F2*0.0275%</f>
+        <v>2.6015000000000001</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.47300000000000003</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="J2" s="3">
+        <f>I2*5%</f>
+        <v>0.12450000000000001</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>9465.6890000000003</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>42996</v>
+      </c>
+      <c r="B3" s="9">
+        <v>168102</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="9">
+        <v>700</v>
+      </c>
+      <c r="E3" s="8">
+        <v>10.5</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3*E3</f>
+        <v>7350</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" si="0"/>
+        <v>2.0212500000000002</v>
+      </c>
+      <c r="H3" s="8">
+        <f>F3*0.005%</f>
+        <v>0.36749999999999999</v>
+      </c>
+      <c r="I3" s="8">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="J3" s="8">
+        <f>I3*5%</f>
+        <v>0.12450000000000001</v>
+      </c>
+      <c r="K3" s="8">
+        <v>0</v>
+      </c>
+      <c r="L3" s="8">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>7355.0032499999998</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f t="shared" ref="F4:K4" si="1">SUM(F2:F3)</f>
+        <v>16810</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" si="1"/>
+        <v>4.6227499999999999</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="1"/>
+        <v>0.84050000000000002</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="1"/>
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="1"/>
+        <v>0.24900000000000003</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f>L3-L2</f>
+        <v>-2110.6857500000006</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF39107-DEBE-454A-A911-9FAC6360BB3B}">
   <dimension ref="A1:AC4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Prevents a 'BrokerageNotesWorksheetReader' from being created when a negative 'Price' is found.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A8B2B2-9456-4EEE-832A-4B5C8AB9915B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D746DBA0-BCE7-4D88-95E2-08FFE0661A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="11" activeTab="13" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="12" activeTab="14" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="NotUsed" sheetId="2" r:id="rId1"/>
@@ -27,33 +27,34 @@
     <sheet name="QtyExtraneousCharacters" sheetId="45" r:id="rId12"/>
     <sheet name="QtyBlack" sheetId="46" r:id="rId13"/>
     <sheet name="PriceMissing" sheetId="47" r:id="rId14"/>
-    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId15"/>
-    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId16"/>
-    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId17"/>
-    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId18"/>
-    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId19"/>
-    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId20"/>
-    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId21"/>
-    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId22"/>
-    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId23"/>
-    <sheet name="SingleLineGroups" sheetId="10" r:id="rId24"/>
-    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId25"/>
-    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId26"/>
-    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId27"/>
-    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId28"/>
-    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId29"/>
-    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId30"/>
-    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId31"/>
-    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId32"/>
-    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId33"/>
-    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId34"/>
-    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId35"/>
-    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId36"/>
-    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId37"/>
-    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId38"/>
-    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId39"/>
-    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId40"/>
-    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId41"/>
+    <sheet name="PriceNegative" sheetId="48" r:id="rId15"/>
+    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId16"/>
+    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId17"/>
+    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId18"/>
+    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId19"/>
+    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId20"/>
+    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId21"/>
+    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId22"/>
+    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId23"/>
+    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId24"/>
+    <sheet name="SingleLineGroups" sheetId="10" r:id="rId25"/>
+    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId26"/>
+    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId27"/>
+    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId28"/>
+    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId29"/>
+    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId30"/>
+    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId31"/>
+    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId32"/>
+    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId33"/>
+    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId34"/>
+    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId35"/>
+    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId36"/>
+    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId37"/>
+    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId38"/>
+    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId39"/>
+    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId40"/>
+    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId41"/>
+    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId42"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -179,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="27">
   <si>
     <t>BBAS3</t>
   </si>
@@ -1429,6 +1430,150 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EAB37C1-DC87-4BE0-9B0C-DB97F9056CC1}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="18"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="24"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>16.79</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F142533D-F42E-4015-8648-EEB2343B1768}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
@@ -1521,18 +1666,20 @@
       <c r="D2" s="4">
         <v>100</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3">
+        <v>-15.34</v>
+      </c>
       <c r="F2" s="3">
         <f>D2*E2</f>
-        <v>0</v>
+        <v>-1534</v>
       </c>
       <c r="G2" s="3">
         <f>F2*0.0275%</f>
-        <v>0</v>
+        <v>-0.42185</v>
       </c>
       <c r="H2" s="3">
         <f>F2*0.007%</f>
-        <v>0</v>
+        <v>-0.10738000000000002</v>
       </c>
       <c r="I2" s="3">
         <v>15.99</v>
@@ -1545,7 +1692,7 @@
       </c>
       <c r="L2" s="3">
         <f>F2+G2+H2+I2+J2</f>
-        <v>16.79</v>
+        <v>-1517.7392299999999</v>
       </c>
       <c r="M2" s="6"/>
       <c r="R2" s="3"/>
@@ -1569,7 +1716,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF98C6E-C61C-4098-8811-20C737B2746F}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -2156,7 +2303,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -2743,7 +2890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F27D22B-36B9-402D-A19C-031FF2332945}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
@@ -2912,7 +3059,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7579CBF-C87A-40BF-91B5-CE83CDC20ECE}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -3100,308 +3247,6 @@
         <f>SUM(L1:L3)</f>
         <v>22611.018699999997</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384BB7C-DF07-4187-ADF0-23E50C2BA287}">
-  <dimension ref="A1:AC7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="1" sqref="B3 A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.140625" style="12"/>
-    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="18"/>
-    </row>
-    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4">
-        <v>100</v>
-      </c>
-      <c r="E2" s="3">
-        <v>15.34</v>
-      </c>
-      <c r="F2" s="3">
-        <f>D2*E2</f>
-        <v>1534</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.0275%</f>
-        <v>0.42185</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.007%</f>
-        <v>0.10738000000000002</v>
-      </c>
-      <c r="I2" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>1551.3192299999998</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-    </row>
-    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B3" s="22">
-        <v>1662</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" s="3">
-        <v>25.19</v>
-      </c>
-      <c r="F3" s="3">
-        <f>D3*E3</f>
-        <v>5038</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
-        <v>1.3854500000000001</v>
-      </c>
-      <c r="H3" s="3">
-        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
-        <v>0.35266000000000003</v>
-      </c>
-      <c r="I3" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>5056.5281099999993</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4">
-        <v>100</v>
-      </c>
-      <c r="E4" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F4" s="3">
-        <f>D4*E4</f>
-        <v>2750</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" si="0"/>
-        <v>0.75625000000000009</v>
-      </c>
-      <c r="H4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.19250000000000003</v>
-      </c>
-      <c r="I4" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3">
-        <f>F4+G4+H4+I4+J4</f>
-        <v>2767.73875</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="7">
-        <f>-SUM(F2:F4)</f>
-        <v>-9322</v>
-      </c>
-      <c r="G5" s="7">
-        <f t="shared" ref="G5:K5" si="2">SUM(G2:G4)</f>
-        <v>2.5635500000000002</v>
-      </c>
-      <c r="H5" s="7">
-        <f t="shared" si="2"/>
-        <v>0.65254000000000012</v>
-      </c>
-      <c r="I5" s="7">
-        <f t="shared" si="2"/>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="7">
-        <f t="shared" si="2"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L5" s="7">
-        <f>-SUM(L2:L4)</f>
-        <v>-9375.5860899999989</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3554,6 +3399,308 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384BB7C-DF07-4187-ADF0-23E50C2BA287}">
+  <dimension ref="A1:AC7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="1" sqref="B3 A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="12"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="18"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2*E2</f>
+        <v>1534</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0.10738000000000002</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>1551.3192299999998</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B3" s="22">
+        <v>1662</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>200</v>
+      </c>
+      <c r="E3" s="3">
+        <v>25.19</v>
+      </c>
+      <c r="F3" s="3">
+        <f>D3*E3</f>
+        <v>5038</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.3854500000000001</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.35266000000000003</v>
+      </c>
+      <c r="I3" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>5056.5281099999993</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4">
+        <v>100</v>
+      </c>
+      <c r="E4" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F4" s="3">
+        <f>D4*E4</f>
+        <v>2750</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.75625000000000009</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.19250000000000003</v>
+      </c>
+      <c r="I4" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <f>F4+G4+H4+I4+J4</f>
+        <v>2767.73875</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="7">
+        <f>-SUM(F2:F4)</f>
+        <v>-9322</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" ref="G5:K5" si="2">SUM(G2:G4)</f>
+        <v>2.5635500000000002</v>
+      </c>
+      <c r="H5" s="7">
+        <f t="shared" si="2"/>
+        <v>0.65254000000000012</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="shared" si="2"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" si="2"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="7">
+        <f>-SUM(L2:L4)</f>
+        <v>-9375.5860899999989</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EC0A3F-FFB0-437C-B726-EA72E0B69675}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -3805,7 +3952,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -4392,7 +4539,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
@@ -4919,7 +5066,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
@@ -5828,7 +5975,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -6084,7 +6231,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7618D34E-0B33-4181-8E63-6765777C5B7E}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
@@ -6376,7 +6523,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19EF43A-AB48-4760-8CB3-D62FBA7ABFD8}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6592,7 +6739,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6808,7 +6955,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1583F5-F968-4E69-BCCF-4B8530FA0CCB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -7021,305 +7168,6 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
-  <dimension ref="A1:AC6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="9">
-        <v>200</v>
-      </c>
-      <c r="E2" s="8">
-        <v>40</v>
-      </c>
-      <c r="F2" s="8">
-        <f>D2*E2</f>
-        <v>8000</v>
-      </c>
-      <c r="G2" s="8">
-        <f>F2*0.0275%</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H2" s="8">
-        <f>F2*0.007%</f>
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="I2" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="8">
-        <v>0.19</v>
-      </c>
-      <c r="L2" s="8">
-        <f>F2-G2-H2-I2-K2</f>
-        <v>7981.06</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-    </row>
-    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B3" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9">
-        <v>200</v>
-      </c>
-      <c r="E3" s="8">
-        <v>34.479999999999997</v>
-      </c>
-      <c r="F3" s="8">
-        <f>D3*E3</f>
-        <v>6895.9999999999991</v>
-      </c>
-      <c r="G3" s="8">
-        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
-        <v>1.8963999999999999</v>
-      </c>
-      <c r="H3" s="8">
-        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
-        <v>0.48271999999999998</v>
-      </c>
-      <c r="I3" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="8">
-        <f>((F3 - G3 - H3 - I3 - J3) - (18.5 * D3)) * 0.005%</f>
-        <v>0.15884154399999997</v>
-      </c>
-      <c r="L3" s="8">
-        <f>F3-G3-H3-I3-K3</f>
-        <v>6877.4720384559996</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-    </row>
-    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="9">
-        <v>200</v>
-      </c>
-      <c r="E4" s="8">
-        <v>27.45</v>
-      </c>
-      <c r="F4" s="8">
-        <f>D4*E4</f>
-        <v>5490</v>
-      </c>
-      <c r="G4" s="8">
-        <f t="shared" si="0"/>
-        <v>1.5097500000000001</v>
-      </c>
-      <c r="H4" s="8">
-        <f t="shared" si="1"/>
-        <v>0.38430000000000003</v>
-      </c>
-      <c r="I4" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="8">
-        <f>((F4 - G4 - H4 - I4 - J4) - (22.3 * D4)) * 0.005%</f>
-        <v>5.0565797500000009E-2</v>
-      </c>
-      <c r="L4" s="8">
-        <f>F4-G4-H4-I4-K4</f>
-        <v>5472.0653842025004</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-    </row>
-    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="11">
-        <f t="shared" ref="F5:L5" si="2">SUM(F2:F4)</f>
-        <v>20386</v>
-      </c>
-      <c r="G5" s="11">
-        <f t="shared" si="2"/>
-        <v>5.6061500000000004</v>
-      </c>
-      <c r="H5" s="11">
-        <f t="shared" si="2"/>
-        <v>1.4270200000000002</v>
-      </c>
-      <c r="I5" s="11">
-        <f t="shared" si="2"/>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="11">
-        <f t="shared" si="2"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="11">
-        <f t="shared" si="2"/>
-        <v>0.39940734150000001</v>
-      </c>
-      <c r="L5" s="11">
-        <f t="shared" si="2"/>
-        <v>20330.597422658502</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="8"/>
-      <c r="AB5" s="8"/>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E6" s="21"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7470,6 +7318,305 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
+  <dimension ref="A1:AC6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9">
+        <v>200</v>
+      </c>
+      <c r="E2" s="8">
+        <v>40</v>
+      </c>
+      <c r="F2" s="8">
+        <f>D2*E2</f>
+        <v>8000</v>
+      </c>
+      <c r="G2" s="8">
+        <f>F2*0.0275%</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H2" s="8">
+        <f>F2*0.007%</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I2" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="L2" s="8">
+        <f>F2-G2-H2-I2-K2</f>
+        <v>7981.06</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9">
+        <v>200</v>
+      </c>
+      <c r="E3" s="8">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3*E3</f>
+        <v>6895.9999999999991</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
+        <v>1.8963999999999999</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
+        <v>0.48271999999999998</v>
+      </c>
+      <c r="I3" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="8">
+        <f>((F3 - G3 - H3 - I3 - J3) - (18.5 * D3)) * 0.005%</f>
+        <v>0.15884154399999997</v>
+      </c>
+      <c r="L3" s="8">
+        <f>F3-G3-H3-I3-K3</f>
+        <v>6877.4720384559996</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="9">
+        <v>200</v>
+      </c>
+      <c r="E4" s="8">
+        <v>27.45</v>
+      </c>
+      <c r="F4" s="8">
+        <f>D4*E4</f>
+        <v>5490</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5097500000000001</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" si="1"/>
+        <v>0.38430000000000003</v>
+      </c>
+      <c r="I4" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="8">
+        <f>((F4 - G4 - H4 - I4 - J4) - (22.3 * D4)) * 0.005%</f>
+        <v>5.0565797500000009E-2</v>
+      </c>
+      <c r="L4" s="8">
+        <f>F4-G4-H4-I4-K4</f>
+        <v>5472.0653842025004</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="11">
+        <f t="shared" ref="F5:L5" si="2">SUM(F2:F4)</f>
+        <v>20386</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="2"/>
+        <v>5.6061500000000004</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="2"/>
+        <v>1.4270200000000002</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="2"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="2"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="2"/>
+        <v>0.39940734150000001</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="2"/>
+        <v>20330.597422658502</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E6" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E3E40E-BCAE-41DB-80FC-C74D9CCDCD28}">
   <dimension ref="A1:AC13"/>
   <sheetViews>
@@ -7908,7 +8055,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F402F95-319A-4797-B7E1-F3EB07A82FDD}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8125,7 +8272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A590E594-CB91-4439-95F2-7F159495761F}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8342,7 +8489,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34F43A8-C89C-44C0-BF29-1F8134A0151F}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -8640,7 +8787,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5AE87-00E8-4CF9-A517-EB6C0CA40610}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8856,7 +9003,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B51BEB4-905E-4036-959A-F9A0226AF070}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9073,7 +9220,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B7349E-D984-4817-800E-2EB4836D5B5D}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9290,7 +9437,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA65F892-A6B4-4288-ADB5-125D04E295EB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9507,7 +9654,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421F9D80-1D28-4F3C-95F7-8DE9883A26F0}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9717,305 +9864,6 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D25BF0F-8645-49A4-A6C8-BE755BFA7BE7}">
-  <dimension ref="A1:AC8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="9">
-        <v>200</v>
-      </c>
-      <c r="E2" s="8">
-        <v>35.15</v>
-      </c>
-      <c r="F2" s="8">
-        <f>D2*E2</f>
-        <v>7030</v>
-      </c>
-      <c r="G2" s="8">
-        <f>F2*0.0275%</f>
-        <v>1.9332500000000001</v>
-      </c>
-      <c r="H2" s="8">
-        <f>F2*0.007%</f>
-        <v>0.49210000000000004</v>
-      </c>
-      <c r="I2" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J2" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="8">
-        <f>((F2 - G2 - H2 - I2 - J2) - (30.88 * D2)) * 0.005%</f>
-        <v>4.173923249999998E-2</v>
-      </c>
-      <c r="L2" s="8">
-        <f t="shared" ref="L2:L4" si="0">F2-G2-H2-I2-J2</f>
-        <v>7010.7846499999996</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-    </row>
-    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B3" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="9">
-        <v>200</v>
-      </c>
-      <c r="E3" s="8">
-        <v>34.479999999999997</v>
-      </c>
-      <c r="F3" s="8">
-        <f>D3*E3</f>
-        <v>6895.9999999999991</v>
-      </c>
-      <c r="G3" s="8">
-        <f t="shared" ref="G3:G4" si="1">F3*0.0275%</f>
-        <v>1.8963999999999999</v>
-      </c>
-      <c r="H3" s="8">
-        <f t="shared" ref="H3:H4" si="2">F3*0.007%</f>
-        <v>0.48271999999999998</v>
-      </c>
-      <c r="I3" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="8">
-        <f>((F3 - G3 - H3 - I3 - J3) - (30.88 * D3)) * 0.005%</f>
-        <v>3.504154399999998E-2</v>
-      </c>
-      <c r="L3" s="8">
-        <f t="shared" si="0"/>
-        <v>6876.8308799999995</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-    </row>
-    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>40073</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1462</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="9">
-        <v>200</v>
-      </c>
-      <c r="E4" s="8">
-        <v>31</v>
-      </c>
-      <c r="F4" s="8">
-        <f>D4*E4</f>
-        <v>6200</v>
-      </c>
-      <c r="G4" s="8">
-        <f t="shared" si="1"/>
-        <v>1.7050000000000001</v>
-      </c>
-      <c r="H4" s="8">
-        <f t="shared" si="2"/>
-        <v>0.43400000000000005</v>
-      </c>
-      <c r="I4" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="8">
-        <f>((F4 - G4 - H4 - I4 - J4) - (30.88 * D4)) * 0.005%</f>
-        <v>2.5354999999999567E-4</v>
-      </c>
-      <c r="L4" s="8">
-        <f t="shared" si="0"/>
-        <v>6181.0709999999999</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-    </row>
-    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="11">
-        <f t="shared" ref="F5:L5" si="3">SUM(F2:F4)</f>
-        <v>20126</v>
-      </c>
-      <c r="G5" s="11">
-        <f t="shared" si="3"/>
-        <v>5.5346500000000001</v>
-      </c>
-      <c r="H5" s="11">
-        <f t="shared" si="3"/>
-        <v>1.40882</v>
-      </c>
-      <c r="I5" s="11">
-        <f t="shared" si="3"/>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="11">
-        <f t="shared" si="3"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="11">
-        <f>SUM(K2:K4) - 0.03</f>
-        <v>4.7034326499999946E-2</v>
-      </c>
-      <c r="L5" s="11">
-        <f t="shared" si="3"/>
-        <v>20068.686529999999</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="8"/>
-      <c r="AB5" s="8"/>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E8" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -10167,6 +10015,305 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D25BF0F-8645-49A4-A6C8-BE755BFA7BE7}">
+  <dimension ref="A1:AC8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9">
+        <v>200</v>
+      </c>
+      <c r="E2" s="8">
+        <v>35.15</v>
+      </c>
+      <c r="F2" s="8">
+        <f>D2*E2</f>
+        <v>7030</v>
+      </c>
+      <c r="G2" s="8">
+        <f>F2*0.0275%</f>
+        <v>1.9332500000000001</v>
+      </c>
+      <c r="H2" s="8">
+        <f>F2*0.007%</f>
+        <v>0.49210000000000004</v>
+      </c>
+      <c r="I2" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="8">
+        <f>((F2 - G2 - H2 - I2 - J2) - (30.88 * D2)) * 0.005%</f>
+        <v>4.173923249999998E-2</v>
+      </c>
+      <c r="L2" s="8">
+        <f t="shared" ref="L2:L4" si="0">F2-G2-H2-I2-J2</f>
+        <v>7010.7846499999996</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9">
+        <v>200</v>
+      </c>
+      <c r="E3" s="8">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3*E3</f>
+        <v>6895.9999999999991</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" ref="G3:G4" si="1">F3*0.0275%</f>
+        <v>1.8963999999999999</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" ref="H3:H4" si="2">F3*0.007%</f>
+        <v>0.48271999999999998</v>
+      </c>
+      <c r="I3" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="8">
+        <f>((F3 - G3 - H3 - I3 - J3) - (30.88 * D3)) * 0.005%</f>
+        <v>3.504154399999998E-2</v>
+      </c>
+      <c r="L3" s="8">
+        <f t="shared" si="0"/>
+        <v>6876.8308799999995</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>40073</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1462</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9">
+        <v>200</v>
+      </c>
+      <c r="E4" s="8">
+        <v>31</v>
+      </c>
+      <c r="F4" s="8">
+        <f>D4*E4</f>
+        <v>6200</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" si="1"/>
+        <v>1.7050000000000001</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" si="2"/>
+        <v>0.43400000000000005</v>
+      </c>
+      <c r="I4" s="8">
+        <v>15.99</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="8">
+        <f>((F4 - G4 - H4 - I4 - J4) - (30.88 * D4)) * 0.005%</f>
+        <v>2.5354999999999567E-4</v>
+      </c>
+      <c r="L4" s="8">
+        <f t="shared" si="0"/>
+        <v>6181.0709999999999</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="11">
+        <f t="shared" ref="F5:L5" si="3">SUM(F2:F4)</f>
+        <v>20126</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="3"/>
+        <v>5.5346500000000001</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="3"/>
+        <v>1.40882</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="3"/>
+        <v>47.97</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="3"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K5" s="11">
+        <f>SUM(K2:K4) - 0.03</f>
+        <v>4.7034326499999946E-2</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="3"/>
+        <v>20068.686529999999</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E8" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4721B46-AB87-4CAA-ABF7-E48CFDA36C4A}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -10401,7 +10548,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF39107-DEBE-454A-A911-9FAC6360BB3B}">
   <dimension ref="A1:AC4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Renames 'NegotiationFess' to 'TradingFees'.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D746DBA0-BCE7-4D88-95E2-08FFE0661A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915807A1-6B2F-4E1E-B8D1-8E0D851C2728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="12" activeTab="14" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="27" activeTab="27" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="NotUsed" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <sheet name="SingleLineGroups" sheetId="10" r:id="rId25"/>
     <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId26"/>
     <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId27"/>
-    <sheet name="InvalidNegotiationsFee" sheetId="17" r:id="rId28"/>
+    <sheet name="InvalidTradingFees" sheetId="17" r:id="rId28"/>
     <sheet name="InvalidServiceTax" sheetId="18" r:id="rId29"/>
     <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId30"/>
     <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId31"/>
@@ -49,7 +49,7 @@
     <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId34"/>
     <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId35"/>
     <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId36"/>
-    <sheet name="InvalidNegotiationFeesSummary" sheetId="27" r:id="rId37"/>
+    <sheet name="InvalidTradingFeesSummary" sheetId="27" r:id="rId37"/>
     <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId38"/>
     <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId39"/>
     <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId40"/>
@@ -1574,7 +1574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F142533D-F42E-4015-8648-EEB2343B1768}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
@@ -6743,7 +6743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>

</xml_diff>

<commit_message>
Prevents a 'BrokerageNotesWorksheetReader' from being created when a 'Price' contains extraneous characters that prevent it from being interpreted as a currency.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915807A1-6B2F-4E1E-B8D1-8E0D851C2728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89918E47-2922-4B64-90AA-6BCF99CAF2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="27" activeTab="27" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="14" activeTab="15" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="NotUsed" sheetId="2" r:id="rId1"/>
@@ -28,33 +28,34 @@
     <sheet name="QtyBlack" sheetId="46" r:id="rId13"/>
     <sheet name="PriceMissing" sheetId="47" r:id="rId14"/>
     <sheet name="PriceNegative" sheetId="48" r:id="rId15"/>
-    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId16"/>
-    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId17"/>
-    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId18"/>
-    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId19"/>
-    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId20"/>
-    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId21"/>
-    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId22"/>
-    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId23"/>
-    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId24"/>
-    <sheet name="SingleLineGroups" sheetId="10" r:id="rId25"/>
-    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId26"/>
-    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId27"/>
-    <sheet name="InvalidTradingFees" sheetId="17" r:id="rId28"/>
-    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId29"/>
-    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId30"/>
-    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId31"/>
-    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId32"/>
-    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId33"/>
-    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId34"/>
-    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId35"/>
-    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId36"/>
-    <sheet name="InvalidTradingFeesSummary" sheetId="27" r:id="rId37"/>
-    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId38"/>
-    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId39"/>
-    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId40"/>
-    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId41"/>
-    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId42"/>
+    <sheet name="PriceExtraneousCharacters" sheetId="49" r:id="rId16"/>
+    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId17"/>
+    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId18"/>
+    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId19"/>
+    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId20"/>
+    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId21"/>
+    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId22"/>
+    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId23"/>
+    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId24"/>
+    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId25"/>
+    <sheet name="SingleLineGroups" sheetId="10" r:id="rId26"/>
+    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId27"/>
+    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId28"/>
+    <sheet name="InvalidTradingFees" sheetId="17" r:id="rId29"/>
+    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId30"/>
+    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId31"/>
+    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId32"/>
+    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId33"/>
+    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId34"/>
+    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId35"/>
+    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId36"/>
+    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId37"/>
+    <sheet name="InvalidTradingFeesSummary" sheetId="27" r:id="rId38"/>
+    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId39"/>
+    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId40"/>
+    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId41"/>
+    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId42"/>
+    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId43"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -180,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="28">
   <si>
     <t>BBAS3</t>
   </si>
@@ -261,6 +262,9 @@
   </si>
   <si>
     <t>l00</t>
+  </si>
+  <si>
+    <t>R$ l5,34</t>
   </si>
 </sst>
 </file>
@@ -1717,6 +1721,152 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8090141B-6275-4BED-906A-014C761C4DEF}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="18"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="24"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="3" t="e">
+        <f>D2*E2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G2" s="3" t="e">
+        <f>F2*0.0275%</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H2" s="3" t="e">
+        <f>F2*0.007%</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3" t="e">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF98C6E-C61C-4098-8811-20C737B2746F}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -2303,7 +2453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -2890,7 +3040,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F27D22B-36B9-402D-A19C-031FF2332945}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
@@ -3051,201 +3201,6 @@
       <c r="L3" s="3">
         <f>F3+G3+H3+I3+J3</f>
         <v>11605.599349999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7579CBF-C87A-40BF-91B5-CE83CDC20ECE}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B2" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
-        <v>11000</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.025%</f>
-        <v>2.75</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>11005.419349999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B3" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500</v>
-      </c>
-      <c r="E3" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" si="0"/>
-        <v>11600</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*0.025%</f>
-        <v>2.9</v>
-      </c>
-      <c r="H3" s="3">
-        <f>F3*0.005%</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>11605.599349999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="F4" s="7">
-        <f>SUM(F1:F3)</f>
-        <v>22600</v>
-      </c>
-      <c r="G4" s="7">
-        <v>5.65</v>
-      </c>
-      <c r="H4" s="7">
-        <f>SUM(H1:H3)</f>
-        <v>1.1300000000000001</v>
-      </c>
-      <c r="I4" s="7">
-        <f>SUM(I1:I3)</f>
-        <v>3.98</v>
-      </c>
-      <c r="J4" s="7">
-        <f>SUM(J1:J3)</f>
-        <v>0.25869999999999999</v>
-      </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7">
-        <f>SUM(L1:L3)</f>
-        <v>22611.018699999997</v>
       </c>
     </row>
   </sheetData>
@@ -3399,6 +3354,201 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7579CBF-C87A-40BF-91B5-CE83CDC20ECE}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="F4" s="7">
+        <f>SUM(F1:F3)</f>
+        <v>22600</v>
+      </c>
+      <c r="G4" s="7">
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f>SUM(H1:H3)</f>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f>SUM(I1:I3)</f>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f>SUM(J1:J3)</f>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7">
+        <f>SUM(L1:L3)</f>
+        <v>22611.018699999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384BB7C-DF07-4187-ADF0-23E50C2BA287}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -3700,7 +3850,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EC0A3F-FFB0-437C-B726-EA72E0B69675}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -3952,7 +4102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -4539,7 +4689,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
@@ -5066,7 +5216,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
@@ -5975,7 +6125,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -6231,7 +6381,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7618D34E-0B33-4181-8E63-6765777C5B7E}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
@@ -6523,7 +6673,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19EF43A-AB48-4760-8CB3-D62FBA7ABFD8}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6739,11 +6889,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
@@ -6935,222 +7085,6 @@
       <c r="L4" s="7">
         <f>-SUM(L2:L3)</f>
         <v>-22611.028699999995</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1583F5-F968-4E69-BCCF-4B8530FA0CCB}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B2" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
-        <v>11000</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.025%</f>
-        <v>2.75</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J2" s="3">
-        <v>0.12</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>11005.41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B3" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500</v>
-      </c>
-      <c r="E3" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" si="0"/>
-        <v>11600</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*0.025%</f>
-        <v>2.9</v>
-      </c>
-      <c r="H3" s="3">
-        <f>F3*0.005%</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" ref="J3" si="1">I3*6.5%</f>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>11605.599349999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7">
-        <f>-SUM(F2:F3)</f>
-        <v>-22600</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
-        <v>5.65</v>
-      </c>
-      <c r="H4" s="7">
-        <f t="shared" si="2"/>
-        <v>1.1300000000000001</v>
-      </c>
-      <c r="I4" s="7">
-        <f t="shared" si="2"/>
-        <v>3.98</v>
-      </c>
-      <c r="J4" s="7">
-        <f t="shared" si="2"/>
-        <v>0.24934999999999999</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="7">
-        <f>-SUM(L2:L3)</f>
-        <v>-22611.00935</v>
       </c>
       <c r="M4" s="6"/>
       <c r="R4" s="3"/>
@@ -7318,6 +7252,222 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1583F5-F968-4E69-BCCF-4B8530FA0CCB}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" ref="J3" si="1">I3*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.24934999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.00935</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -7616,7 +7766,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E3E40E-BCAE-41DB-80FC-C74D9CCDCD28}">
   <dimension ref="A1:AC13"/>
   <sheetViews>
@@ -8055,7 +8205,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F402F95-319A-4797-B7E1-F3EB07A82FDD}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8272,7 +8422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A590E594-CB91-4439-95F2-7F159495761F}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8489,7 +8639,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34F43A8-C89C-44C0-BF29-1F8134A0151F}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -8787,7 +8937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5AE87-00E8-4CF9-A517-EB6C0CA40610}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9003,7 +9153,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B51BEB4-905E-4036-959A-F9A0226AF070}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9220,7 +9370,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B7349E-D984-4817-800E-2EB4836D5B5D}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9437,7 +9587,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA65F892-A6B4-4288-ADB5-125D04E295EB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9626,223 +9776,6 @@
       <c r="J4" s="7">
         <f t="shared" si="2"/>
         <v>0.25869999999999999</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="7">
-        <f>-SUM(L2:L3)</f>
-        <v>-22611.018699999997</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421F9D80-1D28-4F3C-95F7-8DE9883A26F0}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B2" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
-        <v>11000</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.025%</f>
-        <v>2.75</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>11005.419349999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B3" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500</v>
-      </c>
-      <c r="E3" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" si="0"/>
-        <v>11600</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*0.025%</f>
-        <v>2.9</v>
-      </c>
-      <c r="H3" s="3">
-        <f>F3*0.005%</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>11605.599349999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7">
-        <f>-SUM(F2:F3)</f>
-        <v>-22600</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
-        <v>5.65</v>
-      </c>
-      <c r="H4" s="7">
-        <f>SUM(H2:H3)</f>
-        <v>1.1300000000000001</v>
-      </c>
-      <c r="I4" s="7">
-        <f>SUM(I2:I3)</f>
-        <v>3.98</v>
-      </c>
-      <c r="J4" s="7">
-        <f>SUM(J2:J3) + 0.03</f>
-        <v>0.28869999999999996</v>
       </c>
       <c r="K4" s="7">
         <f t="shared" si="2"/>
@@ -10015,6 +9948,223 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421F9D80-1D28-4F3C-95F7-8DE9883A26F0}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f>SUM(H2:H3)</f>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f>SUM(I2:I3)</f>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f>SUM(J2:J3) + 0.03</f>
+        <v>0.28869999999999996</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.018699999997</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D25BF0F-8645-49A4-A6C8-BE755BFA7BE7}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -10313,7 +10463,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4721B46-AB87-4CAA-ABF7-E48CFDA36C4A}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -10548,7 +10698,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF39107-DEBE-454A-A911-9FAC6360BB3B}">
   <dimension ref="A1:AC4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Prevents a 'BrokerageNotesWorksheetReader' from being created when a 'Price' has an invalid font color.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89918E47-2922-4B64-90AA-6BCF99CAF2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913A50B7-AA21-47C3-BB9B-F6727DF79F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="14" activeTab="15" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="15" activeTab="16" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="NotUsed" sheetId="2" r:id="rId1"/>
@@ -29,33 +29,34 @@
     <sheet name="PriceMissing" sheetId="47" r:id="rId14"/>
     <sheet name="PriceNegative" sheetId="48" r:id="rId15"/>
     <sheet name="PriceExtraneousCharacters" sheetId="49" r:id="rId16"/>
-    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId17"/>
-    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId18"/>
-    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId19"/>
-    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId20"/>
-    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId21"/>
-    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId22"/>
-    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId23"/>
-    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId24"/>
-    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId25"/>
-    <sheet name="SingleLineGroups" sheetId="10" r:id="rId26"/>
-    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId27"/>
-    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId28"/>
-    <sheet name="InvalidTradingFees" sheetId="17" r:id="rId29"/>
-    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId30"/>
-    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId31"/>
-    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId32"/>
-    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId33"/>
-    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId34"/>
-    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId35"/>
-    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId36"/>
-    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId37"/>
-    <sheet name="InvalidTradingFeesSummary" sheetId="27" r:id="rId38"/>
-    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId39"/>
-    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId40"/>
-    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId41"/>
-    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId42"/>
-    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId43"/>
+    <sheet name="PriceBlack" sheetId="50" r:id="rId17"/>
+    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId18"/>
+    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId19"/>
+    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId20"/>
+    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId21"/>
+    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId22"/>
+    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId23"/>
+    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId24"/>
+    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId25"/>
+    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId26"/>
+    <sheet name="SingleLineGroups" sheetId="10" r:id="rId27"/>
+    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId28"/>
+    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId29"/>
+    <sheet name="InvalidTradingFees" sheetId="17" r:id="rId30"/>
+    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId31"/>
+    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId32"/>
+    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId33"/>
+    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId34"/>
+    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId35"/>
+    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId36"/>
+    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId37"/>
+    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId38"/>
+    <sheet name="InvalidTradingFeesSummary" sheetId="27" r:id="rId39"/>
+    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId40"/>
+    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId41"/>
+    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId42"/>
+    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId43"/>
+    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId44"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -181,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="28">
   <si>
     <t>BBAS3</t>
   </si>
@@ -1724,6 +1725,152 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8090141B-6275-4BED-906A-014C761C4DEF}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="18"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="24"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="3" t="e">
+        <f>D2*E2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G2" s="3" t="e">
+        <f>F2*0.0275%</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H2" s="3" t="e">
+        <f>F2*0.007%</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3" t="e">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF4EE6C-614E-4BC3-897D-82A4742A252F}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
@@ -1816,20 +1963,20 @@
       <c r="D2" s="4">
         <v>100</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="3" t="e">
+      <c r="E2" s="13">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3">
         <f>D2*E2</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G2" s="3" t="e">
+        <v>1534</v>
+      </c>
+      <c r="G2" s="3">
         <f>F2*0.0275%</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H2" s="3" t="e">
+        <v>0.42185</v>
+      </c>
+      <c r="H2" s="3">
         <f>F2*0.007%</f>
-        <v>#VALUE!</v>
+        <v>0.10738000000000002</v>
       </c>
       <c r="I2" s="3">
         <v>15.99</v>
@@ -1840,9 +1987,9 @@
       <c r="K2" s="3">
         <v>0</v>
       </c>
-      <c r="L2" s="3" t="e">
+      <c r="L2" s="3">
         <f>F2+G2+H2+I2+J2</f>
-        <v>#VALUE!</v>
+        <v>1551.3192299999998</v>
       </c>
       <c r="M2" s="6"/>
       <c r="R2" s="3"/>
@@ -1866,7 +2013,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF98C6E-C61C-4098-8811-20C737B2746F}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -2453,7 +2600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -3033,175 +3180,6 @@
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F27D22B-36B9-402D-A19C-031FF2332945}">
-  <dimension ref="A1:AC3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B2" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
-        <v>11000</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.025%</f>
-        <v>2.75</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>11005.419349999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B3" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500</v>
-      </c>
-      <c r="E3" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" si="0"/>
-        <v>11600</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*0.025%</f>
-        <v>2.9</v>
-      </c>
-      <c r="H3" s="3">
-        <f>F3*0.005%</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>11605.599349999999</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3354,6 +3332,175 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F27D22B-36B9-402D-A19C-031FF2332945}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7579CBF-C87A-40BF-91B5-CE83CDC20ECE}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -3548,7 +3695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384BB7C-DF07-4187-ADF0-23E50C2BA287}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -3850,7 +3997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EC0A3F-FFB0-437C-B726-EA72E0B69675}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -4102,7 +4249,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F2574-DA99-472C-9CA5-5D547CFEDE2C}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -4689,7 +4836,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA113515-2383-42E9-8F47-B3DA9BDEB959}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
@@ -5216,7 +5363,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108430EF-5A58-4F6E-9535-CEBB2732DF3C}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
@@ -6125,7 +6272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7BE703-EA17-4053-8FF6-597C4A72A15B}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -6381,7 +6528,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7618D34E-0B33-4181-8E63-6765777C5B7E}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
@@ -6673,7 +6820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19EF43A-AB48-4760-8CB3-D62FBA7ABFD8}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -6853,222 +7000,6 @@
       <c r="H4" s="7">
         <f t="shared" si="2"/>
         <v>1.1300000000000001</v>
-      </c>
-      <c r="I4" s="7">
-        <f t="shared" si="2"/>
-        <v>3.98</v>
-      </c>
-      <c r="J4" s="7">
-        <f t="shared" si="2"/>
-        <v>0.25869999999999999</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="7">
-        <f>-SUM(L2:L3)</f>
-        <v>-22611.028699999995</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B2" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
-        <v>11000</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.025%</f>
-        <v>2.75</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>11005.429349999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B3" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500</v>
-      </c>
-      <c r="E3" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" si="0"/>
-        <v>11600</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*0.025%</f>
-        <v>2.9</v>
-      </c>
-      <c r="H3" s="3">
-        <f>F3*0.005%</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>11605.599349999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7">
-        <f>-SUM(F2:F3)</f>
-        <v>-22600</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
-        <v>5.65</v>
-      </c>
-      <c r="H4" s="7">
-        <f t="shared" si="2"/>
-        <v>1.1400000000000001</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" si="2"/>
@@ -7252,6 +7183,222 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7D75-65E8-45D7-9B4A-EEFFE176C4A2}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.429349999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1400000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>3.98</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.028699999995</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1583F5-F968-4E69-BCCF-4B8530FA0CCB}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -7467,7 +7614,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B8EB-77D4-4A9D-ADC2-145B24A5415F}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -7766,7 +7913,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E3E40E-BCAE-41DB-80FC-C74D9CCDCD28}">
   <dimension ref="A1:AC13"/>
   <sheetViews>
@@ -8205,7 +8352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F402F95-319A-4797-B7E1-F3EB07A82FDD}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8422,7 +8569,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A590E594-CB91-4439-95F2-7F159495761F}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -8639,7 +8786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34F43A8-C89C-44C0-BF29-1F8134A0151F}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -8937,7 +9084,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5AE87-00E8-4CF9-A517-EB6C0CA40610}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9153,7 +9300,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B51BEB4-905E-4036-959A-F9A0226AF070}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9370,7 +9517,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B7349E-D984-4817-800E-2EB4836D5B5D}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -9555,223 +9702,6 @@
       <c r="I4" s="7">
         <f t="shared" si="2"/>
         <v>3.98</v>
-      </c>
-      <c r="J4" s="7">
-        <f t="shared" si="2"/>
-        <v>0.25869999999999999</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="7">
-        <f>-SUM(L2:L3)</f>
-        <v>-22611.018699999997</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA65F892-A6B4-4288-ADB5-125D04E295EB}">
-  <dimension ref="A1:AC4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="Q108" sqref="Q108"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="16"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B2" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>400</v>
-      </c>
-      <c r="E2" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
-        <v>11000</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*0.025%</f>
-        <v>2.75</v>
-      </c>
-      <c r="H2" s="3">
-        <f>F2*0.005%</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f>F2+G2+H2+I2+J2</f>
-        <v>11005.419349999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44491</v>
-      </c>
-      <c r="B3" s="4">
-        <v>85060</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500</v>
-      </c>
-      <c r="E3" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" si="0"/>
-        <v>11600</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*0.025%</f>
-        <v>2.9</v>
-      </c>
-      <c r="H3" s="3">
-        <f>F3*0.005%</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.12934999999999999</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f>F3+G3+H3+I3+J3</f>
-        <v>11605.599349999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7">
-        <f>-SUM(F2:F3)</f>
-        <v>-22600</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
-        <v>5.65</v>
-      </c>
-      <c r="H4" s="7">
-        <f>SUM(H2:H3)</f>
-        <v>1.1300000000000001</v>
-      </c>
-      <c r="I4" s="7">
-        <f>SUM(I2:I3) - 0.03</f>
-        <v>3.95</v>
       </c>
       <c r="J4" s="7">
         <f t="shared" si="2"/>
@@ -9948,6 +9878,223 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA65F892-A6B4-4288-ADB5-125D04E295EB}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B2" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>400</v>
+      </c>
+      <c r="E2" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>11000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*0.025%</f>
+        <v>2.75</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.005%</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J3" si="1">I2*6.5%</f>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>11005.419349999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B3" s="4">
+        <v>85060</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*0.025%</f>
+        <v>2.9</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*0.005%</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12934999999999999</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>11605.599349999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <f>-SUM(F2:F3)</f>
+        <v>-22600</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
+        <v>5.65</v>
+      </c>
+      <c r="H4" s="7">
+        <f>SUM(H2:H3)</f>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f>SUM(I2:I3) - 0.03</f>
+        <v>3.95</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f>-SUM(L2:L3)</f>
+        <v>-22611.018699999997</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421F9D80-1D28-4F3C-95F7-8DE9883A26F0}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -10164,7 +10311,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D25BF0F-8645-49A4-A6C8-BE755BFA7BE7}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
@@ -10463,7 +10610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4721B46-AB87-4CAA-ABF7-E48CFDA36C4A}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
@@ -10698,7 +10845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF39107-DEBE-454A-A911-9FAC6360BB3B}">
   <dimension ref="A1:AC4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Prevents a 'BrokerageNotesWorksheetReader' from being created when a 'Volume' is missing.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/BrokerageNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913A50B7-AA21-47C3-BB9B-F6727DF79F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412F5EE4-1614-4D49-BF8B-42A07E119E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="15" activeTab="16" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" firstSheet="15" activeTab="17" xr2:uid="{51326E95-EE54-495F-AB8A-B57AD14A8498}"/>
   </bookViews>
   <sheets>
     <sheet name="NotUsed" sheetId="2" r:id="rId1"/>
@@ -30,33 +30,34 @@
     <sheet name="PriceNegative" sheetId="48" r:id="rId15"/>
     <sheet name="PriceExtraneousCharacters" sheetId="49" r:id="rId16"/>
     <sheet name="PriceBlack" sheetId="50" r:id="rId17"/>
-    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId18"/>
-    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId19"/>
-    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId20"/>
-    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId21"/>
-    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId22"/>
-    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId23"/>
-    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId24"/>
-    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId25"/>
-    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId26"/>
-    <sheet name="SingleLineGroups" sheetId="10" r:id="rId27"/>
-    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId28"/>
-    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId29"/>
-    <sheet name="InvalidTradingFees" sheetId="17" r:id="rId30"/>
-    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId31"/>
-    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId32"/>
-    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId33"/>
-    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId34"/>
-    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId35"/>
-    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId36"/>
-    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId37"/>
-    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId38"/>
-    <sheet name="InvalidTradingFeesSummary" sheetId="27" r:id="rId39"/>
-    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId40"/>
-    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId41"/>
-    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId42"/>
-    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId43"/>
-    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId44"/>
+    <sheet name="VolumeMissing" sheetId="51" r:id="rId18"/>
+    <sheet name="GroupWithDifferentTradingDates" sheetId="34" r:id="rId19"/>
+    <sheet name="GroupWithDifferentNoteNumbers" sheetId="12" r:id="rId20"/>
+    <sheet name="MultiLineGroupWithNoSummary" sheetId="25" r:id="rId21"/>
+    <sheet name="GroupWithInvalidSummary" sheetId="26" r:id="rId22"/>
+    <sheet name="LineWithDifferentFontColors" sheetId="13" r:id="rId23"/>
+    <sheet name="LineWithBlackFontColor" sheetId="14" r:id="rId24"/>
+    <sheet name="GroupsWithSameTradingDate&amp;Note" sheetId="7" r:id="rId25"/>
+    <sheet name="GroupsWithSummary" sheetId="8" r:id="rId26"/>
+    <sheet name="BuyingAndSellingOperations" sheetId="9" r:id="rId27"/>
+    <sheet name="SingleLineGroups" sheetId="10" r:id="rId28"/>
+    <sheet name="VolumeDoesNotMatchQtyTimesPrice" sheetId="15" r:id="rId29"/>
+    <sheet name="SettlementFeeNotVolumeTimesRate" sheetId="16" r:id="rId30"/>
+    <sheet name="InvalidTradingFees" sheetId="17" r:id="rId31"/>
+    <sheet name="InvalidServiceTax" sheetId="18" r:id="rId32"/>
+    <sheet name="InvalidIncomeTaxAtSource" sheetId="19" r:id="rId33"/>
+    <sheet name="_BugInGroupFormation_" sheetId="33" r:id="rId34"/>
+    <sheet name="IncomeTaxAtSourceNot$OnBuying" sheetId="20" r:id="rId35"/>
+    <sheet name="NonZeroIncomeTaxAtSourceBuying" sheetId="21" r:id="rId36"/>
+    <sheet name="InvalidTotalForSelling" sheetId="22" r:id="rId37"/>
+    <sheet name="InvalidTotalForBuying" sheetId="23" r:id="rId38"/>
+    <sheet name="InvalidSettlementFeeSummary" sheetId="24" r:id="rId39"/>
+    <sheet name="InvalidTradingFeesSummary" sheetId="27" r:id="rId40"/>
+    <sheet name="InvalidBrokerageSummary" sheetId="28" r:id="rId41"/>
+    <sheet name="InvalidServiceTaxSummary" sheetId="29" r:id="rId42"/>
+    <sheet name="InvalidIncomeTaxAtSourceSummary" sheetId="30" r:id="rId43"/>
+    <sheet name="InvalidVolumeSummaryMixedOps" sheetId="31" r:id="rId44"/>
+    <sheet name="InvalidTotalSummaryMixedOps" sheetId="32" r:id="rId45"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -182,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="28">
   <si>
     <t>BBAS3</t>
   </si>
@@ -1871,7 +1872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF4EE6C-614E-4BC3-897D-82A4742A252F}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q108" sqref="Q108"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
@@ -2014,6 +2015,149 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B1771A0-8299-4AE5-A539-1A7261885D0B}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="Q108" sqref="Q108"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="18"/>
+    <col min="18" max="18" width="10.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="24"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1662</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
+        <f>F2*0.0275%</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*0.007%</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15.99</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f>F2+G2+H2+I2+J2</f>
+        <v>16.79</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF98C6E-C61C-4098-8811-20C737B2746F}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
@@ -2156,593 +2300,6 @@
       </c>
       <c r="B3" s="4">
         <v>1662</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" s="3">
-        <v>25.19</v>
-      </c>
-      <c r="F3" s="3">
-        <f>D3*E3</f>
-        <v>5038</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G4" si="0">F3*0.0275%</f>
-        <v>1.3854500000000001</v>
-      </c>
-      <c r="H3" s="3">
-        <f t="shared" ref="H3:H4" si="1">F3*0.007%</f>
-        <v>0.35266000000000003</v>
-      </c>
-      <c r="I3" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J3" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f t="shared" ref="L3:L4" si="2">F3+G3+H3+I3+J3</f>
-        <v>5056.5281099999993</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>39757</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1662</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4">
-        <v>100</v>
-      </c>
-      <c r="E4" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="F4" s="3">
-        <f>D4*E4</f>
-        <v>2750</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" si="0"/>
-        <v>0.75625000000000009</v>
-      </c>
-      <c r="H4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.19250000000000003</v>
-      </c>
-      <c r="I4" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3">
-        <f t="shared" si="2"/>
-        <v>2767.73875</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-    <row r="5" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3">
-        <f>-SUM(F2:F4)</f>
-        <v>-9322</v>
-      </c>
-      <c r="G5" s="3">
-        <f t="shared" ref="G5:K5" si="3">SUM(G2:G4)</f>
-        <v>2.5635500000000002</v>
-      </c>
-      <c r="H5" s="3">
-        <f t="shared" si="3"/>
-        <v>0.65254000000000012</v>
-      </c>
-      <c r="I5" s="3">
-        <f t="shared" si="3"/>
-        <v>47.97</v>
-      </c>
-      <c r="J5" s="3">
-        <f t="shared" si="3"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K5" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L5" s="3">
-        <f>-SUM(L2:L4)</f>
-        <v>-9375.5860899999989</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-    </row>
-    <row r="6" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="6"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-    </row>
-    <row r="7" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>100</v>
-      </c>
-      <c r="E7" s="3">
-        <v>15.2</v>
-      </c>
-      <c r="F7" s="3">
-        <f>D7*E7</f>
-        <v>1520</v>
-      </c>
-      <c r="G7" s="3">
-        <f>F7*0.0275%</f>
-        <v>0.41800000000000004</v>
-      </c>
-      <c r="H7" s="3">
-        <f>F7*0.007%</f>
-        <v>0.10640000000000001</v>
-      </c>
-      <c r="I7" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K7" s="3">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3">
-        <f>F7+G7+H7+I7+J7</f>
-        <v>1537.3143999999998</v>
-      </c>
-      <c r="M7" s="6"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-    </row>
-    <row r="8" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>39758</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="4">
-        <v>100</v>
-      </c>
-      <c r="E8" s="3">
-        <v>7.69</v>
-      </c>
-      <c r="F8" s="3">
-        <f>D8*E8</f>
-        <v>769</v>
-      </c>
-      <c r="G8" s="3">
-        <f>F8*0.0275%</f>
-        <v>0.21147500000000002</v>
-      </c>
-      <c r="H8" s="3">
-        <f>F8*0.007%</f>
-        <v>5.3830000000000003E-2</v>
-      </c>
-      <c r="I8" s="3">
-        <v>15.99</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3">
-        <f>F8+G8+H8+I8+J8</f>
-        <v>786.05530499999986</v>
-      </c>
-      <c r="M8" s="6"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-    </row>
-    <row r="9" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3">
-        <f>-SUM(F7:F8)</f>
-        <v>-2289</v>
-      </c>
-      <c r="G9" s="3">
-        <f t="shared" ref="G9:K9" si="4">SUM(G7:G8)</f>
-        <v>0.62947500000000001</v>
-      </c>
-      <c r="H9" s="3">
-        <f t="shared" si="4"/>
-        <v>0.16023000000000001</v>
-      </c>
-      <c r="I9" s="3">
-        <f t="shared" si="4"/>
-        <v>31.98</v>
-      </c>
-      <c r="J9" s="3">
-        <f t="shared" si="4"/>
-        <v>1.6</v>
-      </c>
-      <c r="K9" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L9" s="3">
-        <f>-SUM(L7:L8)</f>
-        <v>-2323.3697049999996</v>
-      </c>
-      <c r="M9" s="6"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-    </row>
-    <row r="11" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
-        <v>39849</v>
-      </c>
-      <c r="B11" s="9">
-        <v>1319</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="9">
-        <v>100</v>
-      </c>
-      <c r="E11" s="8">
-        <v>31.5</v>
-      </c>
-      <c r="F11" s="8">
-        <f>D11*E11</f>
-        <v>3150</v>
-      </c>
-      <c r="G11" s="8">
-        <f>F11*0.0275%</f>
-        <v>0.86625000000000008</v>
-      </c>
-      <c r="H11" s="8">
-        <f>F11*0.007%</f>
-        <v>0.22050000000000003</v>
-      </c>
-      <c r="I11" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J11" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K11" s="8">
-        <v>0</v>
-      </c>
-      <c r="L11" s="8">
-        <f>F11-G11-H11-I11-J11</f>
-        <v>3132.1232500000001</v>
-      </c>
-      <c r="M11" s="6"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
-      <c r="AA11" s="8"/>
-      <c r="AB11" s="8"/>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-    </row>
-    <row r="13" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
-        <v>39853</v>
-      </c>
-      <c r="B13" s="9">
-        <v>1362</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="9">
-        <v>100</v>
-      </c>
-      <c r="E13" s="8">
-        <v>31.5</v>
-      </c>
-      <c r="F13" s="8">
-        <f>D13*E13</f>
-        <v>3150</v>
-      </c>
-      <c r="G13" s="8">
-        <f>F13*0.0275%</f>
-        <v>0.86625000000000008</v>
-      </c>
-      <c r="H13" s="8">
-        <f>F13*0.007%</f>
-        <v>0.22050000000000003</v>
-      </c>
-      <c r="I13" s="8">
-        <v>15.99</v>
-      </c>
-      <c r="J13" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K13" s="8">
-        <v>0</v>
-      </c>
-      <c r="L13" s="8">
-        <f>F13-G13-H13-I13-J13</f>
-        <v>3132.1232500000001</v>
-      </c>
-      <c r="M13" s="6"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="8"/>
-      <c r="AA13" s="8"/>
-      <c r="AB13" s="8"/>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB907D2-9E80-482F-8923-3F644E2641BF}">
-  <dimension ref="A1:AC14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/